<commit_message>
more type I error tests and prox/logprox checks
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CE24E2-7E65-4C7B-ADF3-A6158303E892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FFC19A-12CF-4DC1-B64A-299D40657714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="36">
   <si>
     <t>Population</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>100% NFE</t>
-  </si>
-  <si>
-    <t>R RAREsim</t>
   </si>
   <si>
     <t>120% fun, 100% syn</t>
@@ -170,13 +167,16 @@
     <t>Sequentially-
 --f_only 
 --s_only</t>
+  </si>
+  <si>
+    <t>─</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +191,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -213,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -224,6 +230,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -539,11 +548,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660476C5-A4B0-4780-BD43-FC7746B114D2}">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,7 +575,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -575,7 +584,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -613,43 +622,43 @@
         <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="R2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -666,16 +675,52 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="1">
         <v>0.14000000000000001</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:20" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -692,19 +737,52 @@
         <v>0.99</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" s="1">
         <v>0.21</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>20</v>
+      <c r="I4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
@@ -721,16 +799,52 @@
         <v>0.95</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5">
         <v>0.22</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
@@ -747,16 +861,52 @@
         <v>0.9</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" s="1">
         <v>0.23</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
@@ -773,16 +923,52 @@
         <v>0.8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H7" s="1">
         <v>0.26</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
@@ -799,16 +985,52 @@
         <v>0.99</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8">
         <v>0.16</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
@@ -825,16 +1047,52 @@
         <v>0.95</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" s="1">
         <v>0.15</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
@@ -851,16 +1109,52 @@
         <v>0.9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H10" s="1">
         <v>0.14000000000000001</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
@@ -877,16 +1171,52 @@
         <v>0.8</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H11" s="1">
         <v>0.13</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
@@ -903,13 +1233,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H12">
         <v>0.1</v>
@@ -965,13 +1295,13 @@
         <v>0.99</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H13">
         <v>0.21</v>
@@ -1027,13 +1357,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="H14">
         <v>7.0000000000000007E-2</v>
@@ -1089,16 +1419,52 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N15" t="s">
-        <v>20</v>
+        <v>34</v>
+      </c>
+      <c r="H15">
+        <v>0.11</v>
+      </c>
+      <c r="I15">
+        <v>0.15</v>
+      </c>
+      <c r="J15">
+        <v>0.06</v>
+      </c>
+      <c r="K15">
+        <v>0.11</v>
+      </c>
+      <c r="L15">
+        <v>0.09</v>
+      </c>
+      <c r="M15">
+        <v>0.03</v>
+      </c>
+      <c r="N15">
+        <v>0.03</v>
+      </c>
+      <c r="O15">
+        <v>0.06</v>
+      </c>
+      <c r="P15">
+        <v>0.06</v>
+      </c>
+      <c r="Q15">
+        <v>0.04</v>
+      </c>
+      <c r="R15">
+        <v>0.04</v>
+      </c>
+      <c r="S15">
+        <v>0.05</v>
+      </c>
+      <c r="T15">
+        <v>0.06</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -1115,16 +1481,55 @@
         <v>0.8</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="H16">
+        <v>0.03</v>
+      </c>
+      <c r="I16">
+        <v>0.06</v>
+      </c>
+      <c r="J16">
+        <v>0.02</v>
+      </c>
+      <c r="K16">
+        <v>0.05</v>
+      </c>
+      <c r="L16">
+        <v>0.05</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0.01</v>
+      </c>
+      <c r="O16">
+        <v>0.04</v>
+      </c>
+      <c r="P16">
+        <v>0.04</v>
+      </c>
+      <c r="Q16">
+        <v>0.02</v>
+      </c>
+      <c r="R16">
+        <v>0.01</v>
+      </c>
+      <c r="S16">
+        <v>0.02</v>
+      </c>
+      <c r="T16">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1138,13 +1543,57 @@
         <v>0.8</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>33</v>
+      <c r="H17">
+        <v>0.08</v>
+      </c>
+      <c r="I17">
+        <v>0.09</v>
+      </c>
+      <c r="J17">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K17">
+        <v>0.06</v>
+      </c>
+      <c r="L17">
+        <v>0.06</v>
+      </c>
+      <c r="M17">
+        <v>0.04</v>
+      </c>
+      <c r="N17">
+        <v>0.03</v>
+      </c>
+      <c r="O17">
+        <v>0.03</v>
+      </c>
+      <c r="P17">
+        <v>0.05</v>
+      </c>
+      <c r="Q17">
+        <v>0.02</v>
+      </c>
+      <c r="R17">
+        <v>0.04</v>
+      </c>
+      <c r="S17">
+        <v>0.08</v>
+      </c>
+      <c r="T17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R18" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new type I error results
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FFC19A-12CF-4DC1-B64A-299D40657714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A54741-FC34-4271-9C8F-8AA28201A63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="39">
   <si>
     <t>Population</t>
   </si>
@@ -170,6 +170,20 @@
   </si>
   <si>
     <t>─</t>
+  </si>
+  <si>
+    <t>NOTE: all results above this line used the version of proxECAT that was not filtering out common variants properly. All results below this line will have the correct version of proxECAT implemented</t>
+  </si>
+  <si>
+    <t>RAREsim-Python and RAREsim-R</t>
+  </si>
+  <si>
+    <t>1. Separately-
+--functional_bins 100%
+--synonymous_bins 100%
+2. Then-
+80% fun bins
+80% syn bins</t>
   </si>
 </sst>
 </file>
@@ -207,7 +221,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -215,11 +229,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -228,11 +251,24 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -548,11 +584,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660476C5-A4B0-4780-BD43-FC7746B114D2}">
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:AE24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V4" sqref="V4"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,7 +598,7 @@
     <col min="4" max="4" width="14.5546875" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="9.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" customWidth="1"/>
     <col min="13" max="13" width="17.21875" customWidth="1"/>
     <col min="14" max="14" width="17.77734375" customWidth="1"/>
     <col min="15" max="15" width="17.109375" customWidth="1"/>
@@ -574,30 +610,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -686,40 +722,40 @@
       <c r="H3" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T3" s="5" t="s">
+      <c r="I3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T3" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -748,40 +784,40 @@
       <c r="H4" s="1">
         <v>0.21</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T4" s="5" t="s">
+      <c r="I4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T4" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -810,40 +846,40 @@
       <c r="H5">
         <v>0.22</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T5" s="5" t="s">
+      <c r="I5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T5" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -872,40 +908,40 @@
       <c r="H6" s="1">
         <v>0.23</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="S6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T6" s="5" t="s">
+      <c r="I6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T6" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -934,40 +970,40 @@
       <c r="H7" s="1">
         <v>0.26</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="S7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T7" s="5" t="s">
+      <c r="I7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T7" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -996,40 +1032,40 @@
       <c r="H8">
         <v>0.16</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="S8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T8" s="5" t="s">
+      <c r="I8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T8" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1058,40 +1094,40 @@
       <c r="H9" s="1">
         <v>0.15</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="S9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T9" s="5" t="s">
+      <c r="I9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T9" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1120,40 +1156,40 @@
       <c r="H10" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="S10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T10" s="5" t="s">
+      <c r="I10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T10" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1182,40 +1218,40 @@
       <c r="H11" s="1">
         <v>0.13</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="S11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T11" s="5" t="s">
+      <c r="I11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T11" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1529,7 +1565,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1590,9 +1626,338 @@
       <c r="T17">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="R18" t="s">
+      <c r="V17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="J18" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="K18" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="L18" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="M18" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="N18" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="O18" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="P18" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="R18" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="S18" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="T18" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="7"/>
+      <c r="AE18" s="7"/>
+    </row>
+    <row r="19" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19">
+        <v>0.02</v>
+      </c>
+      <c r="I19">
+        <v>0.05</v>
+      </c>
+      <c r="J19">
+        <v>0.02</v>
+      </c>
+      <c r="K19">
+        <v>0.05</v>
+      </c>
+      <c r="L19">
+        <v>0.05</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0.01</v>
+      </c>
+      <c r="O19">
+        <v>0.04</v>
+      </c>
+      <c r="P19">
+        <v>0.04</v>
+      </c>
+      <c r="Q19">
+        <v>0.02</v>
+      </c>
+      <c r="R19">
+        <v>0.01</v>
+      </c>
+      <c r="S19">
+        <v>0.02</v>
+      </c>
+      <c r="T19">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="C20" s="10">
+        <v>1</v>
+      </c>
+      <c r="D20" s="10">
+        <v>1</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20">
+        <v>0.03</v>
+      </c>
+      <c r="I20">
+        <v>0.06</v>
+      </c>
+      <c r="J20">
+        <v>0.03</v>
+      </c>
+      <c r="K20">
+        <v>0.06</v>
+      </c>
+      <c r="L20">
+        <v>0.06</v>
+      </c>
+      <c r="M20">
+        <v>0.02</v>
+      </c>
+      <c r="N20">
+        <v>0.02</v>
+      </c>
+      <c r="O20">
+        <v>0.03</v>
+      </c>
+      <c r="P20">
+        <v>0.03</v>
+      </c>
+      <c r="Q20">
+        <v>0.01</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0.03</v>
+      </c>
+      <c r="T20">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="C21" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21">
+        <v>0.04</v>
+      </c>
+      <c r="I21">
+        <v>0.05</v>
+      </c>
+      <c r="J21">
+        <v>0.04</v>
+      </c>
+      <c r="K21">
+        <v>0.05</v>
+      </c>
+      <c r="L21">
+        <v>0.05</v>
+      </c>
+      <c r="M21">
+        <v>0.03</v>
+      </c>
+      <c r="N21">
+        <v>0.02</v>
+      </c>
+      <c r="O21">
+        <v>0.02</v>
+      </c>
+      <c r="P21">
+        <v>0.04</v>
+      </c>
+      <c r="Q21">
+        <v>0.02</v>
+      </c>
+      <c r="R21">
+        <v>0.02</v>
+      </c>
+      <c r="S21">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T21">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="C22" s="10">
+        <v>1</v>
+      </c>
+      <c r="D22" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I22">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J22">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K22">
+        <v>0.08</v>
+      </c>
+      <c r="L22">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M22">
+        <v>0.02</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0.99</v>
+      </c>
+      <c r="P22">
+        <v>0.83</v>
+      </c>
+      <c r="Q22">
+        <v>0.03</v>
+      </c>
+      <c r="R22">
+        <v>0.03</v>
+      </c>
+      <c r="S22">
+        <v>0.82</v>
+      </c>
+      <c r="T22">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="R24" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more type I error plots
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A54741-FC34-4271-9C8F-8AA28201A63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52AD292-3FA8-42B5-9AC8-47FA720871B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="44">
   <si>
     <t>Population</t>
   </si>
@@ -99,9 +99,6 @@
     <t>iECAT-O 
 Internal + External
 (Syn Variants Only)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Separately-
@@ -184,6 +181,41 @@
 2. Then-
 80% fun bins
 80% syn bins</t>
+  </si>
+  <si>
+    <t>1. Separately-
+--functional_bins 100%
+--synonymous_bins 100%
+2. Then-
+90% fun bins
+90% syn bins</t>
+  </si>
+  <si>
+    <t>SKAT-O Internal
+(Syn Variants Only)</t>
+  </si>
+  <si>
+    <t>SKAT-O External (Syn Variants Only)</t>
+  </si>
+  <si>
+    <t>SKAT-O 
+Internal + External (Syn Variants Only)</t>
+  </si>
+  <si>
+    <t>1. Separately-
+--functional_bins 100%
+--synonymous_bins 100%
+2. Then-
+95% fun bins
+95% syn bins</t>
+  </si>
+  <si>
+    <t>1. Separately-
+--functional_bins 100%
+--synonymous_bins 100%
+2. Then-
+99% fun bins
+99% syn bins</t>
   </si>
 </sst>
 </file>
@@ -242,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -254,9 +286,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -264,11 +293,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -584,11 +610,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660476C5-A4B0-4780-BD43-FC7746B114D2}">
-  <dimension ref="A1:AE24"/>
+  <dimension ref="A1:AE33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,30 +636,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -688,13 +714,13 @@
         <v>18</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -711,52 +737,52 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" s="1">
         <v>0.14000000000000001</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:20" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -773,52 +799,52 @@
         <v>0.99</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="1">
         <v>0.21</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
@@ -835,52 +861,52 @@
         <v>0.95</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5">
         <v>0.22</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
@@ -897,52 +923,52 @@
         <v>0.9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="1">
         <v>0.23</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
@@ -959,52 +985,52 @@
         <v>0.8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="1">
         <v>0.26</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
@@ -1021,52 +1047,52 @@
         <v>0.99</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8">
         <v>0.16</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
@@ -1083,52 +1109,52 @@
         <v>0.95</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9" s="1">
         <v>0.15</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
@@ -1145,52 +1171,52 @@
         <v>0.9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H10" s="1">
         <v>0.14000000000000001</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
@@ -1207,52 +1233,52 @@
         <v>0.8</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H11" s="1">
         <v>0.13</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
@@ -1269,13 +1295,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H12">
         <v>0.1</v>
@@ -1331,13 +1357,13 @@
         <v>0.99</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13">
         <v>0.21</v>
@@ -1393,13 +1419,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="H14">
         <v>7.0000000000000007E-2</v>
@@ -1455,13 +1481,13 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H15">
         <v>0.11</v>
@@ -1517,13 +1543,13 @@
         <v>0.8</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H16">
         <v>0.03</v>
@@ -1579,13 +1605,13 @@
         <v>0.8</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="H17">
         <v>0.08</v>
@@ -1627,103 +1653,103 @@
         <v>0.06</v>
       </c>
       <c r="V17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:31" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="C18" s="8">
-        <v>1</v>
-      </c>
-      <c r="D18" s="8">
-        <v>1</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="6">
+      <c r="A18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="5">
         <v>0.06</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="5">
         <v>0.05</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="5">
         <v>0.06</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="5">
         <v>0.04</v>
       </c>
-      <c r="L18" s="6">
+      <c r="L18" s="5">
         <v>0.05</v>
       </c>
-      <c r="M18" s="6">
-        <v>0.02</v>
-      </c>
-      <c r="N18" s="6">
-        <v>0.03</v>
-      </c>
-      <c r="O18" s="6">
-        <v>0.02</v>
-      </c>
-      <c r="P18" s="6">
-        <v>0.02</v>
-      </c>
-      <c r="Q18" s="6">
-        <v>0.02</v>
-      </c>
-      <c r="R18" s="6">
-        <v>0.03</v>
-      </c>
-      <c r="S18" s="6">
-        <v>0.03</v>
-      </c>
-      <c r="T18" s="6">
+      <c r="M18" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="N18" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="O18" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="P18" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="R18" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="S18" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="T18" s="5">
         <v>0.06</v>
       </c>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="7"/>
-      <c r="Z18" s="7"/>
-      <c r="AA18" s="7"/>
-      <c r="AB18" s="7"/>
-      <c r="AC18" s="7"/>
-      <c r="AD18" s="7"/>
-      <c r="AE18" s="7"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="6"/>
+      <c r="AD18" s="6"/>
+      <c r="AE18" s="6"/>
     </row>
     <row r="19" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="C19" s="10">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C19" s="3">
         <v>0.8</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="3">
         <v>0.8</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>33</v>
+      <c r="E19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="H19">
         <v>0.02</v>
@@ -1766,26 +1792,26 @@
       </c>
     </row>
     <row r="20" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="C20" s="10">
-        <v>1</v>
-      </c>
-      <c r="D20" s="10">
-        <v>1</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="9" t="s">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>30</v>
       </c>
       <c r="H20">
         <v>0.03</v>
@@ -1828,26 +1854,26 @@
       </c>
     </row>
     <row r="21" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="C21" s="10">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C21" s="3">
         <v>0.8</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="3">
         <v>0.8</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" s="9" t="s">
+      <c r="E21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>30</v>
       </c>
       <c r="H21">
         <v>0.04</v>
@@ -1890,26 +1916,26 @@
       </c>
     </row>
     <row r="22" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="C22" s="10">
-        <v>1</v>
-      </c>
-      <c r="D22" s="10">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
         <v>0.8</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>38</v>
       </c>
       <c r="H22">
         <v>0.14000000000000001</v>
@@ -1951,14 +1977,686 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="R24" t="s">
-        <v>19</v>
+    <row r="23" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23">
+        <v>0.02</v>
+      </c>
+      <c r="I23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J23">
+        <v>0.02</v>
+      </c>
+      <c r="K23">
+        <v>0.06</v>
+      </c>
+      <c r="L23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M23">
+        <v>0.01</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0.02</v>
+      </c>
+      <c r="P23">
+        <v>0.03</v>
+      </c>
+      <c r="Q23">
+        <v>0.03</v>
+      </c>
+      <c r="R23">
+        <v>0.03</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24">
+        <v>0.03</v>
+      </c>
+      <c r="I24">
+        <v>0.08</v>
+      </c>
+      <c r="J24">
+        <v>0.03</v>
+      </c>
+      <c r="K24">
+        <v>0.1</v>
+      </c>
+      <c r="L24">
+        <v>0.08</v>
+      </c>
+      <c r="M24">
+        <v>0.01</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0.02</v>
+      </c>
+      <c r="P24">
+        <v>0.04</v>
+      </c>
+      <c r="Q24">
+        <v>0.03</v>
+      </c>
+      <c r="R24">
+        <v>0.03</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25">
+        <v>0.13</v>
+      </c>
+      <c r="I25">
+        <v>0.03</v>
+      </c>
+      <c r="J25">
+        <v>0.13</v>
+      </c>
+      <c r="K25">
+        <v>0.03</v>
+      </c>
+      <c r="L25">
+        <v>0.03</v>
+      </c>
+      <c r="M25">
+        <v>0.03</v>
+      </c>
+      <c r="N25">
+        <v>0.02</v>
+      </c>
+      <c r="O25">
+        <v>0.59</v>
+      </c>
+      <c r="P25">
+        <v>0.38</v>
+      </c>
+      <c r="Q25">
+        <v>0.01</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0.63</v>
+      </c>
+      <c r="T25">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26">
+        <v>0.05</v>
+      </c>
+      <c r="I26">
+        <v>0.03</v>
+      </c>
+      <c r="J26">
+        <v>0.05</v>
+      </c>
+      <c r="K26">
+        <v>0.03</v>
+      </c>
+      <c r="L26">
+        <v>0.03</v>
+      </c>
+      <c r="M26">
+        <v>0.03</v>
+      </c>
+      <c r="N26">
+        <v>0.02</v>
+      </c>
+      <c r="O26">
+        <v>0.06</v>
+      </c>
+      <c r="P26">
+        <v>0.06</v>
+      </c>
+      <c r="Q26">
+        <v>0.01</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0.04</v>
+      </c>
+      <c r="T26">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27">
+        <v>0.04</v>
+      </c>
+      <c r="I27">
+        <v>0.01</v>
+      </c>
+      <c r="J27">
+        <v>0.04</v>
+      </c>
+      <c r="K27">
+        <v>0.02</v>
+      </c>
+      <c r="L27">
+        <v>0.01</v>
+      </c>
+      <c r="M27">
+        <v>0.03</v>
+      </c>
+      <c r="N27">
+        <v>0.01</v>
+      </c>
+      <c r="O27">
+        <v>0.05</v>
+      </c>
+      <c r="P27">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q27">
+        <v>0.02</v>
+      </c>
+      <c r="R27">
+        <v>0.03</v>
+      </c>
+      <c r="S27">
+        <v>0.03</v>
+      </c>
+      <c r="T27">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I28">
+        <v>0.03</v>
+      </c>
+      <c r="J28">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K28">
+        <v>0.03</v>
+      </c>
+      <c r="L28">
+        <v>0.03</v>
+      </c>
+      <c r="M28">
+        <v>0.05</v>
+      </c>
+      <c r="N28">
+        <v>0.03</v>
+      </c>
+      <c r="O28">
+        <v>0.45</v>
+      </c>
+      <c r="P28">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="Q28">
+        <v>0.02</v>
+      </c>
+      <c r="R28">
+        <v>0.02</v>
+      </c>
+      <c r="S28">
+        <v>0.41</v>
+      </c>
+      <c r="T28">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29">
+        <v>0.04</v>
+      </c>
+      <c r="I29">
+        <v>0.03</v>
+      </c>
+      <c r="J29">
+        <v>0.04</v>
+      </c>
+      <c r="K29">
+        <v>0.03</v>
+      </c>
+      <c r="L29">
+        <v>0.03</v>
+      </c>
+      <c r="M29">
+        <v>0.05</v>
+      </c>
+      <c r="N29">
+        <v>0.03</v>
+      </c>
+      <c r="O29">
+        <v>0.03</v>
+      </c>
+      <c r="P29">
+        <v>0.04</v>
+      </c>
+      <c r="Q29">
+        <v>0.02</v>
+      </c>
+      <c r="R29">
+        <v>0.02</v>
+      </c>
+      <c r="S29">
+        <v>0.04</v>
+      </c>
+      <c r="T29">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H30">
+        <v>0.02</v>
+      </c>
+      <c r="I30">
+        <v>0.02</v>
+      </c>
+      <c r="J30">
+        <v>0.02</v>
+      </c>
+      <c r="K30">
+        <v>0.03</v>
+      </c>
+      <c r="L30">
+        <v>0.02</v>
+      </c>
+      <c r="M30">
+        <v>0.03</v>
+      </c>
+      <c r="N30">
+        <v>0.03</v>
+      </c>
+      <c r="O30">
+        <v>0.05</v>
+      </c>
+      <c r="P30">
+        <v>0.05</v>
+      </c>
+      <c r="Q30">
+        <v>0.02</v>
+      </c>
+      <c r="R30">
+        <v>0.02</v>
+      </c>
+      <c r="S30">
+        <v>0.04</v>
+      </c>
+      <c r="T30">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H31">
+        <v>0.13</v>
+      </c>
+      <c r="I31">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J31">
+        <v>0.13</v>
+      </c>
+      <c r="K31">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L31">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M31">
+        <v>0.03</v>
+      </c>
+      <c r="N31">
+        <v>0.02</v>
+      </c>
+      <c r="O31">
+        <v>0.36</v>
+      </c>
+      <c r="P31">
+        <v>0.18</v>
+      </c>
+      <c r="Q31">
+        <v>0.01</v>
+      </c>
+      <c r="R31">
+        <v>0.02</v>
+      </c>
+      <c r="S31">
+        <v>0.27</v>
+      </c>
+      <c r="T31">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H32">
+        <v>0.03</v>
+      </c>
+      <c r="I32">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J32">
+        <v>0.03</v>
+      </c>
+      <c r="K32">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L32">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M32">
+        <v>0.02</v>
+      </c>
+      <c r="N32">
+        <v>0.02</v>
+      </c>
+      <c r="O32">
+        <v>0.01</v>
+      </c>
+      <c r="P32">
+        <v>0.01</v>
+      </c>
+      <c r="Q32">
+        <v>0.01</v>
+      </c>
+      <c r="R32">
+        <v>0.03</v>
+      </c>
+      <c r="S32">
+        <v>0.02</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H33">
+        <v>0.02</v>
+      </c>
+      <c r="I33">
+        <v>0.09</v>
+      </c>
+      <c r="J33">
+        <v>0.02</v>
+      </c>
+      <c r="K33">
+        <v>0.09</v>
+      </c>
+      <c r="L33">
+        <v>0.09</v>
+      </c>
+      <c r="M33">
+        <v>0.03</v>
+      </c>
+      <c r="N33">
+        <v>0.02</v>
+      </c>
+      <c r="O33">
+        <v>0.01</v>
+      </c>
+      <c r="P33">
+        <v>0.01</v>
+      </c>
+      <c r="Q33">
+        <v>0.01</v>
+      </c>
+      <c r="R33">
+        <v>0.02</v>
+      </c>
+      <c r="S33">
+        <v>0.01</v>
+      </c>
+      <c r="T33">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
simulation updates and new pipeline
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52AD292-3FA8-42B5-9AC8-47FA720871B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9ACBC85-A6B6-47D5-9EA7-C29974A35CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="47">
   <si>
     <t>Population</t>
   </si>
@@ -216,6 +216,21 @@
 2. Then-
 99% fun bins
 99% syn bins</t>
+  </si>
+  <si>
+    <t>Separately-
+--functional_bins 99%
+--synonymous_bins 99%</t>
+  </si>
+  <si>
+    <t>Separately-
+--functional_bins 100%
+--synonymous_bins 100%</t>
+  </si>
+  <si>
+    <t>Separately-
+--functional_bins 80%
+--synonymous_bins 80%</t>
   </si>
 </sst>
 </file>
@@ -610,11 +625,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660476C5-A4B0-4780-BD43-FC7746B114D2}">
-  <dimension ref="A1:AE33"/>
+  <dimension ref="A1:AE34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,10 +708,10 @@
         <v>11</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>14</v>
@@ -1811,7 +1826,7 @@
         <v>28</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="H20">
         <v>0.03</v>
@@ -1873,7 +1888,7 @@
         <v>28</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="H21">
         <v>0.04</v>
@@ -2657,6 +2672,68 @@
       </c>
       <c r="T33">
         <v>0.01</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H34">
+        <v>0.05</v>
+      </c>
+      <c r="I34">
+        <v>0.06</v>
+      </c>
+      <c r="J34">
+        <v>0.04</v>
+      </c>
+      <c r="K34">
+        <v>0.06</v>
+      </c>
+      <c r="L34">
+        <v>0.06</v>
+      </c>
+      <c r="M34">
+        <v>0.03</v>
+      </c>
+      <c r="N34">
+        <v>0.04</v>
+      </c>
+      <c r="O34">
+        <v>0.03</v>
+      </c>
+      <c r="P34">
+        <v>0.03</v>
+      </c>
+      <c r="Q34">
+        <v>0.08</v>
+      </c>
+      <c r="R34">
+        <v>0.04</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add rows of zeros back into pruned haplotype
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221C5287-3DBF-482B-9B41-7B18076EB3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46789F30-2647-4D02-84A4-80251A750371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="60">
   <si>
     <t>Population</t>
   </si>
@@ -295,6 +295,9 @@
 --f_only 100%
 2. Sequentially-RAREsim R
 100% syn bins</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -381,14 +384,14 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,11 +706,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660476C5-A4B0-4780-BD43-FC7746B114D2}">
-  <dimension ref="A1:AG35"/>
+  <dimension ref="A1:AG38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,31 +734,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -829,7 +832,7 @@
       </c>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>45189</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -897,7 +900,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>45182</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -965,7 +968,7 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <v>45184</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1033,7 +1036,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <v>45184</v>
       </c>
       <c r="B6" t="s">
@@ -1101,7 +1104,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>45182</v>
       </c>
       <c r="B7" t="s">
@@ -1169,7 +1172,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+      <c r="A8" s="9">
         <v>45188</v>
       </c>
       <c r="B8" t="s">
@@ -1237,7 +1240,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+      <c r="A9" s="9">
         <v>45188</v>
       </c>
       <c r="B9" t="s">
@@ -1305,7 +1308,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+      <c r="A10" s="9">
         <v>45188</v>
       </c>
       <c r="B10" t="s">
@@ -1373,7 +1376,7 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+      <c r="A11" s="9">
         <v>45188</v>
       </c>
       <c r="B11" t="s">
@@ -1441,7 +1444,7 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
+      <c r="A12" s="9">
         <v>45189</v>
       </c>
       <c r="B12" t="s">
@@ -1509,7 +1512,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
+      <c r="A13" s="9">
         <v>45189</v>
       </c>
       <c r="B13" t="s">
@@ -1577,7 +1580,7 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
+      <c r="A14" s="9">
         <v>45190</v>
       </c>
       <c r="B14" t="s">
@@ -1645,7 +1648,7 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
+      <c r="A15" s="9">
         <v>45194</v>
       </c>
       <c r="B15" t="s">
@@ -1713,7 +1716,7 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
+      <c r="A16" s="9">
         <v>45194</v>
       </c>
       <c r="B16" t="s">
@@ -1781,7 +1784,7 @@
       </c>
     </row>
     <row r="17" spans="1:33" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="11">
+      <c r="A17" s="10">
         <v>45194</v>
       </c>
       <c r="B17" t="s">
@@ -1852,7 +1855,7 @@
       </c>
     </row>
     <row r="18" spans="1:33" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="9">
+      <c r="A18" s="8">
         <v>45196</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -1931,7 +1934,7 @@
       <c r="AG18" s="6"/>
     </row>
     <row r="19" spans="1:33" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
+      <c r="A19" s="9">
         <v>45196</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1999,7 +2002,7 @@
       </c>
     </row>
     <row r="20" spans="1:33" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
+      <c r="A20" s="9">
         <v>45196</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2067,7 +2070,7 @@
       </c>
     </row>
     <row r="21" spans="1:33" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
+      <c r="A21" s="9">
         <v>45196</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2135,7 +2138,7 @@
       </c>
     </row>
     <row r="22" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="10">
+      <c r="A22" s="9">
         <v>45196</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2203,7 +2206,7 @@
       </c>
     </row>
     <row r="23" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="10">
+      <c r="A23" s="9">
         <v>45197</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2271,7 +2274,7 @@
       </c>
     </row>
     <row r="24" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="10">
+      <c r="A24" s="9">
         <v>45197</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -2339,7 +2342,7 @@
       </c>
     </row>
     <row r="25" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="10">
+      <c r="A25" s="9">
         <v>45197</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -2407,7 +2410,7 @@
       </c>
     </row>
     <row r="26" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="10">
+      <c r="A26" s="9">
         <v>45197</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2475,7 +2478,7 @@
       </c>
     </row>
     <row r="27" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="10">
+      <c r="A27" s="9">
         <v>45197</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2543,7 +2546,7 @@
       </c>
     </row>
     <row r="28" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="10">
+      <c r="A28" s="9">
         <v>45198</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2611,7 +2614,7 @@
       </c>
     </row>
     <row r="29" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="10">
+      <c r="A29" s="9">
         <v>45198</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2679,7 +2682,7 @@
       </c>
     </row>
     <row r="30" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="10">
+      <c r="A30" s="9">
         <v>45198</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2747,7 +2750,7 @@
       </c>
     </row>
     <row r="31" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="10">
+      <c r="A31" s="9">
         <v>45198</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2815,7 +2818,7 @@
       </c>
     </row>
     <row r="32" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="10">
+      <c r="A32" s="9">
         <v>45198</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2883,7 +2886,7 @@
       </c>
     </row>
     <row r="33" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="10">
+      <c r="A33" s="9">
         <v>45198</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -2951,7 +2954,7 @@
       </c>
     </row>
     <row r="34" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="10">
+      <c r="A34" s="9">
         <v>45198</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -3019,6 +3022,9 @@
       </c>
     </row>
     <row r="35" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+      <c r="A35" s="9">
+        <v>45203</v>
+      </c>
       <c r="B35" s="1" t="s">
         <v>7</v>
       </c>
@@ -3042,6 +3048,50 @@
       </c>
       <c r="I35" s="1" t="s">
         <v>58</v>
+      </c>
+      <c r="J35">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K35">
+        <v>0.04</v>
+      </c>
+      <c r="L35">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M35">
+        <v>0.04</v>
+      </c>
+      <c r="N35">
+        <v>0.04</v>
+      </c>
+      <c r="O35">
+        <v>0.05</v>
+      </c>
+      <c r="P35">
+        <v>0.03</v>
+      </c>
+      <c r="Q35">
+        <v>0.03</v>
+      </c>
+      <c r="R35">
+        <v>0.03</v>
+      </c>
+      <c r="S35">
+        <v>0.03</v>
+      </c>
+      <c r="T35">
+        <v>0.02</v>
+      </c>
+      <c r="U35">
+        <v>0.03</v>
+      </c>
+      <c r="V35">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="U38" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
100v80 results from RAREsim v2.1.1 only pipeline
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46789F30-2647-4D02-84A4-80251A750371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3C381F-07EA-4B50-B6A6-C548470A5D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="60">
   <si>
     <t>Population</t>
   </si>
@@ -297,7 +297,14 @@
 100% syn bins</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>1. Separately-RAREsim v2.1.1
+--functional_bins 100%
+--synonymous_bins 100%
+2. RAREsim v2.1.1: Convert 100% pruned hap file to .sm file using convert.py
+3. Separately-RAREsim v2.1.1
+--functional_bins 80% 6 MAC BINS
+--synonymous_bins 80% 6 MAC BINS
+4. R: add pruned variants back in as rows of 0 and extract datasets</t>
   </si>
 </sst>
 </file>
@@ -709,8 +716,8 @@
   <dimension ref="A1:AG38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+      <pane ySplit="2" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,7 +728,7 @@
     <col min="5" max="6" width="14.5546875" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" customWidth="1"/>
     <col min="8" max="8" width="9.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="32.44140625" customWidth="1"/>
     <col min="15" max="15" width="17.21875" customWidth="1"/>
     <col min="16" max="16" width="17.77734375" customWidth="1"/>
     <col min="17" max="17" width="17.109375" customWidth="1"/>
@@ -3089,9 +3096,208 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="U38" t="s">
+    <row r="36" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="9">
+        <v>45205</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>59</v>
+      </c>
+      <c r="J36">
+        <v>0.02</v>
+      </c>
+      <c r="K36">
+        <v>0.03</v>
+      </c>
+      <c r="L36">
+        <v>0.02</v>
+      </c>
+      <c r="M36">
+        <v>0.03</v>
+      </c>
+      <c r="N36">
+        <v>0.03</v>
+      </c>
+      <c r="O36">
+        <v>0.04</v>
+      </c>
+      <c r="P36">
+        <v>0.03</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>0.01</v>
+      </c>
+      <c r="S36">
+        <v>0.01</v>
+      </c>
+      <c r="T36">
+        <v>0.03</v>
+      </c>
+      <c r="U36">
+        <v>0.04</v>
+      </c>
+      <c r="V36">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="9">
+        <v>45205</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J37">
+        <v>0.22</v>
+      </c>
+      <c r="K37">
+        <v>0.03</v>
+      </c>
+      <c r="L37">
+        <v>0.22</v>
+      </c>
+      <c r="M37">
+        <v>0.03</v>
+      </c>
+      <c r="N37">
+        <v>0.03</v>
+      </c>
+      <c r="O37">
+        <v>0.03</v>
+      </c>
+      <c r="P37">
+        <v>0.03</v>
+      </c>
+      <c r="Q37">
+        <v>0.97</v>
+      </c>
+      <c r="R37">
+        <v>0.84</v>
+      </c>
+      <c r="S37">
+        <v>0.02</v>
+      </c>
+      <c r="T37">
+        <v>0.02</v>
+      </c>
+      <c r="U37">
+        <v>0.79</v>
+      </c>
+      <c r="V37">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="9">
+        <v>45205</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J38">
+        <v>0.01</v>
+      </c>
+      <c r="K38">
+        <v>0.04</v>
+      </c>
+      <c r="L38">
+        <v>0.01</v>
+      </c>
+      <c r="M38">
+        <v>0.03</v>
+      </c>
+      <c r="N38">
+        <v>0.04</v>
+      </c>
+      <c r="O38">
+        <v>0.04</v>
+      </c>
+      <c r="P38">
+        <v>0.04</v>
+      </c>
+      <c r="Q38">
+        <v>0.02</v>
+      </c>
+      <c r="R38">
+        <v>0.02</v>
+      </c>
+      <c r="S38">
+        <v>0.01</v>
+      </c>
+      <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <v>0.01</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
t1e for 100v99 R pruning pipeline
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C51F95-11DA-4415-BBED-8E27A08A9D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E01379-5FFB-4DA0-A254-C3DF91200D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="64">
   <si>
     <t>Population</t>
   </si>
@@ -328,6 +328,16 @@
 80% fun bins
 80% syn bins
 4. Extract datasets from 80% pruned haplotype</t>
+  </si>
+  <si>
+    <t>1. Separately-R
+100% fun bins
+100% syn bins
+2. Extract datasets from 100% pruned haplotype
+3. Separately-R
+99% fun bins
+99% syn bins
+4. Extract datasets from 99% pruned haplotype</t>
   </si>
 </sst>
 </file>
@@ -736,16 +746,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660476C5-A4B0-4780-BD43-FC7746B114D2}">
-  <dimension ref="A1:AG44"/>
+  <dimension ref="A1:AG47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q53" sqref="Q53"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O48" sqref="O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.88671875" customWidth="1"/>
     <col min="4" max="4" width="14.109375" customWidth="1"/>
     <col min="5" max="6" width="14.5546875" customWidth="1"/>
@@ -3731,6 +3741,210 @@
         <v>0.06</v>
       </c>
     </row>
+    <row r="45" spans="1:22" ht="144" x14ac:dyDescent="0.3">
+      <c r="A45" s="9">
+        <v>45209</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D45" s="2">
+        <v>1</v>
+      </c>
+      <c r="E45" s="2">
+        <v>1</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J45">
+        <v>0.09</v>
+      </c>
+      <c r="K45">
+        <v>0.11</v>
+      </c>
+      <c r="L45">
+        <v>0.09</v>
+      </c>
+      <c r="M45">
+        <v>0.1</v>
+      </c>
+      <c r="N45">
+        <v>0.11</v>
+      </c>
+      <c r="O45">
+        <v>0.02</v>
+      </c>
+      <c r="P45">
+        <v>0.02</v>
+      </c>
+      <c r="Q45">
+        <v>0.01</v>
+      </c>
+      <c r="R45">
+        <v>0.03</v>
+      </c>
+      <c r="S45">
+        <v>0.05</v>
+      </c>
+      <c r="T45">
+        <v>0.06</v>
+      </c>
+      <c r="U45">
+        <v>0.05</v>
+      </c>
+      <c r="V45">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" ht="144" x14ac:dyDescent="0.3">
+      <c r="A46" s="9">
+        <v>45209</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D46" s="2">
+        <v>1</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J46">
+        <v>0.13</v>
+      </c>
+      <c r="K46">
+        <v>0.11</v>
+      </c>
+      <c r="L46">
+        <v>0.13</v>
+      </c>
+      <c r="M46">
+        <v>0.1</v>
+      </c>
+      <c r="N46">
+        <v>0.11</v>
+      </c>
+      <c r="O46">
+        <v>0.02</v>
+      </c>
+      <c r="P46">
+        <v>0.02</v>
+      </c>
+      <c r="Q46">
+        <v>0.3</v>
+      </c>
+      <c r="R46">
+        <v>0.1</v>
+      </c>
+      <c r="S46">
+        <v>0.05</v>
+      </c>
+      <c r="T46">
+        <v>0.06</v>
+      </c>
+      <c r="U46">
+        <v>0.37</v>
+      </c>
+      <c r="V46">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" ht="144" x14ac:dyDescent="0.3">
+      <c r="A47" s="9">
+        <v>45209</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="E47" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J47">
+        <v>0.1</v>
+      </c>
+      <c r="K47">
+        <v>0.11</v>
+      </c>
+      <c r="L47">
+        <v>0.1</v>
+      </c>
+      <c r="M47">
+        <v>0.11</v>
+      </c>
+      <c r="N47">
+        <v>0.11</v>
+      </c>
+      <c r="O47">
+        <v>0.02</v>
+      </c>
+      <c r="P47">
+        <v>0.02</v>
+      </c>
+      <c r="Q47">
+        <v>0.02</v>
+      </c>
+      <c r="R47">
+        <v>0.03</v>
+      </c>
+      <c r="S47">
+        <v>0.05</v>
+      </c>
+      <c r="T47">
+        <v>0.05</v>
+      </c>
+      <c r="U47">
+        <v>0.04</v>
+      </c>
+      <c r="V47">
+        <v>0.05</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:I1"/>

</xml_diff>

<commit_message>
99% int v 99% ext results RAREsim v2.1.1 pruning pipeline
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E01379-5FFB-4DA0-A254-C3DF91200D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E5361F-CEA6-4A6C-8008-DF6214536045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="66">
   <si>
     <t>Population</t>
   </si>
@@ -338,6 +338,24 @@
 99% fun bins
 99% syn bins
 4. Extract datasets from 99% pruned haplotype</t>
+  </si>
+  <si>
+    <t>1. Separately-RAREsim v2.1.1
+--functional_bins 100%
+--synonymous_bins 100%
+2. RAREsim v2.1.1: Convert 100% pruned hap file to .sm file using convert.py
+3.1: Internal Data
+Separately-RAREsim v2.1.1
+--functional_bins 99% 6 MAC BINS
+--synonymous_bins 99% 6 MAC BINS
+3.2: External Data
+Separately-RAREsim v2.1.1
+--functional_bins 99% 6 MAC BINS
+--synonymous_bins 99% 6 MAC BINS
+4. R: add pruned variants back in as rows of 0 and extract datasets from internal data and external data</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -746,11 +764,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660476C5-A4B0-4780-BD43-FC7746B114D2}">
-  <dimension ref="A1:AG47"/>
+  <dimension ref="A1:AG52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O48" sqref="O48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P53" sqref="P53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3945,6 +3963,79 @@
         <v>0.05</v>
       </c>
     </row>
+    <row r="48" spans="1:22" ht="249.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="9">
+        <v>45210</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="E48" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J48">
+        <v>0.06</v>
+      </c>
+      <c r="K48">
+        <v>0.02</v>
+      </c>
+      <c r="L48">
+        <v>0.06</v>
+      </c>
+      <c r="M48">
+        <v>0.02</v>
+      </c>
+      <c r="N48">
+        <v>0.02</v>
+      </c>
+      <c r="O48">
+        <v>0.01</v>
+      </c>
+      <c r="P48">
+        <v>0.02</v>
+      </c>
+      <c r="Q48">
+        <v>0.35</v>
+      </c>
+      <c r="R48">
+        <v>0.17</v>
+      </c>
+      <c r="S48">
+        <v>0.02</v>
+      </c>
+      <c r="T48">
+        <v>0.03</v>
+      </c>
+      <c r="U48">
+        <v>0.27</v>
+      </c>
+      <c r="V48">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="52" spans="20:20" x14ac:dyDescent="0.3">
+      <c r="T52" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:I1"/>

</xml_diff>

<commit_message>
results from 99% int v 99% ext RAREsim v2.1.1 pipeline
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E5361F-CEA6-4A6C-8008-DF6214536045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA817F02-675D-41AF-9F1F-FD3B8C4CD4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="69">
   <si>
     <t>Population</t>
   </si>
@@ -356,6 +356,18 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>100v99/
+internal v external data</t>
+  </si>
+  <si>
+    <t>100v99/
+external v external data</t>
+  </si>
+  <si>
+    <t>100v99/
+internal v internal data</t>
   </si>
 </sst>
 </file>
@@ -767,8 +779,8 @@
   <dimension ref="A1:AG52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P53" sqref="P53"/>
+      <pane ySplit="2" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3980,7 +3992,7 @@
         <v>0.99</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>40</v>
@@ -4031,7 +4043,143 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="52" spans="20:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="9">
+        <v>45211</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J49">
+        <v>0.04</v>
+      </c>
+      <c r="K49">
+        <v>0.03</v>
+      </c>
+      <c r="L49">
+        <v>0.04</v>
+      </c>
+      <c r="M49">
+        <v>0.03</v>
+      </c>
+      <c r="N49">
+        <v>0.03</v>
+      </c>
+      <c r="O49">
+        <v>0.01</v>
+      </c>
+      <c r="P49">
+        <v>0.02</v>
+      </c>
+      <c r="Q49">
+        <v>0.02</v>
+      </c>
+      <c r="R49">
+        <v>0.02</v>
+      </c>
+      <c r="S49">
+        <v>0.02</v>
+      </c>
+      <c r="T49">
+        <v>0.04</v>
+      </c>
+      <c r="U49">
+        <v>0.02</v>
+      </c>
+      <c r="V49">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="9">
+        <v>45211</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="E50" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J50">
+        <v>0.04</v>
+      </c>
+      <c r="K50">
+        <v>0.02</v>
+      </c>
+      <c r="L50">
+        <v>0.04</v>
+      </c>
+      <c r="M50">
+        <v>0.02</v>
+      </c>
+      <c r="N50">
+        <v>0.02</v>
+      </c>
+      <c r="O50">
+        <v>0.02</v>
+      </c>
+      <c r="P50">
+        <v>0.02</v>
+      </c>
+      <c r="Q50">
+        <v>0.04</v>
+      </c>
+      <c r="R50">
+        <v>0.02</v>
+      </c>
+      <c r="S50">
+        <v>0.02</v>
+      </c>
+      <c r="T50">
+        <v>0.03</v>
+      </c>
+      <c r="U50">
+        <v>0.02</v>
+      </c>
+      <c r="V50">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
       <c r="T52" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
80% int v 80% ext RAREsim v2.1.1 pruning results
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA817F02-675D-41AF-9F1F-FD3B8C4CD4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0923F990-E946-4AB8-A289-9D6A612C3329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="72">
   <si>
     <t>Population</t>
   </si>
@@ -355,9 +355,6 @@
 4. R: add pruned variants back in as rows of 0 and extract datasets from internal data and external data</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>100v99/
 internal v external data</t>
   </si>
@@ -367,6 +364,33 @@
   </si>
   <si>
     <t>100v99/
+internal v internal data</t>
+  </si>
+  <si>
+    <t>100v80/
+internal v external data</t>
+  </si>
+  <si>
+    <t>1. Separately-RAREsim v2.1.1
+--functional_bins 100%
+--synonymous_bins 100%
+2. RAREsim v2.1.1: Convert 100% pruned hap file to .sm file using convert.py
+3.1: Internal Data
+Separately-RAREsim v2.1.1
+--functional_bins 80% 6 MAC BINS
+--synonymous_bins 80% 6 MAC BINS
+3.2: External Data
+Separately-RAREsim v2.1.1
+--functional_bins 80% 6 MAC BINS
+--synonymous_bins 80% 6 MAC BINS
+4. R: add pruned variants back in as rows of 0 and extract datasets from internal data and external data</t>
+  </si>
+  <si>
+    <t>100v80/
+external v external data</t>
+  </si>
+  <si>
+    <t>100v80/
 internal v internal data</t>
   </si>
 </sst>
@@ -776,11 +800,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660476C5-A4B0-4780-BD43-FC7746B114D2}">
-  <dimension ref="A1:AG52"/>
+  <dimension ref="A1:AG53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
+      <pane ySplit="2" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3992,7 +4016,7 @@
         <v>0.99</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>40</v>
@@ -4060,7 +4084,7 @@
         <v>0.99</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>40</v>
@@ -4128,7 +4152,7 @@
         <v>0.99</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>40</v>
@@ -4179,9 +4203,208 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="T52" t="s">
-        <v>65</v>
+    <row r="51" spans="1:22" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="9">
+        <v>45215</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E51" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J51">
+        <v>0.11</v>
+      </c>
+      <c r="K51">
+        <v>0.03</v>
+      </c>
+      <c r="L51">
+        <v>0.11</v>
+      </c>
+      <c r="M51">
+        <v>0.03</v>
+      </c>
+      <c r="N51">
+        <v>0.03</v>
+      </c>
+      <c r="O51">
+        <v>0.01</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <v>0.89</v>
+      </c>
+      <c r="R51">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S51">
+        <v>0.02</v>
+      </c>
+      <c r="T51">
+        <v>0.01</v>
+      </c>
+      <c r="U51">
+        <v>0.67</v>
+      </c>
+      <c r="V51">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="9">
+        <v>45215</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J52">
+        <v>0.02</v>
+      </c>
+      <c r="K52">
+        <v>0.03</v>
+      </c>
+      <c r="L52">
+        <v>0.02</v>
+      </c>
+      <c r="M52">
+        <v>0.03</v>
+      </c>
+      <c r="N52">
+        <v>0.03</v>
+      </c>
+      <c r="O52">
+        <v>0.01</v>
+      </c>
+      <c r="P52">
+        <v>0.02</v>
+      </c>
+      <c r="Q52">
+        <v>0</v>
+      </c>
+      <c r="R52">
+        <v>0</v>
+      </c>
+      <c r="S52">
+        <v>0.02</v>
+      </c>
+      <c r="T52">
+        <v>0.01</v>
+      </c>
+      <c r="U52">
+        <v>0.03</v>
+      </c>
+      <c r="V52">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="9">
+        <v>45215</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E53" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J53">
+        <v>0.03</v>
+      </c>
+      <c r="K53">
+        <v>0.03</v>
+      </c>
+      <c r="L53">
+        <v>0.03</v>
+      </c>
+      <c r="M53">
+        <v>0.03</v>
+      </c>
+      <c r="N53">
+        <v>0.03</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <v>0.03</v>
+      </c>
+      <c r="R53">
+        <v>0.02</v>
+      </c>
+      <c r="S53">
+        <v>0.01</v>
+      </c>
+      <c r="T53">
+        <v>0.01</v>
+      </c>
+      <c r="U53">
+        <v>0.03</v>
+      </c>
+      <c r="V53">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
results for 99% and 80% int v ext for SKAT and Burden
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0923F990-E946-4AB8-A289-9D6A612C3329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F45F495-DEA5-41C7-99FF-4F130FC539E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="88">
   <si>
     <t>Population</t>
   </si>
@@ -355,22 +355,6 @@
 4. R: add pruned variants back in as rows of 0 and extract datasets from internal data and external data</t>
   </si>
   <si>
-    <t>100v99/
-internal v external data</t>
-  </si>
-  <si>
-    <t>100v99/
-external v external data</t>
-  </si>
-  <si>
-    <t>100v99/
-internal v internal data</t>
-  </si>
-  <si>
-    <t>100v80/
-internal v external data</t>
-  </si>
-  <si>
     <t>1. Separately-RAREsim v2.1.1
 --functional_bins 100%
 --synonymous_bins 100%
@@ -386,12 +370,91 @@
 4. R: add pruned variants back in as rows of 0 and extract datasets from internal data and external data</t>
   </si>
   <si>
-    <t>100v80/
+    <t>99v99/
+internal v external data</t>
+  </si>
+  <si>
+    <t>99v99/
 external v external data</t>
   </si>
   <si>
-    <t>100v80/
+    <t>99v99/
 internal v internal data</t>
+  </si>
+  <si>
+    <t>80v80/
+internal v external data</t>
+  </si>
+  <si>
+    <t>80v80/
+external v external data</t>
+  </si>
+  <si>
+    <t>80v80/
+internal v internal data</t>
+  </si>
+  <si>
+    <t>Burden Internal (Fun Variants Only)</t>
+  </si>
+  <si>
+    <t>SKAT Internal 
+(Fun Variants Only)</t>
+  </si>
+  <si>
+    <t>SKAT External 
+(Fun Variants Only)</t>
+  </si>
+  <si>
+    <t>SKAT 
+Internal + External 
+(Fun Variants Only)</t>
+  </si>
+  <si>
+    <t>Burden External 
+(Fun Variants Only)</t>
+  </si>
+  <si>
+    <t>Burden 
+Internal + External 
+(Fun Variants Only)</t>
+  </si>
+  <si>
+    <t>SKAT Internal 
+(Syn Variants Only)</t>
+  </si>
+  <si>
+    <t>SKAT External 
+(Syn Variants Only)</t>
+  </si>
+  <si>
+    <t>SKAT 
+Internal + External 
+(Syn Variants Only)</t>
+  </si>
+  <si>
+    <t>Burden Internal 
+(Syn Variants Only)</t>
+  </si>
+  <si>
+    <t>Burden External 
+(Syn Variants Only)</t>
+  </si>
+  <si>
+    <t>Burden 
+Internal + External 
+(Syn Variants Only)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>10/11/2023 &amp; 10/18/23 (SKAT and Burden)</t>
+  </si>
+  <si>
+    <t>10/12/2023 &amp; 10/18/23 (SKAT and Burden)</t>
+  </si>
+  <si>
+    <t>10/16/2023 &amp; 10/18/23 (SKAT and Burden)</t>
   </si>
 </sst>
 </file>
@@ -459,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -481,8 +544,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -800,16 +864,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660476C5-A4B0-4780-BD43-FC7746B114D2}">
-  <dimension ref="A1:AG53"/>
+  <dimension ref="A1:AL53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I56" sqref="I56"/>
+      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.88671875" customWidth="1"/>
     <col min="4" max="4" width="14.109375" customWidth="1"/>
     <col min="5" max="6" width="14.5546875" customWidth="1"/>
@@ -824,37 +888,48 @@
     <col min="20" max="20" width="16.21875" customWidth="1"/>
     <col min="21" max="21" width="16.77734375" customWidth="1"/>
     <col min="22" max="22" width="18.109375" customWidth="1"/>
-    <col min="23" max="23" width="10.21875" customWidth="1"/>
+    <col min="23" max="23" width="17" customWidth="1"/>
+    <col min="24" max="24" width="17.33203125" customWidth="1"/>
+    <col min="25" max="25" width="17.21875" customWidth="1"/>
+    <col min="26" max="26" width="16.77734375" customWidth="1"/>
+    <col min="27" max="27" width="17" customWidth="1"/>
+    <col min="28" max="28" width="16.77734375" customWidth="1"/>
+    <col min="29" max="29" width="16.6640625" customWidth="1"/>
+    <col min="30" max="30" width="17" customWidth="1"/>
+    <col min="31" max="31" width="17.109375" customWidth="1"/>
+    <col min="32" max="33" width="16.88671875" customWidth="1"/>
+    <col min="34" max="34" width="17.88671875" customWidth="1"/>
+    <col min="35" max="35" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
     </row>
-    <row r="2" spans="1:23" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -922,10 +997,46 @@
         <v>27</v>
       </c>
       <c r="W2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI2" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>45189</v>
       </c>
@@ -992,8 +1103,44 @@
       <c r="V3" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="W3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH3" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>45182</v>
       </c>
@@ -1060,9 +1207,45 @@
       <c r="V4" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="W4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH4" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
+    <row r="5" spans="1:35" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
         <v>45184</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1128,9 +1311,45 @@
       <c r="V5" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="W5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH5" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+    <row r="6" spans="1:35" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
         <v>45184</v>
       </c>
       <c r="B6" t="s">
@@ -1196,9 +1415,45 @@
       <c r="V6" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="W6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH6" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
+    <row r="7" spans="1:35" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
         <v>45182</v>
       </c>
       <c r="B7" t="s">
@@ -1264,9 +1519,45 @@
       <c r="V7" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="W7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH7" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
+    <row r="8" spans="1:35" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
         <v>45188</v>
       </c>
       <c r="B8" t="s">
@@ -1332,9 +1623,45 @@
       <c r="V8" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="W8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH8" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="9" spans="1:23" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="9">
+    <row r="9" spans="1:35" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
         <v>45188</v>
       </c>
       <c r="B9" t="s">
@@ -1400,9 +1727,45 @@
       <c r="V9" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="W9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH9" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="10" spans="1:23" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
+    <row r="10" spans="1:35" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
         <v>45188</v>
       </c>
       <c r="B10" t="s">
@@ -1468,9 +1831,45 @@
       <c r="V10" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="W10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH10" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="11" spans="1:23" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
+    <row r="11" spans="1:35" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
         <v>45188</v>
       </c>
       <c r="B11" t="s">
@@ -1536,9 +1935,45 @@
       <c r="V11" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="W11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH11" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="12" spans="1:23" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
+    <row r="12" spans="1:35" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
         <v>45189</v>
       </c>
       <c r="B12" t="s">
@@ -1604,9 +2039,45 @@
       <c r="V12">
         <v>0.03</v>
       </c>
+      <c r="W12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH12" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="13" spans="1:23" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
+    <row r="13" spans="1:35" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
         <v>45189</v>
       </c>
       <c r="B13" t="s">
@@ -1672,9 +2143,45 @@
       <c r="V13">
         <v>0.16</v>
       </c>
+      <c r="W13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH13" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="14" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
+    <row r="14" spans="1:35" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
         <v>45190</v>
       </c>
       <c r="B14" t="s">
@@ -1740,9 +2247,45 @@
       <c r="V14">
         <v>0.03</v>
       </c>
+      <c r="W14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH14" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="15" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
+    <row r="15" spans="1:35" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
         <v>45194</v>
       </c>
       <c r="B15" t="s">
@@ -1808,9 +2351,45 @@
       <c r="V15">
         <v>0.06</v>
       </c>
+      <c r="W15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH15" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="16" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
+    <row r="16" spans="1:35" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
         <v>45194</v>
       </c>
       <c r="B16" t="s">
@@ -1876,9 +2455,45 @@
       <c r="V16">
         <v>0.02</v>
       </c>
+      <c r="W16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH16" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="17" spans="1:33" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
+    <row r="17" spans="1:34" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
         <v>45194</v>
       </c>
       <c r="B17" t="s">
@@ -1948,7 +2563,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:33" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:34" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>45196</v>
       </c>
@@ -2015,20 +2630,45 @@
       <c r="V18" s="5">
         <v>0.06</v>
       </c>
-      <c r="W18" s="6"/>
-      <c r="X18" s="6"/>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="6"/>
-      <c r="AA18" s="6"/>
-      <c r="AB18" s="6"/>
-      <c r="AC18" s="6"/>
-      <c r="AD18" s="6"/>
-      <c r="AE18" s="6"/>
-      <c r="AF18" s="6"/>
-      <c r="AG18" s="6"/>
+      <c r="W18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH18" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="19" spans="1:33" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="9">
+    <row r="19" spans="1:34" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
         <v>45196</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2094,9 +2734,45 @@
       <c r="V19">
         <v>0.02</v>
       </c>
+      <c r="W19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH19" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="20" spans="1:33" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="9">
+    <row r="20" spans="1:34" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
         <v>45196</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2162,9 +2838,45 @@
       <c r="V20">
         <v>0.03</v>
       </c>
+      <c r="W20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH20" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="21" spans="1:33" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="9">
+    <row r="21" spans="1:34" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
         <v>45196</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2230,9 +2942,45 @@
       <c r="V21">
         <v>7.0000000000000007E-2</v>
       </c>
+      <c r="W21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH21" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="22" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="9">
+    <row r="22" spans="1:34" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
         <v>45196</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2298,9 +3046,45 @@
       <c r="V22">
         <v>0.61</v>
       </c>
+      <c r="W22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH22" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="23" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="9">
+    <row r="23" spans="1:34" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
         <v>45197</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2366,9 +3150,45 @@
       <c r="V23">
         <v>0.01</v>
       </c>
+      <c r="W23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH23" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="24" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="9">
+    <row r="24" spans="1:34" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="8">
         <v>45197</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -2434,9 +3254,45 @@
       <c r="V24">
         <v>0.03</v>
       </c>
+      <c r="W24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH24" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="25" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="9">
+    <row r="25" spans="1:34" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="8">
         <v>45197</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -2502,9 +3358,45 @@
       <c r="V25">
         <v>0.39</v>
       </c>
+      <c r="W25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH25" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="26" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="9">
+    <row r="26" spans="1:34" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
         <v>45197</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2570,9 +3462,45 @@
       <c r="V26">
         <v>0.03</v>
       </c>
+      <c r="W26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH26" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="27" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="9">
+    <row r="27" spans="1:34" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
         <v>45197</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2638,9 +3566,45 @@
       <c r="V27">
         <v>0.04</v>
       </c>
+      <c r="W27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH27" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="28" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
+    <row r="28" spans="1:34" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
         <v>45198</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2706,9 +3670,45 @@
       <c r="V28">
         <v>0.21</v>
       </c>
+      <c r="W28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH28" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="29" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="9">
+    <row r="29" spans="1:34" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="8">
         <v>45198</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2774,9 +3774,45 @@
       <c r="V29">
         <v>0.05</v>
       </c>
+      <c r="W29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH29" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="30" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="9">
+    <row r="30" spans="1:34" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="8">
         <v>45198</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2842,9 +3878,45 @@
       <c r="V30">
         <v>0.05</v>
       </c>
+      <c r="W30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH30" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="31" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="9">
+    <row r="31" spans="1:34" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="8">
         <v>45198</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2910,9 +3982,45 @@
       <c r="V31">
         <v>0.1</v>
       </c>
+      <c r="W31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH31" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="32" spans="1:33" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="9">
+    <row r="32" spans="1:34" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="8">
         <v>45198</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2978,9 +4086,45 @@
       <c r="V32">
         <v>0</v>
       </c>
+      <c r="W32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH32" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="33" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="9">
+    <row r="33" spans="1:34" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
         <v>45198</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -3046,9 +4190,45 @@
       <c r="V33">
         <v>0.01</v>
       </c>
+      <c r="W33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH33" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="34" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="9">
+    <row r="34" spans="1:34" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="8">
         <v>45198</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -3114,9 +4294,45 @@
       <c r="V34">
         <v>0.04</v>
       </c>
+      <c r="W34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH34" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="35" spans="1:22" ht="72" x14ac:dyDescent="0.3">
-      <c r="A35" s="9">
+    <row r="35" spans="1:34" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="8">
         <v>45203</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -3182,9 +4398,45 @@
       <c r="V35">
         <v>0.03</v>
       </c>
+      <c r="W35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH35" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="36" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="9">
+    <row r="36" spans="1:34" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="8">
         <v>45205</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -3250,9 +4502,45 @@
       <c r="V36">
         <v>0.02</v>
       </c>
+      <c r="W36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH36" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="37" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="9">
+    <row r="37" spans="1:34" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="8">
         <v>45205</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -3318,9 +4606,45 @@
       <c r="V37">
         <v>0.56000000000000005</v>
       </c>
+      <c r="W37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH37" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="38" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="9">
+    <row r="38" spans="1:34" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="8">
         <v>45205</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -3386,9 +4710,45 @@
       <c r="V38">
         <v>0</v>
       </c>
+      <c r="W38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH38" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="39" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A39" s="9">
+    <row r="39" spans="1:34" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="8">
         <v>45208</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -3454,9 +4814,45 @@
       <c r="V39">
         <v>0.01</v>
       </c>
+      <c r="W39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH39" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="40" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="9">
+    <row r="40" spans="1:34" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="8">
         <v>45208</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -3522,9 +4918,45 @@
       <c r="V40">
         <v>0.08</v>
       </c>
+      <c r="W40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH40" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="41" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="9">
+    <row r="41" spans="1:34" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="8">
         <v>45208</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -3590,9 +5022,45 @@
       <c r="V41">
         <v>0.02</v>
       </c>
+      <c r="W41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH41" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="42" spans="1:22" ht="144" x14ac:dyDescent="0.3">
-      <c r="A42" s="9">
+    <row r="42" spans="1:34" ht="144" x14ac:dyDescent="0.3">
+      <c r="A42" s="8">
         <v>45208</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -3658,9 +5126,45 @@
       <c r="V42">
         <v>0.04</v>
       </c>
+      <c r="W42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH42" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="43" spans="1:22" ht="144" x14ac:dyDescent="0.3">
-      <c r="A43" s="9">
+    <row r="43" spans="1:34" ht="144" x14ac:dyDescent="0.3">
+      <c r="A43" s="8">
         <v>45208</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -3726,9 +5230,45 @@
       <c r="V43">
         <v>0.68</v>
       </c>
+      <c r="W43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH43" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="44" spans="1:22" ht="144" x14ac:dyDescent="0.3">
-      <c r="A44" s="9">
+    <row r="44" spans="1:34" ht="144" x14ac:dyDescent="0.3">
+      <c r="A44" s="8">
         <v>45208</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -3794,9 +5334,45 @@
       <c r="V44">
         <v>0.06</v>
       </c>
+      <c r="W44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH44" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="45" spans="1:22" ht="144" x14ac:dyDescent="0.3">
-      <c r="A45" s="9">
+    <row r="45" spans="1:34" ht="144" x14ac:dyDescent="0.3">
+      <c r="A45" s="8">
         <v>45209</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -3862,9 +5438,45 @@
       <c r="V45">
         <v>0.04</v>
       </c>
+      <c r="W45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH45" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="46" spans="1:22" ht="144" x14ac:dyDescent="0.3">
-      <c r="A46" s="9">
+    <row r="46" spans="1:34" ht="144" x14ac:dyDescent="0.3">
+      <c r="A46" s="8">
         <v>45209</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -3930,9 +5542,45 @@
       <c r="V46">
         <v>0.21</v>
       </c>
+      <c r="W46" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X46" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y46" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z46" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA46" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB46" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC46" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD46" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE46" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF46" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG46" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH46" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="47" spans="1:22" ht="144" x14ac:dyDescent="0.3">
-      <c r="A47" s="9">
+    <row r="47" spans="1:34" ht="144" x14ac:dyDescent="0.3">
+      <c r="A47" s="8">
         <v>45209</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -3998,10 +5646,46 @@
       <c r="V47">
         <v>0.05</v>
       </c>
+      <c r="W47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH47" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="48" spans="1:22" ht="249.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="9">
-        <v>45210</v>
+    <row r="48" spans="1:34" ht="249.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>7</v>
@@ -4016,7 +5700,7 @@
         <v>0.99</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>40</v>
@@ -4066,10 +5750,46 @@
       <c r="V48">
         <v>0.12</v>
       </c>
+      <c r="W48">
+        <v>0.03</v>
+      </c>
+      <c r="X48">
+        <v>0.36</v>
+      </c>
+      <c r="Y48">
+        <v>0.19</v>
+      </c>
+      <c r="Z48">
+        <v>0</v>
+      </c>
+      <c r="AA48">
+        <v>0.08</v>
+      </c>
+      <c r="AB48">
+        <v>0.05</v>
+      </c>
+      <c r="AC48">
+        <v>0.01</v>
+      </c>
+      <c r="AD48">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AE48">
+        <v>0.13</v>
+      </c>
+      <c r="AF48">
+        <v>0.05</v>
+      </c>
+      <c r="AG48">
+        <v>0.05</v>
+      </c>
+      <c r="AH48">
+        <v>0.04</v>
+      </c>
     </row>
-    <row r="49" spans="1:22" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="9">
-        <v>45211</v>
+    <row r="49" spans="1:38" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>7</v>
@@ -4084,7 +5804,7 @@
         <v>0.99</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>40</v>
@@ -4134,10 +5854,46 @@
       <c r="V49">
         <v>0.03</v>
       </c>
+      <c r="W49">
+        <v>0.01</v>
+      </c>
+      <c r="X49">
+        <v>0</v>
+      </c>
+      <c r="Y49">
+        <v>0</v>
+      </c>
+      <c r="Z49">
+        <v>0</v>
+      </c>
+      <c r="AA49">
+        <v>0.08</v>
+      </c>
+      <c r="AB49">
+        <v>0.06</v>
+      </c>
+      <c r="AC49">
+        <v>0.02</v>
+      </c>
+      <c r="AD49">
+        <v>0</v>
+      </c>
+      <c r="AE49">
+        <v>0</v>
+      </c>
+      <c r="AF49">
+        <v>0.05</v>
+      </c>
+      <c r="AG49">
+        <v>0.04</v>
+      </c>
+      <c r="AH49">
+        <v>0.05</v>
+      </c>
     </row>
-    <row r="50" spans="1:22" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="9">
-        <v>45211</v>
+    <row r="50" spans="1:38" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>7</v>
@@ -4152,7 +5908,7 @@
         <v>0.99</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>40</v>
@@ -4202,10 +5958,46 @@
       <c r="V50">
         <v>0.02</v>
       </c>
+      <c r="W50">
+        <v>0.03</v>
+      </c>
+      <c r="X50">
+        <v>0</v>
+      </c>
+      <c r="Y50">
+        <v>0</v>
+      </c>
+      <c r="Z50">
+        <v>0</v>
+      </c>
+      <c r="AA50">
+        <v>0.09</v>
+      </c>
+      <c r="AB50">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC50">
+        <v>0.01</v>
+      </c>
+      <c r="AD50">
+        <v>0</v>
+      </c>
+      <c r="AE50">
+        <v>0</v>
+      </c>
+      <c r="AF50">
+        <v>0.05</v>
+      </c>
+      <c r="AG50">
+        <v>0.03</v>
+      </c>
+      <c r="AH50">
+        <v>0.04</v>
+      </c>
     </row>
-    <row r="51" spans="1:22" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="9">
-        <v>45215</v>
+    <row r="51" spans="1:38" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>7</v>
@@ -4220,7 +6012,7 @@
         <v>0.8</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>40</v>
@@ -4229,7 +6021,7 @@
         <v>22</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J51">
         <v>0.11</v>
@@ -4270,10 +6062,46 @@
       <c r="V51">
         <v>0.35</v>
       </c>
+      <c r="W51">
+        <v>0</v>
+      </c>
+      <c r="X51">
+        <v>0.92</v>
+      </c>
+      <c r="Y51">
+        <v>0.61</v>
+      </c>
+      <c r="Z51">
+        <v>0.04</v>
+      </c>
+      <c r="AA51">
+        <v>0.11</v>
+      </c>
+      <c r="AB51">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC51">
+        <v>0.01</v>
+      </c>
+      <c r="AD51">
+        <v>0.69</v>
+      </c>
+      <c r="AE51">
+        <v>0.42</v>
+      </c>
+      <c r="AF51">
+        <v>0.06</v>
+      </c>
+      <c r="AG51">
+        <v>0.11</v>
+      </c>
+      <c r="AH51">
+        <v>0.06</v>
+      </c>
     </row>
-    <row r="52" spans="1:22" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="9">
-        <v>45215</v>
+    <row r="52" spans="1:38" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>7</v>
@@ -4297,7 +6125,7 @@
         <v>22</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J52">
         <v>0.02</v>
@@ -4338,10 +6166,46 @@
       <c r="V52">
         <v>0.02</v>
       </c>
+      <c r="W52">
+        <v>0.01</v>
+      </c>
+      <c r="X52">
+        <v>0</v>
+      </c>
+      <c r="Y52">
+        <v>0</v>
+      </c>
+      <c r="Z52">
+        <v>0.01</v>
+      </c>
+      <c r="AA52">
+        <v>0.02</v>
+      </c>
+      <c r="AB52">
+        <v>0.01</v>
+      </c>
+      <c r="AC52">
+        <v>0</v>
+      </c>
+      <c r="AD52">
+        <v>0</v>
+      </c>
+      <c r="AE52">
+        <v>0</v>
+      </c>
+      <c r="AF52">
+        <v>0.04</v>
+      </c>
+      <c r="AG52">
+        <v>0.04</v>
+      </c>
+      <c r="AH52">
+        <v>0.03</v>
+      </c>
     </row>
-    <row r="53" spans="1:22" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="9">
-        <v>45215</v>
+    <row r="53" spans="1:38" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>7</v>
@@ -4365,7 +6229,7 @@
         <v>22</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J53">
         <v>0.03</v>
@@ -4405,6 +6269,45 @@
       </c>
       <c r="V53">
         <v>0.01</v>
+      </c>
+      <c r="W53">
+        <v>0</v>
+      </c>
+      <c r="X53">
+        <v>0</v>
+      </c>
+      <c r="Y53">
+        <v>0</v>
+      </c>
+      <c r="Z53">
+        <v>0.04</v>
+      </c>
+      <c r="AA53">
+        <v>0.04</v>
+      </c>
+      <c r="AB53">
+        <v>0.04</v>
+      </c>
+      <c r="AC53">
+        <v>0.01</v>
+      </c>
+      <c r="AD53">
+        <v>0.01</v>
+      </c>
+      <c r="AE53">
+        <v>0.01</v>
+      </c>
+      <c r="AF53">
+        <v>0.06</v>
+      </c>
+      <c r="AG53">
+        <v>0.06</v>
+      </c>
+      <c r="AH53">
+        <v>0.04</v>
+      </c>
+      <c r="AL53" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
100v99 and 100v80 SKAT and Burden results added
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F45F495-DEA5-41C7-99FF-4F130FC539E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F3C8D6-9E4D-4E41-BE00-88F2DD4BE124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="90">
   <si>
     <t>Population</t>
   </si>
@@ -455,6 +455,12 @@
   </si>
   <si>
     <t>10/16/2023 &amp; 10/18/23 (SKAT and Burden)</t>
+  </si>
+  <si>
+    <t>10/6/2023 &amp; 10/19/23 for SKAT and Burden</t>
+  </si>
+  <si>
+    <t>10/9/2023 &amp; 10/19/23 for SKAT and Burden</t>
   </si>
 </sst>
 </file>
@@ -522,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -546,6 +552,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -866,9 +875,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660476C5-A4B0-4780-BD43-FC7746B114D2}">
   <dimension ref="A1:AL53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -903,31 +912,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
     </row>
     <row r="2" spans="1:35" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -4436,8 +4445,8 @@
       </c>
     </row>
     <row r="36" spans="1:34" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="8">
-        <v>45205</v>
+      <c r="A36" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>7</v>
@@ -4502,46 +4511,46 @@
       <c r="V36">
         <v>0.02</v>
       </c>
-      <c r="W36" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="X36" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y36" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z36" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA36" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB36" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC36" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD36" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE36" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF36" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG36" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AH36" s="4" t="s">
-        <v>23</v>
+      <c r="W36">
+        <v>0</v>
+      </c>
+      <c r="X36">
+        <v>0</v>
+      </c>
+      <c r="Y36">
+        <v>0</v>
+      </c>
+      <c r="Z36">
+        <v>0.05</v>
+      </c>
+      <c r="AA36">
+        <v>0.04</v>
+      </c>
+      <c r="AB36">
+        <v>0.04</v>
+      </c>
+      <c r="AC36">
+        <v>0</v>
+      </c>
+      <c r="AD36">
+        <v>0.01</v>
+      </c>
+      <c r="AE36">
+        <v>0</v>
+      </c>
+      <c r="AF36">
+        <v>0.03</v>
+      </c>
+      <c r="AG36">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AH36">
+        <v>0.04</v>
       </c>
     </row>
     <row r="37" spans="1:34" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="8">
-        <v>45205</v>
+      <c r="A37" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>7</v>
@@ -4606,46 +4615,46 @@
       <c r="V37">
         <v>0.56000000000000005</v>
       </c>
-      <c r="W37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="X37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AH37" s="4" t="s">
-        <v>23</v>
+      <c r="W37">
+        <v>0</v>
+      </c>
+      <c r="X37">
+        <v>0.85</v>
+      </c>
+      <c r="Y37">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Z37">
+        <v>0.05</v>
+      </c>
+      <c r="AA37">
+        <v>0.97</v>
+      </c>
+      <c r="AB37">
+        <v>0.82</v>
+      </c>
+      <c r="AC37">
+        <v>0</v>
+      </c>
+      <c r="AD37">
+        <v>0.7</v>
+      </c>
+      <c r="AE37">
+        <v>0.39</v>
+      </c>
+      <c r="AF37">
+        <v>0.03</v>
+      </c>
+      <c r="AG37">
+        <v>0.7</v>
+      </c>
+      <c r="AH37">
+        <v>0.52</v>
       </c>
     </row>
     <row r="38" spans="1:34" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="8">
-        <v>45205</v>
+      <c r="A38" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>7</v>
@@ -4710,46 +4719,46 @@
       <c r="V38">
         <v>0</v>
       </c>
-      <c r="W38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="X38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AH38" s="4" t="s">
-        <v>23</v>
+      <c r="W38">
+        <v>0</v>
+      </c>
+      <c r="X38">
+        <v>0</v>
+      </c>
+      <c r="Y38">
+        <v>0</v>
+      </c>
+      <c r="Z38">
+        <v>0.02</v>
+      </c>
+      <c r="AA38">
+        <v>0.04</v>
+      </c>
+      <c r="AB38">
+        <v>0.04</v>
+      </c>
+      <c r="AC38">
+        <v>0.01</v>
+      </c>
+      <c r="AD38">
+        <v>0</v>
+      </c>
+      <c r="AE38">
+        <v>0.02</v>
+      </c>
+      <c r="AF38">
+        <v>0.02</v>
+      </c>
+      <c r="AG38">
+        <v>0.03</v>
+      </c>
+      <c r="AH38">
+        <v>0.02</v>
       </c>
     </row>
     <row r="39" spans="1:34" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A39" s="8">
-        <v>45208</v>
+      <c r="A39" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>7</v>
@@ -4814,46 +4823,46 @@
       <c r="V39">
         <v>0.01</v>
       </c>
-      <c r="W39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="X39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AH39" s="4" t="s">
-        <v>23</v>
+      <c r="W39" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="X39" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="Y39" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="Z39" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="AA39" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AB39" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC39" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD39" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AE39" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="AF39" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AG39" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH39" s="10">
+        <v>0.02</v>
       </c>
     </row>
     <row r="40" spans="1:34" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="8">
-        <v>45208</v>
+      <c r="A40" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>7</v>
@@ -4918,46 +4927,46 @@
       <c r="V40">
         <v>0.08</v>
       </c>
-      <c r="W40" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="X40" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y40" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z40" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA40" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB40" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC40" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD40" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE40" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF40" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG40" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AH40" s="4" t="s">
-        <v>23</v>
+      <c r="W40">
+        <v>0.01</v>
+      </c>
+      <c r="X40">
+        <v>0.19</v>
+      </c>
+      <c r="Y40">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z40">
+        <v>0.04</v>
+      </c>
+      <c r="AA40">
+        <v>0.12</v>
+      </c>
+      <c r="AB40">
+        <v>0.06</v>
+      </c>
+      <c r="AC40">
+        <v>0</v>
+      </c>
+      <c r="AD40">
+        <v>0.2</v>
+      </c>
+      <c r="AE40">
+        <v>0.1</v>
+      </c>
+      <c r="AF40">
+        <v>0.03</v>
+      </c>
+      <c r="AG40">
+        <v>0.08</v>
+      </c>
+      <c r="AH40">
+        <v>0.06</v>
       </c>
     </row>
     <row r="41" spans="1:34" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="8">
-        <v>45208</v>
+      <c r="A41" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>7</v>
@@ -5022,41 +5031,41 @@
       <c r="V41">
         <v>0.02</v>
       </c>
-      <c r="W41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="X41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AH41" s="4" t="s">
-        <v>23</v>
+      <c r="W41">
+        <v>0.01</v>
+      </c>
+      <c r="X41">
+        <v>0.02</v>
+      </c>
+      <c r="Y41">
+        <v>0.03</v>
+      </c>
+      <c r="Z41">
+        <v>0.03</v>
+      </c>
+      <c r="AA41">
+        <v>0.03</v>
+      </c>
+      <c r="AB41">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC41">
+        <v>0</v>
+      </c>
+      <c r="AD41">
+        <v>0.02</v>
+      </c>
+      <c r="AE41">
+        <v>0.01</v>
+      </c>
+      <c r="AF41">
+        <v>0.02</v>
+      </c>
+      <c r="AG41">
+        <v>0.01</v>
+      </c>
+      <c r="AH41">
+        <v>0.03</v>
       </c>
     </row>
     <row r="42" spans="1:34" ht="144" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added 100v90 and 100v95 RAREsim v2.1.1 results
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F3C8D6-9E4D-4E41-BE00-88F2DD4BE124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90362831-46CA-4461-9366-B206EBDE7DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="92">
   <si>
     <t>Population</t>
   </si>
@@ -461,6 +461,26 @@
   </si>
   <si>
     <t>10/9/2023 &amp; 10/19/23 for SKAT and Burden</t>
+  </si>
+  <si>
+    <t>1. Separately-RAREsim v2.1.1
+--functional_bins 100%
+--synonymous_bins 100%
+2. RAREsim v2.1.1: Convert 100% pruned hap file to .sm file using convert.py
+3. Separately-RAREsim v2.1.1
+--functional_bins 90% 6 MAC BINS
+--synonymous_bins 90% 6 MAC BINS
+4. R: add pruned variants back in as rows of 0 and extract datasets</t>
+  </si>
+  <si>
+    <t>1. Separately-RAREsim v2.1.1
+--functional_bins 100%
+--synonymous_bins 100%
+2. RAREsim v2.1.1: Convert 100% pruned hap file to .sm file using convert.py
+3. Separately-RAREsim v2.1.1
+--functional_bins 95% 6 MAC BINS
+--synonymous_bins 95% 6 MAC BINS
+4. R: add pruned variants back in as rows of 0 and extract datasets</t>
   </si>
 </sst>
 </file>
@@ -873,11 +893,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660476C5-A4B0-4780-BD43-FC7746B114D2}">
-  <dimension ref="A1:AL53"/>
+  <dimension ref="A1:AL59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6319,6 +6339,630 @@
         <v>84</v>
       </c>
     </row>
+    <row r="54" spans="1:38" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A54" s="8">
+        <v>45219</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D54" s="2">
+        <v>1</v>
+      </c>
+      <c r="E54" s="2">
+        <v>1</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J54">
+        <v>0.03</v>
+      </c>
+      <c r="K54">
+        <v>0.05</v>
+      </c>
+      <c r="L54">
+        <v>0.03</v>
+      </c>
+      <c r="M54">
+        <v>0.04</v>
+      </c>
+      <c r="N54">
+        <v>0.05</v>
+      </c>
+      <c r="O54">
+        <v>0.03</v>
+      </c>
+      <c r="P54">
+        <v>0.01</v>
+      </c>
+      <c r="Q54">
+        <v>0.06</v>
+      </c>
+      <c r="R54">
+        <v>0.04</v>
+      </c>
+      <c r="S54">
+        <v>0.04</v>
+      </c>
+      <c r="T54">
+        <v>0.03</v>
+      </c>
+      <c r="U54">
+        <v>0.01</v>
+      </c>
+      <c r="V54">
+        <v>0.01</v>
+      </c>
+      <c r="W54">
+        <v>0.02</v>
+      </c>
+      <c r="X54">
+        <v>0.02</v>
+      </c>
+      <c r="Y54">
+        <v>0.04</v>
+      </c>
+      <c r="Z54">
+        <v>0.06</v>
+      </c>
+      <c r="AA54">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB54">
+        <v>0.04</v>
+      </c>
+      <c r="AC54">
+        <v>0</v>
+      </c>
+      <c r="AD54">
+        <v>0</v>
+      </c>
+      <c r="AE54">
+        <v>0.01</v>
+      </c>
+      <c r="AF54">
+        <v>0.05</v>
+      </c>
+      <c r="AG54">
+        <v>0.05</v>
+      </c>
+      <c r="AH54">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="55" spans="1:38" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A55" s="8">
+        <v>45219</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1</v>
+      </c>
+      <c r="E55" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J55">
+        <v>0.16</v>
+      </c>
+      <c r="K55">
+        <v>0.05</v>
+      </c>
+      <c r="L55">
+        <v>0.16</v>
+      </c>
+      <c r="M55">
+        <v>0.04</v>
+      </c>
+      <c r="N55">
+        <v>0.05</v>
+      </c>
+      <c r="O55">
+        <v>0.03</v>
+      </c>
+      <c r="P55">
+        <v>0.01</v>
+      </c>
+      <c r="Q55">
+        <v>0.68</v>
+      </c>
+      <c r="R55">
+        <v>0.43</v>
+      </c>
+      <c r="S55">
+        <v>0.04</v>
+      </c>
+      <c r="T55">
+        <v>0.03</v>
+      </c>
+      <c r="U55">
+        <v>0.49</v>
+      </c>
+      <c r="V55">
+        <v>0.34</v>
+      </c>
+      <c r="W55">
+        <v>0.02</v>
+      </c>
+      <c r="X55">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Y55">
+        <v>0.25</v>
+      </c>
+      <c r="Z55">
+        <v>0.06</v>
+      </c>
+      <c r="AA55">
+        <v>0.59</v>
+      </c>
+      <c r="AB55">
+        <v>0.39</v>
+      </c>
+      <c r="AC55">
+        <v>0</v>
+      </c>
+      <c r="AD55">
+        <v>0.45</v>
+      </c>
+      <c r="AE55">
+        <v>0.26</v>
+      </c>
+      <c r="AF55">
+        <v>0.05</v>
+      </c>
+      <c r="AG55">
+        <v>0.46</v>
+      </c>
+      <c r="AH55">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:38" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A56" s="8">
+        <v>45219</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E56" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J56">
+        <v>0.04</v>
+      </c>
+      <c r="K56">
+        <v>0.05</v>
+      </c>
+      <c r="L56">
+        <v>0.04</v>
+      </c>
+      <c r="M56">
+        <v>0.06</v>
+      </c>
+      <c r="N56">
+        <v>0.05</v>
+      </c>
+      <c r="O56">
+        <v>0.03</v>
+      </c>
+      <c r="P56">
+        <v>0.03</v>
+      </c>
+      <c r="Q56">
+        <v>0.05</v>
+      </c>
+      <c r="R56">
+        <v>0.03</v>
+      </c>
+      <c r="S56">
+        <v>0.03</v>
+      </c>
+      <c r="T56">
+        <v>0.02</v>
+      </c>
+      <c r="U56">
+        <v>0.02</v>
+      </c>
+      <c r="V56">
+        <v>0.02</v>
+      </c>
+      <c r="W56">
+        <v>0.01</v>
+      </c>
+      <c r="X56">
+        <v>0.05</v>
+      </c>
+      <c r="Y56">
+        <v>0.03</v>
+      </c>
+      <c r="Z56">
+        <v>0.02</v>
+      </c>
+      <c r="AA56">
+        <v>0.05</v>
+      </c>
+      <c r="AB56">
+        <v>0.03</v>
+      </c>
+      <c r="AC56">
+        <v>0</v>
+      </c>
+      <c r="AD56">
+        <v>0</v>
+      </c>
+      <c r="AE56">
+        <v>0.02</v>
+      </c>
+      <c r="AF56">
+        <v>0.05</v>
+      </c>
+      <c r="AG56">
+        <v>0.06</v>
+      </c>
+      <c r="AH56">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="57" spans="1:38" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A57" s="8">
+        <v>45219</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
+      <c r="E57" s="2">
+        <v>1</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J57">
+        <v>0.06</v>
+      </c>
+      <c r="K57">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L57">
+        <v>0.06</v>
+      </c>
+      <c r="M57">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N57">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O57">
+        <v>0</v>
+      </c>
+      <c r="P57">
+        <v>0.01</v>
+      </c>
+      <c r="Q57">
+        <v>0</v>
+      </c>
+      <c r="R57">
+        <v>0.02</v>
+      </c>
+      <c r="S57">
+        <v>0.01</v>
+      </c>
+      <c r="T57">
+        <v>0.01</v>
+      </c>
+      <c r="U57">
+        <v>0.04</v>
+      </c>
+      <c r="V57">
+        <v>0.03</v>
+      </c>
+      <c r="W57">
+        <v>0.01</v>
+      </c>
+      <c r="X57">
+        <v>0</v>
+      </c>
+      <c r="Y57">
+        <v>0.01</v>
+      </c>
+      <c r="Z57">
+        <v>0.04</v>
+      </c>
+      <c r="AA57">
+        <v>0.05</v>
+      </c>
+      <c r="AB57">
+        <v>0.03</v>
+      </c>
+      <c r="AC57">
+        <v>0.01</v>
+      </c>
+      <c r="AD57">
+        <v>0</v>
+      </c>
+      <c r="AE57">
+        <v>0.01</v>
+      </c>
+      <c r="AF57">
+        <v>0.08</v>
+      </c>
+      <c r="AG57">
+        <v>0.05</v>
+      </c>
+      <c r="AH57">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="58" spans="1:38" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A58" s="8">
+        <v>45219</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D58" s="2">
+        <v>1</v>
+      </c>
+      <c r="E58" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J58">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K58">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L58">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M58">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N58">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O58">
+        <v>0.01</v>
+      </c>
+      <c r="P58">
+        <v>0.01</v>
+      </c>
+      <c r="Q58">
+        <v>0.45</v>
+      </c>
+      <c r="R58">
+        <v>0.25</v>
+      </c>
+      <c r="S58">
+        <v>0.02</v>
+      </c>
+      <c r="T58">
+        <v>0.01</v>
+      </c>
+      <c r="U58">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="V58">
+        <v>0.17</v>
+      </c>
+      <c r="W58">
+        <v>0.01</v>
+      </c>
+      <c r="X58">
+        <v>0.4</v>
+      </c>
+      <c r="Y58">
+        <v>0.23</v>
+      </c>
+      <c r="Z58">
+        <v>0.04</v>
+      </c>
+      <c r="AA58">
+        <v>0.36</v>
+      </c>
+      <c r="AB58">
+        <v>0.22</v>
+      </c>
+      <c r="AC58">
+        <v>0.01</v>
+      </c>
+      <c r="AD58">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AE58">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AF58">
+        <v>0.08</v>
+      </c>
+      <c r="AG58">
+        <v>0.23</v>
+      </c>
+      <c r="AH58">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:38" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A59" s="8">
+        <v>45219</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="E59" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J59">
+        <v>0.05</v>
+      </c>
+      <c r="K59">
+        <v>0.08</v>
+      </c>
+      <c r="L59">
+        <v>0.05</v>
+      </c>
+      <c r="M59">
+        <v>0.08</v>
+      </c>
+      <c r="N59">
+        <v>0.08</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <v>0.01</v>
+      </c>
+      <c r="Q59">
+        <v>0.03</v>
+      </c>
+      <c r="R59">
+        <v>0.03</v>
+      </c>
+      <c r="S59">
+        <v>0.02</v>
+      </c>
+      <c r="T59">
+        <v>0.02</v>
+      </c>
+      <c r="U59">
+        <v>0.03</v>
+      </c>
+      <c r="V59">
+        <v>0.02</v>
+      </c>
+      <c r="W59">
+        <v>0.01</v>
+      </c>
+      <c r="X59">
+        <v>0</v>
+      </c>
+      <c r="Y59">
+        <v>0</v>
+      </c>
+      <c r="Z59">
+        <v>0.06</v>
+      </c>
+      <c r="AA59">
+        <v>0.06</v>
+      </c>
+      <c r="AB59">
+        <v>0.06</v>
+      </c>
+      <c r="AC59">
+        <v>0.01</v>
+      </c>
+      <c r="AD59">
+        <v>0.01</v>
+      </c>
+      <c r="AE59">
+        <v>0.01</v>
+      </c>
+      <c r="AF59">
+        <v>0.04</v>
+      </c>
+      <c r="AG59">
+        <v>0.06</v>
+      </c>
+      <c r="AH59">
+        <v>0.03</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:I1"/>

</xml_diff>

<commit_message>
added 100v80 by gene results
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90362831-46CA-4461-9366-B206EBDE7DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A9B421-83C1-42B7-9FC1-91F071199CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="gene_region" sheetId="1" r:id="rId1"/>
+    <sheet name="by_gene" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="119">
   <si>
     <t>Population</t>
   </si>
@@ -481,6 +482,87 @@
 --functional_bins 95% 6 MAC BINS
 --synonymous_bins 95% 6 MAC BINS
 4. R: add pruned variants back in as rows of 0 and extract datasets</t>
+  </si>
+  <si>
+    <t>Gene</t>
+  </si>
+  <si>
+    <t>Megan's Haplotype</t>
+  </si>
+  <si>
+    <t>ProxECAT Internal</t>
+  </si>
+  <si>
+    <t>ProwECAT-weighted Internal</t>
+  </si>
+  <si>
+    <t>proxECAT-weighted External</t>
+  </si>
+  <si>
+    <t>iECAT-O Internal + External</t>
+  </si>
+  <si>
+    <t>SKAT-O Internal</t>
+  </si>
+  <si>
+    <t>SKAT-O External</t>
+  </si>
+  <si>
+    <t>SKAT-O Internal + External</t>
+  </si>
+  <si>
+    <t>SKAT Internal</t>
+  </si>
+  <si>
+    <t>SKAT External</t>
+  </si>
+  <si>
+    <t>SKAT Internal + External</t>
+  </si>
+  <si>
+    <t>Burden Internal</t>
+  </si>
+  <si>
+    <t>Burden External</t>
+  </si>
+  <si>
+    <t>Burden Internal + External</t>
+  </si>
+  <si>
+    <t>ADGRE2</t>
+  </si>
+  <si>
+    <t>ADGRE3</t>
+  </si>
+  <si>
+    <t>ADGRE5</t>
+  </si>
+  <si>
+    <t>CLEC17A</t>
+  </si>
+  <si>
+    <t>DDX39A</t>
+  </si>
+  <si>
+    <t>DNAJB1</t>
+  </si>
+  <si>
+    <t>GIPC1</t>
+  </si>
+  <si>
+    <t>NDUFB7</t>
+  </si>
+  <si>
+    <t>PKN1</t>
+  </si>
+  <si>
+    <t>PTGER1</t>
+  </si>
+  <si>
+    <t>TECR</t>
+  </si>
+  <si>
+    <t>ZNF333</t>
   </si>
 </sst>
 </file>
@@ -548,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -579,6 +661,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -895,9 +978,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660476C5-A4B0-4780-BD43-FC7746B114D2}">
   <dimension ref="A1:AL59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J61" sqref="J61"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6971,4 +7054,850 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DDB312-960A-4A06-81C4-77814F5815B8}">
+  <dimension ref="A1:AA14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="30.77734375" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="K1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+    </row>
+    <row r="2" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="162" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12">
+        <v>45225</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>1E-3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K3">
+        <v>0.06</v>
+      </c>
+      <c r="L3">
+        <v>0.15</v>
+      </c>
+      <c r="M3">
+        <v>0.05</v>
+      </c>
+      <c r="N3">
+        <v>0.08</v>
+      </c>
+      <c r="O3">
+        <v>0.06</v>
+      </c>
+      <c r="P3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Q3">
+        <v>0.06</v>
+      </c>
+      <c r="R3">
+        <v>0.04</v>
+      </c>
+      <c r="S3">
+        <v>0.01</v>
+      </c>
+      <c r="T3">
+        <v>0.38</v>
+      </c>
+      <c r="U3">
+        <v>0.19</v>
+      </c>
+      <c r="V3">
+        <v>0.01</v>
+      </c>
+      <c r="W3">
+        <v>0.36</v>
+      </c>
+      <c r="X3">
+        <v>0.15</v>
+      </c>
+      <c r="Y3">
+        <v>0.05</v>
+      </c>
+      <c r="Z3">
+        <v>0.36</v>
+      </c>
+      <c r="AA3">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>108</v>
+      </c>
+      <c r="K4">
+        <v>0.05</v>
+      </c>
+      <c r="L4">
+        <v>0.06</v>
+      </c>
+      <c r="M4">
+        <v>0.01</v>
+      </c>
+      <c r="N4">
+        <v>0.08</v>
+      </c>
+      <c r="O4">
+        <v>0.05</v>
+      </c>
+      <c r="P4">
+        <v>0.06</v>
+      </c>
+      <c r="Q4">
+        <v>0.05</v>
+      </c>
+      <c r="R4">
+        <v>0.04</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0.41</v>
+      </c>
+      <c r="U4">
+        <v>0.19</v>
+      </c>
+      <c r="V4">
+        <v>0.02</v>
+      </c>
+      <c r="W4">
+        <v>0.35</v>
+      </c>
+      <c r="X4">
+        <v>0.21</v>
+      </c>
+      <c r="Y4">
+        <v>0.03</v>
+      </c>
+      <c r="Z4">
+        <v>0.43</v>
+      </c>
+      <c r="AA4">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K5">
+        <v>0.06</v>
+      </c>
+      <c r="L5">
+        <v>0.12</v>
+      </c>
+      <c r="M5">
+        <v>0.05</v>
+      </c>
+      <c r="N5">
+        <v>0.05</v>
+      </c>
+      <c r="O5">
+        <v>0.06</v>
+      </c>
+      <c r="P5">
+        <v>0.12</v>
+      </c>
+      <c r="Q5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R5">
+        <v>0.02</v>
+      </c>
+      <c r="S5">
+        <v>0.04</v>
+      </c>
+      <c r="T5">
+        <v>0.48</v>
+      </c>
+      <c r="U5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="V5">
+        <v>0.02</v>
+      </c>
+      <c r="W5">
+        <v>0.41</v>
+      </c>
+      <c r="X5">
+        <v>0.16</v>
+      </c>
+      <c r="Y5">
+        <v>0.06</v>
+      </c>
+      <c r="Z5">
+        <v>0.44</v>
+      </c>
+      <c r="AA5">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L6">
+        <v>0.08</v>
+      </c>
+      <c r="M6">
+        <v>0.04</v>
+      </c>
+      <c r="N6">
+        <v>0.04</v>
+      </c>
+      <c r="O6">
+        <v>0.04</v>
+      </c>
+      <c r="P6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q6">
+        <v>0.04</v>
+      </c>
+      <c r="R6">
+        <v>0.03</v>
+      </c>
+      <c r="S6">
+        <v>0.1</v>
+      </c>
+      <c r="T6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="U6">
+        <v>0.21</v>
+      </c>
+      <c r="V6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W6">
+        <v>0.27</v>
+      </c>
+      <c r="X6">
+        <v>0.15</v>
+      </c>
+      <c r="Y6">
+        <v>0.11</v>
+      </c>
+      <c r="Z6">
+        <v>0.22</v>
+      </c>
+      <c r="AA6">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>111</v>
+      </c>
+      <c r="K7">
+        <v>0.04</v>
+      </c>
+      <c r="L7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M7">
+        <v>0.01</v>
+      </c>
+      <c r="N7">
+        <v>0.05</v>
+      </c>
+      <c r="O7">
+        <v>0.04</v>
+      </c>
+      <c r="P7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q7">
+        <v>0.05</v>
+      </c>
+      <c r="R7">
+        <v>0.05</v>
+      </c>
+      <c r="S7">
+        <v>0.03</v>
+      </c>
+      <c r="T7">
+        <v>0.31</v>
+      </c>
+      <c r="U7">
+        <v>0.17</v>
+      </c>
+      <c r="V7">
+        <v>0.03</v>
+      </c>
+      <c r="W7">
+        <v>0.3</v>
+      </c>
+      <c r="X7">
+        <v>0.2</v>
+      </c>
+      <c r="Y7">
+        <v>0.03</v>
+      </c>
+      <c r="Z7">
+        <v>0.32</v>
+      </c>
+      <c r="AA7">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>112</v>
+      </c>
+      <c r="K8">
+        <v>0.03</v>
+      </c>
+      <c r="L8">
+        <v>0.15</v>
+      </c>
+      <c r="M8">
+        <v>0.03</v>
+      </c>
+      <c r="N8">
+        <v>0.1</v>
+      </c>
+      <c r="O8">
+        <v>0.03</v>
+      </c>
+      <c r="P8">
+        <v>0.13</v>
+      </c>
+      <c r="Q8">
+        <v>0.03</v>
+      </c>
+      <c r="R8">
+        <v>0.03</v>
+      </c>
+      <c r="S8">
+        <v>0.03</v>
+      </c>
+      <c r="T8">
+        <v>0.26</v>
+      </c>
+      <c r="U8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V8">
+        <v>0.03</v>
+      </c>
+      <c r="W8">
+        <v>0.25</v>
+      </c>
+      <c r="X8">
+        <v>0.17</v>
+      </c>
+      <c r="Y8">
+        <v>0.05</v>
+      </c>
+      <c r="Z8">
+        <v>0.19</v>
+      </c>
+      <c r="AA8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J9" t="s">
+        <v>113</v>
+      </c>
+      <c r="K9">
+        <v>0.05</v>
+      </c>
+      <c r="L9">
+        <v>0.12</v>
+      </c>
+      <c r="M9">
+        <v>0.01</v>
+      </c>
+      <c r="N9">
+        <v>0.06</v>
+      </c>
+      <c r="O9">
+        <v>0.05</v>
+      </c>
+      <c r="P9">
+        <v>0.12</v>
+      </c>
+      <c r="Q9">
+        <v>0.06</v>
+      </c>
+      <c r="R9">
+        <v>0.03</v>
+      </c>
+      <c r="S9">
+        <v>0.04</v>
+      </c>
+      <c r="T9">
+        <v>0.31</v>
+      </c>
+      <c r="U9">
+        <v>0.17</v>
+      </c>
+      <c r="V9">
+        <v>0.04</v>
+      </c>
+      <c r="W9">
+        <v>0.3</v>
+      </c>
+      <c r="X9">
+        <v>0.18</v>
+      </c>
+      <c r="Y9">
+        <v>0.03</v>
+      </c>
+      <c r="Z9">
+        <v>0.26</v>
+      </c>
+      <c r="AA9">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
+        <v>114</v>
+      </c>
+      <c r="K10">
+        <v>0.09</v>
+      </c>
+      <c r="L10">
+        <v>0.06</v>
+      </c>
+      <c r="M10">
+        <v>4.49438202247191E-2</v>
+      </c>
+      <c r="N10">
+        <v>4.1237113402061903E-2</v>
+      </c>
+      <c r="O10">
+        <v>0.02</v>
+      </c>
+      <c r="P10">
+        <v>0.05</v>
+      </c>
+      <c r="Q10">
+        <v>0.02</v>
+      </c>
+      <c r="R10">
+        <v>0.01</v>
+      </c>
+      <c r="S10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T10">
+        <v>0.17</v>
+      </c>
+      <c r="U10">
+        <v>0.11</v>
+      </c>
+      <c r="V10">
+        <v>0.05</v>
+      </c>
+      <c r="W10">
+        <v>0.21</v>
+      </c>
+      <c r="X10">
+        <v>0.12</v>
+      </c>
+      <c r="Y10">
+        <v>0.05</v>
+      </c>
+      <c r="Z10">
+        <v>0.18</v>
+      </c>
+      <c r="AA10">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
+        <v>115</v>
+      </c>
+      <c r="K11">
+        <v>0.03</v>
+      </c>
+      <c r="L11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M11">
+        <v>0.03</v>
+      </c>
+      <c r="N11">
+        <v>0.08</v>
+      </c>
+      <c r="O11">
+        <v>0.03</v>
+      </c>
+      <c r="P11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Q11">
+        <v>0.03</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0.02</v>
+      </c>
+      <c r="T11">
+        <v>0.49</v>
+      </c>
+      <c r="U11">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="V11">
+        <v>0.03</v>
+      </c>
+      <c r="W11">
+        <v>0.44</v>
+      </c>
+      <c r="X11">
+        <v>0.2</v>
+      </c>
+      <c r="Y11">
+        <v>0.03</v>
+      </c>
+      <c r="Z11">
+        <v>0.43</v>
+      </c>
+      <c r="AA11">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>116</v>
+      </c>
+      <c r="K12">
+        <v>0.06</v>
+      </c>
+      <c r="L12">
+        <v>0.08</v>
+      </c>
+      <c r="M12">
+        <v>0.04</v>
+      </c>
+      <c r="N12">
+        <v>0.04</v>
+      </c>
+      <c r="O12">
+        <v>0.06</v>
+      </c>
+      <c r="P12">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q12">
+        <v>0.06</v>
+      </c>
+      <c r="R12">
+        <v>0.04</v>
+      </c>
+      <c r="S12">
+        <v>0.04</v>
+      </c>
+      <c r="T12">
+        <v>0.37</v>
+      </c>
+      <c r="U12">
+        <v>0.16</v>
+      </c>
+      <c r="V12">
+        <v>0.04</v>
+      </c>
+      <c r="W12">
+        <v>0.36</v>
+      </c>
+      <c r="X12">
+        <v>0.17</v>
+      </c>
+      <c r="Y12">
+        <v>0.02</v>
+      </c>
+      <c r="Z12">
+        <v>0.31</v>
+      </c>
+      <c r="AA12">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J13" t="s">
+        <v>117</v>
+      </c>
+      <c r="K13">
+        <v>0.06</v>
+      </c>
+      <c r="L13">
+        <v>0.11</v>
+      </c>
+      <c r="M13">
+        <v>0.01</v>
+      </c>
+      <c r="N13">
+        <v>0.09</v>
+      </c>
+      <c r="O13">
+        <v>0.06</v>
+      </c>
+      <c r="P13">
+        <v>0.11</v>
+      </c>
+      <c r="Q13">
+        <v>0.06</v>
+      </c>
+      <c r="R13">
+        <v>0.01</v>
+      </c>
+      <c r="S13">
+        <v>0.04</v>
+      </c>
+      <c r="T13">
+        <v>0.3</v>
+      </c>
+      <c r="U13">
+        <v>0.19</v>
+      </c>
+      <c r="V13">
+        <v>0.01</v>
+      </c>
+      <c r="W13">
+        <v>0.2</v>
+      </c>
+      <c r="X13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Y13">
+        <v>0.06</v>
+      </c>
+      <c r="Z13">
+        <v>0.22</v>
+      </c>
+      <c r="AA13">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J14" t="s">
+        <v>118</v>
+      </c>
+      <c r="K14">
+        <v>0.06</v>
+      </c>
+      <c r="L14">
+        <v>0.13</v>
+      </c>
+      <c r="M14">
+        <v>0.06</v>
+      </c>
+      <c r="N14">
+        <v>0.05</v>
+      </c>
+      <c r="O14">
+        <v>0.06</v>
+      </c>
+      <c r="P14">
+        <v>0.13</v>
+      </c>
+      <c r="Q14">
+        <v>0.06</v>
+      </c>
+      <c r="R14">
+        <v>0.02</v>
+      </c>
+      <c r="S14">
+        <v>0.02</v>
+      </c>
+      <c r="T14">
+        <v>0.44</v>
+      </c>
+      <c r="U14">
+        <v>0.23</v>
+      </c>
+      <c r="V14">
+        <v>0.03</v>
+      </c>
+      <c r="W14">
+        <v>0.39</v>
+      </c>
+      <c r="X14">
+        <v>0.18</v>
+      </c>
+      <c r="Y14">
+        <v>0.02</v>
+      </c>
+      <c r="Z14">
+        <v>0.37</v>
+      </c>
+      <c r="AA14">
+        <v>0.23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="K1:AA1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added results from 100v80 by gene
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A9B421-83C1-42B7-9FC1-91F071199CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55E7DFA-BE26-4E9F-BCE9-1B2B20E1E09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="122">
   <si>
     <t>Population</t>
   </si>
@@ -563,6 +563,15 @@
   </si>
   <si>
     <t>ZNF333</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These were done using updated code so that LogProx was filtering out genes with ACs &lt; 5 in the same way proxECAT and proxECAT-weighted </t>
+  </si>
+  <si>
+    <t>These were done using code that did not have LogProx and proxECAT filtering out genes with low Acs in the same way</t>
   </si>
 </sst>
 </file>
@@ -658,10 +667,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1015,31 +1024,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
     </row>
     <row r="2" spans="1:35" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -7058,11 +7067,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DDB312-960A-4A06-81C4-77814F5815B8}">
-  <dimension ref="A1:AA14"/>
+  <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB45" sqref="AB45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7077,41 +7086,42 @@
     <col min="10" max="10" width="13.44140625" customWidth="1"/>
     <col min="13" max="13" width="12.21875" customWidth="1"/>
     <col min="14" max="14" width="9.88671875" customWidth="1"/>
+    <col min="28" max="28" width="20.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="K1" s="11" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="K1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-    </row>
-    <row r="2" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+    </row>
+    <row r="2" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -7193,9 +7203,12 @@
       <c r="AA2" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" ht="162" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12">
+      <c r="AB2" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="162" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
         <v>45225</v>
       </c>
       <c r="B3" t="s">
@@ -7276,8 +7289,11 @@
       <c r="AA3">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AB3" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J4" t="s">
         <v>108</v>
       </c>
@@ -7333,7 +7349,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J5" t="s">
         <v>109</v>
       </c>
@@ -7389,7 +7405,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J6" t="s">
         <v>110</v>
       </c>
@@ -7445,7 +7461,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J7" t="s">
         <v>111</v>
       </c>
@@ -7501,7 +7517,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J8" t="s">
         <v>112</v>
       </c>
@@ -7557,7 +7573,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J9" t="s">
         <v>113</v>
       </c>
@@ -7613,7 +7629,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J10" t="s">
         <v>114</v>
       </c>
@@ -7669,7 +7685,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J11" t="s">
         <v>115</v>
       </c>
@@ -7725,7 +7741,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J12" t="s">
         <v>116</v>
       </c>
@@ -7781,7 +7797,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J13" t="s">
         <v>117</v>
       </c>
@@ -7837,7 +7853,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J14" t="s">
         <v>118</v>
       </c>
@@ -7891,6 +7907,2112 @@
       </c>
       <c r="AA14">
         <v>0.23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="11">
+        <v>45232</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>1E-3</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" t="s">
+        <v>93</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" t="s">
+        <v>107</v>
+      </c>
+      <c r="K15">
+        <v>0.06</v>
+      </c>
+      <c r="L15">
+        <v>0.04</v>
+      </c>
+      <c r="M15">
+        <v>0.05</v>
+      </c>
+      <c r="N15">
+        <v>0.04</v>
+      </c>
+      <c r="O15">
+        <v>0.06</v>
+      </c>
+      <c r="P15">
+        <v>0.04</v>
+      </c>
+      <c r="Q15">
+        <v>0.06</v>
+      </c>
+      <c r="R15">
+        <v>0.04</v>
+      </c>
+      <c r="S15">
+        <v>0.01</v>
+      </c>
+      <c r="T15">
+        <v>0.06</v>
+      </c>
+      <c r="U15">
+        <v>0.03</v>
+      </c>
+      <c r="V15">
+        <v>0.01</v>
+      </c>
+      <c r="W15">
+        <v>0.03</v>
+      </c>
+      <c r="X15">
+        <v>0.02</v>
+      </c>
+      <c r="Y15">
+        <v>0.05</v>
+      </c>
+      <c r="Z15">
+        <v>0.04</v>
+      </c>
+      <c r="AA15">
+        <v>0.05</v>
+      </c>
+      <c r="AB15" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
+        <v>108</v>
+      </c>
+      <c r="K16">
+        <v>0.05</v>
+      </c>
+      <c r="L16">
+        <v>0.04</v>
+      </c>
+      <c r="M16">
+        <v>0.01</v>
+      </c>
+      <c r="N16">
+        <v>0.04</v>
+      </c>
+      <c r="O16">
+        <v>0.05</v>
+      </c>
+      <c r="P16">
+        <v>0.04</v>
+      </c>
+      <c r="Q16">
+        <v>0.06</v>
+      </c>
+      <c r="R16">
+        <v>0.01</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0.05</v>
+      </c>
+      <c r="U16">
+        <v>0.03</v>
+      </c>
+      <c r="V16">
+        <v>0.02</v>
+      </c>
+      <c r="W16">
+        <v>0.05</v>
+      </c>
+      <c r="X16">
+        <v>0.06</v>
+      </c>
+      <c r="Y16">
+        <v>0.03</v>
+      </c>
+      <c r="Z16">
+        <v>0.03</v>
+      </c>
+      <c r="AA16">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J17" t="s">
+        <v>109</v>
+      </c>
+      <c r="K17">
+        <v>0.06</v>
+      </c>
+      <c r="L17">
+        <v>0.05</v>
+      </c>
+      <c r="M17">
+        <v>0.05</v>
+      </c>
+      <c r="N17">
+        <v>0.02</v>
+      </c>
+      <c r="O17">
+        <v>0.06</v>
+      </c>
+      <c r="P17">
+        <v>0.04</v>
+      </c>
+      <c r="Q17">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R17">
+        <v>0.02</v>
+      </c>
+      <c r="S17">
+        <v>0.04</v>
+      </c>
+      <c r="T17">
+        <v>0.03</v>
+      </c>
+      <c r="U17">
+        <v>0.04</v>
+      </c>
+      <c r="V17">
+        <v>0.02</v>
+      </c>
+      <c r="W17">
+        <v>0.03</v>
+      </c>
+      <c r="X17">
+        <v>0.03</v>
+      </c>
+      <c r="Y17">
+        <v>0.06</v>
+      </c>
+      <c r="Z17">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA17">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J18" t="s">
+        <v>110</v>
+      </c>
+      <c r="K18">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L18">
+        <v>0.05</v>
+      </c>
+      <c r="M18">
+        <v>0.04</v>
+      </c>
+      <c r="N18">
+        <v>0.03</v>
+      </c>
+      <c r="O18">
+        <v>0.04</v>
+      </c>
+      <c r="P18">
+        <v>0.04</v>
+      </c>
+      <c r="Q18">
+        <v>0.04</v>
+      </c>
+      <c r="R18">
+        <v>0.03</v>
+      </c>
+      <c r="S18">
+        <v>0.1</v>
+      </c>
+      <c r="T18">
+        <v>0.03</v>
+      </c>
+      <c r="U18">
+        <v>0.04</v>
+      </c>
+      <c r="V18">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W18">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="X18">
+        <v>0.06</v>
+      </c>
+      <c r="Y18">
+        <v>0.11</v>
+      </c>
+      <c r="Z18">
+        <v>0.03</v>
+      </c>
+      <c r="AA18">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J19" t="s">
+        <v>111</v>
+      </c>
+      <c r="K19">
+        <v>0.04</v>
+      </c>
+      <c r="L19">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M19">
+        <v>0.01</v>
+      </c>
+      <c r="N19">
+        <v>0.02</v>
+      </c>
+      <c r="O19">
+        <v>0.04</v>
+      </c>
+      <c r="P19">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q19">
+        <v>0.05</v>
+      </c>
+      <c r="R19">
+        <v>0.05</v>
+      </c>
+      <c r="S19">
+        <v>0.03</v>
+      </c>
+      <c r="T19">
+        <v>0.04</v>
+      </c>
+      <c r="U19">
+        <v>0.04</v>
+      </c>
+      <c r="V19">
+        <v>0.03</v>
+      </c>
+      <c r="W19">
+        <v>0.03</v>
+      </c>
+      <c r="X19">
+        <v>0.02</v>
+      </c>
+      <c r="Y19">
+        <v>0.03</v>
+      </c>
+      <c r="Z19">
+        <v>0.08</v>
+      </c>
+      <c r="AA19">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J20" t="s">
+        <v>112</v>
+      </c>
+      <c r="K20">
+        <v>0.03</v>
+      </c>
+      <c r="L20">
+        <v>0.08</v>
+      </c>
+      <c r="M20">
+        <v>0.03</v>
+      </c>
+      <c r="N20">
+        <v>0.05</v>
+      </c>
+      <c r="O20">
+        <v>0.03</v>
+      </c>
+      <c r="P20">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q20">
+        <v>0.03</v>
+      </c>
+      <c r="R20">
+        <v>0.02</v>
+      </c>
+      <c r="S20">
+        <v>0.03</v>
+      </c>
+      <c r="T20">
+        <v>0.02</v>
+      </c>
+      <c r="U20">
+        <v>0.03</v>
+      </c>
+      <c r="V20">
+        <v>0.03</v>
+      </c>
+      <c r="W20">
+        <v>0.01</v>
+      </c>
+      <c r="X20">
+        <v>0.02</v>
+      </c>
+      <c r="Y20">
+        <v>0.05</v>
+      </c>
+      <c r="Z20">
+        <v>0.04</v>
+      </c>
+      <c r="AA20">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J21" t="s">
+        <v>113</v>
+      </c>
+      <c r="K21">
+        <v>0.05</v>
+      </c>
+      <c r="L21">
+        <v>0.05</v>
+      </c>
+      <c r="M21">
+        <v>0.01</v>
+      </c>
+      <c r="N21">
+        <v>0.02</v>
+      </c>
+      <c r="O21">
+        <v>0.05</v>
+      </c>
+      <c r="P21">
+        <v>0.05</v>
+      </c>
+      <c r="Q21">
+        <v>0.06</v>
+      </c>
+      <c r="R21">
+        <v>0.02</v>
+      </c>
+      <c r="S21">
+        <v>0.04</v>
+      </c>
+      <c r="T21">
+        <v>0.03</v>
+      </c>
+      <c r="U21">
+        <v>0.01</v>
+      </c>
+      <c r="V21">
+        <v>0.04</v>
+      </c>
+      <c r="W21">
+        <v>0.05</v>
+      </c>
+      <c r="X21">
+        <v>0.04</v>
+      </c>
+      <c r="Y21">
+        <v>0.03</v>
+      </c>
+      <c r="Z21">
+        <v>0.02</v>
+      </c>
+      <c r="AA21">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J22" t="s">
+        <v>114</v>
+      </c>
+      <c r="K22">
+        <v>7.69230769230769E-2</v>
+      </c>
+      <c r="L22">
+        <v>2.02020202020202E-2</v>
+      </c>
+      <c r="M22">
+        <v>4.49438202247191E-2</v>
+      </c>
+      <c r="N22">
+        <v>1.02040816326531E-2</v>
+      </c>
+      <c r="O22">
+        <v>2.1978021978022001E-2</v>
+      </c>
+      <c r="P22">
+        <v>2.02020202020202E-2</v>
+      </c>
+      <c r="Q22">
+        <v>2.02020202020202E-2</v>
+      </c>
+      <c r="R22">
+        <v>0.01</v>
+      </c>
+      <c r="S22">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T22">
+        <v>0.02</v>
+      </c>
+      <c r="U22">
+        <v>0.03</v>
+      </c>
+      <c r="V22">
+        <v>0.05</v>
+      </c>
+      <c r="W22">
+        <v>0.02</v>
+      </c>
+      <c r="X22">
+        <v>0.02</v>
+      </c>
+      <c r="Y22">
+        <v>0.05</v>
+      </c>
+      <c r="Z22">
+        <v>0.02</v>
+      </c>
+      <c r="AA22">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J23" t="s">
+        <v>115</v>
+      </c>
+      <c r="K23">
+        <v>0.03</v>
+      </c>
+      <c r="L23">
+        <v>0.06</v>
+      </c>
+      <c r="M23">
+        <v>0.03</v>
+      </c>
+      <c r="N23">
+        <v>0.04</v>
+      </c>
+      <c r="O23">
+        <v>0.03</v>
+      </c>
+      <c r="P23">
+        <v>0.05</v>
+      </c>
+      <c r="Q23">
+        <v>0.03</v>
+      </c>
+      <c r="R23">
+        <v>0.01</v>
+      </c>
+      <c r="S23">
+        <v>0.02</v>
+      </c>
+      <c r="T23">
+        <v>0.02</v>
+      </c>
+      <c r="U23">
+        <v>0.02</v>
+      </c>
+      <c r="V23">
+        <v>0.03</v>
+      </c>
+      <c r="W23">
+        <v>0.02</v>
+      </c>
+      <c r="X23">
+        <v>0.01</v>
+      </c>
+      <c r="Y23">
+        <v>0.03</v>
+      </c>
+      <c r="Z23">
+        <v>0.02</v>
+      </c>
+      <c r="AA23">
+        <v>0.02</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J24" t="s">
+        <v>116</v>
+      </c>
+      <c r="K24">
+        <v>0.06</v>
+      </c>
+      <c r="L24">
+        <v>0.06</v>
+      </c>
+      <c r="M24">
+        <v>0.04</v>
+      </c>
+      <c r="N24">
+        <v>0.02</v>
+      </c>
+      <c r="O24">
+        <v>0.06</v>
+      </c>
+      <c r="P24">
+        <v>0.05</v>
+      </c>
+      <c r="Q24">
+        <v>0.06</v>
+      </c>
+      <c r="R24">
+        <v>0.03</v>
+      </c>
+      <c r="S24">
+        <v>0.04</v>
+      </c>
+      <c r="T24">
+        <v>0.05</v>
+      </c>
+      <c r="U24">
+        <v>0.04</v>
+      </c>
+      <c r="V24">
+        <v>0.04</v>
+      </c>
+      <c r="W24">
+        <v>0.05</v>
+      </c>
+      <c r="X24">
+        <v>0.03</v>
+      </c>
+      <c r="Y24">
+        <v>0.02</v>
+      </c>
+      <c r="Z24">
+        <v>0.05</v>
+      </c>
+      <c r="AA24">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J25" t="s">
+        <v>117</v>
+      </c>
+      <c r="K25">
+        <v>0.06</v>
+      </c>
+      <c r="L25">
+        <v>0.06</v>
+      </c>
+      <c r="M25">
+        <v>0.01</v>
+      </c>
+      <c r="N25">
+        <v>0.03</v>
+      </c>
+      <c r="O25">
+        <v>0.06</v>
+      </c>
+      <c r="P25">
+        <v>0.06</v>
+      </c>
+      <c r="Q25">
+        <v>0.06</v>
+      </c>
+      <c r="R25">
+        <v>0.01</v>
+      </c>
+      <c r="S25">
+        <v>0.04</v>
+      </c>
+      <c r="T25">
+        <v>0.09</v>
+      </c>
+      <c r="U25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V25">
+        <v>0.01</v>
+      </c>
+      <c r="W25">
+        <v>0.04</v>
+      </c>
+      <c r="X25">
+        <v>0.04</v>
+      </c>
+      <c r="Y25">
+        <v>0.06</v>
+      </c>
+      <c r="Z25">
+        <v>0.09</v>
+      </c>
+      <c r="AA25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J26" t="s">
+        <v>118</v>
+      </c>
+      <c r="K26">
+        <v>0.06</v>
+      </c>
+      <c r="L26">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M26">
+        <v>0.06</v>
+      </c>
+      <c r="N26">
+        <v>0.03</v>
+      </c>
+      <c r="O26">
+        <v>0.06</v>
+      </c>
+      <c r="P26">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q26">
+        <v>0.06</v>
+      </c>
+      <c r="R26">
+        <v>0.01</v>
+      </c>
+      <c r="S26">
+        <v>0.02</v>
+      </c>
+      <c r="T26">
+        <v>0.02</v>
+      </c>
+      <c r="U26">
+        <v>0.04</v>
+      </c>
+      <c r="V26">
+        <v>0.03</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <v>0.02</v>
+      </c>
+      <c r="Z26">
+        <v>0.08</v>
+      </c>
+      <c r="AA26">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="11">
+        <v>45232</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>1E-3</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" t="s">
+        <v>93</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J27" t="s">
+        <v>107</v>
+      </c>
+      <c r="K27">
+        <v>0.06</v>
+      </c>
+      <c r="L27">
+        <v>0.15</v>
+      </c>
+      <c r="M27">
+        <v>0.05</v>
+      </c>
+      <c r="N27">
+        <v>0.08</v>
+      </c>
+      <c r="O27">
+        <v>0.06</v>
+      </c>
+      <c r="P27">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Q27">
+        <v>0.06</v>
+      </c>
+      <c r="R27">
+        <v>0.04</v>
+      </c>
+      <c r="S27">
+        <v>0.01</v>
+      </c>
+      <c r="T27">
+        <v>0.38</v>
+      </c>
+      <c r="U27">
+        <v>0.19</v>
+      </c>
+      <c r="V27">
+        <v>0.01</v>
+      </c>
+      <c r="W27">
+        <v>0.36</v>
+      </c>
+      <c r="X27">
+        <v>0.15</v>
+      </c>
+      <c r="Y27">
+        <v>0.05</v>
+      </c>
+      <c r="Z27">
+        <v>0.36</v>
+      </c>
+      <c r="AA27">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J28" t="s">
+        <v>108</v>
+      </c>
+      <c r="K28">
+        <v>0.05</v>
+      </c>
+      <c r="L28">
+        <v>0.06</v>
+      </c>
+      <c r="M28">
+        <v>0.01</v>
+      </c>
+      <c r="N28">
+        <v>0.08</v>
+      </c>
+      <c r="O28">
+        <v>0.05</v>
+      </c>
+      <c r="P28">
+        <v>0.06</v>
+      </c>
+      <c r="Q28">
+        <v>0.05</v>
+      </c>
+      <c r="R28">
+        <v>0.04</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0.41</v>
+      </c>
+      <c r="U28">
+        <v>0.19</v>
+      </c>
+      <c r="V28">
+        <v>0.02</v>
+      </c>
+      <c r="W28">
+        <v>0.35</v>
+      </c>
+      <c r="X28">
+        <v>0.21</v>
+      </c>
+      <c r="Y28">
+        <v>0.03</v>
+      </c>
+      <c r="Z28">
+        <v>0.43</v>
+      </c>
+      <c r="AA28">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J29" t="s">
+        <v>109</v>
+      </c>
+      <c r="K29">
+        <v>0.06</v>
+      </c>
+      <c r="L29">
+        <v>0.12</v>
+      </c>
+      <c r="M29">
+        <v>0.05</v>
+      </c>
+      <c r="N29">
+        <v>0.05</v>
+      </c>
+      <c r="O29">
+        <v>0.06</v>
+      </c>
+      <c r="P29">
+        <v>0.12</v>
+      </c>
+      <c r="Q29">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R29">
+        <v>0.02</v>
+      </c>
+      <c r="S29">
+        <v>0.04</v>
+      </c>
+      <c r="T29">
+        <v>0.48</v>
+      </c>
+      <c r="U29">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="V29">
+        <v>0.02</v>
+      </c>
+      <c r="W29">
+        <v>0.41</v>
+      </c>
+      <c r="X29">
+        <v>0.16</v>
+      </c>
+      <c r="Y29">
+        <v>0.06</v>
+      </c>
+      <c r="Z29">
+        <v>0.44</v>
+      </c>
+      <c r="AA29">
+        <v>0.26</v>
+      </c>
+      <c r="AB29" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J30" t="s">
+        <v>110</v>
+      </c>
+      <c r="K30">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L30">
+        <v>0.08</v>
+      </c>
+      <c r="M30">
+        <v>0.04</v>
+      </c>
+      <c r="N30">
+        <v>0.04</v>
+      </c>
+      <c r="O30">
+        <v>0.04</v>
+      </c>
+      <c r="P30">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q30">
+        <v>0.04</v>
+      </c>
+      <c r="R30">
+        <v>0.03</v>
+      </c>
+      <c r="S30">
+        <v>0.1</v>
+      </c>
+      <c r="T30">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="U30">
+        <v>0.21</v>
+      </c>
+      <c r="V30">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W30">
+        <v>0.27</v>
+      </c>
+      <c r="X30">
+        <v>0.15</v>
+      </c>
+      <c r="Y30">
+        <v>0.11</v>
+      </c>
+      <c r="Z30">
+        <v>0.22</v>
+      </c>
+      <c r="AA30">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J31" t="s">
+        <v>111</v>
+      </c>
+      <c r="K31">
+        <v>0.04</v>
+      </c>
+      <c r="L31">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M31">
+        <v>0.01</v>
+      </c>
+      <c r="N31">
+        <v>0.05</v>
+      </c>
+      <c r="O31">
+        <v>0.04</v>
+      </c>
+      <c r="P31">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q31">
+        <v>0.05</v>
+      </c>
+      <c r="R31">
+        <v>0.05</v>
+      </c>
+      <c r="S31">
+        <v>0.03</v>
+      </c>
+      <c r="T31">
+        <v>0.31</v>
+      </c>
+      <c r="U31">
+        <v>0.17</v>
+      </c>
+      <c r="V31">
+        <v>0.03</v>
+      </c>
+      <c r="W31">
+        <v>0.3</v>
+      </c>
+      <c r="X31">
+        <v>0.2</v>
+      </c>
+      <c r="Y31">
+        <v>0.03</v>
+      </c>
+      <c r="Z31">
+        <v>0.32</v>
+      </c>
+      <c r="AA31">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J32" t="s">
+        <v>112</v>
+      </c>
+      <c r="K32">
+        <v>0.03</v>
+      </c>
+      <c r="L32">
+        <v>0.15</v>
+      </c>
+      <c r="M32">
+        <v>0.03</v>
+      </c>
+      <c r="N32">
+        <v>0.1</v>
+      </c>
+      <c r="O32">
+        <v>0.03</v>
+      </c>
+      <c r="P32">
+        <v>0.13</v>
+      </c>
+      <c r="Q32">
+        <v>0.03</v>
+      </c>
+      <c r="R32">
+        <v>0.03</v>
+      </c>
+      <c r="S32">
+        <v>0.03</v>
+      </c>
+      <c r="T32">
+        <v>0.26</v>
+      </c>
+      <c r="U32">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V32">
+        <v>0.03</v>
+      </c>
+      <c r="W32">
+        <v>0.25</v>
+      </c>
+      <c r="X32">
+        <v>0.17</v>
+      </c>
+      <c r="Y32">
+        <v>0.05</v>
+      </c>
+      <c r="Z32">
+        <v>0.19</v>
+      </c>
+      <c r="AA32">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J33" t="s">
+        <v>113</v>
+      </c>
+      <c r="K33">
+        <v>0.05</v>
+      </c>
+      <c r="L33">
+        <v>0.12</v>
+      </c>
+      <c r="M33">
+        <v>0.01</v>
+      </c>
+      <c r="N33">
+        <v>0.06</v>
+      </c>
+      <c r="O33">
+        <v>0.05</v>
+      </c>
+      <c r="P33">
+        <v>0.12</v>
+      </c>
+      <c r="Q33">
+        <v>0.06</v>
+      </c>
+      <c r="R33">
+        <v>0.03</v>
+      </c>
+      <c r="S33">
+        <v>0.04</v>
+      </c>
+      <c r="T33">
+        <v>0.31</v>
+      </c>
+      <c r="U33">
+        <v>0.17</v>
+      </c>
+      <c r="V33">
+        <v>0.04</v>
+      </c>
+      <c r="W33">
+        <v>0.3</v>
+      </c>
+      <c r="X33">
+        <v>0.18</v>
+      </c>
+      <c r="Y33">
+        <v>0.03</v>
+      </c>
+      <c r="Z33">
+        <v>0.26</v>
+      </c>
+      <c r="AA33">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J34" t="s">
+        <v>114</v>
+      </c>
+      <c r="K34">
+        <v>7.69230769230769E-2</v>
+      </c>
+      <c r="L34">
+        <v>6.1224489795918401E-2</v>
+      </c>
+      <c r="M34">
+        <v>4.49438202247191E-2</v>
+      </c>
+      <c r="N34">
+        <v>4.1237113402061903E-2</v>
+      </c>
+      <c r="O34">
+        <v>2.1978021978022001E-2</v>
+      </c>
+      <c r="P34">
+        <v>5.10204081632653E-2</v>
+      </c>
+      <c r="Q34">
+        <v>2.02020202020202E-2</v>
+      </c>
+      <c r="R34">
+        <v>0.01</v>
+      </c>
+      <c r="S34">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T34">
+        <v>0.17</v>
+      </c>
+      <c r="U34">
+        <v>0.11</v>
+      </c>
+      <c r="V34">
+        <v>0.05</v>
+      </c>
+      <c r="W34">
+        <v>0.21</v>
+      </c>
+      <c r="X34">
+        <v>0.12</v>
+      </c>
+      <c r="Y34">
+        <v>0.05</v>
+      </c>
+      <c r="Z34">
+        <v>0.18</v>
+      </c>
+      <c r="AA34">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J35" t="s">
+        <v>115</v>
+      </c>
+      <c r="K35">
+        <v>0.03</v>
+      </c>
+      <c r="L35">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M35">
+        <v>0.03</v>
+      </c>
+      <c r="N35">
+        <v>0.08</v>
+      </c>
+      <c r="O35">
+        <v>0.03</v>
+      </c>
+      <c r="P35">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Q35">
+        <v>0.03</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>0.02</v>
+      </c>
+      <c r="T35">
+        <v>0.49</v>
+      </c>
+      <c r="U35">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="V35">
+        <v>0.03</v>
+      </c>
+      <c r="W35">
+        <v>0.44</v>
+      </c>
+      <c r="X35">
+        <v>0.2</v>
+      </c>
+      <c r="Y35">
+        <v>0.03</v>
+      </c>
+      <c r="Z35">
+        <v>0.43</v>
+      </c>
+      <c r="AA35">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J36" t="s">
+        <v>116</v>
+      </c>
+      <c r="K36">
+        <v>0.06</v>
+      </c>
+      <c r="L36">
+        <v>0.08</v>
+      </c>
+      <c r="M36">
+        <v>0.04</v>
+      </c>
+      <c r="N36">
+        <v>0.04</v>
+      </c>
+      <c r="O36">
+        <v>0.06</v>
+      </c>
+      <c r="P36">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q36">
+        <v>0.06</v>
+      </c>
+      <c r="R36">
+        <v>0.04</v>
+      </c>
+      <c r="S36">
+        <v>0.04</v>
+      </c>
+      <c r="T36">
+        <v>0.37</v>
+      </c>
+      <c r="U36">
+        <v>0.16</v>
+      </c>
+      <c r="V36">
+        <v>0.04</v>
+      </c>
+      <c r="W36">
+        <v>0.36</v>
+      </c>
+      <c r="X36">
+        <v>0.17</v>
+      </c>
+      <c r="Y36">
+        <v>0.02</v>
+      </c>
+      <c r="Z36">
+        <v>0.31</v>
+      </c>
+      <c r="AA36">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J37" t="s">
+        <v>117</v>
+      </c>
+      <c r="K37">
+        <v>0.06</v>
+      </c>
+      <c r="L37">
+        <v>0.11</v>
+      </c>
+      <c r="M37">
+        <v>0.01</v>
+      </c>
+      <c r="N37">
+        <v>0.09</v>
+      </c>
+      <c r="O37">
+        <v>0.06</v>
+      </c>
+      <c r="P37">
+        <v>0.11</v>
+      </c>
+      <c r="Q37">
+        <v>0.06</v>
+      </c>
+      <c r="R37">
+        <v>0.01</v>
+      </c>
+      <c r="S37">
+        <v>0.04</v>
+      </c>
+      <c r="T37">
+        <v>0.3</v>
+      </c>
+      <c r="U37">
+        <v>0.19</v>
+      </c>
+      <c r="V37">
+        <v>0.01</v>
+      </c>
+      <c r="W37">
+        <v>0.2</v>
+      </c>
+      <c r="X37">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Y37">
+        <v>0.06</v>
+      </c>
+      <c r="Z37">
+        <v>0.22</v>
+      </c>
+      <c r="AA37">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J38" t="s">
+        <v>118</v>
+      </c>
+      <c r="K38">
+        <v>0.06</v>
+      </c>
+      <c r="L38">
+        <v>0.13</v>
+      </c>
+      <c r="M38">
+        <v>0.06</v>
+      </c>
+      <c r="N38">
+        <v>0.05</v>
+      </c>
+      <c r="O38">
+        <v>0.06</v>
+      </c>
+      <c r="P38">
+        <v>0.13</v>
+      </c>
+      <c r="Q38">
+        <v>0.06</v>
+      </c>
+      <c r="R38">
+        <v>0.02</v>
+      </c>
+      <c r="S38">
+        <v>0.02</v>
+      </c>
+      <c r="T38">
+        <v>0.44</v>
+      </c>
+      <c r="U38">
+        <v>0.23</v>
+      </c>
+      <c r="V38">
+        <v>0.03</v>
+      </c>
+      <c r="W38">
+        <v>0.38</v>
+      </c>
+      <c r="X38">
+        <v>0.18</v>
+      </c>
+      <c r="Y38">
+        <v>0.02</v>
+      </c>
+      <c r="Z38">
+        <v>0.37</v>
+      </c>
+      <c r="AA38">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="11">
+        <v>45232</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39">
+        <v>1E-3</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F39" t="s">
+        <v>37</v>
+      </c>
+      <c r="G39" t="s">
+        <v>40</v>
+      </c>
+      <c r="H39" t="s">
+        <v>93</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J39" t="s">
+        <v>107</v>
+      </c>
+      <c r="K39">
+        <v>0.06</v>
+      </c>
+      <c r="L39">
+        <v>0.08</v>
+      </c>
+      <c r="M39">
+        <v>0.06</v>
+      </c>
+      <c r="N39">
+        <v>0.05</v>
+      </c>
+      <c r="O39">
+        <v>0.06</v>
+      </c>
+      <c r="P39">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q39">
+        <v>0.04</v>
+      </c>
+      <c r="R39">
+        <v>0.03</v>
+      </c>
+      <c r="S39">
+        <v>0.05</v>
+      </c>
+      <c r="T39">
+        <v>0.05</v>
+      </c>
+      <c r="U39">
+        <v>0.03</v>
+      </c>
+      <c r="V39">
+        <v>0.02</v>
+      </c>
+      <c r="W39">
+        <v>0.04</v>
+      </c>
+      <c r="X39">
+        <v>0.01</v>
+      </c>
+      <c r="Y39">
+        <v>0.08</v>
+      </c>
+      <c r="Z39">
+        <v>0.05</v>
+      </c>
+      <c r="AA39">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J40" t="s">
+        <v>108</v>
+      </c>
+      <c r="K40">
+        <v>0.06</v>
+      </c>
+      <c r="L40">
+        <v>0.02</v>
+      </c>
+      <c r="M40">
+        <v>0.03</v>
+      </c>
+      <c r="N40">
+        <v>0.03</v>
+      </c>
+      <c r="O40">
+        <v>0.06</v>
+      </c>
+      <c r="P40">
+        <v>0.02</v>
+      </c>
+      <c r="Q40">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R40">
+        <v>0.01</v>
+      </c>
+      <c r="S40">
+        <v>0.03</v>
+      </c>
+      <c r="T40">
+        <v>0.05</v>
+      </c>
+      <c r="U40">
+        <v>0.06</v>
+      </c>
+      <c r="V40">
+        <v>0.02</v>
+      </c>
+      <c r="W40">
+        <v>0.06</v>
+      </c>
+      <c r="X40">
+        <v>0.05</v>
+      </c>
+      <c r="Y40">
+        <v>0.05</v>
+      </c>
+      <c r="Z40">
+        <v>0.03</v>
+      </c>
+      <c r="AA40">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J41" t="s">
+        <v>109</v>
+      </c>
+      <c r="K41">
+        <v>0.08</v>
+      </c>
+      <c r="L41">
+        <v>0.06</v>
+      </c>
+      <c r="M41">
+        <v>0.03</v>
+      </c>
+      <c r="N41">
+        <v>0.05</v>
+      </c>
+      <c r="O41">
+        <v>0.08</v>
+      </c>
+      <c r="P41">
+        <v>0.06</v>
+      </c>
+      <c r="Q41">
+        <v>0.09</v>
+      </c>
+      <c r="R41">
+        <v>0.03</v>
+      </c>
+      <c r="S41">
+        <v>0.05</v>
+      </c>
+      <c r="T41">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U41">
+        <v>0.05</v>
+      </c>
+      <c r="V41">
+        <v>0.02</v>
+      </c>
+      <c r="W41">
+        <v>0.02</v>
+      </c>
+      <c r="X41">
+        <v>0.04</v>
+      </c>
+      <c r="Y41">
+        <v>0.08</v>
+      </c>
+      <c r="Z41">
+        <v>0.09</v>
+      </c>
+      <c r="AA41">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J42" t="s">
+        <v>110</v>
+      </c>
+      <c r="K42">
+        <v>0.05</v>
+      </c>
+      <c r="L42">
+        <v>0.06</v>
+      </c>
+      <c r="M42">
+        <v>0.03</v>
+      </c>
+      <c r="N42">
+        <v>0.01</v>
+      </c>
+      <c r="O42">
+        <v>0.05</v>
+      </c>
+      <c r="P42">
+        <v>0.04</v>
+      </c>
+      <c r="Q42">
+        <v>0.05</v>
+      </c>
+      <c r="R42">
+        <v>0.01</v>
+      </c>
+      <c r="S42">
+        <v>0.08</v>
+      </c>
+      <c r="T42">
+        <v>0.04</v>
+      </c>
+      <c r="U42">
+        <v>0.04</v>
+      </c>
+      <c r="V42">
+        <v>0.04</v>
+      </c>
+      <c r="W42">
+        <v>0.05</v>
+      </c>
+      <c r="X42">
+        <v>0.03</v>
+      </c>
+      <c r="Y42">
+        <v>0.11</v>
+      </c>
+      <c r="Z42">
+        <v>0.04</v>
+      </c>
+      <c r="AA42">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J43" t="s">
+        <v>111</v>
+      </c>
+      <c r="K43">
+        <v>0.04</v>
+      </c>
+      <c r="L43">
+        <v>0.03</v>
+      </c>
+      <c r="M43">
+        <v>0.01</v>
+      </c>
+      <c r="N43">
+        <v>0.01</v>
+      </c>
+      <c r="O43">
+        <v>0.04</v>
+      </c>
+      <c r="P43">
+        <v>0.03</v>
+      </c>
+      <c r="Q43">
+        <v>0.04</v>
+      </c>
+      <c r="R43">
+        <v>0.05</v>
+      </c>
+      <c r="S43">
+        <v>0.05</v>
+      </c>
+      <c r="T43">
+        <v>0.04</v>
+      </c>
+      <c r="U43">
+        <v>0.05</v>
+      </c>
+      <c r="V43">
+        <v>0.05</v>
+      </c>
+      <c r="W43">
+        <v>0.05</v>
+      </c>
+      <c r="X43">
+        <v>0.04</v>
+      </c>
+      <c r="Y43">
+        <v>0.04</v>
+      </c>
+      <c r="Z43">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA43">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J44" t="s">
+        <v>112</v>
+      </c>
+      <c r="K44">
+        <v>0.03</v>
+      </c>
+      <c r="L44">
+        <v>0.06</v>
+      </c>
+      <c r="M44">
+        <v>0.02</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0.01</v>
+      </c>
+      <c r="P44">
+        <v>0.06</v>
+      </c>
+      <c r="Q44">
+        <v>0.01</v>
+      </c>
+      <c r="R44">
+        <v>0.02</v>
+      </c>
+      <c r="S44">
+        <v>0.01</v>
+      </c>
+      <c r="T44">
+        <v>0.03</v>
+      </c>
+      <c r="U44">
+        <v>0.03</v>
+      </c>
+      <c r="V44">
+        <v>0.01</v>
+      </c>
+      <c r="W44">
+        <v>0.03</v>
+      </c>
+      <c r="X44">
+        <v>0.03</v>
+      </c>
+      <c r="Y44">
+        <v>0.02</v>
+      </c>
+      <c r="Z44">
+        <v>0.05</v>
+      </c>
+      <c r="AA44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J45" t="s">
+        <v>113</v>
+      </c>
+      <c r="K45">
+        <v>0.05</v>
+      </c>
+      <c r="L45">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M45">
+        <v>0.02</v>
+      </c>
+      <c r="N45">
+        <v>0.03</v>
+      </c>
+      <c r="O45">
+        <v>0.03</v>
+      </c>
+      <c r="P45">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q45">
+        <v>0.05</v>
+      </c>
+      <c r="R45">
+        <v>0.01</v>
+      </c>
+      <c r="S45">
+        <v>0.06</v>
+      </c>
+      <c r="T45">
+        <v>0.06</v>
+      </c>
+      <c r="U45">
+        <v>0.05</v>
+      </c>
+      <c r="V45">
+        <v>0.04</v>
+      </c>
+      <c r="W45">
+        <v>0.03</v>
+      </c>
+      <c r="X45">
+        <v>0.04</v>
+      </c>
+      <c r="Y45">
+        <v>0.05</v>
+      </c>
+      <c r="Z45">
+        <v>0.05</v>
+      </c>
+      <c r="AA45">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J46" t="s">
+        <v>114</v>
+      </c>
+      <c r="K46">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L46">
+        <v>5.2083333333333301E-2</v>
+      </c>
+      <c r="M46">
+        <v>2.7027027027027001E-2</v>
+      </c>
+      <c r="N46">
+        <v>2.1276595744680899E-2</v>
+      </c>
+      <c r="O46">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="P46">
+        <v>3.125E-2</v>
+      </c>
+      <c r="Q46">
+        <v>2.04081632653061E-2</v>
+      </c>
+      <c r="R46">
+        <v>0.02</v>
+      </c>
+      <c r="S46">
+        <v>0.06</v>
+      </c>
+      <c r="T46">
+        <v>0.02</v>
+      </c>
+      <c r="U46">
+        <v>0.04</v>
+      </c>
+      <c r="V46">
+        <v>0.05</v>
+      </c>
+      <c r="W46">
+        <v>0.04</v>
+      </c>
+      <c r="X46">
+        <v>0.03</v>
+      </c>
+      <c r="Y46">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z46">
+        <v>0.02</v>
+      </c>
+      <c r="AA46">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J47" t="s">
+        <v>115</v>
+      </c>
+      <c r="K47">
+        <v>0.01</v>
+      </c>
+      <c r="L47">
+        <v>0.06</v>
+      </c>
+      <c r="M47">
+        <v>0.02</v>
+      </c>
+      <c r="N47">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O47">
+        <v>0.01</v>
+      </c>
+      <c r="P47">
+        <v>0.06</v>
+      </c>
+      <c r="Q47">
+        <v>0.01</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>0.02</v>
+      </c>
+      <c r="T47">
+        <v>0.02</v>
+      </c>
+      <c r="U47">
+        <v>0.01</v>
+      </c>
+      <c r="V47">
+        <v>0.01</v>
+      </c>
+      <c r="W47">
+        <v>0.03</v>
+      </c>
+      <c r="X47">
+        <v>0.02</v>
+      </c>
+      <c r="Y47">
+        <v>0.02</v>
+      </c>
+      <c r="Z47">
+        <v>0.03</v>
+      </c>
+      <c r="AA47">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J48" t="s">
+        <v>116</v>
+      </c>
+      <c r="K48">
+        <v>0.03</v>
+      </c>
+      <c r="L48">
+        <v>0.05</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0.03</v>
+      </c>
+      <c r="O48">
+        <v>0.03</v>
+      </c>
+      <c r="P48">
+        <v>0.04</v>
+      </c>
+      <c r="Q48">
+        <v>0.03</v>
+      </c>
+      <c r="R48">
+        <v>0.02</v>
+      </c>
+      <c r="S48">
+        <v>0.05</v>
+      </c>
+      <c r="T48">
+        <v>0.02</v>
+      </c>
+      <c r="U48">
+        <v>0.03</v>
+      </c>
+      <c r="V48">
+        <v>0.06</v>
+      </c>
+      <c r="W48">
+        <v>0.03</v>
+      </c>
+      <c r="X48">
+        <v>0.05</v>
+      </c>
+      <c r="Y48">
+        <v>0.02</v>
+      </c>
+      <c r="Z48">
+        <v>0.05</v>
+      </c>
+      <c r="AA48">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="49" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="J49" t="s">
+        <v>117</v>
+      </c>
+      <c r="K49">
+        <v>0.08</v>
+      </c>
+      <c r="L49">
+        <v>0.08</v>
+      </c>
+      <c r="M49">
+        <v>0.04</v>
+      </c>
+      <c r="N49">
+        <v>0.03</v>
+      </c>
+      <c r="O49">
+        <v>0.06</v>
+      </c>
+      <c r="P49">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q49">
+        <v>0.06</v>
+      </c>
+      <c r="R49">
+        <v>0.01</v>
+      </c>
+      <c r="S49">
+        <v>0.01</v>
+      </c>
+      <c r="T49">
+        <v>0.08</v>
+      </c>
+      <c r="U49">
+        <v>0.06</v>
+      </c>
+      <c r="V49">
+        <v>0.01</v>
+      </c>
+      <c r="W49">
+        <v>0.05</v>
+      </c>
+      <c r="X49">
+        <v>0.06</v>
+      </c>
+      <c r="Y49">
+        <v>0.02</v>
+      </c>
+      <c r="Z49">
+        <v>0.06</v>
+      </c>
+      <c r="AA49">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="J50" t="s">
+        <v>118</v>
+      </c>
+      <c r="K50">
+        <v>0.04</v>
+      </c>
+      <c r="L50">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M50">
+        <v>0.03</v>
+      </c>
+      <c r="N50">
+        <v>0.05</v>
+      </c>
+      <c r="O50">
+        <v>0.04</v>
+      </c>
+      <c r="P50">
+        <v>0.06</v>
+      </c>
+      <c r="Q50">
+        <v>0.04</v>
+      </c>
+      <c r="R50">
+        <v>0.02</v>
+      </c>
+      <c r="S50">
+        <v>0.01</v>
+      </c>
+      <c r="T50">
+        <v>0.04</v>
+      </c>
+      <c r="U50">
+        <v>0.03</v>
+      </c>
+      <c r="V50">
+        <v>0.01</v>
+      </c>
+      <c r="W50">
+        <v>0.01</v>
+      </c>
+      <c r="X50">
+        <v>0.01</v>
+      </c>
+      <c r="Y50">
+        <v>0.01</v>
+      </c>
+      <c r="Z50">
+        <v>0.06</v>
+      </c>
+      <c r="AA50">
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
results from 100v90, 95, 99 by gene
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55E7DFA-BE26-4E9F-BCE9-1B2B20E1E09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AAD8CB-11E3-4C65-832C-6B028926FA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="122">
   <si>
     <t>Population</t>
   </si>
@@ -7067,11 +7067,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DDB312-960A-4A06-81C4-77814F5815B8}">
-  <dimension ref="A1:AB50"/>
+  <dimension ref="A1:AB86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB45" sqref="AB45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB88" sqref="AB88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9903,7 +9903,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="49" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J49" t="s">
         <v>117</v>
       </c>
@@ -9959,7 +9959,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="50" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J50" t="s">
         <v>118</v>
       </c>
@@ -10013,6 +10013,2106 @@
       </c>
       <c r="AA50">
         <v>0.04</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="11">
+        <v>45233</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51">
+        <v>1E-3</v>
+      </c>
+      <c r="D51" s="2">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F51" t="s">
+        <v>36</v>
+      </c>
+      <c r="G51" t="s">
+        <v>40</v>
+      </c>
+      <c r="H51" t="s">
+        <v>93</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J51" t="s">
+        <v>107</v>
+      </c>
+      <c r="K51">
+        <v>0.09</v>
+      </c>
+      <c r="L51">
+        <v>0.11</v>
+      </c>
+      <c r="M51">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N51">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O51">
+        <v>0.08</v>
+      </c>
+      <c r="P51">
+        <v>0.11</v>
+      </c>
+      <c r="Q51">
+        <v>0.08</v>
+      </c>
+      <c r="R51">
+        <v>0.05</v>
+      </c>
+      <c r="S51">
+        <v>0.04</v>
+      </c>
+      <c r="T51">
+        <v>0.2</v>
+      </c>
+      <c r="U51">
+        <v>0.12</v>
+      </c>
+      <c r="V51">
+        <v>0.02</v>
+      </c>
+      <c r="W51">
+        <v>0.18</v>
+      </c>
+      <c r="X51">
+        <v>0.1</v>
+      </c>
+      <c r="Y51">
+        <v>0.05</v>
+      </c>
+      <c r="Z51">
+        <v>0.13</v>
+      </c>
+      <c r="AA51">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J52" t="s">
+        <v>108</v>
+      </c>
+      <c r="K52">
+        <v>0.06</v>
+      </c>
+      <c r="L52">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>0.03</v>
+      </c>
+      <c r="O52">
+        <v>0.05</v>
+      </c>
+      <c r="P52">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q52">
+        <v>0.05</v>
+      </c>
+      <c r="R52">
+        <v>0.02</v>
+      </c>
+      <c r="S52">
+        <v>0.03</v>
+      </c>
+      <c r="T52">
+        <v>0.2</v>
+      </c>
+      <c r="U52">
+        <v>0.11</v>
+      </c>
+      <c r="V52">
+        <v>0.01</v>
+      </c>
+      <c r="W52">
+        <v>0.15</v>
+      </c>
+      <c r="X52">
+        <v>0.08</v>
+      </c>
+      <c r="Y52">
+        <v>0.05</v>
+      </c>
+      <c r="Z52">
+        <v>0.13</v>
+      </c>
+      <c r="AA52">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J53" t="s">
+        <v>109</v>
+      </c>
+      <c r="K53">
+        <v>0.02</v>
+      </c>
+      <c r="L53">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M53">
+        <v>0.01</v>
+      </c>
+      <c r="N53">
+        <v>0.08</v>
+      </c>
+      <c r="O53">
+        <v>0.02</v>
+      </c>
+      <c r="P53">
+        <v>0.06</v>
+      </c>
+      <c r="Q53">
+        <v>0.02</v>
+      </c>
+      <c r="R53">
+        <v>0.02</v>
+      </c>
+      <c r="S53">
+        <v>0.04</v>
+      </c>
+      <c r="T53">
+        <v>0.23</v>
+      </c>
+      <c r="U53">
+        <v>0.13</v>
+      </c>
+      <c r="V53">
+        <v>0.05</v>
+      </c>
+      <c r="W53">
+        <v>0.21</v>
+      </c>
+      <c r="X53">
+        <v>0.11</v>
+      </c>
+      <c r="Y53">
+        <v>0.04</v>
+      </c>
+      <c r="Z53">
+        <v>0.18</v>
+      </c>
+      <c r="AA53">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J54" t="s">
+        <v>110</v>
+      </c>
+      <c r="K54">
+        <v>0.05</v>
+      </c>
+      <c r="L54">
+        <v>0.09</v>
+      </c>
+      <c r="M54">
+        <v>0.04</v>
+      </c>
+      <c r="N54">
+        <v>0.05</v>
+      </c>
+      <c r="O54">
+        <v>0.05</v>
+      </c>
+      <c r="P54">
+        <v>0.08</v>
+      </c>
+      <c r="Q54">
+        <v>0.05</v>
+      </c>
+      <c r="R54">
+        <v>0.03</v>
+      </c>
+      <c r="S54">
+        <v>0.04</v>
+      </c>
+      <c r="T54">
+        <v>0.13</v>
+      </c>
+      <c r="U54">
+        <v>0.09</v>
+      </c>
+      <c r="V54">
+        <v>0.01</v>
+      </c>
+      <c r="W54">
+        <v>0.11</v>
+      </c>
+      <c r="X54">
+        <v>0.08</v>
+      </c>
+      <c r="Y54">
+        <v>0.03</v>
+      </c>
+      <c r="Z54">
+        <v>0.1</v>
+      </c>
+      <c r="AA54">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J55" t="s">
+        <v>111</v>
+      </c>
+      <c r="K55">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L55">
+        <v>0.1</v>
+      </c>
+      <c r="M55">
+        <v>0.03</v>
+      </c>
+      <c r="N55">
+        <v>0.05</v>
+      </c>
+      <c r="O55">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P55">
+        <v>0.11</v>
+      </c>
+      <c r="Q55">
+        <v>0.08</v>
+      </c>
+      <c r="R55">
+        <v>0.06</v>
+      </c>
+      <c r="S55">
+        <v>0.04</v>
+      </c>
+      <c r="T55">
+        <v>0.22</v>
+      </c>
+      <c r="U55">
+        <v>0.17</v>
+      </c>
+      <c r="V55">
+        <v>0.02</v>
+      </c>
+      <c r="W55">
+        <v>0.17</v>
+      </c>
+      <c r="X55">
+        <v>0.09</v>
+      </c>
+      <c r="Y55">
+        <v>0.08</v>
+      </c>
+      <c r="Z55">
+        <v>0.21</v>
+      </c>
+      <c r="AA55">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J56" t="s">
+        <v>112</v>
+      </c>
+      <c r="K56">
+        <v>0.05</v>
+      </c>
+      <c r="L56">
+        <v>0.1</v>
+      </c>
+      <c r="M56">
+        <v>0.04</v>
+      </c>
+      <c r="N56">
+        <v>0.06</v>
+      </c>
+      <c r="O56">
+        <v>0.05</v>
+      </c>
+      <c r="P56">
+        <v>0.09</v>
+      </c>
+      <c r="Q56">
+        <v>0.05</v>
+      </c>
+      <c r="R56">
+        <v>0.04</v>
+      </c>
+      <c r="S56">
+        <v>0.04</v>
+      </c>
+      <c r="T56">
+        <v>0.25</v>
+      </c>
+      <c r="U56">
+        <v>0.12</v>
+      </c>
+      <c r="V56">
+        <v>0.04</v>
+      </c>
+      <c r="W56">
+        <v>0.25</v>
+      </c>
+      <c r="X56">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Y56">
+        <v>0.05</v>
+      </c>
+      <c r="Z56">
+        <v>0.12</v>
+      </c>
+      <c r="AA56">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J57" t="s">
+        <v>113</v>
+      </c>
+      <c r="K57">
+        <v>0.04</v>
+      </c>
+      <c r="L57">
+        <v>0.09</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <v>0.05</v>
+      </c>
+      <c r="O57">
+        <v>0.03</v>
+      </c>
+      <c r="P57">
+        <v>0.09</v>
+      </c>
+      <c r="Q57">
+        <v>0.03</v>
+      </c>
+      <c r="R57">
+        <v>0.04</v>
+      </c>
+      <c r="S57">
+        <v>0.06</v>
+      </c>
+      <c r="T57">
+        <v>0.16</v>
+      </c>
+      <c r="U57">
+        <v>0.1</v>
+      </c>
+      <c r="V57">
+        <v>0.05</v>
+      </c>
+      <c r="W57">
+        <v>0.16</v>
+      </c>
+      <c r="X57">
+        <v>0.12</v>
+      </c>
+      <c r="Y57">
+        <v>0.04</v>
+      </c>
+      <c r="Z57">
+        <v>0.09</v>
+      </c>
+      <c r="AA57">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J58" t="s">
+        <v>114</v>
+      </c>
+      <c r="K58">
+        <v>5.4945054945054903E-2</v>
+      </c>
+      <c r="L58">
+        <v>0.10101010101010099</v>
+      </c>
+      <c r="M58">
+        <v>1.1235955056179799E-2</v>
+      </c>
+      <c r="N58">
+        <v>5.0505050505050497E-2</v>
+      </c>
+      <c r="O58">
+        <v>4.3956043956044001E-2</v>
+      </c>
+      <c r="P58">
+        <v>7.0707070707070704E-2</v>
+      </c>
+      <c r="Q58">
+        <v>5.10204081632653E-2</v>
+      </c>
+      <c r="R58">
+        <v>0.03</v>
+      </c>
+      <c r="S58">
+        <v>0.02</v>
+      </c>
+      <c r="T58">
+        <v>0.11</v>
+      </c>
+      <c r="U58">
+        <v>0.09</v>
+      </c>
+      <c r="V58">
+        <v>0.04</v>
+      </c>
+      <c r="W58">
+        <v>0.11</v>
+      </c>
+      <c r="X58">
+        <v>0.1</v>
+      </c>
+      <c r="Y58">
+        <v>0.04</v>
+      </c>
+      <c r="Z58">
+        <v>0.11</v>
+      </c>
+      <c r="AA58">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J59" t="s">
+        <v>115</v>
+      </c>
+      <c r="K59">
+        <v>0.04</v>
+      </c>
+      <c r="L59">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M59">
+        <v>0.01</v>
+      </c>
+      <c r="N59">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O59">
+        <v>0.04</v>
+      </c>
+      <c r="P59">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Q59">
+        <v>0.04</v>
+      </c>
+      <c r="R59">
+        <v>0.03</v>
+      </c>
+      <c r="S59">
+        <v>0.02</v>
+      </c>
+      <c r="T59">
+        <v>0.21</v>
+      </c>
+      <c r="U59">
+        <v>0.08</v>
+      </c>
+      <c r="V59">
+        <v>0.02</v>
+      </c>
+      <c r="W59">
+        <v>0.21</v>
+      </c>
+      <c r="X59">
+        <v>0.11</v>
+      </c>
+      <c r="Y59">
+        <v>0.02</v>
+      </c>
+      <c r="Z59">
+        <v>0.17</v>
+      </c>
+      <c r="AA59">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J60" t="s">
+        <v>116</v>
+      </c>
+      <c r="K60">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L60">
+        <v>0.12</v>
+      </c>
+      <c r="M60">
+        <v>0.04</v>
+      </c>
+      <c r="N60">
+        <v>0.09</v>
+      </c>
+      <c r="O60">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P60">
+        <v>0.11</v>
+      </c>
+      <c r="Q60">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R60">
+        <v>0.02</v>
+      </c>
+      <c r="S60">
+        <v>0.03</v>
+      </c>
+      <c r="T60">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U60">
+        <v>0.08</v>
+      </c>
+      <c r="V60">
+        <v>0.01</v>
+      </c>
+      <c r="W60">
+        <v>0.18</v>
+      </c>
+      <c r="X60">
+        <v>0.08</v>
+      </c>
+      <c r="Y60">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z60">
+        <v>0.11</v>
+      </c>
+      <c r="AA60">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J61" t="s">
+        <v>117</v>
+      </c>
+      <c r="K61">
+        <v>0.05</v>
+      </c>
+      <c r="L61">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M61">
+        <v>0.03</v>
+      </c>
+      <c r="N61">
+        <v>0.05</v>
+      </c>
+      <c r="O61">
+        <v>0.04</v>
+      </c>
+      <c r="P61">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q61">
+        <v>0.05</v>
+      </c>
+      <c r="R61">
+        <v>0.03</v>
+      </c>
+      <c r="S61">
+        <v>0.02</v>
+      </c>
+      <c r="T61">
+        <v>0.16</v>
+      </c>
+      <c r="U61">
+        <v>0.05</v>
+      </c>
+      <c r="V61">
+        <v>0.01</v>
+      </c>
+      <c r="W61">
+        <v>0.19</v>
+      </c>
+      <c r="X61">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y61">
+        <v>0.03</v>
+      </c>
+      <c r="Z61">
+        <v>0.13</v>
+      </c>
+      <c r="AA61">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J62" t="s">
+        <v>118</v>
+      </c>
+      <c r="K62">
+        <v>0.02</v>
+      </c>
+      <c r="L62">
+        <v>0.08</v>
+      </c>
+      <c r="M62">
+        <v>0.08</v>
+      </c>
+      <c r="N62">
+        <v>0.05</v>
+      </c>
+      <c r="O62">
+        <v>0.02</v>
+      </c>
+      <c r="P62">
+        <v>0.08</v>
+      </c>
+      <c r="Q62">
+        <v>0.02</v>
+      </c>
+      <c r="R62">
+        <v>0.01</v>
+      </c>
+      <c r="S62">
+        <v>0.02</v>
+      </c>
+      <c r="T62">
+        <v>0.23</v>
+      </c>
+      <c r="U62">
+        <v>0.09</v>
+      </c>
+      <c r="V62">
+        <v>0.01</v>
+      </c>
+      <c r="W62">
+        <v>0.24</v>
+      </c>
+      <c r="X62">
+        <v>0.12</v>
+      </c>
+      <c r="Y62">
+        <v>0.03</v>
+      </c>
+      <c r="Z62">
+        <v>0.17</v>
+      </c>
+      <c r="AA62">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="11">
+        <v>45233</v>
+      </c>
+      <c r="B63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63">
+        <v>1E-3</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1</v>
+      </c>
+      <c r="E63" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="F63" t="s">
+        <v>35</v>
+      </c>
+      <c r="G63" t="s">
+        <v>40</v>
+      </c>
+      <c r="H63" t="s">
+        <v>93</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J63" t="s">
+        <v>107</v>
+      </c>
+      <c r="K63">
+        <v>0.04</v>
+      </c>
+      <c r="L63">
+        <v>0.06</v>
+      </c>
+      <c r="M63">
+        <v>0.02</v>
+      </c>
+      <c r="N63">
+        <v>0.03</v>
+      </c>
+      <c r="O63">
+        <v>0.04</v>
+      </c>
+      <c r="P63">
+        <v>0.06</v>
+      </c>
+      <c r="Q63">
+        <v>0.04</v>
+      </c>
+      <c r="R63">
+        <v>0.03</v>
+      </c>
+      <c r="S63">
+        <v>0</v>
+      </c>
+      <c r="T63">
+        <v>0.17</v>
+      </c>
+      <c r="U63">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V63">
+        <v>0.01</v>
+      </c>
+      <c r="W63">
+        <v>0.2</v>
+      </c>
+      <c r="X63">
+        <v>0.08</v>
+      </c>
+      <c r="Y63">
+        <v>0</v>
+      </c>
+      <c r="Z63">
+        <v>0.08</v>
+      </c>
+      <c r="AA63">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J64" t="s">
+        <v>108</v>
+      </c>
+      <c r="K64">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L64">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M64">
+        <v>0.03</v>
+      </c>
+      <c r="N64">
+        <v>0.01</v>
+      </c>
+      <c r="O64">
+        <v>0.06</v>
+      </c>
+      <c r="P64">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q64">
+        <v>0.06</v>
+      </c>
+      <c r="R64">
+        <v>0.02</v>
+      </c>
+      <c r="S64">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T64">
+        <v>0.16</v>
+      </c>
+      <c r="U64">
+        <v>0.12</v>
+      </c>
+      <c r="V64">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W64">
+        <v>0.19</v>
+      </c>
+      <c r="X64">
+        <v>0.12</v>
+      </c>
+      <c r="Y64">
+        <v>0.09</v>
+      </c>
+      <c r="Z64">
+        <v>0.1</v>
+      </c>
+      <c r="AA64">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="65" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J65" t="s">
+        <v>109</v>
+      </c>
+      <c r="K65">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L65">
+        <v>0.1</v>
+      </c>
+      <c r="M65">
+        <v>0.05</v>
+      </c>
+      <c r="N65">
+        <v>0.06</v>
+      </c>
+      <c r="O65">
+        <v>0.06</v>
+      </c>
+      <c r="P65">
+        <v>0.08</v>
+      </c>
+      <c r="Q65">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R65">
+        <v>0.04</v>
+      </c>
+      <c r="S65">
+        <v>0.06</v>
+      </c>
+      <c r="T65">
+        <v>0.17</v>
+      </c>
+      <c r="U65">
+        <v>0.11</v>
+      </c>
+      <c r="V65">
+        <v>0.03</v>
+      </c>
+      <c r="W65">
+        <v>0.16</v>
+      </c>
+      <c r="X65">
+        <v>0.12</v>
+      </c>
+      <c r="Y65">
+        <v>0.06</v>
+      </c>
+      <c r="Z65">
+        <v>0.11</v>
+      </c>
+      <c r="AA65">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J66" t="s">
+        <v>110</v>
+      </c>
+      <c r="K66">
+        <v>0.05</v>
+      </c>
+      <c r="L66">
+        <v>0.04</v>
+      </c>
+      <c r="M66">
+        <v>0.02</v>
+      </c>
+      <c r="N66">
+        <v>0.04</v>
+      </c>
+      <c r="O66">
+        <v>0.05</v>
+      </c>
+      <c r="P66">
+        <v>0.04</v>
+      </c>
+      <c r="Q66">
+        <v>0.04</v>
+      </c>
+      <c r="R66">
+        <v>0.03</v>
+      </c>
+      <c r="S66">
+        <v>0.04</v>
+      </c>
+      <c r="T66">
+        <v>0.15</v>
+      </c>
+      <c r="U66">
+        <v>0.06</v>
+      </c>
+      <c r="V66">
+        <v>0.03</v>
+      </c>
+      <c r="W66">
+        <v>0.15</v>
+      </c>
+      <c r="X66">
+        <v>0.08</v>
+      </c>
+      <c r="Y66">
+        <v>0.02</v>
+      </c>
+      <c r="Z66">
+        <v>0.1</v>
+      </c>
+      <c r="AA66">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J67" t="s">
+        <v>111</v>
+      </c>
+      <c r="K67">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L67">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M67">
+        <v>0.03</v>
+      </c>
+      <c r="N67">
+        <v>0.02</v>
+      </c>
+      <c r="O67">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P67">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q67">
+        <v>0.08</v>
+      </c>
+      <c r="R67">
+        <v>0.02</v>
+      </c>
+      <c r="S67">
+        <v>0.03</v>
+      </c>
+      <c r="T67">
+        <v>0.13</v>
+      </c>
+      <c r="U67">
+        <v>0.09</v>
+      </c>
+      <c r="V67">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W67">
+        <v>0.12</v>
+      </c>
+      <c r="X67">
+        <v>0.1</v>
+      </c>
+      <c r="Y67">
+        <v>0.04</v>
+      </c>
+      <c r="Z67">
+        <v>0.1</v>
+      </c>
+      <c r="AA67">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J68" t="s">
+        <v>112</v>
+      </c>
+      <c r="K68">
+        <v>0.03</v>
+      </c>
+      <c r="L68">
+        <v>0.1</v>
+      </c>
+      <c r="M68">
+        <v>0.03</v>
+      </c>
+      <c r="N68">
+        <v>0.03</v>
+      </c>
+      <c r="O68">
+        <v>0.03</v>
+      </c>
+      <c r="P68">
+        <v>0.1</v>
+      </c>
+      <c r="Q68">
+        <v>0.03</v>
+      </c>
+      <c r="R68">
+        <v>0.03</v>
+      </c>
+      <c r="S68">
+        <v>0.04</v>
+      </c>
+      <c r="T68">
+        <v>0.15</v>
+      </c>
+      <c r="U68">
+        <v>0.1</v>
+      </c>
+      <c r="V68">
+        <v>0.02</v>
+      </c>
+      <c r="W68">
+        <v>0.13</v>
+      </c>
+      <c r="X68">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y68">
+        <v>0.03</v>
+      </c>
+      <c r="Z68">
+        <v>0.08</v>
+      </c>
+      <c r="AA68">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J69" t="s">
+        <v>113</v>
+      </c>
+      <c r="K69">
+        <v>0.06</v>
+      </c>
+      <c r="L69">
+        <v>0.08</v>
+      </c>
+      <c r="M69">
+        <v>0.03</v>
+      </c>
+      <c r="N69">
+        <v>0.06</v>
+      </c>
+      <c r="O69">
+        <v>0.06</v>
+      </c>
+      <c r="P69">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q69">
+        <v>0.06</v>
+      </c>
+      <c r="R69">
+        <v>0.05</v>
+      </c>
+      <c r="S69">
+        <v>0.04</v>
+      </c>
+      <c r="T69">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U69">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V69">
+        <v>0.02</v>
+      </c>
+      <c r="W69">
+        <v>0.11</v>
+      </c>
+      <c r="X69">
+        <v>0.04</v>
+      </c>
+      <c r="Y69">
+        <v>0.05</v>
+      </c>
+      <c r="Z69">
+        <v>0.12</v>
+      </c>
+      <c r="AA69">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J70" t="s">
+        <v>114</v>
+      </c>
+      <c r="K70">
+        <v>6.25E-2</v>
+      </c>
+      <c r="L70">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M70">
+        <v>2.1505376344085999E-2</v>
+      </c>
+      <c r="N70">
+        <v>0.04</v>
+      </c>
+      <c r="O70">
+        <v>3.125E-2</v>
+      </c>
+      <c r="P70">
+        <v>0.06</v>
+      </c>
+      <c r="Q70">
+        <v>0.03</v>
+      </c>
+      <c r="R70">
+        <v>0</v>
+      </c>
+      <c r="S70">
+        <v>0.02</v>
+      </c>
+      <c r="T70">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U70">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V70">
+        <v>0.04</v>
+      </c>
+      <c r="W70">
+        <v>0.15</v>
+      </c>
+      <c r="X70">
+        <v>0.09</v>
+      </c>
+      <c r="Y70">
+        <v>0.05</v>
+      </c>
+      <c r="Z70">
+        <v>0.13</v>
+      </c>
+      <c r="AA70">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J71" t="s">
+        <v>115</v>
+      </c>
+      <c r="K71">
+        <v>0.03</v>
+      </c>
+      <c r="L71">
+        <v>0.06</v>
+      </c>
+      <c r="M71">
+        <v>0.01</v>
+      </c>
+      <c r="N71">
+        <v>0.08</v>
+      </c>
+      <c r="O71">
+        <v>0.03</v>
+      </c>
+      <c r="P71">
+        <v>0.06</v>
+      </c>
+      <c r="Q71">
+        <v>0.03</v>
+      </c>
+      <c r="R71">
+        <v>0.03</v>
+      </c>
+      <c r="S71">
+        <v>0.05</v>
+      </c>
+      <c r="T71">
+        <v>0.18</v>
+      </c>
+      <c r="U71">
+        <v>0.1</v>
+      </c>
+      <c r="V71">
+        <v>0.04</v>
+      </c>
+      <c r="W71">
+        <v>0.21</v>
+      </c>
+      <c r="X71">
+        <v>0.08</v>
+      </c>
+      <c r="Y71">
+        <v>0.04</v>
+      </c>
+      <c r="Z71">
+        <v>0.12</v>
+      </c>
+      <c r="AA71">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J72" t="s">
+        <v>116</v>
+      </c>
+      <c r="K72">
+        <v>0.09</v>
+      </c>
+      <c r="L72">
+        <v>0.11</v>
+      </c>
+      <c r="M72">
+        <v>0.03</v>
+      </c>
+      <c r="N72">
+        <v>0.01</v>
+      </c>
+      <c r="O72">
+        <v>0.09</v>
+      </c>
+      <c r="P72">
+        <v>0.1</v>
+      </c>
+      <c r="Q72">
+        <v>0.1</v>
+      </c>
+      <c r="R72">
+        <v>0.04</v>
+      </c>
+      <c r="S72">
+        <v>0.03</v>
+      </c>
+      <c r="T72">
+        <v>0.13</v>
+      </c>
+      <c r="U72">
+        <v>0.08</v>
+      </c>
+      <c r="V72">
+        <v>0.01</v>
+      </c>
+      <c r="W72">
+        <v>0.13</v>
+      </c>
+      <c r="X72">
+        <v>0.05</v>
+      </c>
+      <c r="Y72">
+        <v>0.06</v>
+      </c>
+      <c r="Z72">
+        <v>0.11</v>
+      </c>
+      <c r="AA72">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="73" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J73" t="s">
+        <v>117</v>
+      </c>
+      <c r="K73">
+        <v>0.06</v>
+      </c>
+      <c r="L73">
+        <v>0.08</v>
+      </c>
+      <c r="M73">
+        <v>0.02</v>
+      </c>
+      <c r="N73">
+        <v>0.04</v>
+      </c>
+      <c r="O73">
+        <v>0.05</v>
+      </c>
+      <c r="P73">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q73">
+        <v>0.04</v>
+      </c>
+      <c r="R73">
+        <v>0.01</v>
+      </c>
+      <c r="S73">
+        <v>0.01</v>
+      </c>
+      <c r="T73">
+        <v>0.2</v>
+      </c>
+      <c r="U73">
+        <v>0.09</v>
+      </c>
+      <c r="V73">
+        <v>0.02</v>
+      </c>
+      <c r="W73">
+        <v>0.16</v>
+      </c>
+      <c r="X73">
+        <v>0.1</v>
+      </c>
+      <c r="Y73">
+        <v>0.08</v>
+      </c>
+      <c r="Z73">
+        <v>0.11</v>
+      </c>
+      <c r="AA73">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="74" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J74" t="s">
+        <v>118</v>
+      </c>
+      <c r="K74">
+        <v>0.04</v>
+      </c>
+      <c r="L74">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M74">
+        <v>0.02</v>
+      </c>
+      <c r="N74">
+        <v>0.05</v>
+      </c>
+      <c r="O74">
+        <v>0.03</v>
+      </c>
+      <c r="P74">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q74">
+        <v>0.03</v>
+      </c>
+      <c r="R74">
+        <v>0.02</v>
+      </c>
+      <c r="S74">
+        <v>0</v>
+      </c>
+      <c r="T74">
+        <v>0.15</v>
+      </c>
+      <c r="U74">
+        <v>0.1</v>
+      </c>
+      <c r="V74">
+        <v>0.02</v>
+      </c>
+      <c r="W74">
+        <v>0.17</v>
+      </c>
+      <c r="X74">
+        <v>0.09</v>
+      </c>
+      <c r="Y74">
+        <v>0.02</v>
+      </c>
+      <c r="Z74">
+        <v>0.09</v>
+      </c>
+      <c r="AA74">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A75" s="11">
+        <v>45233</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75">
+        <v>1E-3</v>
+      </c>
+      <c r="D75" s="2">
+        <v>1</v>
+      </c>
+      <c r="E75" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F75" t="s">
+        <v>34</v>
+      </c>
+      <c r="G75" t="s">
+        <v>40</v>
+      </c>
+      <c r="H75" t="s">
+        <v>93</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J75" t="s">
+        <v>107</v>
+      </c>
+      <c r="K75">
+        <v>0.03</v>
+      </c>
+      <c r="L75">
+        <v>0.08</v>
+      </c>
+      <c r="M75">
+        <v>0.05</v>
+      </c>
+      <c r="N75">
+        <v>0.05</v>
+      </c>
+      <c r="O75">
+        <v>0.03</v>
+      </c>
+      <c r="P75">
+        <v>0.08</v>
+      </c>
+      <c r="Q75">
+        <v>0.04</v>
+      </c>
+      <c r="R75">
+        <v>0.03</v>
+      </c>
+      <c r="S75">
+        <v>0.02</v>
+      </c>
+      <c r="T75">
+        <v>0.11</v>
+      </c>
+      <c r="U75">
+        <v>0.06</v>
+      </c>
+      <c r="V75">
+        <v>0.02</v>
+      </c>
+      <c r="W75">
+        <v>0.12</v>
+      </c>
+      <c r="X75">
+        <v>0.08</v>
+      </c>
+      <c r="Y75">
+        <v>0.04</v>
+      </c>
+      <c r="Z75">
+        <v>0.06</v>
+      </c>
+      <c r="AA75">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J76" t="s">
+        <v>108</v>
+      </c>
+      <c r="K76">
+        <v>0.02</v>
+      </c>
+      <c r="L76">
+        <v>0.04</v>
+      </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+      <c r="N76">
+        <v>0.01</v>
+      </c>
+      <c r="O76">
+        <v>0.02</v>
+      </c>
+      <c r="P76">
+        <v>0.04</v>
+      </c>
+      <c r="Q76">
+        <v>0.02</v>
+      </c>
+      <c r="R76">
+        <v>0.01</v>
+      </c>
+      <c r="S76">
+        <v>0.03</v>
+      </c>
+      <c r="T76">
+        <v>0.11</v>
+      </c>
+      <c r="U76">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V76">
+        <v>0.01</v>
+      </c>
+      <c r="W76">
+        <v>0.11</v>
+      </c>
+      <c r="X76">
+        <v>0.05</v>
+      </c>
+      <c r="Y76">
+        <v>0.03</v>
+      </c>
+      <c r="Z76">
+        <v>0.09</v>
+      </c>
+      <c r="AA76">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J77" t="s">
+        <v>109</v>
+      </c>
+      <c r="K77">
+        <v>0.09</v>
+      </c>
+      <c r="L77">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M77">
+        <v>0.06</v>
+      </c>
+      <c r="N77">
+        <v>0.06</v>
+      </c>
+      <c r="O77">
+        <v>0.09</v>
+      </c>
+      <c r="P77">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q77">
+        <v>0.09</v>
+      </c>
+      <c r="R77">
+        <v>0.03</v>
+      </c>
+      <c r="S77">
+        <v>0.04</v>
+      </c>
+      <c r="T77">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U77">
+        <v>0.04</v>
+      </c>
+      <c r="V77">
+        <v>0.08</v>
+      </c>
+      <c r="W77">
+        <v>0.05</v>
+      </c>
+      <c r="X77">
+        <v>0.03</v>
+      </c>
+      <c r="Y77">
+        <v>0.03</v>
+      </c>
+      <c r="Z77">
+        <v>0.05</v>
+      </c>
+      <c r="AA77">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="78" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J78" t="s">
+        <v>110</v>
+      </c>
+      <c r="K78">
+        <v>0.04</v>
+      </c>
+      <c r="L78">
+        <v>0.03</v>
+      </c>
+      <c r="M78">
+        <v>0.04</v>
+      </c>
+      <c r="N78">
+        <v>0.03</v>
+      </c>
+      <c r="O78">
+        <v>0.04</v>
+      </c>
+      <c r="P78">
+        <v>0.03</v>
+      </c>
+      <c r="Q78">
+        <v>0.04</v>
+      </c>
+      <c r="R78">
+        <v>0.05</v>
+      </c>
+      <c r="S78">
+        <v>0.02</v>
+      </c>
+      <c r="T78">
+        <v>0.06</v>
+      </c>
+      <c r="U78">
+        <v>0.05</v>
+      </c>
+      <c r="V78">
+        <v>0.02</v>
+      </c>
+      <c r="W78">
+        <v>0.1</v>
+      </c>
+      <c r="X78">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y78">
+        <v>0</v>
+      </c>
+      <c r="Z78">
+        <v>0.03</v>
+      </c>
+      <c r="AA78">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="79" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J79" t="s">
+        <v>111</v>
+      </c>
+      <c r="K79">
+        <v>0.03</v>
+      </c>
+      <c r="L79">
+        <v>0.04</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+      <c r="N79">
+        <v>0.03</v>
+      </c>
+      <c r="O79">
+        <v>0.03</v>
+      </c>
+      <c r="P79">
+        <v>0.04</v>
+      </c>
+      <c r="Q79">
+        <v>0.02</v>
+      </c>
+      <c r="R79">
+        <v>0.02</v>
+      </c>
+      <c r="S79">
+        <v>0.03</v>
+      </c>
+      <c r="T79">
+        <v>0.03</v>
+      </c>
+      <c r="U79">
+        <v>0.03</v>
+      </c>
+      <c r="V79">
+        <v>0.06</v>
+      </c>
+      <c r="W79">
+        <v>0.06</v>
+      </c>
+      <c r="X79">
+        <v>0.04</v>
+      </c>
+      <c r="Y79">
+        <v>0.02</v>
+      </c>
+      <c r="Z79">
+        <v>0.02</v>
+      </c>
+      <c r="AA79">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="80" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J80" t="s">
+        <v>112</v>
+      </c>
+      <c r="K80">
+        <v>0.01</v>
+      </c>
+      <c r="L80">
+        <v>0.06</v>
+      </c>
+      <c r="M80">
+        <v>0</v>
+      </c>
+      <c r="N80">
+        <v>0.02</v>
+      </c>
+      <c r="O80">
+        <v>0.01</v>
+      </c>
+      <c r="P80">
+        <v>0.05</v>
+      </c>
+      <c r="Q80">
+        <v>0.01</v>
+      </c>
+      <c r="R80">
+        <v>0</v>
+      </c>
+      <c r="S80">
+        <v>0.04</v>
+      </c>
+      <c r="T80">
+        <v>0.05</v>
+      </c>
+      <c r="U80">
+        <v>0.01</v>
+      </c>
+      <c r="V80">
+        <v>0.06</v>
+      </c>
+      <c r="W80">
+        <v>0.05</v>
+      </c>
+      <c r="X80">
+        <v>0</v>
+      </c>
+      <c r="Y80">
+        <v>0.04</v>
+      </c>
+      <c r="Z80">
+        <v>0.04</v>
+      </c>
+      <c r="AA80">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="81" spans="10:28" x14ac:dyDescent="0.3">
+      <c r="J81" t="s">
+        <v>113</v>
+      </c>
+      <c r="K81">
+        <v>0.02</v>
+      </c>
+      <c r="L81">
+        <v>0.03</v>
+      </c>
+      <c r="M81">
+        <v>0.04</v>
+      </c>
+      <c r="N81">
+        <v>0.03</v>
+      </c>
+      <c r="O81">
+        <v>0.02</v>
+      </c>
+      <c r="P81">
+        <v>0.03</v>
+      </c>
+      <c r="Q81">
+        <v>0.03</v>
+      </c>
+      <c r="R81">
+        <v>0.02</v>
+      </c>
+      <c r="S81">
+        <v>0.02</v>
+      </c>
+      <c r="T81">
+        <v>0.08</v>
+      </c>
+      <c r="U81">
+        <v>0.05</v>
+      </c>
+      <c r="V81">
+        <v>0.04</v>
+      </c>
+      <c r="W81">
+        <v>0.06</v>
+      </c>
+      <c r="X81">
+        <v>0.03</v>
+      </c>
+      <c r="Y81">
+        <v>0.04</v>
+      </c>
+      <c r="Z81">
+        <v>0.04</v>
+      </c>
+      <c r="AA81">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="82" spans="10:28" x14ac:dyDescent="0.3">
+      <c r="J82" t="s">
+        <v>114</v>
+      </c>
+      <c r="K82">
+        <v>7.8651685393258397E-2</v>
+      </c>
+      <c r="L82">
+        <v>5.1546391752577303E-2</v>
+      </c>
+      <c r="M82">
+        <v>8.04597701149425E-2</v>
+      </c>
+      <c r="N82">
+        <v>2.06185567010309E-2</v>
+      </c>
+      <c r="O82">
+        <v>6.7415730337078594E-2</v>
+      </c>
+      <c r="P82">
+        <v>3.09278350515464E-2</v>
+      </c>
+      <c r="Q82">
+        <v>6.0606060606060601E-2</v>
+      </c>
+      <c r="R82">
+        <v>0.02</v>
+      </c>
+      <c r="S82">
+        <v>0.04</v>
+      </c>
+      <c r="T82">
+        <v>0.06</v>
+      </c>
+      <c r="U82">
+        <v>0.05</v>
+      </c>
+      <c r="V82">
+        <v>0.03</v>
+      </c>
+      <c r="W82">
+        <v>0.06</v>
+      </c>
+      <c r="X82">
+        <v>0.03</v>
+      </c>
+      <c r="Y82">
+        <v>0.04</v>
+      </c>
+      <c r="Z82">
+        <v>0.05</v>
+      </c>
+      <c r="AA82">
+        <v>0.06</v>
+      </c>
+      <c r="AB82" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83" spans="10:28" x14ac:dyDescent="0.3">
+      <c r="J83" t="s">
+        <v>115</v>
+      </c>
+      <c r="K83">
+        <v>0.04</v>
+      </c>
+      <c r="L83">
+        <v>0.1</v>
+      </c>
+      <c r="M83">
+        <v>0.02</v>
+      </c>
+      <c r="N83">
+        <v>0.08</v>
+      </c>
+      <c r="O83">
+        <v>0.04</v>
+      </c>
+      <c r="P83">
+        <v>0.1</v>
+      </c>
+      <c r="Q83">
+        <v>0.04</v>
+      </c>
+      <c r="R83">
+        <v>0</v>
+      </c>
+      <c r="S83">
+        <v>0.02</v>
+      </c>
+      <c r="T83">
+        <v>0.1</v>
+      </c>
+      <c r="U83">
+        <v>0.06</v>
+      </c>
+      <c r="V83">
+        <v>0.01</v>
+      </c>
+      <c r="W83">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="X83">
+        <v>0.03</v>
+      </c>
+      <c r="Y83">
+        <v>0.03</v>
+      </c>
+      <c r="Z83">
+        <v>0.08</v>
+      </c>
+      <c r="AA83">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="84" spans="10:28" x14ac:dyDescent="0.3">
+      <c r="J84" t="s">
+        <v>116</v>
+      </c>
+      <c r="K84">
+        <v>0.06</v>
+      </c>
+      <c r="L84">
+        <v>0.04</v>
+      </c>
+      <c r="M84">
+        <v>0.03</v>
+      </c>
+      <c r="N84">
+        <v>0.05</v>
+      </c>
+      <c r="O84">
+        <v>0.06</v>
+      </c>
+      <c r="P84">
+        <v>0.04</v>
+      </c>
+      <c r="Q84">
+        <v>0.06</v>
+      </c>
+      <c r="R84">
+        <v>0.02</v>
+      </c>
+      <c r="S84">
+        <v>0.02</v>
+      </c>
+      <c r="T84">
+        <v>0.13</v>
+      </c>
+      <c r="U84">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V84">
+        <v>0.01</v>
+      </c>
+      <c r="W84">
+        <v>0.09</v>
+      </c>
+      <c r="X84">
+        <v>0.09</v>
+      </c>
+      <c r="Y84">
+        <v>0.04</v>
+      </c>
+      <c r="Z84">
+        <v>0.09</v>
+      </c>
+      <c r="AA84">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="10:28" x14ac:dyDescent="0.3">
+      <c r="J85" t="s">
+        <v>117</v>
+      </c>
+      <c r="K85">
+        <v>0.1</v>
+      </c>
+      <c r="L85">
+        <v>0.15</v>
+      </c>
+      <c r="M85">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N85">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O85">
+        <v>0.1</v>
+      </c>
+      <c r="P85">
+        <v>0.16</v>
+      </c>
+      <c r="Q85">
+        <v>0.1</v>
+      </c>
+      <c r="R85">
+        <v>0.03</v>
+      </c>
+      <c r="S85">
+        <v>0.06</v>
+      </c>
+      <c r="T85">
+        <v>0.09</v>
+      </c>
+      <c r="U85">
+        <v>0.06</v>
+      </c>
+      <c r="V85">
+        <v>0.04</v>
+      </c>
+      <c r="W85">
+        <v>0.06</v>
+      </c>
+      <c r="X85">
+        <v>0.04</v>
+      </c>
+      <c r="Y85">
+        <v>0.06</v>
+      </c>
+      <c r="Z85">
+        <v>0.09</v>
+      </c>
+      <c r="AA85">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="86" spans="10:28" x14ac:dyDescent="0.3">
+      <c r="J86" t="s">
+        <v>118</v>
+      </c>
+      <c r="K86">
+        <v>0.05</v>
+      </c>
+      <c r="L86">
+        <v>0.05</v>
+      </c>
+      <c r="M86">
+        <v>0.02</v>
+      </c>
+      <c r="N86">
+        <v>0.03</v>
+      </c>
+      <c r="O86">
+        <v>0.05</v>
+      </c>
+      <c r="P86">
+        <v>0.05</v>
+      </c>
+      <c r="Q86">
+        <v>0.05</v>
+      </c>
+      <c r="R86">
+        <v>0.03</v>
+      </c>
+      <c r="S86">
+        <v>0.01</v>
+      </c>
+      <c r="T86">
+        <v>0.13</v>
+      </c>
+      <c r="U86">
+        <v>0.06</v>
+      </c>
+      <c r="V86">
+        <v>0.02</v>
+      </c>
+      <c r="W86">
+        <v>0.13</v>
+      </c>
+      <c r="X86">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y86">
+        <v>0.03</v>
+      </c>
+      <c r="Z86">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA86">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
power and t1e results from 140v100v80 pruning scneario
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5137AF5-C342-43E6-91BE-FCD063A86976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE53C76-14B7-44B8-8D72-3C46B75F5525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="128">
   <si>
     <t>Population</t>
   </si>
@@ -595,6 +595,27 @@
 120% fun 100% syn
 internal controls: 100% fun 100% syn</t>
   </si>
+  <si>
+    <t>140v100v80</t>
+  </si>
+  <si>
+    <t>1. Separately-RAREsim v2.1.1
+--functional_bins 140%
+--synonymous_bins 100%
+2. RAREsim v2.1.1: Convert 140% fun 100% syn pruned hap file to .sm file using convert.py
+3. Sequentially-RAREsimv2.1.1
+--f_only 100% 6 MAC bins
+4. RAREsim v2.1.1: Convert 100% fun 100% syn pruned hap file to .sm file using convert .py 
+5. Separately-RAREsim v2.1.1
+--functional_bins 80% 6 MAC BINS
+--synonymous_bins 80% 6 MAC BINS
+6. R: add pruned variants back in as rows of 0 and extract datasets</t>
+  </si>
+  <si>
+    <t>cases: 
+140% fun 100% syn
+internal controls: 100% fun 100% syn</t>
+  </si>
 </sst>
 </file>
 
@@ -693,12 +714,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7096,11 +7117,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DDB312-960A-4A06-81C4-77814F5815B8}">
-  <dimension ref="A1:AD95"/>
+  <dimension ref="A1:AD104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G92" sqref="G92"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I97" sqref="I97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12680,6 +12701,537 @@
         <v>0.25</v>
       </c>
     </row>
+    <row r="96" spans="1:28" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A96" s="11">
+        <v>45243</v>
+      </c>
+      <c r="B96" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96">
+        <v>1E-3</v>
+      </c>
+      <c r="D96" s="2">
+        <v>1</v>
+      </c>
+      <c r="E96" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F96" t="s">
+        <v>125</v>
+      </c>
+      <c r="G96" t="s">
+        <v>40</v>
+      </c>
+      <c r="H96" t="s">
+        <v>93</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J96" t="s">
+        <v>107</v>
+      </c>
+      <c r="K96">
+        <v>0.04</v>
+      </c>
+      <c r="L96">
+        <v>0.1</v>
+      </c>
+      <c r="M96">
+        <v>0.05</v>
+      </c>
+      <c r="N96">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O96">
+        <v>0.04</v>
+      </c>
+      <c r="P96">
+        <v>0.1</v>
+      </c>
+      <c r="Q96">
+        <v>0.04</v>
+      </c>
+      <c r="R96">
+        <v>0.02</v>
+      </c>
+      <c r="S96">
+        <v>0.05</v>
+      </c>
+      <c r="T96">
+        <v>0.46</v>
+      </c>
+      <c r="U96">
+        <v>0.25</v>
+      </c>
+      <c r="V96">
+        <v>0.04</v>
+      </c>
+      <c r="W96">
+        <v>0.38</v>
+      </c>
+      <c r="X96">
+        <v>0.18</v>
+      </c>
+      <c r="Y96">
+        <v>0.02</v>
+      </c>
+      <c r="Z96">
+        <v>0.38</v>
+      </c>
+      <c r="AA96">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="97" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="J97" t="s">
+        <v>110</v>
+      </c>
+      <c r="K97">
+        <v>0.05</v>
+      </c>
+      <c r="L97">
+        <v>0.11</v>
+      </c>
+      <c r="M97">
+        <v>0.01</v>
+      </c>
+      <c r="N97">
+        <v>0.05</v>
+      </c>
+      <c r="O97">
+        <v>0.02</v>
+      </c>
+      <c r="P97">
+        <v>0.1</v>
+      </c>
+      <c r="Q97">
+        <v>0.02</v>
+      </c>
+      <c r="R97">
+        <v>0.03</v>
+      </c>
+      <c r="S97">
+        <v>0.03</v>
+      </c>
+      <c r="T97">
+        <v>0.31</v>
+      </c>
+      <c r="U97">
+        <v>0.19</v>
+      </c>
+      <c r="V97">
+        <v>0.01</v>
+      </c>
+      <c r="W97">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="X97">
+        <v>0.18</v>
+      </c>
+      <c r="Y97">
+        <v>0.05</v>
+      </c>
+      <c r="Z97">
+        <v>0.27</v>
+      </c>
+      <c r="AA97">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="98" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="J98" t="s">
+        <v>111</v>
+      </c>
+      <c r="K98">
+        <v>0.02</v>
+      </c>
+      <c r="L98">
+        <v>0.08</v>
+      </c>
+      <c r="M98">
+        <v>0.01</v>
+      </c>
+      <c r="N98">
+        <v>0.06</v>
+      </c>
+      <c r="O98">
+        <v>0.02</v>
+      </c>
+      <c r="P98">
+        <v>0.08</v>
+      </c>
+      <c r="Q98">
+        <v>0.03</v>
+      </c>
+      <c r="R98">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S98">
+        <v>0.05</v>
+      </c>
+      <c r="T98">
+        <v>0.19</v>
+      </c>
+      <c r="U98">
+        <v>0.11</v>
+      </c>
+      <c r="V98">
+        <v>0.05</v>
+      </c>
+      <c r="W98">
+        <v>0.2</v>
+      </c>
+      <c r="X98">
+        <v>0.13</v>
+      </c>
+      <c r="Y98">
+        <v>0.04</v>
+      </c>
+      <c r="Z98">
+        <v>0.16</v>
+      </c>
+      <c r="AA98">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="99" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="J99" t="s">
+        <v>112</v>
+      </c>
+      <c r="K99">
+        <v>0.03</v>
+      </c>
+      <c r="L99">
+        <v>0.09</v>
+      </c>
+      <c r="M99">
+        <v>0.02</v>
+      </c>
+      <c r="N99">
+        <v>0.02</v>
+      </c>
+      <c r="O99">
+        <v>0.03</v>
+      </c>
+      <c r="P99">
+        <v>0.08</v>
+      </c>
+      <c r="Q99">
+        <v>0.03</v>
+      </c>
+      <c r="R99">
+        <v>0.02</v>
+      </c>
+      <c r="S99">
+        <v>0.01</v>
+      </c>
+      <c r="T99">
+        <v>0.24</v>
+      </c>
+      <c r="U99">
+        <v>0.11</v>
+      </c>
+      <c r="V99">
+        <v>0.01</v>
+      </c>
+      <c r="W99">
+        <v>0.24</v>
+      </c>
+      <c r="X99">
+        <v>0.13</v>
+      </c>
+      <c r="Y99">
+        <v>0.02</v>
+      </c>
+      <c r="Z99">
+        <v>0.17</v>
+      </c>
+      <c r="AA99">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="100" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="J100" t="s">
+        <v>113</v>
+      </c>
+      <c r="K100">
+        <v>0.03</v>
+      </c>
+      <c r="L100">
+        <v>0.09</v>
+      </c>
+      <c r="M100">
+        <v>0</v>
+      </c>
+      <c r="N100">
+        <v>0.04</v>
+      </c>
+      <c r="O100">
+        <v>0.03</v>
+      </c>
+      <c r="P100">
+        <v>0.09</v>
+      </c>
+      <c r="Q100">
+        <v>0.03</v>
+      </c>
+      <c r="R100">
+        <v>0.04</v>
+      </c>
+      <c r="S100">
+        <v>0.01</v>
+      </c>
+      <c r="T100">
+        <v>0.26</v>
+      </c>
+      <c r="U100">
+        <v>0.16</v>
+      </c>
+      <c r="V100">
+        <v>0</v>
+      </c>
+      <c r="W100">
+        <v>0.22</v>
+      </c>
+      <c r="X100">
+        <v>0.11</v>
+      </c>
+      <c r="Y100">
+        <v>0.05</v>
+      </c>
+      <c r="Z100">
+        <v>0.21</v>
+      </c>
+      <c r="AA100">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="101" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="J101" t="s">
+        <v>114</v>
+      </c>
+      <c r="K101">
+        <v>4.4444444444444398E-2</v>
+      </c>
+      <c r="L101">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="M101">
+        <v>3.4883720930232599E-2</v>
+      </c>
+      <c r="N101">
+        <v>4.2553191489361701E-2</v>
+      </c>
+      <c r="O101">
+        <v>3.3333333333333298E-2</v>
+      </c>
+      <c r="P101">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q101">
+        <v>3.06122448979592E-2</v>
+      </c>
+      <c r="R101">
+        <v>0</v>
+      </c>
+      <c r="S101">
+        <v>0.03</v>
+      </c>
+      <c r="T101">
+        <v>0.23</v>
+      </c>
+      <c r="U101">
+        <v>0.11</v>
+      </c>
+      <c r="V101">
+        <v>0.04</v>
+      </c>
+      <c r="W101">
+        <v>0.24</v>
+      </c>
+      <c r="X101">
+        <v>0.13</v>
+      </c>
+      <c r="Y101">
+        <v>0.06</v>
+      </c>
+      <c r="Z101">
+        <v>0.17</v>
+      </c>
+      <c r="AA101">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="102" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="J102" t="s">
+        <v>115</v>
+      </c>
+      <c r="K102">
+        <v>0.05</v>
+      </c>
+      <c r="L102">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M102">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N102">
+        <v>0.09</v>
+      </c>
+      <c r="O102">
+        <v>0.05</v>
+      </c>
+      <c r="P102">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q102">
+        <v>0.05</v>
+      </c>
+      <c r="R102">
+        <v>0.05</v>
+      </c>
+      <c r="S102">
+        <v>0.05</v>
+      </c>
+      <c r="T102">
+        <v>0.5</v>
+      </c>
+      <c r="U102">
+        <v>0.3</v>
+      </c>
+      <c r="V102">
+        <v>0.05</v>
+      </c>
+      <c r="W102">
+        <v>0.46</v>
+      </c>
+      <c r="X102">
+        <v>0.23</v>
+      </c>
+      <c r="Y102">
+        <v>0.04</v>
+      </c>
+      <c r="Z102">
+        <v>0.4</v>
+      </c>
+      <c r="AA102">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="103" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="J103" t="s">
+        <v>116</v>
+      </c>
+      <c r="K103">
+        <v>0.03</v>
+      </c>
+      <c r="L103">
+        <v>0.09</v>
+      </c>
+      <c r="M103">
+        <v>0.01</v>
+      </c>
+      <c r="N103">
+        <v>0.04</v>
+      </c>
+      <c r="O103">
+        <v>0.03</v>
+      </c>
+      <c r="P103">
+        <v>0.08</v>
+      </c>
+      <c r="Q103">
+        <v>0.04</v>
+      </c>
+      <c r="R103">
+        <v>0.03</v>
+      </c>
+      <c r="S103">
+        <v>0.04</v>
+      </c>
+      <c r="T103">
+        <v>0.32</v>
+      </c>
+      <c r="U103">
+        <v>0.16</v>
+      </c>
+      <c r="V103">
+        <v>0.05</v>
+      </c>
+      <c r="W103">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="X103">
+        <v>0.2</v>
+      </c>
+      <c r="Y103">
+        <v>0.04</v>
+      </c>
+      <c r="Z103">
+        <v>0.27</v>
+      </c>
+      <c r="AA103">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="104" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="J104" t="s">
+        <v>118</v>
+      </c>
+      <c r="K104">
+        <v>0.06</v>
+      </c>
+      <c r="L104">
+        <v>0.16</v>
+      </c>
+      <c r="M104">
+        <v>0.05</v>
+      </c>
+      <c r="N104">
+        <v>0.09</v>
+      </c>
+      <c r="O104">
+        <v>0.06</v>
+      </c>
+      <c r="P104">
+        <v>0.16</v>
+      </c>
+      <c r="Q104">
+        <v>0.06</v>
+      </c>
+      <c r="R104">
+        <v>0.05</v>
+      </c>
+      <c r="S104">
+        <v>0.03</v>
+      </c>
+      <c r="T104">
+        <v>0.47</v>
+      </c>
+      <c r="U104">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="V104">
+        <v>0.04</v>
+      </c>
+      <c r="W104">
+        <v>0.41</v>
+      </c>
+      <c r="X104">
+        <v>0.26</v>
+      </c>
+      <c r="Y104">
+        <v>0.01</v>
+      </c>
+      <c r="Z104">
+        <v>0.42</v>
+      </c>
+      <c r="AA104">
+        <v>0.26</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="K1:AA1"/>
@@ -12691,11 +13243,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5E01F1-9A92-4DEF-99E5-C0BF38433A3D}">
-  <dimension ref="A1:AB5"/>
+  <dimension ref="A1:AB8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12713,18 +13265,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
       <c r="K1" s="12" t="s">
         <v>20</v>
       </c>
@@ -13027,6 +13579,201 @@
         <v>0.43</v>
       </c>
     </row>
+    <row r="6" spans="1:28" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>45243</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>1E-3</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J6" t="s">
+        <v>108</v>
+      </c>
+      <c r="K6">
+        <v>0.25</v>
+      </c>
+      <c r="L6">
+        <v>0.27</v>
+      </c>
+      <c r="M6">
+        <v>0.11</v>
+      </c>
+      <c r="N6">
+        <v>0.1</v>
+      </c>
+      <c r="O6">
+        <v>0.25</v>
+      </c>
+      <c r="P6">
+        <v>0.27</v>
+      </c>
+      <c r="Q6">
+        <v>0.24</v>
+      </c>
+      <c r="R6">
+        <v>0.52</v>
+      </c>
+      <c r="S6">
+        <v>0.59</v>
+      </c>
+      <c r="T6">
+        <v>0.96</v>
+      </c>
+      <c r="U6">
+        <v>0.93</v>
+      </c>
+      <c r="V6">
+        <v>0.39</v>
+      </c>
+      <c r="W6">
+        <v>0.85</v>
+      </c>
+      <c r="X6">
+        <v>0.79</v>
+      </c>
+      <c r="Y6">
+        <v>0.6</v>
+      </c>
+      <c r="Z6">
+        <v>0.96</v>
+      </c>
+      <c r="AA6">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>109</v>
+      </c>
+      <c r="K7">
+        <v>0.2</v>
+      </c>
+      <c r="L7">
+        <v>0.33</v>
+      </c>
+      <c r="M7">
+        <v>0.09</v>
+      </c>
+      <c r="N7">
+        <v>0.18</v>
+      </c>
+      <c r="O7">
+        <v>0.2</v>
+      </c>
+      <c r="P7">
+        <v>0.33</v>
+      </c>
+      <c r="Q7">
+        <v>0.2</v>
+      </c>
+      <c r="R7">
+        <v>0.61</v>
+      </c>
+      <c r="S7">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="T7">
+        <v>0.99</v>
+      </c>
+      <c r="U7">
+        <v>0.99</v>
+      </c>
+      <c r="V7">
+        <v>0.37</v>
+      </c>
+      <c r="W7">
+        <v>0.87</v>
+      </c>
+      <c r="X7">
+        <v>0.9</v>
+      </c>
+      <c r="Y7">
+        <v>0.6</v>
+      </c>
+      <c r="Z7">
+        <v>0.95</v>
+      </c>
+      <c r="AA7">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K8">
+        <v>0.18</v>
+      </c>
+      <c r="L8">
+        <v>0.25</v>
+      </c>
+      <c r="M8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N8">
+        <v>0.15</v>
+      </c>
+      <c r="O8">
+        <v>0.17</v>
+      </c>
+      <c r="P8">
+        <v>0.25</v>
+      </c>
+      <c r="Q8">
+        <v>0.18</v>
+      </c>
+      <c r="R8">
+        <v>0.31</v>
+      </c>
+      <c r="S8">
+        <v>0.36</v>
+      </c>
+      <c r="T8">
+        <v>0.81</v>
+      </c>
+      <c r="U8">
+        <v>0.73</v>
+      </c>
+      <c r="V8">
+        <v>0.26</v>
+      </c>
+      <c r="W8">
+        <v>0.67</v>
+      </c>
+      <c r="X8">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Y8">
+        <v>0.37</v>
+      </c>
+      <c r="Z8">
+        <v>0.79</v>
+      </c>
+      <c r="AA8">
+        <v>0.76</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="K1:AA1"/>

</xml_diff>

<commit_message>
power and t1e results for 160v100v80 by gene
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE53C76-14B7-44B8-8D72-3C46B75F5525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4FB87A-B78A-436D-BDEE-4D9DFA0AB347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="131">
   <si>
     <t>Population</t>
   </si>
@@ -488,9 +488,6 @@
     <t>Gene</t>
   </si>
   <si>
-    <t>Megan's Haplotype</t>
-  </si>
-  <si>
     <t>ProxECAT Internal</t>
   </si>
   <si>
@@ -614,6 +611,30 @@
   <si>
     <t>cases: 
 140% fun 100% syn
+internal controls: 100% fun 100% syn</t>
+  </si>
+  <si>
+    <t>160v100v80</t>
+  </si>
+  <si>
+    <t>1. Separately-RAREsim v2.1.1
+--functional_bins 160%
+--synonymous_bins 100%
+2. RAREsim v2.1.1: Convert 160% fun 100% syn pruned hap file to .sm file using convert.py
+3. Sequentially-RAREsimv2.1.1
+--f_only 100% 6 MAC bins
+4. RAREsim v2.1.1: Convert 100% fun 100% syn pruned hap file to .sm file using convert .py 
+5. Separately-RAREsim v2.1.1
+--functional_bins 80% 6 MAC BINS
+--synonymous_bins 80% 6 MAC BINS
+6. R: add pruned variants back in as rows of 0 and extract datasets</t>
+  </si>
+  <si>
+    <t>Megan's Haplotypes</t>
+  </si>
+  <si>
+    <t>cases: 
+160% fun 100% syn
 internal controls: 100% fun 100% syn</t>
   </si>
 </sst>
@@ -1037,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660476C5-A4B0-4780-BD43-FC7746B114D2}">
   <dimension ref="A1:AL59"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
@@ -7117,11 +7138,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DDB312-960A-4A06-81C4-77814F5815B8}">
-  <dimension ref="A1:AD104"/>
+  <dimension ref="A1:AD113"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I97" sqref="I97"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB108" sqref="AB108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7132,7 +7153,7 @@
     <col min="5" max="5" width="14.5546875" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1"/>
     <col min="9" max="9" width="30.77734375" customWidth="1"/>
     <col min="10" max="10" width="13.44140625" customWidth="1"/>
     <col min="13" max="13" width="12.21875" customWidth="1"/>
@@ -7205,16 +7226,16 @@
         <v>92</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>12</v>
@@ -7226,37 +7247,37 @@
         <v>13</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AA2" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="AB2" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="162" customHeight="1" x14ac:dyDescent="0.3">
@@ -7282,13 +7303,13 @@
         <v>40</v>
       </c>
       <c r="H3" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>59</v>
       </c>
       <c r="J3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K3">
         <v>0.06</v>
@@ -7342,7 +7363,7 @@
         <v>0.21</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AD3" t="s">
         <v>84</v>
@@ -7350,7 +7371,7 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="J4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K4">
         <v>0.05</v>
@@ -7406,7 +7427,7 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="J5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K5">
         <v>0.06</v>
@@ -7462,7 +7483,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="J6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K6">
         <v>7.0000000000000007E-2</v>
@@ -7518,7 +7539,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="J7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K7">
         <v>0.04</v>
@@ -7574,7 +7595,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="J8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K8">
         <v>0.03</v>
@@ -7630,7 +7651,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="J9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K9">
         <v>0.05</v>
@@ -7686,7 +7707,7 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="J10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K10">
         <v>0.09</v>
@@ -7742,7 +7763,7 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="J11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K11">
         <v>0.03</v>
@@ -7798,7 +7819,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="J12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K12">
         <v>0.06</v>
@@ -7854,7 +7875,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="J13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K13">
         <v>0.06</v>
@@ -7910,7 +7931,7 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="J14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K14">
         <v>0.06</v>
@@ -7987,13 +8008,13 @@
         <v>40</v>
       </c>
       <c r="H15" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>59</v>
       </c>
       <c r="J15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K15">
         <v>0.06</v>
@@ -8047,12 +8068,12 @@
         <v>0.05</v>
       </c>
       <c r="AB15" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="J16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K16">
         <v>0.05</v>
@@ -8108,7 +8129,7 @@
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K17">
         <v>0.06</v>
@@ -8164,7 +8185,7 @@
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K18">
         <v>7.0000000000000007E-2</v>
@@ -8220,7 +8241,7 @@
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K19">
         <v>0.04</v>
@@ -8276,7 +8297,7 @@
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K20">
         <v>0.03</v>
@@ -8332,7 +8353,7 @@
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K21">
         <v>0.05</v>
@@ -8388,7 +8409,7 @@
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K22">
         <v>7.69230769230769E-2</v>
@@ -8444,7 +8465,7 @@
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K23">
         <v>0.03</v>
@@ -8503,7 +8524,7 @@
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K24">
         <v>0.06</v>
@@ -8559,7 +8580,7 @@
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K25">
         <v>0.06</v>
@@ -8615,7 +8636,7 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K26">
         <v>0.06</v>
@@ -8692,13 +8713,13 @@
         <v>40</v>
       </c>
       <c r="H27" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>59</v>
       </c>
       <c r="J27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K27">
         <v>0.06</v>
@@ -8754,7 +8775,7 @@
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K28">
         <v>0.05</v>
@@ -8810,7 +8831,7 @@
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K29">
         <v>0.06</v>
@@ -8869,7 +8890,7 @@
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K30">
         <v>7.0000000000000007E-2</v>
@@ -8925,7 +8946,7 @@
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K31">
         <v>0.04</v>
@@ -8981,7 +9002,7 @@
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K32">
         <v>0.03</v>
@@ -9037,7 +9058,7 @@
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K33">
         <v>0.05</v>
@@ -9093,7 +9114,7 @@
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K34">
         <v>7.69230769230769E-2</v>
@@ -9149,7 +9170,7 @@
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K35">
         <v>0.03</v>
@@ -9205,7 +9226,7 @@
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K36">
         <v>0.06</v>
@@ -9261,7 +9282,7 @@
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K37">
         <v>0.06</v>
@@ -9317,7 +9338,7 @@
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K38">
         <v>0.06</v>
@@ -9394,13 +9415,13 @@
         <v>40</v>
       </c>
       <c r="H39" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>59</v>
       </c>
       <c r="J39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K39">
         <v>0.06</v>
@@ -9456,7 +9477,7 @@
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K40">
         <v>0.06</v>
@@ -9512,7 +9533,7 @@
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K41">
         <v>0.08</v>
@@ -9568,7 +9589,7 @@
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K42">
         <v>0.05</v>
@@ -9624,7 +9645,7 @@
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K43">
         <v>0.04</v>
@@ -9680,7 +9701,7 @@
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K44">
         <v>0.03</v>
@@ -9736,7 +9757,7 @@
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K45">
         <v>0.05</v>
@@ -9792,7 +9813,7 @@
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K46">
         <v>2.5000000000000001E-2</v>
@@ -9848,7 +9869,7 @@
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K47">
         <v>0.01</v>
@@ -9904,7 +9925,7 @@
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K48">
         <v>0.03</v>
@@ -9960,7 +9981,7 @@
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K49">
         <v>0.08</v>
@@ -10016,7 +10037,7 @@
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K50">
         <v>0.04</v>
@@ -10093,13 +10114,13 @@
         <v>40</v>
       </c>
       <c r="H51" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>90</v>
       </c>
       <c r="J51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K51">
         <v>0.09</v>
@@ -10155,7 +10176,7 @@
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K52">
         <v>0.06</v>
@@ -10211,7 +10232,7 @@
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J53" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K53">
         <v>0.02</v>
@@ -10267,7 +10288,7 @@
     </row>
     <row r="54" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K54">
         <v>0.05</v>
@@ -10323,7 +10344,7 @@
     </row>
     <row r="55" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K55">
         <v>7.0000000000000007E-2</v>
@@ -10379,7 +10400,7 @@
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K56">
         <v>0.05</v>
@@ -10435,7 +10456,7 @@
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K57">
         <v>0.04</v>
@@ -10491,7 +10512,7 @@
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K58">
         <v>5.4945054945054903E-2</v>
@@ -10547,7 +10568,7 @@
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K59">
         <v>0.04</v>
@@ -10603,7 +10624,7 @@
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J60" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K60">
         <v>7.0000000000000007E-2</v>
@@ -10659,7 +10680,7 @@
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J61" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K61">
         <v>0.05</v>
@@ -10715,7 +10736,7 @@
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J62" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K62">
         <v>0.02</v>
@@ -10792,13 +10813,13 @@
         <v>40</v>
       </c>
       <c r="H63" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>91</v>
       </c>
       <c r="J63" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K63">
         <v>0.04</v>
@@ -10854,7 +10875,7 @@
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J64" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K64">
         <v>7.0000000000000007E-2</v>
@@ -10910,7 +10931,7 @@
     </row>
     <row r="65" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K65">
         <v>7.0000000000000007E-2</v>
@@ -10966,7 +10987,7 @@
     </row>
     <row r="66" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J66" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K66">
         <v>0.05</v>
@@ -11022,7 +11043,7 @@
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J67" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K67">
         <v>7.0000000000000007E-2</v>
@@ -11078,7 +11099,7 @@
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J68" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K68">
         <v>0.03</v>
@@ -11134,7 +11155,7 @@
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J69" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K69">
         <v>0.06</v>
@@ -11190,7 +11211,7 @@
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J70" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K70">
         <v>6.25E-2</v>
@@ -11246,7 +11267,7 @@
     </row>
     <row r="71" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J71" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K71">
         <v>0.03</v>
@@ -11302,7 +11323,7 @@
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J72" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K72">
         <v>0.09</v>
@@ -11358,7 +11379,7 @@
     </row>
     <row r="73" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J73" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K73">
         <v>0.06</v>
@@ -11414,7 +11435,7 @@
     </row>
     <row r="74" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J74" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K74">
         <v>0.04</v>
@@ -11491,13 +11512,13 @@
         <v>40</v>
       </c>
       <c r="H75" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>60</v>
       </c>
       <c r="J75" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K75">
         <v>0.03</v>
@@ -11553,7 +11574,7 @@
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J76" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K76">
         <v>0.02</v>
@@ -11609,7 +11630,7 @@
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J77" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K77">
         <v>0.09</v>
@@ -11665,7 +11686,7 @@
     </row>
     <row r="78" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J78" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K78">
         <v>0.04</v>
@@ -11721,7 +11742,7 @@
     </row>
     <row r="79" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K79">
         <v>0.03</v>
@@ -11777,7 +11798,7 @@
     </row>
     <row r="80" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J80" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K80">
         <v>0.01</v>
@@ -11833,7 +11854,7 @@
     </row>
     <row r="81" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J81" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K81">
         <v>0.02</v>
@@ -11889,7 +11910,7 @@
     </row>
     <row r="82" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J82" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K82">
         <v>7.8651685393258397E-2</v>
@@ -11948,7 +11969,7 @@
     </row>
     <row r="83" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J83" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K83">
         <v>0.04</v>
@@ -12004,7 +12025,7 @@
     </row>
     <row r="84" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J84" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K84">
         <v>0.06</v>
@@ -12060,7 +12081,7 @@
     </row>
     <row r="85" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J85" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K85">
         <v>0.1</v>
@@ -12116,7 +12137,7 @@
     </row>
     <row r="86" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J86" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K86">
         <v>0.05</v>
@@ -12187,19 +12208,19 @@
         <v>0.8</v>
       </c>
       <c r="F87" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G87" t="s">
         <v>40</v>
       </c>
       <c r="H87" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J87" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K87">
         <v>0.02</v>
@@ -12255,7 +12276,7 @@
     </row>
     <row r="88" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J88" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K88">
         <v>0.05</v>
@@ -12311,7 +12332,7 @@
     </row>
     <row r="89" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J89" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K89">
         <v>0.06</v>
@@ -12367,7 +12388,7 @@
     </row>
     <row r="90" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J90" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K90">
         <v>7.0000000000000007E-2</v>
@@ -12423,7 +12444,7 @@
     </row>
     <row r="91" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J91" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K91">
         <v>0.08</v>
@@ -12479,7 +12500,7 @@
     </row>
     <row r="92" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J92" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K92">
         <v>7.5268817204301106E-2</v>
@@ -12535,7 +12556,7 @@
     </row>
     <row r="93" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J93" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K93">
         <v>0.06</v>
@@ -12591,7 +12612,7 @@
     </row>
     <row r="94" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J94" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K94">
         <v>0.05</v>
@@ -12647,7 +12668,7 @@
     </row>
     <row r="95" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J95" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K95">
         <v>7.0000000000000007E-2</v>
@@ -12718,19 +12739,19 @@
         <v>0.8</v>
       </c>
       <c r="F96" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G96" t="s">
         <v>40</v>
       </c>
       <c r="H96" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J96" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K96">
         <v>0.04</v>
@@ -12784,9 +12805,9 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="97" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J97" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K97">
         <v>0.05</v>
@@ -12840,9 +12861,9 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="98" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J98" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K98">
         <v>0.02</v>
@@ -12896,9 +12917,9 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="99" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J99" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K99">
         <v>0.03</v>
@@ -12952,9 +12973,9 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="100" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J100" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K100">
         <v>0.03</v>
@@ -13008,9 +13029,9 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="101" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J101" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K101">
         <v>4.4444444444444398E-2</v>
@@ -13064,9 +13085,9 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="102" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J102" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K102">
         <v>0.05</v>
@@ -13120,9 +13141,9 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="103" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J103" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K103">
         <v>0.03</v>
@@ -13176,9 +13197,9 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="104" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J104" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K104">
         <v>0.06</v>
@@ -13230,6 +13251,537 @@
       </c>
       <c r="AA104">
         <v>0.26</v>
+      </c>
+    </row>
+    <row r="105" spans="1:27" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A105" s="11">
+        <v>45245</v>
+      </c>
+      <c r="B105" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105">
+        <v>1E-3</v>
+      </c>
+      <c r="D105" s="2">
+        <v>1</v>
+      </c>
+      <c r="E105" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F105" t="s">
+        <v>127</v>
+      </c>
+      <c r="G105" t="s">
+        <v>40</v>
+      </c>
+      <c r="H105" t="s">
+        <v>129</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J105" t="s">
+        <v>106</v>
+      </c>
+      <c r="K105">
+        <v>0.03</v>
+      </c>
+      <c r="L105">
+        <v>0.09</v>
+      </c>
+      <c r="M105">
+        <v>0.03</v>
+      </c>
+      <c r="N105">
+        <v>0.13</v>
+      </c>
+      <c r="O105">
+        <v>0.03</v>
+      </c>
+      <c r="P105">
+        <v>0.09</v>
+      </c>
+      <c r="Q105">
+        <v>0.03</v>
+      </c>
+      <c r="R105">
+        <v>0.04</v>
+      </c>
+      <c r="S105">
+        <v>0.05</v>
+      </c>
+      <c r="T105">
+        <v>0.5</v>
+      </c>
+      <c r="U105">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="V105">
+        <v>0.05</v>
+      </c>
+      <c r="W105">
+        <v>0.44</v>
+      </c>
+      <c r="X105">
+        <v>0.23</v>
+      </c>
+      <c r="Y105">
+        <v>0.05</v>
+      </c>
+      <c r="Z105">
+        <v>0.4</v>
+      </c>
+      <c r="AA105">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="106" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J106" t="s">
+        <v>109</v>
+      </c>
+      <c r="K106">
+        <v>0.04</v>
+      </c>
+      <c r="L106">
+        <v>0.1</v>
+      </c>
+      <c r="M106">
+        <v>0.01</v>
+      </c>
+      <c r="N106">
+        <v>0.04</v>
+      </c>
+      <c r="O106">
+        <v>0.04</v>
+      </c>
+      <c r="P106">
+        <v>0.1</v>
+      </c>
+      <c r="Q106">
+        <v>0.05</v>
+      </c>
+      <c r="R106">
+        <v>0.08</v>
+      </c>
+      <c r="S106">
+        <v>0.09</v>
+      </c>
+      <c r="T106">
+        <v>0.32</v>
+      </c>
+      <c r="U106">
+        <v>0.19</v>
+      </c>
+      <c r="V106">
+        <v>0.05</v>
+      </c>
+      <c r="W106">
+        <v>0.3</v>
+      </c>
+      <c r="X106">
+        <v>0.19</v>
+      </c>
+      <c r="Y106">
+        <v>0.09</v>
+      </c>
+      <c r="Z106">
+        <v>0.32</v>
+      </c>
+      <c r="AA106">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="107" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J107" t="s">
+        <v>110</v>
+      </c>
+      <c r="K107">
+        <v>0.08</v>
+      </c>
+      <c r="L107">
+        <v>0.15</v>
+      </c>
+      <c r="M107">
+        <v>0.06</v>
+      </c>
+      <c r="N107">
+        <v>0.06</v>
+      </c>
+      <c r="O107">
+        <v>0.06</v>
+      </c>
+      <c r="P107">
+        <v>0.15</v>
+      </c>
+      <c r="Q107">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R107">
+        <v>0.06</v>
+      </c>
+      <c r="S107">
+        <v>0.05</v>
+      </c>
+      <c r="T107">
+        <v>0.35</v>
+      </c>
+      <c r="U107">
+        <v>0.17</v>
+      </c>
+      <c r="V107">
+        <v>0.06</v>
+      </c>
+      <c r="W107">
+        <v>0.36</v>
+      </c>
+      <c r="X107">
+        <v>0.19</v>
+      </c>
+      <c r="Y107">
+        <v>0.02</v>
+      </c>
+      <c r="Z107">
+        <v>0.21</v>
+      </c>
+      <c r="AA107">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="108" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J108" t="s">
+        <v>111</v>
+      </c>
+      <c r="K108">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L108">
+        <v>0.13</v>
+      </c>
+      <c r="M108">
+        <v>0.05</v>
+      </c>
+      <c r="N108">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O108">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P108">
+        <v>0.12</v>
+      </c>
+      <c r="Q108">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R108">
+        <v>0.03</v>
+      </c>
+      <c r="S108">
+        <v>0.04</v>
+      </c>
+      <c r="T108">
+        <v>0.31</v>
+      </c>
+      <c r="U108">
+        <v>0.19</v>
+      </c>
+      <c r="V108">
+        <v>0.04</v>
+      </c>
+      <c r="W108">
+        <v>0.3</v>
+      </c>
+      <c r="X108">
+        <v>0.15</v>
+      </c>
+      <c r="Y108">
+        <v>0</v>
+      </c>
+      <c r="Z108">
+        <v>0.26</v>
+      </c>
+      <c r="AA108">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J109" t="s">
+        <v>112</v>
+      </c>
+      <c r="K109">
+        <v>0.08</v>
+      </c>
+      <c r="L109">
+        <v>0.18</v>
+      </c>
+      <c r="M109">
+        <v>0.04</v>
+      </c>
+      <c r="N109">
+        <v>0.11</v>
+      </c>
+      <c r="O109">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P109">
+        <v>0.18</v>
+      </c>
+      <c r="Q109">
+        <v>0.08</v>
+      </c>
+      <c r="R109">
+        <v>0.03</v>
+      </c>
+      <c r="S109">
+        <v>0.05</v>
+      </c>
+      <c r="T109">
+        <v>0.3</v>
+      </c>
+      <c r="U109">
+        <v>0.19</v>
+      </c>
+      <c r="V109">
+        <v>0.01</v>
+      </c>
+      <c r="W109">
+        <v>0.27</v>
+      </c>
+      <c r="X109">
+        <v>0.15</v>
+      </c>
+      <c r="Y109">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z109">
+        <v>0.23</v>
+      </c>
+      <c r="AA109">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="110" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J110" t="s">
+        <v>113</v>
+      </c>
+      <c r="K110">
+        <v>4.3478260869565202E-2</v>
+      </c>
+      <c r="L110">
+        <v>8.1632653061224497E-2</v>
+      </c>
+      <c r="M110">
+        <v>2.27272727272727E-2</v>
+      </c>
+      <c r="N110">
+        <v>5.1546391752577303E-2</v>
+      </c>
+      <c r="O110">
+        <v>2.1739130434782601E-2</v>
+      </c>
+      <c r="P110">
+        <v>6.1224489795918401E-2</v>
+      </c>
+      <c r="Q110">
+        <v>2.02020202020202E-2</v>
+      </c>
+      <c r="R110">
+        <v>0.02</v>
+      </c>
+      <c r="S110">
+        <v>0.03</v>
+      </c>
+      <c r="T110">
+        <v>0.23</v>
+      </c>
+      <c r="U110">
+        <v>0.11</v>
+      </c>
+      <c r="V110">
+        <v>0.04</v>
+      </c>
+      <c r="W110">
+        <v>0.18</v>
+      </c>
+      <c r="X110">
+        <v>0.12</v>
+      </c>
+      <c r="Y110">
+        <v>0.05</v>
+      </c>
+      <c r="Z110">
+        <v>0.18</v>
+      </c>
+      <c r="AA110">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="111" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J111" t="s">
+        <v>114</v>
+      </c>
+      <c r="K111">
+        <v>0.03</v>
+      </c>
+      <c r="L111">
+        <v>0.11</v>
+      </c>
+      <c r="M111">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N111">
+        <v>0.1</v>
+      </c>
+      <c r="O111">
+        <v>0.03</v>
+      </c>
+      <c r="P111">
+        <v>0.11</v>
+      </c>
+      <c r="Q111">
+        <v>0.03</v>
+      </c>
+      <c r="R111">
+        <v>0</v>
+      </c>
+      <c r="S111">
+        <v>0.01</v>
+      </c>
+      <c r="T111">
+        <v>0.46</v>
+      </c>
+      <c r="U111">
+        <v>0.27</v>
+      </c>
+      <c r="V111">
+        <v>0.01</v>
+      </c>
+      <c r="W111">
+        <v>0.4</v>
+      </c>
+      <c r="X111">
+        <v>0.21</v>
+      </c>
+      <c r="Y111">
+        <v>0.02</v>
+      </c>
+      <c r="Z111">
+        <v>0.38</v>
+      </c>
+      <c r="AA111">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="112" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J112" t="s">
+        <v>115</v>
+      </c>
+      <c r="K112">
+        <v>0.06</v>
+      </c>
+      <c r="L112">
+        <v>0.11</v>
+      </c>
+      <c r="M112">
+        <v>0.04</v>
+      </c>
+      <c r="N112">
+        <v>0.01</v>
+      </c>
+      <c r="O112">
+        <v>0.06</v>
+      </c>
+      <c r="P112">
+        <v>0.11</v>
+      </c>
+      <c r="Q112">
+        <v>0.04</v>
+      </c>
+      <c r="R112">
+        <v>0.04</v>
+      </c>
+      <c r="S112">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T112">
+        <v>0.35</v>
+      </c>
+      <c r="U112">
+        <v>0.22</v>
+      </c>
+      <c r="V112">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W112">
+        <v>0.34</v>
+      </c>
+      <c r="X112">
+        <v>0.24</v>
+      </c>
+      <c r="Y112">
+        <v>0.06</v>
+      </c>
+      <c r="Z112">
+        <v>0.3</v>
+      </c>
+      <c r="AA112">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="113" spans="10:27" x14ac:dyDescent="0.3">
+      <c r="J113" t="s">
+        <v>117</v>
+      </c>
+      <c r="K113">
+        <v>0.04</v>
+      </c>
+      <c r="L113">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M113">
+        <v>0.02</v>
+      </c>
+      <c r="N113">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O113">
+        <v>0.04</v>
+      </c>
+      <c r="P113">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q113">
+        <v>0.04</v>
+      </c>
+      <c r="R113">
+        <v>0.01</v>
+      </c>
+      <c r="S113">
+        <v>0.03</v>
+      </c>
+      <c r="T113">
+        <v>0.41</v>
+      </c>
+      <c r="U113">
+        <v>0.23</v>
+      </c>
+      <c r="V113">
+        <v>0.04</v>
+      </c>
+      <c r="W113">
+        <v>0.33</v>
+      </c>
+      <c r="X113">
+        <v>0.21</v>
+      </c>
+      <c r="Y113">
+        <v>0.04</v>
+      </c>
+      <c r="Z113">
+        <v>0.38</v>
+      </c>
+      <c r="AA113">
+        <v>0.22</v>
       </c>
     </row>
   </sheetData>
@@ -13243,11 +13795,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5E01F1-9A92-4DEF-99E5-C0BF38433A3D}">
-  <dimension ref="A1:AB8"/>
+  <dimension ref="A1:AB11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13258,7 +13810,7 @@
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
     <col min="6" max="6" width="13.21875" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" customWidth="1"/>
     <col min="9" max="9" width="35.6640625" customWidth="1"/>
     <col min="13" max="13" width="13.5546875" customWidth="1"/>
     <col min="14" max="14" width="10.109375" customWidth="1"/>
@@ -13330,16 +13882,16 @@
         <v>92</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>12</v>
@@ -13351,37 +13903,37 @@
         <v>13</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AA2" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="AB2" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="230.4" x14ac:dyDescent="0.3">
@@ -13395,25 +13947,25 @@
         <v>1E-3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3" s="2">
         <v>0.8</v>
       </c>
       <c r="F3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G3" t="s">
         <v>40</v>
       </c>
       <c r="H3" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K3">
         <v>0.12</v>
@@ -13469,7 +14021,7 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K4">
         <v>0.1</v>
@@ -13525,7 +14077,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K5">
         <v>7.0000000000000007E-2</v>
@@ -13590,25 +14142,25 @@
         <v>1E-3</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E6" s="2">
         <v>0.8</v>
       </c>
       <c r="F6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G6" t="s">
         <v>40</v>
       </c>
       <c r="H6" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K6">
         <v>0.25</v>
@@ -13664,7 +14216,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K7">
         <v>0.2</v>
@@ -13720,7 +14272,7 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="J8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K8">
         <v>0.18</v>
@@ -13772,6 +14324,201 @@
       </c>
       <c r="AA8">
         <v>0.76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>45245</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>1E-3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" t="s">
+        <v>129</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J9" t="s">
+        <v>107</v>
+      </c>
+      <c r="K9">
+        <v>0.43</v>
+      </c>
+      <c r="L9">
+        <v>0.54</v>
+      </c>
+      <c r="M9">
+        <v>0.16</v>
+      </c>
+      <c r="N9">
+        <v>0.25</v>
+      </c>
+      <c r="O9">
+        <v>0.43</v>
+      </c>
+      <c r="P9">
+        <v>0.54</v>
+      </c>
+      <c r="Q9">
+        <v>0.43</v>
+      </c>
+      <c r="R9">
+        <v>0.78</v>
+      </c>
+      <c r="S9">
+        <v>0.87</v>
+      </c>
+      <c r="T9">
+        <v>0.99</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="W9">
+        <v>0.97</v>
+      </c>
+      <c r="X9">
+        <v>0.95</v>
+      </c>
+      <c r="Y9">
+        <v>0.86</v>
+      </c>
+      <c r="Z9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
+        <v>108</v>
+      </c>
+      <c r="K10">
+        <v>0.45</v>
+      </c>
+      <c r="L10">
+        <v>0.5</v>
+      </c>
+      <c r="M10">
+        <v>0.15</v>
+      </c>
+      <c r="N10">
+        <v>0.17</v>
+      </c>
+      <c r="O10">
+        <v>0.45</v>
+      </c>
+      <c r="P10">
+        <v>0.5</v>
+      </c>
+      <c r="Q10">
+        <v>0.45</v>
+      </c>
+      <c r="R10">
+        <v>0.76</v>
+      </c>
+      <c r="S10">
+        <v>0.9</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>0.99</v>
+      </c>
+      <c r="V10">
+        <v>0.61</v>
+      </c>
+      <c r="W10">
+        <v>0.97</v>
+      </c>
+      <c r="X10">
+        <v>0.99</v>
+      </c>
+      <c r="Y10">
+        <v>0.9</v>
+      </c>
+      <c r="Z10">
+        <v>1</v>
+      </c>
+      <c r="AA10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
+        <v>116</v>
+      </c>
+      <c r="K11">
+        <v>0.3</v>
+      </c>
+      <c r="L11">
+        <v>0.31</v>
+      </c>
+      <c r="M11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N11">
+        <v>0.16</v>
+      </c>
+      <c r="O11">
+        <v>0.3</v>
+      </c>
+      <c r="P11">
+        <v>0.31</v>
+      </c>
+      <c r="Q11">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="R11">
+        <v>0.46</v>
+      </c>
+      <c r="S11">
+        <v>0.48</v>
+      </c>
+      <c r="T11">
+        <v>0.81</v>
+      </c>
+      <c r="U11">
+        <v>0.86</v>
+      </c>
+      <c r="V11">
+        <v>0.38</v>
+      </c>
+      <c r="W11">
+        <v>0.69</v>
+      </c>
+      <c r="X11">
+        <v>0.67</v>
+      </c>
+      <c r="Y11">
+        <v>0.46</v>
+      </c>
+      <c r="Z11">
+        <v>0.82</v>
+      </c>
+      <c r="AA11">
+        <v>0.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 20K AFR results and admixed t1e 100v100 results
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4FB87A-B78A-436D-BDEE-4D9DFA0AB347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAB21BA-DFB0-4CC1-9265-C395C2C80984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="t1e_gene_region" sheetId="1" r:id="rId1"/>
     <sheet name="t1e_by_gene" sheetId="2" r:id="rId2"/>
     <sheet name="power_by_gene" sheetId="3" r:id="rId3"/>
+    <sheet name="admixed_t1e" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="144">
   <si>
     <t>Population</t>
   </si>
@@ -637,6 +638,59 @@
 160% fun 100% syn
 internal controls: 100% fun 100% syn</t>
   </si>
+  <si>
+    <t>ProxECAT External Adjusted</t>
+  </si>
+  <si>
+    <t>proxECAT-weighted External Adjusted</t>
+  </si>
+  <si>
+    <t>iECAT-O Internal + External Adjusted</t>
+  </si>
+  <si>
+    <t>LogProx External Adjusted</t>
+  </si>
+  <si>
+    <t>LogProx Internal + External Adjusted</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>AFR NFE</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>Nsim</t>
+  </si>
+  <si>
+    <t>23K</t>
+  </si>
+  <si>
+    <t>1. RAREsim v2.1.1: Extract the AFR haplotypes using extract.py
+2. RAREsim v2.1.1: Extract the NFE haplotypes using extract.py
+3. Combine the AFR and NFE haplotypes to create admixed population
+4. RAREsim v2.1.1: Convert the admixed haplotype to a sparse matrix using convert.py
+5. Prune Separately-RAREsim v2.1.1
+--functional_bins 160%
+--synonymous_bins 100%
+6. RAREsim v2.1.1: Convert 160% fun 100% syn pruned hap file to .sm file using convert.py
+7. Prune Sequentially-RAREsimv2.1.1
+--f_only 100% 
+8. RAREsim v2.1.1: Convert 100% fun 100% syn pruned hap file to .sm file using convert .py 
+9. Prune Separately-RAREsim v2.1.1
+--functional_bins 80% 
+--synonymous_bins 80% 
+10. R: add pruned variants back in as rows of 0 and extract datasets</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>100% AFR</t>
+  </si>
 </sst>
 </file>
 
@@ -703,7 +757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -732,6 +786,7 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -760,9 +815,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -800,7 +855,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -906,7 +961,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1048,7 +1103,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1095,31 +1150,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
     </row>
     <row r="2" spans="1:35" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -7138,11 +7193,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DDB312-960A-4A06-81C4-77814F5815B8}">
-  <dimension ref="A1:AD113"/>
+  <dimension ref="A1:AD122"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB108" sqref="AB108"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J129" sqref="J129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7163,36 +7218,36 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="12" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
     </row>
     <row r="2" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -13728,7 +13783,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="113" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J113" t="s">
         <v>117</v>
       </c>
@@ -13782,6 +13837,537 @@
       </c>
       <c r="AA113">
         <v>0.22</v>
+      </c>
+    </row>
+    <row r="114" spans="1:27" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A114" s="11">
+        <v>45279</v>
+      </c>
+      <c r="B114" t="s">
+        <v>143</v>
+      </c>
+      <c r="C114">
+        <v>1E-3</v>
+      </c>
+      <c r="D114" s="2">
+        <v>1</v>
+      </c>
+      <c r="E114" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F114" t="s">
+        <v>127</v>
+      </c>
+      <c r="G114" t="s">
+        <v>40</v>
+      </c>
+      <c r="H114" t="s">
+        <v>129</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J114" t="s">
+        <v>106</v>
+      </c>
+      <c r="K114">
+        <v>0.04</v>
+      </c>
+      <c r="L114">
+        <v>0.15</v>
+      </c>
+      <c r="M114">
+        <v>0.03</v>
+      </c>
+      <c r="N114">
+        <v>0.09</v>
+      </c>
+      <c r="O114">
+        <v>0.04</v>
+      </c>
+      <c r="P114">
+        <v>0.15</v>
+      </c>
+      <c r="Q114">
+        <v>0.05</v>
+      </c>
+      <c r="R114">
+        <v>0.03</v>
+      </c>
+      <c r="S114">
+        <v>0.06</v>
+      </c>
+      <c r="T114">
+        <v>0.44</v>
+      </c>
+      <c r="U114">
+        <v>0.21</v>
+      </c>
+      <c r="V114">
+        <v>0.05</v>
+      </c>
+      <c r="W114">
+        <v>0.39</v>
+      </c>
+      <c r="X114">
+        <v>0.21</v>
+      </c>
+      <c r="Y114">
+        <v>0.03</v>
+      </c>
+      <c r="Z114">
+        <v>0.32</v>
+      </c>
+      <c r="AA114">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="115" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J115" t="s">
+        <v>109</v>
+      </c>
+      <c r="K115">
+        <v>0.03</v>
+      </c>
+      <c r="L115">
+        <v>0.11</v>
+      </c>
+      <c r="M115">
+        <v>0.03</v>
+      </c>
+      <c r="N115">
+        <v>0.09</v>
+      </c>
+      <c r="O115">
+        <v>0.02</v>
+      </c>
+      <c r="P115">
+        <v>0.11</v>
+      </c>
+      <c r="Q115">
+        <v>0.02</v>
+      </c>
+      <c r="R115">
+        <v>0.03</v>
+      </c>
+      <c r="S115">
+        <v>0.01</v>
+      </c>
+      <c r="T115">
+        <v>0.32</v>
+      </c>
+      <c r="U115">
+        <v>0.15</v>
+      </c>
+      <c r="V115">
+        <v>0.02</v>
+      </c>
+      <c r="W115">
+        <v>0.31</v>
+      </c>
+      <c r="X115">
+        <v>0.12</v>
+      </c>
+      <c r="Y115">
+        <v>0.02</v>
+      </c>
+      <c r="Z115">
+        <v>0.24</v>
+      </c>
+      <c r="AA115">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="116" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J116" t="s">
+        <v>110</v>
+      </c>
+      <c r="K116">
+        <v>0.06</v>
+      </c>
+      <c r="L116">
+        <v>0.18</v>
+      </c>
+      <c r="M116">
+        <v>0.03</v>
+      </c>
+      <c r="N116">
+        <v>0.08</v>
+      </c>
+      <c r="O116">
+        <v>0.06</v>
+      </c>
+      <c r="P116">
+        <v>0.18</v>
+      </c>
+      <c r="Q116">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R116">
+        <v>0.03</v>
+      </c>
+      <c r="S116">
+        <v>0.03</v>
+      </c>
+      <c r="T116">
+        <v>0.39</v>
+      </c>
+      <c r="U116">
+        <v>0.17</v>
+      </c>
+      <c r="V116">
+        <v>0.03</v>
+      </c>
+      <c r="W116">
+        <v>0.34</v>
+      </c>
+      <c r="X116">
+        <v>0.19</v>
+      </c>
+      <c r="Y116">
+        <v>0.04</v>
+      </c>
+      <c r="Z116">
+        <v>0.33</v>
+      </c>
+      <c r="AA116">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="117" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J117" t="s">
+        <v>111</v>
+      </c>
+      <c r="K117">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L117">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M117">
+        <v>0.05</v>
+      </c>
+      <c r="N117">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O117">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P117">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q117">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R117">
+        <v>0.04</v>
+      </c>
+      <c r="S117">
+        <v>0.02</v>
+      </c>
+      <c r="T117">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="U117">
+        <v>0.17</v>
+      </c>
+      <c r="V117">
+        <v>0.02</v>
+      </c>
+      <c r="W117">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="X117">
+        <v>0.2</v>
+      </c>
+      <c r="Y117">
+        <v>0.02</v>
+      </c>
+      <c r="Z117">
+        <v>0.21</v>
+      </c>
+      <c r="AA117">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="118" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J118" t="s">
+        <v>112</v>
+      </c>
+      <c r="K118">
+        <v>0.03</v>
+      </c>
+      <c r="L118">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M118">
+        <v>0.02</v>
+      </c>
+      <c r="N118">
+        <v>0.1</v>
+      </c>
+      <c r="O118">
+        <v>0.03</v>
+      </c>
+      <c r="P118">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Q118">
+        <v>0.03</v>
+      </c>
+      <c r="R118">
+        <v>0.03</v>
+      </c>
+      <c r="S118">
+        <v>0.02</v>
+      </c>
+      <c r="T118">
+        <v>0.33</v>
+      </c>
+      <c r="U118">
+        <v>0.16</v>
+      </c>
+      <c r="V118">
+        <v>0.02</v>
+      </c>
+      <c r="W118">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="X118">
+        <v>0.17</v>
+      </c>
+      <c r="Y118">
+        <v>0.02</v>
+      </c>
+      <c r="Z118">
+        <v>0.24</v>
+      </c>
+      <c r="AA118">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="119" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J119" t="s">
+        <v>113</v>
+      </c>
+      <c r="K119">
+        <v>3.1578947368421102E-2</v>
+      </c>
+      <c r="L119">
+        <v>3.09278350515464E-2</v>
+      </c>
+      <c r="M119">
+        <v>0</v>
+      </c>
+      <c r="N119">
+        <v>3.1578947368421102E-2</v>
+      </c>
+      <c r="O119">
+        <v>2.1052631578947399E-2</v>
+      </c>
+      <c r="P119">
+        <v>3.09278350515464E-2</v>
+      </c>
+      <c r="Q119">
+        <v>0.02</v>
+      </c>
+      <c r="R119">
+        <v>0.04</v>
+      </c>
+      <c r="S119">
+        <v>0.05</v>
+      </c>
+      <c r="T119">
+        <v>0.12</v>
+      </c>
+      <c r="U119">
+        <v>0.1</v>
+      </c>
+      <c r="V119">
+        <v>0.03</v>
+      </c>
+      <c r="W119">
+        <v>0.17</v>
+      </c>
+      <c r="X119">
+        <v>0.1</v>
+      </c>
+      <c r="Y119">
+        <v>0.04</v>
+      </c>
+      <c r="Z119">
+        <v>0.12</v>
+      </c>
+      <c r="AA119">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="120" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J120" t="s">
+        <v>114</v>
+      </c>
+      <c r="K120">
+        <v>0.05</v>
+      </c>
+      <c r="L120">
+        <v>0.12</v>
+      </c>
+      <c r="M120">
+        <v>0.05</v>
+      </c>
+      <c r="N120">
+        <v>0.1</v>
+      </c>
+      <c r="O120">
+        <v>0.05</v>
+      </c>
+      <c r="P120">
+        <v>0.12</v>
+      </c>
+      <c r="Q120">
+        <v>0.05</v>
+      </c>
+      <c r="R120">
+        <v>0.02</v>
+      </c>
+      <c r="S120">
+        <v>0.06</v>
+      </c>
+      <c r="T120">
+        <v>0.59</v>
+      </c>
+      <c r="U120">
+        <v>0.36</v>
+      </c>
+      <c r="V120">
+        <v>0.04</v>
+      </c>
+      <c r="W120">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="X120">
+        <v>0.31</v>
+      </c>
+      <c r="Y120">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z120">
+        <v>0.47</v>
+      </c>
+      <c r="AA120">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="121" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J121" t="s">
+        <v>115</v>
+      </c>
+      <c r="K121">
+        <v>0.08</v>
+      </c>
+      <c r="L121">
+        <v>0.16</v>
+      </c>
+      <c r="M121">
+        <v>0.05</v>
+      </c>
+      <c r="N121">
+        <v>0.12</v>
+      </c>
+      <c r="O121">
+        <v>0.08</v>
+      </c>
+      <c r="P121">
+        <v>0.16</v>
+      </c>
+      <c r="Q121">
+        <v>0.08</v>
+      </c>
+      <c r="R121">
+        <v>0.03</v>
+      </c>
+      <c r="S121">
+        <v>0.09</v>
+      </c>
+      <c r="T121">
+        <v>0.35</v>
+      </c>
+      <c r="U121">
+        <v>0.17</v>
+      </c>
+      <c r="V121">
+        <v>0.05</v>
+      </c>
+      <c r="W121">
+        <v>0.24</v>
+      </c>
+      <c r="X121">
+        <v>0.13</v>
+      </c>
+      <c r="Y121">
+        <v>0.08</v>
+      </c>
+      <c r="Z121">
+        <v>0.32</v>
+      </c>
+      <c r="AA121">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="122" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="J122" t="s">
+        <v>117</v>
+      </c>
+      <c r="K122">
+        <v>0.02</v>
+      </c>
+      <c r="L122">
+        <v>0.08</v>
+      </c>
+      <c r="M122">
+        <v>0.06</v>
+      </c>
+      <c r="N122">
+        <v>0.09</v>
+      </c>
+      <c r="O122">
+        <v>0.01</v>
+      </c>
+      <c r="P122">
+        <v>0.08</v>
+      </c>
+      <c r="Q122">
+        <v>0.02</v>
+      </c>
+      <c r="R122">
+        <v>0.05</v>
+      </c>
+      <c r="S122">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T122">
+        <v>0.43</v>
+      </c>
+      <c r="U122">
+        <v>0.19</v>
+      </c>
+      <c r="V122">
+        <v>0.03</v>
+      </c>
+      <c r="W122">
+        <v>0.43</v>
+      </c>
+      <c r="X122">
+        <v>0.18</v>
+      </c>
+      <c r="Y122">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z122">
+        <v>0.37</v>
+      </c>
+      <c r="AA122">
+        <v>0.18</v>
       </c>
     </row>
   </sheetData>
@@ -13795,11 +14381,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5E01F1-9A92-4DEF-99E5-C0BF38433A3D}">
-  <dimension ref="A1:AB11"/>
+  <dimension ref="A1:AB14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13817,37 +14403,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="12" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
       <c r="AB1" s="1"/>
     </row>
     <row r="2" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
@@ -14519,6 +15105,201 @@
       </c>
       <c r="AA11">
         <v>0.83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
+        <v>45269</v>
+      </c>
+      <c r="B12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12">
+        <v>1E-3</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>127</v>
+      </c>
+      <c r="G12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" t="s">
+        <v>129</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J12" t="s">
+        <v>107</v>
+      </c>
+      <c r="K12">
+        <v>0.45</v>
+      </c>
+      <c r="L12">
+        <v>0.54</v>
+      </c>
+      <c r="M12">
+        <v>0.19</v>
+      </c>
+      <c r="N12">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="O12">
+        <v>0.45</v>
+      </c>
+      <c r="P12">
+        <v>0.54</v>
+      </c>
+      <c r="Q12">
+        <v>0.46</v>
+      </c>
+      <c r="R12">
+        <v>0.83</v>
+      </c>
+      <c r="S12">
+        <v>0.83</v>
+      </c>
+      <c r="T12">
+        <v>0.99</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>0.69</v>
+      </c>
+      <c r="W12">
+        <v>0.96</v>
+      </c>
+      <c r="X12">
+        <v>0.97</v>
+      </c>
+      <c r="Y12">
+        <v>0.78</v>
+      </c>
+      <c r="Z12">
+        <v>0.98</v>
+      </c>
+      <c r="AA12">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J13" t="s">
+        <v>108</v>
+      </c>
+      <c r="K13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L13">
+        <v>0.61</v>
+      </c>
+      <c r="M13">
+        <v>0.33</v>
+      </c>
+      <c r="N13">
+        <v>0.31</v>
+      </c>
+      <c r="O13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P13">
+        <v>0.61</v>
+      </c>
+      <c r="Q13">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="R13">
+        <v>0.86</v>
+      </c>
+      <c r="S13">
+        <v>0.88</v>
+      </c>
+      <c r="T13">
+        <v>0.98</v>
+      </c>
+      <c r="U13">
+        <v>0.98</v>
+      </c>
+      <c r="V13">
+        <v>0.62</v>
+      </c>
+      <c r="W13">
+        <v>0.97</v>
+      </c>
+      <c r="X13">
+        <v>0.96</v>
+      </c>
+      <c r="Y13">
+        <v>0.86</v>
+      </c>
+      <c r="Z13">
+        <v>0.99</v>
+      </c>
+      <c r="AA13">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J14" t="s">
+        <v>116</v>
+      </c>
+      <c r="K14">
+        <v>0.23</v>
+      </c>
+      <c r="L14">
+        <v>0.3</v>
+      </c>
+      <c r="M14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N14">
+        <v>0.13</v>
+      </c>
+      <c r="O14">
+        <v>0.23</v>
+      </c>
+      <c r="P14">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="Q14">
+        <v>0.24</v>
+      </c>
+      <c r="R14">
+        <v>0.59</v>
+      </c>
+      <c r="S14">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="T14">
+        <v>0.85</v>
+      </c>
+      <c r="U14">
+        <v>0.83</v>
+      </c>
+      <c r="V14">
+        <v>0.48</v>
+      </c>
+      <c r="W14">
+        <v>0.77</v>
+      </c>
+      <c r="X14">
+        <v>0.76</v>
+      </c>
+      <c r="Y14">
+        <v>0.5</v>
+      </c>
+      <c r="Z14">
+        <v>0.85</v>
+      </c>
+      <c r="AA14">
+        <v>0.85</v>
       </c>
     </row>
   </sheetData>
@@ -14528,4 +15309,1286 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669C6091-A5A6-4DA3-95F0-78E591F91A2C}">
+  <dimension ref="A1:AH26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" customWidth="1"/>
+    <col min="10" max="10" width="17.21875" customWidth="1"/>
+    <col min="11" max="11" width="36.109375" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" customWidth="1"/>
+    <col min="16" max="16" width="11.21875" customWidth="1"/>
+    <col min="17" max="17" width="9.88671875" customWidth="1"/>
+    <col min="18" max="18" width="10.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="1"/>
+    </row>
+    <row r="2" spans="1:34" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+    </row>
+    <row r="3" spans="1:34" ht="360" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>45278</v>
+      </c>
+      <c r="B3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3">
+        <v>1E-3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
+        <v>129</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="L3" t="s">
+        <v>106</v>
+      </c>
+      <c r="M3">
+        <v>0.13</v>
+      </c>
+      <c r="N3">
+        <v>0.1</v>
+      </c>
+      <c r="O3">
+        <v>0.12</v>
+      </c>
+      <c r="P3">
+        <v>0.05</v>
+      </c>
+      <c r="Q3">
+        <v>0.06</v>
+      </c>
+      <c r="R3">
+        <v>0.06</v>
+      </c>
+      <c r="S3">
+        <v>0.04</v>
+      </c>
+      <c r="T3">
+        <v>0.1</v>
+      </c>
+      <c r="U3">
+        <v>0.11</v>
+      </c>
+      <c r="V3">
+        <v>0.12</v>
+      </c>
+      <c r="W3">
+        <v>0.10891089108910899</v>
+      </c>
+      <c r="X3">
+        <v>0.04</v>
+      </c>
+      <c r="Y3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="L4" t="s">
+        <v>107</v>
+      </c>
+      <c r="M4">
+        <v>0.13</v>
+      </c>
+      <c r="N4">
+        <v>0.09</v>
+      </c>
+      <c r="O4">
+        <v>0.09</v>
+      </c>
+      <c r="P4">
+        <v>0.09</v>
+      </c>
+      <c r="Q4">
+        <v>0.06</v>
+      </c>
+      <c r="R4">
+        <v>0.06</v>
+      </c>
+      <c r="S4">
+        <v>0.09</v>
+      </c>
+      <c r="T4">
+        <v>0.09</v>
+      </c>
+      <c r="U4">
+        <v>0.12</v>
+      </c>
+      <c r="V4">
+        <v>0.08</v>
+      </c>
+      <c r="W4">
+        <v>0.12871287128712899</v>
+      </c>
+      <c r="X4">
+        <v>0.01</v>
+      </c>
+      <c r="Y4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="L5" t="s">
+        <v>108</v>
+      </c>
+      <c r="M5">
+        <v>0.05</v>
+      </c>
+      <c r="N5">
+        <v>0.03</v>
+      </c>
+      <c r="O5">
+        <v>0.03</v>
+      </c>
+      <c r="P5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q5">
+        <v>0.03</v>
+      </c>
+      <c r="R5">
+        <v>0.03</v>
+      </c>
+      <c r="S5">
+        <v>0.04</v>
+      </c>
+      <c r="T5">
+        <v>0.03</v>
+      </c>
+      <c r="U5">
+        <v>0.05</v>
+      </c>
+      <c r="V5">
+        <v>0.03</v>
+      </c>
+      <c r="W5">
+        <v>4.95049504950495E-2</v>
+      </c>
+      <c r="X5">
+        <v>0.03</v>
+      </c>
+      <c r="Y5">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>109</v>
+      </c>
+      <c r="M6">
+        <v>0.1</v>
+      </c>
+      <c r="N6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O6">
+        <v>0.08</v>
+      </c>
+      <c r="P6">
+        <v>0.08</v>
+      </c>
+      <c r="Q6">
+        <v>0.04</v>
+      </c>
+      <c r="R6">
+        <v>0.05</v>
+      </c>
+      <c r="S6">
+        <v>0.04</v>
+      </c>
+      <c r="T6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W6">
+        <v>6.9306930693069299E-2</v>
+      </c>
+      <c r="X6">
+        <v>0.02</v>
+      </c>
+      <c r="Y6">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="L7" t="s">
+        <v>110</v>
+      </c>
+      <c r="M7">
+        <v>0.04</v>
+      </c>
+      <c r="N7">
+        <v>0.01</v>
+      </c>
+      <c r="O7">
+        <v>0.01</v>
+      </c>
+      <c r="P7">
+        <v>0.04</v>
+      </c>
+      <c r="Q7">
+        <v>0.02</v>
+      </c>
+      <c r="R7">
+        <v>0.02</v>
+      </c>
+      <c r="S7">
+        <v>0.02</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0.04</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>3.9603960396039598E-2</v>
+      </c>
+      <c r="X7">
+        <v>0.03</v>
+      </c>
+      <c r="Y7">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>111</v>
+      </c>
+      <c r="M8">
+        <v>0.09</v>
+      </c>
+      <c r="N8">
+        <v>0.03</v>
+      </c>
+      <c r="O8">
+        <v>0.03</v>
+      </c>
+      <c r="P8">
+        <v>0.04</v>
+      </c>
+      <c r="Q8">
+        <v>0.02</v>
+      </c>
+      <c r="R8">
+        <v>0.03</v>
+      </c>
+      <c r="S8">
+        <v>0.01</v>
+      </c>
+      <c r="T8">
+        <v>0.03</v>
+      </c>
+      <c r="U8">
+        <v>0.08</v>
+      </c>
+      <c r="V8">
+        <v>0.03</v>
+      </c>
+      <c r="W8">
+        <v>7.9207920792079195E-2</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="L9" t="s">
+        <v>112</v>
+      </c>
+      <c r="M9">
+        <v>0.04</v>
+      </c>
+      <c r="N9">
+        <v>0.06</v>
+      </c>
+      <c r="O9">
+        <v>0.05</v>
+      </c>
+      <c r="P9">
+        <v>0.05</v>
+      </c>
+      <c r="Q9">
+        <v>0.04</v>
+      </c>
+      <c r="R9">
+        <v>0.05</v>
+      </c>
+      <c r="S9">
+        <v>0.03</v>
+      </c>
+      <c r="T9">
+        <v>0.06</v>
+      </c>
+      <c r="U9">
+        <v>0.04</v>
+      </c>
+      <c r="V9">
+        <v>0.05</v>
+      </c>
+      <c r="W9">
+        <v>3.9603960396039598E-2</v>
+      </c>
+      <c r="X9">
+        <v>0.01</v>
+      </c>
+      <c r="Y9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="L10" t="s">
+        <v>113</v>
+      </c>
+      <c r="M10">
+        <v>6.3829787234042507E-2</v>
+      </c>
+      <c r="N10">
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="O10">
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="P10">
+        <v>5.31914893617021E-2</v>
+      </c>
+      <c r="Q10">
+        <v>1.0416666666666701E-2</v>
+      </c>
+      <c r="R10">
+        <v>1.0416666666666701E-2</v>
+      </c>
+      <c r="S10">
+        <v>4.2553191489361701E-2</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0.05</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>4.95049504950495E-2</v>
+      </c>
+      <c r="X10">
+        <v>0.04</v>
+      </c>
+      <c r="Y10">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="L11" t="s">
+        <v>114</v>
+      </c>
+      <c r="M11">
+        <v>0.06</v>
+      </c>
+      <c r="N11">
+        <v>0.01</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0.05</v>
+      </c>
+      <c r="Q11">
+        <v>0.02</v>
+      </c>
+      <c r="R11">
+        <v>0.03</v>
+      </c>
+      <c r="S11">
+        <v>0.05</v>
+      </c>
+      <c r="T11">
+        <v>0.01</v>
+      </c>
+      <c r="U11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>7.9207920792079195E-2</v>
+      </c>
+      <c r="X11">
+        <v>0.03</v>
+      </c>
+      <c r="Y11">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="L12" t="s">
+        <v>115</v>
+      </c>
+      <c r="M12">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N12">
+        <v>0.04</v>
+      </c>
+      <c r="O12">
+        <v>0.03</v>
+      </c>
+      <c r="P12">
+        <v>0.04</v>
+      </c>
+      <c r="Q12">
+        <v>0.02</v>
+      </c>
+      <c r="R12">
+        <v>0.02</v>
+      </c>
+      <c r="S12">
+        <v>0.04</v>
+      </c>
+      <c r="T12">
+        <v>0.04</v>
+      </c>
+      <c r="U12">
+        <v>0.08</v>
+      </c>
+      <c r="V12">
+        <v>0.03</v>
+      </c>
+      <c r="W12">
+        <v>7.9207920792079195E-2</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="L13" t="s">
+        <v>116</v>
+      </c>
+      <c r="M13">
+        <v>0.08</v>
+      </c>
+      <c r="N13">
+        <v>0.04</v>
+      </c>
+      <c r="O13">
+        <v>0.04</v>
+      </c>
+      <c r="P13">
+        <v>0.04</v>
+      </c>
+      <c r="Q13">
+        <v>0.03</v>
+      </c>
+      <c r="R13">
+        <v>0.02</v>
+      </c>
+      <c r="S13">
+        <v>0.03</v>
+      </c>
+      <c r="T13">
+        <v>0.04</v>
+      </c>
+      <c r="U13">
+        <v>0.06</v>
+      </c>
+      <c r="V13">
+        <v>0.03</v>
+      </c>
+      <c r="W13">
+        <v>5.9405940594059403E-2</v>
+      </c>
+      <c r="X13">
+        <v>0.02</v>
+      </c>
+      <c r="Y13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="L14" t="s">
+        <v>117</v>
+      </c>
+      <c r="M14">
+        <v>0.11</v>
+      </c>
+      <c r="N14">
+        <v>0.02</v>
+      </c>
+      <c r="O14">
+        <v>0.02</v>
+      </c>
+      <c r="P14">
+        <v>0.1</v>
+      </c>
+      <c r="Q14">
+        <v>0.01</v>
+      </c>
+      <c r="R14">
+        <v>0.01</v>
+      </c>
+      <c r="S14">
+        <v>0.05</v>
+      </c>
+      <c r="T14">
+        <v>0.02</v>
+      </c>
+      <c r="U14">
+        <v>0.11</v>
+      </c>
+      <c r="V14">
+        <v>0.03</v>
+      </c>
+      <c r="W14">
+        <v>0.118811881188119</v>
+      </c>
+      <c r="X14">
+        <v>0.03</v>
+      </c>
+      <c r="Y14">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" ht="360" x14ac:dyDescent="0.3">
+      <c r="A15" s="11">
+        <v>45279</v>
+      </c>
+      <c r="B15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15">
+        <v>1E-3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15" t="s">
+        <v>140</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>127</v>
+      </c>
+      <c r="I15" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" t="s">
+        <v>129</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="L15" t="s">
+        <v>106</v>
+      </c>
+      <c r="M15">
+        <v>0.05</v>
+      </c>
+      <c r="N15">
+        <v>0.09</v>
+      </c>
+      <c r="O15">
+        <v>0.13</v>
+      </c>
+      <c r="P15">
+        <v>0.01</v>
+      </c>
+      <c r="Q15">
+        <v>0.06</v>
+      </c>
+      <c r="R15">
+        <v>0.06</v>
+      </c>
+      <c r="S15">
+        <v>0.02</v>
+      </c>
+      <c r="T15">
+        <v>0.09</v>
+      </c>
+      <c r="U15">
+        <v>0.05</v>
+      </c>
+      <c r="V15">
+        <v>0.13</v>
+      </c>
+      <c r="W15">
+        <v>4.95049504950495E-2</v>
+      </c>
+      <c r="X15">
+        <v>0.02</v>
+      </c>
+      <c r="Y15">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="L16" t="s">
+        <v>107</v>
+      </c>
+      <c r="M16">
+        <v>0.12</v>
+      </c>
+      <c r="N16">
+        <v>0.12</v>
+      </c>
+      <c r="O16">
+        <v>0.15</v>
+      </c>
+      <c r="P16">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q16">
+        <v>0.09</v>
+      </c>
+      <c r="R16">
+        <v>0.12</v>
+      </c>
+      <c r="S16">
+        <v>0.04</v>
+      </c>
+      <c r="T16">
+        <v>0.11</v>
+      </c>
+      <c r="U16">
+        <v>0.13</v>
+      </c>
+      <c r="V16">
+        <v>0.15</v>
+      </c>
+      <c r="W16">
+        <v>0.12871287128712899</v>
+      </c>
+      <c r="X16">
+        <v>0.02</v>
+      </c>
+      <c r="Y16">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="17" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="L17" t="s">
+        <v>108</v>
+      </c>
+      <c r="M17">
+        <v>0.09</v>
+      </c>
+      <c r="N17">
+        <v>0.11</v>
+      </c>
+      <c r="O17">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="P17">
+        <v>0.09</v>
+      </c>
+      <c r="Q17">
+        <v>0.08</v>
+      </c>
+      <c r="R17">
+        <v>0.09</v>
+      </c>
+      <c r="S17">
+        <v>0.05</v>
+      </c>
+      <c r="T17">
+        <v>0.11</v>
+      </c>
+      <c r="U17">
+        <v>0.1</v>
+      </c>
+      <c r="V17">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W17">
+        <v>9.9009900990099001E-2</v>
+      </c>
+      <c r="X17">
+        <v>0.06</v>
+      </c>
+      <c r="Y17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="18" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="L18" t="s">
+        <v>109</v>
+      </c>
+      <c r="M18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N18">
+        <v>0.15</v>
+      </c>
+      <c r="O18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="P18">
+        <v>0.12</v>
+      </c>
+      <c r="Q18">
+        <v>0.09</v>
+      </c>
+      <c r="R18">
+        <v>0.1</v>
+      </c>
+      <c r="S18">
+        <v>0.08</v>
+      </c>
+      <c r="T18">
+        <v>0.16</v>
+      </c>
+      <c r="U18">
+        <v>0.15</v>
+      </c>
+      <c r="V18">
+        <v>0.12</v>
+      </c>
+      <c r="W18">
+        <v>0.14851485148514901</v>
+      </c>
+      <c r="X18">
+        <v>0.03</v>
+      </c>
+      <c r="Y18">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="19" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="L19" t="s">
+        <v>110</v>
+      </c>
+      <c r="M19">
+        <v>0.12</v>
+      </c>
+      <c r="N19">
+        <v>0.15</v>
+      </c>
+      <c r="O19">
+        <v>0.13</v>
+      </c>
+      <c r="P19">
+        <v>0.06</v>
+      </c>
+      <c r="Q19">
+        <v>0.1</v>
+      </c>
+      <c r="R19">
+        <v>0.12</v>
+      </c>
+      <c r="S19">
+        <v>0.04</v>
+      </c>
+      <c r="T19">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U19">
+        <v>0.12</v>
+      </c>
+      <c r="V19">
+        <v>0.12</v>
+      </c>
+      <c r="W19">
+        <v>0.12871287128712899</v>
+      </c>
+      <c r="X19">
+        <v>0.03</v>
+      </c>
+      <c r="Y19">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="20" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="L20" t="s">
+        <v>111</v>
+      </c>
+      <c r="M20">
+        <v>0.06</v>
+      </c>
+      <c r="N20">
+        <v>0.12</v>
+      </c>
+      <c r="O20">
+        <v>0.13</v>
+      </c>
+      <c r="P20">
+        <v>0.05</v>
+      </c>
+      <c r="Q20">
+        <v>0.1</v>
+      </c>
+      <c r="R20">
+        <v>0.11</v>
+      </c>
+      <c r="S20">
+        <v>0.01</v>
+      </c>
+      <c r="T20">
+        <v>0.12</v>
+      </c>
+      <c r="U20">
+        <v>0.06</v>
+      </c>
+      <c r="V20">
+        <v>0.12</v>
+      </c>
+      <c r="W20">
+        <v>5.9405940594059403E-2</v>
+      </c>
+      <c r="X20">
+        <v>0.04</v>
+      </c>
+      <c r="Y20">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="21" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="L21" t="s">
+        <v>112</v>
+      </c>
+      <c r="M21">
+        <v>0.09</v>
+      </c>
+      <c r="N21">
+        <v>0.15</v>
+      </c>
+      <c r="O21">
+        <v>0.22</v>
+      </c>
+      <c r="P21">
+        <v>0.05</v>
+      </c>
+      <c r="Q21">
+        <v>0.12</v>
+      </c>
+      <c r="R21">
+        <v>0.15</v>
+      </c>
+      <c r="S21">
+        <v>0.03</v>
+      </c>
+      <c r="T21">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U21">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V21">
+        <v>0.21</v>
+      </c>
+      <c r="W21">
+        <v>6.9306930693069299E-2</v>
+      </c>
+      <c r="X21">
+        <v>0.03</v>
+      </c>
+      <c r="Y21">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="22" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="L22" t="s">
+        <v>113</v>
+      </c>
+      <c r="M22">
+        <v>0.104651162790698</v>
+      </c>
+      <c r="N22">
+        <v>0.114583333333333</v>
+      </c>
+      <c r="O22">
+        <v>0.1875</v>
+      </c>
+      <c r="P22">
+        <v>4.81927710843374E-2</v>
+      </c>
+      <c r="Q22">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="R22">
+        <v>0.13541666666666699</v>
+      </c>
+      <c r="S22">
+        <v>2.53164556962025E-2</v>
+      </c>
+      <c r="T22">
+        <v>6.25E-2</v>
+      </c>
+      <c r="U22">
+        <v>4.1237113402061903E-2</v>
+      </c>
+      <c r="V22">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="W22">
+        <v>4.08163265306122E-2</v>
+      </c>
+      <c r="X22">
+        <v>0.02</v>
+      </c>
+      <c r="Y22">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="23" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="L23" t="s">
+        <v>114</v>
+      </c>
+      <c r="M23">
+        <v>0.02</v>
+      </c>
+      <c r="N23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O23">
+        <v>0.17</v>
+      </c>
+      <c r="P23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q23">
+        <v>0.12</v>
+      </c>
+      <c r="R23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S23">
+        <v>0.01</v>
+      </c>
+      <c r="T23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U23">
+        <v>0.02</v>
+      </c>
+      <c r="V23">
+        <v>0.16</v>
+      </c>
+      <c r="W23">
+        <v>1.9801980198019799E-2</v>
+      </c>
+      <c r="X23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="L24" t="s">
+        <v>115</v>
+      </c>
+      <c r="M24">
+        <v>0.05</v>
+      </c>
+      <c r="N24">
+        <v>0.09</v>
+      </c>
+      <c r="O24">
+        <v>0.15</v>
+      </c>
+      <c r="P24">
+        <v>0.04</v>
+      </c>
+      <c r="Q24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R24">
+        <v>0.1</v>
+      </c>
+      <c r="S24">
+        <v>0.02</v>
+      </c>
+      <c r="T24">
+        <v>0.09</v>
+      </c>
+      <c r="U24">
+        <v>0.06</v>
+      </c>
+      <c r="V24">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W24">
+        <v>5.9405940594059403E-2</v>
+      </c>
+      <c r="X24">
+        <v>0.02</v>
+      </c>
+      <c r="Y24">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="25" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="L25" t="s">
+        <v>116</v>
+      </c>
+      <c r="M25">
+        <v>0.1</v>
+      </c>
+      <c r="N25">
+        <v>0.19</v>
+      </c>
+      <c r="O25">
+        <v>0.16</v>
+      </c>
+      <c r="P25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q25">
+        <v>0.08</v>
+      </c>
+      <c r="R25">
+        <v>0.08</v>
+      </c>
+      <c r="S25">
+        <v>5.0505050505050497E-2</v>
+      </c>
+      <c r="T25">
+        <v>0.16</v>
+      </c>
+      <c r="U25">
+        <v>0.1</v>
+      </c>
+      <c r="V25">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W25">
+        <v>9.9009900990099001E-2</v>
+      </c>
+      <c r="X25">
+        <v>0.04</v>
+      </c>
+      <c r="Y25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="L26" t="s">
+        <v>117</v>
+      </c>
+      <c r="M26">
+        <v>0.09</v>
+      </c>
+      <c r="N26">
+        <v>0.06</v>
+      </c>
+      <c r="O26">
+        <v>0.18</v>
+      </c>
+      <c r="P26">
+        <v>0.09</v>
+      </c>
+      <c r="Q26">
+        <v>0.09</v>
+      </c>
+      <c r="R26">
+        <v>0.19</v>
+      </c>
+      <c r="S26">
+        <v>0.04</v>
+      </c>
+      <c r="T26">
+        <v>0.05</v>
+      </c>
+      <c r="U26">
+        <v>0.08</v>
+      </c>
+      <c r="V26">
+        <v>0.17</v>
+      </c>
+      <c r="W26">
+        <v>7.9207920792079195E-2</v>
+      </c>
+      <c r="X26">
+        <v>0.02</v>
+      </c>
+      <c r="Y26">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="M1:Z1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added admixed results from 100v100 s1 and s2
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAB21BA-DFB0-4CC1-9265-C395C2C80984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D923FBC5-4B60-4656-ABED-2CCDF93180E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
   <sheets>
     <sheet name="t1e_gene_region" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="153">
   <si>
     <t>Population</t>
   </si>
@@ -691,6 +691,33 @@
   <si>
     <t>100% AFR</t>
   </si>
+  <si>
+    <t>Ncase/Nint</t>
+  </si>
+  <si>
+    <t>Ncc</t>
+  </si>
+  <si>
+    <t>Nref</t>
+  </si>
+  <si>
+    <t>5k</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>42K</t>
+  </si>
+  <si>
+    <t>Admixture</t>
+  </si>
+  <si>
+    <t>80/20</t>
+  </si>
+  <si>
+    <t>New Simulated 100K haplotypes</t>
+  </si>
 </sst>
 </file>
 
@@ -815,9 +842,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -855,7 +882,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -961,7 +988,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1103,7 +1130,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -14383,7 +14410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5E01F1-9A92-4DEF-99E5-C0BF38433A3D}">
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AC12" sqref="AC12"/>
     </sheetView>
@@ -15313,28 +15340,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669C6091-A5A6-4DA3-95F0-78E591F91A2C}">
-  <dimension ref="A1:AH26"/>
+  <dimension ref="A1:AM50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" customWidth="1"/>
-    <col min="10" max="10" width="17.21875" customWidth="1"/>
-    <col min="11" max="11" width="36.109375" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" customWidth="1"/>
-    <col min="16" max="16" width="11.21875" customWidth="1"/>
-    <col min="17" max="17" width="9.88671875" customWidth="1"/>
-    <col min="18" max="18" width="10.109375" customWidth="1"/>
+    <col min="2" max="3" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" customWidth="1"/>
+    <col min="14" max="14" width="17.21875" customWidth="1"/>
+    <col min="15" max="15" width="36.109375" customWidth="1"/>
+    <col min="19" max="19" width="9.44140625" customWidth="1"/>
+    <col min="20" max="20" width="11.21875" customWidth="1"/>
+    <col min="21" max="21" width="9.88671875" customWidth="1"/>
+    <col min="22" max="22" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="13" t="s">
         <v>19</v>
@@ -15348,14 +15376,14 @@
       <c r="I1" s="13"/>
       <c r="J1" s="13"/>
       <c r="K1" s="13"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="13" t="s">
-        <v>20</v>
-      </c>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="13" t="s">
+        <v>20</v>
+      </c>
       <c r="R1" s="13"/>
       <c r="S1" s="13"/>
       <c r="T1" s="13"/>
@@ -15365,16 +15393,20 @@
       <c r="X1" s="13"/>
       <c r="Y1" s="13"/>
       <c r="Z1" s="13"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
       <c r="AE1" s="12"/>
       <c r="AF1" s="12"/>
       <c r="AG1" s="12"/>
-      <c r="AH1" s="1"/>
-    </row>
-    <row r="2" spans="1:34" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="1"/>
+    </row>
+    <row r="2" spans="1:39" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -15382,184 +15414,215 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM2" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-    </row>
-    <row r="3" spans="1:34" ht="360" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:39" ht="360" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>45278</v>
       </c>
       <c r="B3" t="s">
         <v>137</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3">
         <v>1E-3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>138</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>140</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H3" t="s">
+        <v>148</v>
+      </c>
+      <c r="I3">
+        <v>500</v>
+      </c>
+      <c r="J3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="2">
+      <c r="K3" s="2">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>127</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>40</v>
       </c>
-      <c r="J3" t="s">
+      <c r="N3" t="s">
         <v>129</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="L3" t="s">
+      <c r="P3" t="s">
         <v>106</v>
       </c>
-      <c r="M3">
+      <c r="Q3">
         <v>0.13</v>
       </c>
-      <c r="N3">
+      <c r="R3">
         <v>0.1</v>
       </c>
-      <c r="O3">
+      <c r="S3">
         <v>0.12</v>
       </c>
-      <c r="P3">
-        <v>0.05</v>
-      </c>
-      <c r="Q3">
-        <v>0.06</v>
-      </c>
-      <c r="R3">
-        <v>0.06</v>
-      </c>
-      <c r="S3">
-        <v>0.04</v>
-      </c>
       <c r="T3">
+        <v>0.05</v>
+      </c>
+      <c r="U3">
+        <v>0.06</v>
+      </c>
+      <c r="V3">
+        <v>0.06</v>
+      </c>
+      <c r="W3">
+        <v>0.04</v>
+      </c>
+      <c r="X3">
         <v>0.1</v>
       </c>
-      <c r="U3">
+      <c r="Y3">
         <v>0.11</v>
       </c>
-      <c r="V3">
+      <c r="Z3">
         <v>0.12</v>
       </c>
-      <c r="W3">
+      <c r="AA3">
         <v>0.10891089108910899</v>
       </c>
-      <c r="X3">
-        <v>0.04</v>
-      </c>
-      <c r="Y3">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="L4" t="s">
+      <c r="AB3">
+        <v>0.04</v>
+      </c>
+      <c r="AC3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="P4" t="s">
         <v>107</v>
       </c>
-      <c r="M4">
+      <c r="Q4">
         <v>0.13</v>
       </c>
-      <c r="N4">
+      <c r="R4">
         <v>0.09</v>
-      </c>
-      <c r="O4">
-        <v>0.09</v>
-      </c>
-      <c r="P4">
-        <v>0.09</v>
-      </c>
-      <c r="Q4">
-        <v>0.06</v>
-      </c>
-      <c r="R4">
-        <v>0.06</v>
       </c>
       <c r="S4">
         <v>0.09</v>
@@ -15568,224 +15631,224 @@
         <v>0.09</v>
       </c>
       <c r="U4">
+        <v>0.06</v>
+      </c>
+      <c r="V4">
+        <v>0.06</v>
+      </c>
+      <c r="W4">
+        <v>0.09</v>
+      </c>
+      <c r="X4">
+        <v>0.09</v>
+      </c>
+      <c r="Y4">
         <v>0.12</v>
       </c>
-      <c r="V4">
+      <c r="Z4">
         <v>0.08</v>
       </c>
-      <c r="W4">
+      <c r="AA4">
         <v>0.12871287128712899</v>
       </c>
-      <c r="X4">
-        <v>0.01</v>
-      </c>
-      <c r="Y4">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="L5" t="s">
+      <c r="AB4">
+        <v>0.01</v>
+      </c>
+      <c r="AC4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="P5" t="s">
         <v>108</v>
       </c>
-      <c r="M5">
-        <v>0.05</v>
-      </c>
-      <c r="N5">
-        <v>0.03</v>
-      </c>
-      <c r="O5">
-        <v>0.03</v>
-      </c>
-      <c r="P5">
-        <v>7.0000000000000007E-2</v>
-      </c>
       <c r="Q5">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="R5">
         <v>0.03</v>
       </c>
       <c r="S5">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="T5">
-        <v>0.03</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="U5">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="V5">
         <v>0.03</v>
       </c>
       <c r="W5">
+        <v>0.04</v>
+      </c>
+      <c r="X5">
+        <v>0.03</v>
+      </c>
+      <c r="Y5">
+        <v>0.05</v>
+      </c>
+      <c r="Z5">
+        <v>0.03</v>
+      </c>
+      <c r="AA5">
         <v>4.95049504950495E-2</v>
       </c>
-      <c r="X5">
-        <v>0.03</v>
-      </c>
-      <c r="Y5">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="L6" t="s">
+      <c r="AB5">
+        <v>0.03</v>
+      </c>
+      <c r="AC5">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="P6" t="s">
         <v>109</v>
       </c>
-      <c r="M6">
+      <c r="Q6">
         <v>0.1</v>
       </c>
-      <c r="N6">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="O6">
+      <c r="R6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S6">
         <v>0.08</v>
       </c>
-      <c r="P6">
+      <c r="T6">
         <v>0.08</v>
       </c>
-      <c r="Q6">
-        <v>0.04</v>
-      </c>
-      <c r="R6">
-        <v>0.05</v>
-      </c>
-      <c r="S6">
-        <v>0.04</v>
-      </c>
-      <c r="T6">
-        <v>7.0000000000000007E-2</v>
-      </c>
       <c r="U6">
-        <v>7.0000000000000007E-2</v>
+        <v>0.04</v>
       </c>
       <c r="V6">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="W6">
+        <v>0.04</v>
+      </c>
+      <c r="X6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA6">
         <v>6.9306930693069299E-2</v>
       </c>
-      <c r="X6">
-        <v>0.02</v>
-      </c>
-      <c r="Y6">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="L7" t="s">
+      <c r="AB6">
+        <v>0.02</v>
+      </c>
+      <c r="AC6">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="P7" t="s">
         <v>110</v>
       </c>
-      <c r="M7">
-        <v>0.04</v>
-      </c>
-      <c r="N7">
-        <v>0.01</v>
-      </c>
-      <c r="O7">
-        <v>0.01</v>
-      </c>
-      <c r="P7">
-        <v>0.04</v>
-      </c>
       <c r="Q7">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="R7">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="S7">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="T7">
+        <v>0.04</v>
+      </c>
+      <c r="U7">
+        <v>0.02</v>
+      </c>
+      <c r="V7">
+        <v>0.02</v>
+      </c>
+      <c r="W7">
+        <v>0.02</v>
+      </c>
+      <c r="X7">
         <v>0</v>
       </c>
-      <c r="U7">
-        <v>0.04</v>
-      </c>
-      <c r="V7">
+      <c r="Y7">
+        <v>0.04</v>
+      </c>
+      <c r="Z7">
         <v>0</v>
       </c>
-      <c r="W7">
+      <c r="AA7">
         <v>3.9603960396039598E-2</v>
       </c>
-      <c r="X7">
-        <v>0.03</v>
-      </c>
-      <c r="Y7">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="L8" t="s">
+      <c r="AB7">
+        <v>0.03</v>
+      </c>
+      <c r="AC7">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="P8" t="s">
         <v>111</v>
       </c>
-      <c r="M8">
+      <c r="Q8">
         <v>0.09</v>
       </c>
-      <c r="N8">
-        <v>0.03</v>
-      </c>
-      <c r="O8">
-        <v>0.03</v>
-      </c>
-      <c r="P8">
-        <v>0.04</v>
-      </c>
-      <c r="Q8">
-        <v>0.02</v>
-      </c>
       <c r="R8">
         <v>0.03</v>
       </c>
       <c r="S8">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="T8">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="U8">
+        <v>0.02</v>
+      </c>
+      <c r="V8">
+        <v>0.03</v>
+      </c>
+      <c r="W8">
+        <v>0.01</v>
+      </c>
+      <c r="X8">
+        <v>0.03</v>
+      </c>
+      <c r="Y8">
         <v>0.08</v>
       </c>
-      <c r="V8">
-        <v>0.03</v>
-      </c>
-      <c r="W8">
+      <c r="Z8">
+        <v>0.03</v>
+      </c>
+      <c r="AA8">
         <v>7.9207920792079195E-2</v>
       </c>
-      <c r="X8">
+      <c r="AB8">
         <v>0</v>
       </c>
-      <c r="Y8">
+      <c r="AC8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="L9" t="s">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="P9" t="s">
         <v>112</v>
       </c>
-      <c r="M9">
-        <v>0.04</v>
-      </c>
-      <c r="N9">
-        <v>0.06</v>
-      </c>
-      <c r="O9">
-        <v>0.05</v>
-      </c>
-      <c r="P9">
-        <v>0.05</v>
-      </c>
       <c r="Q9">
         <v>0.04</v>
       </c>
       <c r="R9">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="S9">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="T9">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="U9">
         <v>0.04</v>
@@ -15794,800 +15857,2618 @@
         <v>0.05</v>
       </c>
       <c r="W9">
+        <v>0.03</v>
+      </c>
+      <c r="X9">
+        <v>0.06</v>
+      </c>
+      <c r="Y9">
+        <v>0.04</v>
+      </c>
+      <c r="Z9">
+        <v>0.05</v>
+      </c>
+      <c r="AA9">
         <v>3.9603960396039598E-2</v>
       </c>
-      <c r="X9">
-        <v>0.01</v>
-      </c>
-      <c r="Y9">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="L10" t="s">
+      <c r="AB9">
+        <v>0.01</v>
+      </c>
+      <c r="AC9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="P10" t="s">
         <v>113</v>
       </c>
-      <c r="M10">
+      <c r="Q10">
         <v>6.3829787234042507E-2</v>
       </c>
-      <c r="N10">
+      <c r="R10">
         <v>2.0833333333333301E-2</v>
       </c>
-      <c r="O10">
+      <c r="S10">
         <v>2.0833333333333301E-2</v>
       </c>
-      <c r="P10">
+      <c r="T10">
         <v>5.31914893617021E-2</v>
       </c>
-      <c r="Q10">
+      <c r="U10">
         <v>1.0416666666666701E-2</v>
       </c>
-      <c r="R10">
+      <c r="V10">
         <v>1.0416666666666701E-2</v>
       </c>
-      <c r="S10">
+      <c r="W10">
         <v>4.2553191489361701E-2</v>
       </c>
-      <c r="T10">
+      <c r="X10">
         <v>0</v>
       </c>
-      <c r="U10">
-        <v>0.05</v>
-      </c>
-      <c r="V10">
+      <c r="Y10">
+        <v>0.05</v>
+      </c>
+      <c r="Z10">
         <v>0</v>
       </c>
-      <c r="W10">
+      <c r="AA10">
         <v>4.95049504950495E-2</v>
       </c>
-      <c r="X10">
-        <v>0.04</v>
-      </c>
-      <c r="Y10">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="L11" t="s">
+      <c r="AB10">
+        <v>0.04</v>
+      </c>
+      <c r="AC10">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="P11" t="s">
         <v>114</v>
       </c>
-      <c r="M11">
-        <v>0.06</v>
-      </c>
-      <c r="N11">
-        <v>0.01</v>
-      </c>
-      <c r="O11">
+      <c r="Q11">
+        <v>0.06</v>
+      </c>
+      <c r="R11">
+        <v>0.01</v>
+      </c>
+      <c r="S11">
         <v>0</v>
       </c>
-      <c r="P11">
-        <v>0.05</v>
-      </c>
-      <c r="Q11">
-        <v>0.02</v>
-      </c>
-      <c r="R11">
-        <v>0.03</v>
-      </c>
-      <c r="S11">
-        <v>0.05</v>
-      </c>
       <c r="T11">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="U11">
-        <v>7.0000000000000007E-2</v>
+        <v>0.02</v>
       </c>
       <c r="V11">
+        <v>0.03</v>
+      </c>
+      <c r="W11">
+        <v>0.05</v>
+      </c>
+      <c r="X11">
+        <v>0.01</v>
+      </c>
+      <c r="Y11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z11">
         <v>0</v>
       </c>
-      <c r="W11">
+      <c r="AA11">
         <v>7.9207920792079195E-2</v>
       </c>
-      <c r="X11">
-        <v>0.03</v>
-      </c>
-      <c r="Y11">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="L12" t="s">
+      <c r="AB11">
+        <v>0.03</v>
+      </c>
+      <c r="AC11">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="P12" t="s">
         <v>115</v>
       </c>
-      <c r="M12">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="N12">
-        <v>0.04</v>
-      </c>
-      <c r="O12">
-        <v>0.03</v>
-      </c>
-      <c r="P12">
-        <v>0.04</v>
-      </c>
       <c r="Q12">
-        <v>0.02</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="R12">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="S12">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="T12">
         <v>0.04</v>
       </c>
       <c r="U12">
+        <v>0.02</v>
+      </c>
+      <c r="V12">
+        <v>0.02</v>
+      </c>
+      <c r="W12">
+        <v>0.04</v>
+      </c>
+      <c r="X12">
+        <v>0.04</v>
+      </c>
+      <c r="Y12">
         <v>0.08</v>
       </c>
-      <c r="V12">
-        <v>0.03</v>
-      </c>
-      <c r="W12">
+      <c r="Z12">
+        <v>0.03</v>
+      </c>
+      <c r="AA12">
         <v>7.9207920792079195E-2</v>
       </c>
-      <c r="X12">
+      <c r="AB12">
         <v>0</v>
       </c>
-      <c r="Y12">
+      <c r="AC12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="L13" t="s">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="P13" t="s">
         <v>116</v>
       </c>
-      <c r="M13">
+      <c r="Q13">
         <v>0.08</v>
       </c>
-      <c r="N13">
-        <v>0.04</v>
-      </c>
-      <c r="O13">
-        <v>0.04</v>
-      </c>
-      <c r="P13">
-        <v>0.04</v>
-      </c>
-      <c r="Q13">
-        <v>0.03</v>
-      </c>
       <c r="R13">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="S13">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="T13">
         <v>0.04</v>
       </c>
       <c r="U13">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="V13">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="W13">
+        <v>0.03</v>
+      </c>
+      <c r="X13">
+        <v>0.04</v>
+      </c>
+      <c r="Y13">
+        <v>0.06</v>
+      </c>
+      <c r="Z13">
+        <v>0.03</v>
+      </c>
+      <c r="AA13">
         <v>5.9405940594059403E-2</v>
       </c>
-      <c r="X13">
-        <v>0.02</v>
-      </c>
-      <c r="Y13">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="L14" t="s">
+      <c r="AB13">
+        <v>0.02</v>
+      </c>
+      <c r="AC13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="P14" t="s">
         <v>117</v>
       </c>
-      <c r="M14">
+      <c r="Q14">
         <v>0.11</v>
       </c>
-      <c r="N14">
-        <v>0.02</v>
-      </c>
-      <c r="O14">
-        <v>0.02</v>
-      </c>
-      <c r="P14">
+      <c r="R14">
+        <v>0.02</v>
+      </c>
+      <c r="S14">
+        <v>0.02</v>
+      </c>
+      <c r="T14">
         <v>0.1</v>
       </c>
-      <c r="Q14">
-        <v>0.01</v>
-      </c>
-      <c r="R14">
-        <v>0.01</v>
-      </c>
-      <c r="S14">
-        <v>0.05</v>
-      </c>
-      <c r="T14">
-        <v>0.02</v>
-      </c>
       <c r="U14">
+        <v>0.01</v>
+      </c>
+      <c r="V14">
+        <v>0.01</v>
+      </c>
+      <c r="W14">
+        <v>0.05</v>
+      </c>
+      <c r="X14">
+        <v>0.02</v>
+      </c>
+      <c r="Y14">
         <v>0.11</v>
       </c>
-      <c r="V14">
-        <v>0.03</v>
-      </c>
-      <c r="W14">
+      <c r="Z14">
+        <v>0.03</v>
+      </c>
+      <c r="AA14">
         <v>0.118811881188119</v>
       </c>
-      <c r="X14">
-        <v>0.03</v>
-      </c>
-      <c r="Y14">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" ht="360" x14ac:dyDescent="0.3">
+      <c r="AB14">
+        <v>0.03</v>
+      </c>
+      <c r="AC14">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" ht="360" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>45279</v>
       </c>
       <c r="B15" t="s">
         <v>137</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D15">
         <v>1E-3</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>142</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>140</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" t="s">
+        <v>147</v>
+      </c>
+      <c r="H15" t="s">
+        <v>148</v>
+      </c>
+      <c r="I15">
+        <v>500</v>
+      </c>
+      <c r="J15" s="2">
         <v>1</v>
       </c>
-      <c r="G15" s="2">
+      <c r="K15" s="2">
         <v>1</v>
       </c>
-      <c r="H15" t="s">
+      <c r="L15" t="s">
         <v>127</v>
       </c>
-      <c r="I15" t="s">
+      <c r="M15" t="s">
         <v>40</v>
       </c>
-      <c r="J15" t="s">
+      <c r="N15" t="s">
         <v>129</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="L15" t="s">
+      <c r="P15" t="s">
         <v>106</v>
       </c>
-      <c r="M15">
-        <v>0.05</v>
-      </c>
-      <c r="N15">
+      <c r="Q15">
+        <v>0.05</v>
+      </c>
+      <c r="R15">
         <v>0.09</v>
       </c>
-      <c r="O15">
+      <c r="S15">
         <v>0.13</v>
       </c>
-      <c r="P15">
-        <v>0.01</v>
-      </c>
-      <c r="Q15">
-        <v>0.06</v>
-      </c>
-      <c r="R15">
-        <v>0.06</v>
-      </c>
-      <c r="S15">
-        <v>0.02</v>
-      </c>
       <c r="T15">
+        <v>0.01</v>
+      </c>
+      <c r="U15">
+        <v>0.06</v>
+      </c>
+      <c r="V15">
+        <v>0.06</v>
+      </c>
+      <c r="W15">
+        <v>0.02</v>
+      </c>
+      <c r="X15">
         <v>0.09</v>
       </c>
-      <c r="U15">
-        <v>0.05</v>
-      </c>
-      <c r="V15">
+      <c r="Y15">
+        <v>0.05</v>
+      </c>
+      <c r="Z15">
         <v>0.13</v>
       </c>
-      <c r="W15">
+      <c r="AA15">
         <v>4.95049504950495E-2</v>
       </c>
-      <c r="X15">
-        <v>0.02</v>
-      </c>
-      <c r="Y15">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="L16" t="s">
+      <c r="AB15">
+        <v>0.02</v>
+      </c>
+      <c r="AC15">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="P16" t="s">
         <v>107</v>
       </c>
-      <c r="M16">
+      <c r="Q16">
         <v>0.12</v>
-      </c>
-      <c r="N16">
-        <v>0.12</v>
-      </c>
-      <c r="O16">
-        <v>0.15</v>
-      </c>
-      <c r="P16">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q16">
-        <v>0.09</v>
       </c>
       <c r="R16">
         <v>0.12</v>
       </c>
       <c r="S16">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="T16">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U16">
+        <v>0.09</v>
+      </c>
+      <c r="V16">
+        <v>0.12</v>
+      </c>
+      <c r="W16">
+        <v>0.04</v>
+      </c>
+      <c r="X16">
         <v>0.11</v>
       </c>
-      <c r="U16">
+      <c r="Y16">
         <v>0.13</v>
       </c>
-      <c r="V16">
+      <c r="Z16">
         <v>0.15</v>
       </c>
-      <c r="W16">
+      <c r="AA16">
         <v>0.12871287128712899</v>
       </c>
-      <c r="X16">
-        <v>0.02</v>
-      </c>
-      <c r="Y16">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="17" spans="12:25" x14ac:dyDescent="0.3">
-      <c r="L17" t="s">
+      <c r="AB16">
+        <v>0.02</v>
+      </c>
+      <c r="AC16">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P17" t="s">
         <v>108</v>
       </c>
-      <c r="M17">
+      <c r="Q17">
         <v>0.09</v>
       </c>
-      <c r="N17">
+      <c r="R17">
         <v>0.11</v>
       </c>
-      <c r="O17">
+      <c r="S17">
         <v>0.14000000000000001</v>
       </c>
-      <c r="P17">
+      <c r="T17">
         <v>0.09</v>
       </c>
-      <c r="Q17">
+      <c r="U17">
         <v>0.08</v>
       </c>
-      <c r="R17">
+      <c r="V17">
         <v>0.09</v>
       </c>
-      <c r="S17">
-        <v>0.05</v>
-      </c>
-      <c r="T17">
+      <c r="W17">
+        <v>0.05</v>
+      </c>
+      <c r="X17">
         <v>0.11</v>
       </c>
-      <c r="U17">
+      <c r="Y17">
         <v>0.1</v>
       </c>
-      <c r="V17">
+      <c r="Z17">
         <v>0.14000000000000001</v>
       </c>
-      <c r="W17">
+      <c r="AA17">
         <v>9.9009900990099001E-2</v>
       </c>
-      <c r="X17">
-        <v>0.06</v>
-      </c>
-      <c r="Y17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="18" spans="12:25" x14ac:dyDescent="0.3">
-      <c r="L18" t="s">
+      <c r="AB17">
+        <v>0.06</v>
+      </c>
+      <c r="AC17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P18" t="s">
         <v>109</v>
       </c>
-      <c r="M18">
+      <c r="Q18">
         <v>0.14000000000000001</v>
       </c>
-      <c r="N18">
+      <c r="R18">
         <v>0.15</v>
       </c>
-      <c r="O18">
+      <c r="S18">
         <v>0.14000000000000001</v>
       </c>
-      <c r="P18">
+      <c r="T18">
         <v>0.12</v>
       </c>
-      <c r="Q18">
+      <c r="U18">
         <v>0.09</v>
       </c>
-      <c r="R18">
+      <c r="V18">
         <v>0.1</v>
       </c>
-      <c r="S18">
+      <c r="W18">
         <v>0.08</v>
       </c>
-      <c r="T18">
+      <c r="X18">
         <v>0.16</v>
       </c>
-      <c r="U18">
+      <c r="Y18">
         <v>0.15</v>
       </c>
-      <c r="V18">
+      <c r="Z18">
         <v>0.12</v>
       </c>
-      <c r="W18">
+      <c r="AA18">
         <v>0.14851485148514901</v>
       </c>
-      <c r="X18">
-        <v>0.03</v>
-      </c>
-      <c r="Y18">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="19" spans="12:25" x14ac:dyDescent="0.3">
-      <c r="L19" t="s">
+      <c r="AB18">
+        <v>0.03</v>
+      </c>
+      <c r="AC18">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P19" t="s">
         <v>110</v>
       </c>
-      <c r="M19">
+      <c r="Q19">
         <v>0.12</v>
       </c>
-      <c r="N19">
+      <c r="R19">
         <v>0.15</v>
       </c>
-      <c r="O19">
+      <c r="S19">
         <v>0.13</v>
       </c>
-      <c r="P19">
-        <v>0.06</v>
-      </c>
-      <c r="Q19">
+      <c r="T19">
+        <v>0.06</v>
+      </c>
+      <c r="U19">
         <v>0.1</v>
-      </c>
-      <c r="R19">
-        <v>0.12</v>
-      </c>
-      <c r="S19">
-        <v>0.04</v>
-      </c>
-      <c r="T19">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="U19">
-        <v>0.12</v>
       </c>
       <c r="V19">
         <v>0.12</v>
       </c>
       <c r="W19">
+        <v>0.04</v>
+      </c>
+      <c r="X19">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Y19">
+        <v>0.12</v>
+      </c>
+      <c r="Z19">
+        <v>0.12</v>
+      </c>
+      <c r="AA19">
         <v>0.12871287128712899</v>
       </c>
-      <c r="X19">
-        <v>0.03</v>
-      </c>
-      <c r="Y19">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="20" spans="12:25" x14ac:dyDescent="0.3">
-      <c r="L20" t="s">
+      <c r="AB19">
+        <v>0.03</v>
+      </c>
+      <c r="AC19">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P20" t="s">
         <v>111</v>
       </c>
-      <c r="M20">
-        <v>0.06</v>
-      </c>
-      <c r="N20">
+      <c r="Q20">
+        <v>0.06</v>
+      </c>
+      <c r="R20">
         <v>0.12</v>
       </c>
-      <c r="O20">
+      <c r="S20">
         <v>0.13</v>
       </c>
-      <c r="P20">
-        <v>0.05</v>
-      </c>
-      <c r="Q20">
+      <c r="T20">
+        <v>0.05</v>
+      </c>
+      <c r="U20">
         <v>0.1</v>
       </c>
-      <c r="R20">
+      <c r="V20">
         <v>0.11</v>
       </c>
-      <c r="S20">
-        <v>0.01</v>
-      </c>
-      <c r="T20">
+      <c r="W20">
+        <v>0.01</v>
+      </c>
+      <c r="X20">
         <v>0.12</v>
       </c>
-      <c r="U20">
-        <v>0.06</v>
-      </c>
-      <c r="V20">
+      <c r="Y20">
+        <v>0.06</v>
+      </c>
+      <c r="Z20">
         <v>0.12</v>
       </c>
-      <c r="W20">
+      <c r="AA20">
         <v>5.9405940594059403E-2</v>
       </c>
-      <c r="X20">
-        <v>0.04</v>
-      </c>
-      <c r="Y20">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="21" spans="12:25" x14ac:dyDescent="0.3">
-      <c r="L21" t="s">
+      <c r="AB20">
+        <v>0.04</v>
+      </c>
+      <c r="AC20">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P21" t="s">
         <v>112</v>
       </c>
-      <c r="M21">
+      <c r="Q21">
         <v>0.09</v>
-      </c>
-      <c r="N21">
-        <v>0.15</v>
-      </c>
-      <c r="O21">
-        <v>0.22</v>
-      </c>
-      <c r="P21">
-        <v>0.05</v>
-      </c>
-      <c r="Q21">
-        <v>0.12</v>
       </c>
       <c r="R21">
         <v>0.15</v>
       </c>
       <c r="S21">
-        <v>0.03</v>
+        <v>0.22</v>
       </c>
       <c r="T21">
+        <v>0.05</v>
+      </c>
+      <c r="U21">
+        <v>0.12</v>
+      </c>
+      <c r="V21">
+        <v>0.15</v>
+      </c>
+      <c r="W21">
+        <v>0.03</v>
+      </c>
+      <c r="X21">
         <v>0.14000000000000001</v>
       </c>
-      <c r="U21">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="V21">
+      <c r="Y21">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z21">
         <v>0.21</v>
       </c>
-      <c r="W21">
+      <c r="AA21">
         <v>6.9306930693069299E-2</v>
       </c>
-      <c r="X21">
-        <v>0.03</v>
-      </c>
-      <c r="Y21">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="22" spans="12:25" x14ac:dyDescent="0.3">
-      <c r="L22" t="s">
+      <c r="AB21">
+        <v>0.03</v>
+      </c>
+      <c r="AC21">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P22" t="s">
         <v>113</v>
       </c>
-      <c r="M22">
+      <c r="Q22">
         <v>0.104651162790698</v>
       </c>
-      <c r="N22">
+      <c r="R22">
         <v>0.114583333333333</v>
       </c>
-      <c r="O22">
+      <c r="S22">
         <v>0.1875</v>
       </c>
-      <c r="P22">
+      <c r="T22">
         <v>4.81927710843374E-2</v>
       </c>
-      <c r="Q22">
+      <c r="U22">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="R22">
+      <c r="V22">
         <v>0.13541666666666699</v>
       </c>
-      <c r="S22">
+      <c r="W22">
         <v>2.53164556962025E-2</v>
       </c>
-      <c r="T22">
+      <c r="X22">
         <v>6.25E-2</v>
       </c>
-      <c r="U22">
+      <c r="Y22">
         <v>4.1237113402061903E-2</v>
       </c>
-      <c r="V22">
+      <c r="Z22">
         <v>0.104166666666667</v>
       </c>
-      <c r="W22">
+      <c r="AA22">
         <v>4.08163265306122E-2</v>
       </c>
-      <c r="X22">
-        <v>0.02</v>
-      </c>
-      <c r="Y22">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="23" spans="12:25" x14ac:dyDescent="0.3">
-      <c r="L23" t="s">
+      <c r="AB22">
+        <v>0.02</v>
+      </c>
+      <c r="AC22">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P23" t="s">
         <v>114</v>
       </c>
-      <c r="M23">
-        <v>0.02</v>
-      </c>
-      <c r="N23">
+      <c r="Q23">
+        <v>0.02</v>
+      </c>
+      <c r="R23">
         <v>0.14000000000000001</v>
       </c>
-      <c r="O23">
+      <c r="S23">
         <v>0.17</v>
       </c>
-      <c r="P23">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q23">
+      <c r="T23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U23">
         <v>0.12</v>
       </c>
-      <c r="R23">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="S23">
-        <v>0.01</v>
-      </c>
-      <c r="T23">
+      <c r="V23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W23">
+        <v>0.01</v>
+      </c>
+      <c r="X23">
         <v>0.14000000000000001</v>
       </c>
-      <c r="U23">
-        <v>0.02</v>
-      </c>
-      <c r="V23">
+      <c r="Y23">
+        <v>0.02</v>
+      </c>
+      <c r="Z23">
         <v>0.16</v>
       </c>
-      <c r="W23">
+      <c r="AA23">
         <v>1.9801980198019799E-2</v>
       </c>
-      <c r="X23">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Y23">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="12:25" x14ac:dyDescent="0.3">
-      <c r="L24" t="s">
+      <c r="AB23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P24" t="s">
         <v>115</v>
       </c>
-      <c r="M24">
-        <v>0.05</v>
-      </c>
-      <c r="N24">
+      <c r="Q24">
+        <v>0.05</v>
+      </c>
+      <c r="R24">
         <v>0.09</v>
       </c>
-      <c r="O24">
+      <c r="S24">
         <v>0.15</v>
       </c>
-      <c r="P24">
-        <v>0.04</v>
-      </c>
-      <c r="Q24">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="R24">
+      <c r="T24">
+        <v>0.04</v>
+      </c>
+      <c r="U24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V24">
         <v>0.1</v>
       </c>
-      <c r="S24">
-        <v>0.02</v>
-      </c>
-      <c r="T24">
+      <c r="W24">
+        <v>0.02</v>
+      </c>
+      <c r="X24">
         <v>0.09</v>
       </c>
-      <c r="U24">
-        <v>0.06</v>
-      </c>
-      <c r="V24">
+      <c r="Y24">
+        <v>0.06</v>
+      </c>
+      <c r="Z24">
         <v>0.14000000000000001</v>
       </c>
-      <c r="W24">
+      <c r="AA24">
         <v>5.9405940594059403E-2</v>
       </c>
-      <c r="X24">
-        <v>0.02</v>
-      </c>
-      <c r="Y24">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="25" spans="12:25" x14ac:dyDescent="0.3">
-      <c r="L25" t="s">
+      <c r="AB24">
+        <v>0.02</v>
+      </c>
+      <c r="AC24">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P25" t="s">
         <v>116</v>
       </c>
-      <c r="M25">
+      <c r="Q25">
         <v>0.1</v>
       </c>
-      <c r="N25">
+      <c r="R25">
         <v>0.19</v>
       </c>
-      <c r="O25">
+      <c r="S25">
         <v>0.16</v>
       </c>
-      <c r="P25">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q25">
+      <c r="T25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U25">
         <v>0.08</v>
       </c>
-      <c r="R25">
+      <c r="V25">
         <v>0.08</v>
       </c>
-      <c r="S25">
+      <c r="W25">
         <v>5.0505050505050497E-2</v>
       </c>
-      <c r="T25">
+      <c r="X25">
         <v>0.16</v>
       </c>
-      <c r="U25">
+      <c r="Y25">
         <v>0.1</v>
       </c>
-      <c r="V25">
+      <c r="Z25">
         <v>0.14000000000000001</v>
       </c>
-      <c r="W25">
+      <c r="AA25">
         <v>9.9009900990099001E-2</v>
       </c>
-      <c r="X25">
-        <v>0.04</v>
-      </c>
-      <c r="Y25">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="12:25" x14ac:dyDescent="0.3">
-      <c r="L26" t="s">
+      <c r="AB25">
+        <v>0.04</v>
+      </c>
+      <c r="AC25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P26" t="s">
         <v>117</v>
-      </c>
-      <c r="M26">
-        <v>0.09</v>
-      </c>
-      <c r="N26">
-        <v>0.06</v>
-      </c>
-      <c r="O26">
-        <v>0.18</v>
-      </c>
-      <c r="P26">
-        <v>0.09</v>
       </c>
       <c r="Q26">
         <v>0.09</v>
       </c>
       <c r="R26">
+        <v>0.06</v>
+      </c>
+      <c r="S26">
+        <v>0.18</v>
+      </c>
+      <c r="T26">
+        <v>0.09</v>
+      </c>
+      <c r="U26">
+        <v>0.09</v>
+      </c>
+      <c r="V26">
         <v>0.19</v>
       </c>
-      <c r="S26">
-        <v>0.04</v>
-      </c>
-      <c r="T26">
-        <v>0.05</v>
-      </c>
-      <c r="U26">
+      <c r="W26">
+        <v>0.04</v>
+      </c>
+      <c r="X26">
+        <v>0.05</v>
+      </c>
+      <c r="Y26">
         <v>0.08</v>
       </c>
-      <c r="V26">
+      <c r="Z26">
         <v>0.17</v>
       </c>
-      <c r="W26">
+      <c r="AA26">
         <v>7.9207920792079195E-2</v>
       </c>
-      <c r="X26">
-        <v>0.02</v>
-      </c>
-      <c r="Y26">
-        <v>0.05</v>
+      <c r="AB26">
+        <v>0.02</v>
+      </c>
+      <c r="AC26">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:38" ht="360" x14ac:dyDescent="0.3">
+      <c r="A27" s="11">
+        <v>44963</v>
+      </c>
+      <c r="B27" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" t="s">
+        <v>151</v>
+      </c>
+      <c r="D27">
+        <v>1E-3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>138</v>
+      </c>
+      <c r="F27" t="s">
+        <v>149</v>
+      </c>
+      <c r="G27" t="s">
+        <v>147</v>
+      </c>
+      <c r="H27" t="s">
+        <v>148</v>
+      </c>
+      <c r="I27" t="s">
+        <v>148</v>
+      </c>
+      <c r="J27" s="2">
+        <v>1</v>
+      </c>
+      <c r="K27" s="2">
+        <v>1</v>
+      </c>
+      <c r="L27" t="s">
+        <v>127</v>
+      </c>
+      <c r="M27" t="s">
+        <v>40</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P27" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q27">
+        <v>0.04</v>
+      </c>
+      <c r="R27">
+        <v>0.02</v>
+      </c>
+      <c r="S27">
+        <v>0.02</v>
+      </c>
+      <c r="T27">
+        <v>0.03</v>
+      </c>
+      <c r="U27">
+        <v>0.02</v>
+      </c>
+      <c r="V27">
+        <v>0.02</v>
+      </c>
+      <c r="W27">
+        <v>0.04</v>
+      </c>
+      <c r="X27">
+        <v>0.02</v>
+      </c>
+      <c r="Y27">
+        <v>0.09</v>
+      </c>
+      <c r="Z27">
+        <v>0.02</v>
+      </c>
+      <c r="AA27">
+        <v>0.09</v>
+      </c>
+      <c r="AB27">
+        <v>0.04</v>
+      </c>
+      <c r="AC27">
+        <v>0.04</v>
+      </c>
+      <c r="AD27">
+        <v>0.04</v>
+      </c>
+      <c r="AE27">
+        <v>0.03</v>
+      </c>
+      <c r="AF27">
+        <v>0.03</v>
+      </c>
+      <c r="AG27">
+        <v>0.03</v>
+      </c>
+      <c r="AH27">
+        <v>0.01</v>
+      </c>
+      <c r="AI27">
+        <v>0.01</v>
+      </c>
+      <c r="AJ27">
+        <v>0.06</v>
+      </c>
+      <c r="AK27">
+        <v>0.03</v>
+      </c>
+      <c r="AL27">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P28" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q28">
+        <v>0.03</v>
+      </c>
+      <c r="R28">
+        <v>0.03</v>
+      </c>
+      <c r="S28">
+        <v>0.03</v>
+      </c>
+      <c r="T28">
+        <v>0.02</v>
+      </c>
+      <c r="U28">
+        <v>0.01</v>
+      </c>
+      <c r="V28">
+        <v>0.01</v>
+      </c>
+      <c r="W28">
+        <v>0.03</v>
+      </c>
+      <c r="X28">
+        <v>0.02</v>
+      </c>
+      <c r="Y28">
+        <v>0.04</v>
+      </c>
+      <c r="Z28">
+        <v>0.02</v>
+      </c>
+      <c r="AA28">
+        <v>0.04</v>
+      </c>
+      <c r="AB28">
+        <v>0</v>
+      </c>
+      <c r="AC28">
+        <v>0</v>
+      </c>
+      <c r="AD28">
+        <v>0.02</v>
+      </c>
+      <c r="AE28">
+        <v>0.02</v>
+      </c>
+      <c r="AF28">
+        <v>0.02</v>
+      </c>
+      <c r="AG28">
+        <v>0.02</v>
+      </c>
+      <c r="AH28">
+        <v>0.02</v>
+      </c>
+      <c r="AI28">
+        <v>0.02</v>
+      </c>
+      <c r="AJ28">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AK28">
+        <v>0.03</v>
+      </c>
+      <c r="AL28">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P29" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q29">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R29">
+        <v>0.04</v>
+      </c>
+      <c r="S29">
+        <v>0.04</v>
+      </c>
+      <c r="T29">
+        <v>0.06</v>
+      </c>
+      <c r="U29">
+        <v>0.05</v>
+      </c>
+      <c r="V29">
+        <v>0.05</v>
+      </c>
+      <c r="W29">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="X29">
+        <v>0.04</v>
+      </c>
+      <c r="Y29">
+        <v>0.1</v>
+      </c>
+      <c r="Z29">
+        <v>0.04</v>
+      </c>
+      <c r="AA29">
+        <v>0.1</v>
+      </c>
+      <c r="AB29">
+        <v>0.04</v>
+      </c>
+      <c r="AC29">
+        <v>0.04</v>
+      </c>
+      <c r="AD29">
+        <v>0.04</v>
+      </c>
+      <c r="AE29">
+        <v>0.03</v>
+      </c>
+      <c r="AF29">
+        <v>0.03</v>
+      </c>
+      <c r="AG29">
+        <v>0.02</v>
+      </c>
+      <c r="AH29">
+        <v>0.03</v>
+      </c>
+      <c r="AI29">
+        <v>0.02</v>
+      </c>
+      <c r="AJ29">
+        <v>0.04</v>
+      </c>
+      <c r="AK29">
+        <v>0.06</v>
+      </c>
+      <c r="AL29">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P30" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q30">
+        <v>0.03</v>
+      </c>
+      <c r="R30">
+        <v>0.05</v>
+      </c>
+      <c r="S30">
+        <v>0.06</v>
+      </c>
+      <c r="T30">
+        <v>0.01</v>
+      </c>
+      <c r="U30">
+        <v>0.03</v>
+      </c>
+      <c r="V30">
+        <v>0.03</v>
+      </c>
+      <c r="W30">
+        <v>0.02</v>
+      </c>
+      <c r="X30">
+        <v>0.05</v>
+      </c>
+      <c r="Y30">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z30">
+        <v>0.06</v>
+      </c>
+      <c r="AA30">
+        <v>0.06</v>
+      </c>
+      <c r="AB30">
+        <v>0</v>
+      </c>
+      <c r="AC30">
+        <v>0</v>
+      </c>
+      <c r="AD30">
+        <v>0.02</v>
+      </c>
+      <c r="AE30">
+        <v>0.05</v>
+      </c>
+      <c r="AF30">
+        <v>0.02</v>
+      </c>
+      <c r="AG30">
+        <v>0.01</v>
+      </c>
+      <c r="AH30">
+        <v>0.02</v>
+      </c>
+      <c r="AI30">
+        <v>0.01</v>
+      </c>
+      <c r="AJ30">
+        <v>0.03</v>
+      </c>
+      <c r="AK30">
+        <v>0.06</v>
+      </c>
+      <c r="AL30">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P31" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q31">
+        <v>0.02</v>
+      </c>
+      <c r="R31">
+        <v>0.03</v>
+      </c>
+      <c r="S31">
+        <v>0.03</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>0.03</v>
+      </c>
+      <c r="V31">
+        <v>0.04</v>
+      </c>
+      <c r="W31">
+        <v>0.01</v>
+      </c>
+      <c r="X31">
+        <v>0.03</v>
+      </c>
+      <c r="Y31">
+        <v>0.06</v>
+      </c>
+      <c r="Z31">
+        <v>0.03</v>
+      </c>
+      <c r="AA31">
+        <v>0.06</v>
+      </c>
+      <c r="AB31">
+        <v>0.03</v>
+      </c>
+      <c r="AC31">
+        <v>0.03</v>
+      </c>
+      <c r="AD31">
+        <v>0.03</v>
+      </c>
+      <c r="AE31">
+        <v>0.02</v>
+      </c>
+      <c r="AF31">
+        <v>0.04</v>
+      </c>
+      <c r="AG31">
+        <v>0.05</v>
+      </c>
+      <c r="AH31">
+        <v>0.02</v>
+      </c>
+      <c r="AI31">
+        <v>0.01</v>
+      </c>
+      <c r="AJ31">
+        <v>0.06</v>
+      </c>
+      <c r="AK31">
+        <v>0.06</v>
+      </c>
+      <c r="AL31">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P32" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q32">
+        <v>0.03</v>
+      </c>
+      <c r="R32">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S32">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T32">
+        <v>0.02</v>
+      </c>
+      <c r="U32">
+        <v>0.04</v>
+      </c>
+      <c r="V32">
+        <v>0.03</v>
+      </c>
+      <c r="W32">
+        <v>0.02</v>
+      </c>
+      <c r="X32">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y32">
+        <v>0.05</v>
+      </c>
+      <c r="Z32">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA32">
+        <v>0.06</v>
+      </c>
+      <c r="AB32">
+        <v>0.01</v>
+      </c>
+      <c r="AC32">
+        <v>0.01</v>
+      </c>
+      <c r="AD32">
+        <v>0.05</v>
+      </c>
+      <c r="AE32">
+        <v>0.08</v>
+      </c>
+      <c r="AF32">
+        <v>0.06</v>
+      </c>
+      <c r="AG32">
+        <v>0.03</v>
+      </c>
+      <c r="AH32">
+        <v>0.05</v>
+      </c>
+      <c r="AI32">
+        <v>0.04</v>
+      </c>
+      <c r="AJ32">
+        <v>0.05</v>
+      </c>
+      <c r="AK32">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AL32">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="33" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P33" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q33">
+        <v>0.03</v>
+      </c>
+      <c r="R33">
+        <v>0.04</v>
+      </c>
+      <c r="S33">
+        <v>0.04</v>
+      </c>
+      <c r="T33">
+        <v>0.01</v>
+      </c>
+      <c r="U33">
+        <v>0.03</v>
+      </c>
+      <c r="V33">
+        <v>0.02</v>
+      </c>
+      <c r="W33">
+        <v>0.03</v>
+      </c>
+      <c r="X33">
+        <v>0.04</v>
+      </c>
+      <c r="Y33">
+        <v>0.06</v>
+      </c>
+      <c r="Z33">
+        <v>0.04</v>
+      </c>
+      <c r="AA33">
+        <v>0.06</v>
+      </c>
+      <c r="AB33">
+        <v>0.02</v>
+      </c>
+      <c r="AC33">
+        <v>0.02</v>
+      </c>
+      <c r="AD33">
+        <v>0.08</v>
+      </c>
+      <c r="AE33">
+        <v>0.03</v>
+      </c>
+      <c r="AF33">
+        <v>0.06</v>
+      </c>
+      <c r="AG33">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AH33">
+        <v>0.04</v>
+      </c>
+      <c r="AI33">
+        <v>0.05</v>
+      </c>
+      <c r="AJ33">
+        <v>0.05</v>
+      </c>
+      <c r="AK33">
+        <v>0.04</v>
+      </c>
+      <c r="AL33">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="34" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P34" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q34">
+        <v>4.3478260869565202E-2</v>
+      </c>
+      <c r="R34">
+        <v>3.03030303030303E-2</v>
+      </c>
+      <c r="S34">
+        <v>3.03030303030303E-2</v>
+      </c>
+      <c r="T34">
+        <v>3.2967032967033003E-2</v>
+      </c>
+      <c r="U34">
+        <v>2.04081632653061E-2</v>
+      </c>
+      <c r="V34">
+        <v>2.04081632653061E-2</v>
+      </c>
+      <c r="W34">
+        <v>2.1739130434782601E-2</v>
+      </c>
+      <c r="X34">
+        <v>0</v>
+      </c>
+      <c r="Y34">
+        <v>0.05</v>
+      </c>
+      <c r="Z34">
+        <v>0</v>
+      </c>
+      <c r="AA34">
+        <v>0.05</v>
+      </c>
+      <c r="AB34">
+        <v>0.02</v>
+      </c>
+      <c r="AC34">
+        <v>0.02</v>
+      </c>
+      <c r="AD34">
+        <v>0.06</v>
+      </c>
+      <c r="AE34">
+        <v>0.06</v>
+      </c>
+      <c r="AF34">
+        <v>0.04</v>
+      </c>
+      <c r="AG34">
+        <v>0.06</v>
+      </c>
+      <c r="AH34">
+        <v>0.02</v>
+      </c>
+      <c r="AI34">
+        <v>0.01</v>
+      </c>
+      <c r="AJ34">
+        <v>0.05</v>
+      </c>
+      <c r="AK34">
+        <v>0.06</v>
+      </c>
+      <c r="AL34">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="35" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P35" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q35">
+        <v>0.09</v>
+      </c>
+      <c r="R35">
+        <v>0.05</v>
+      </c>
+      <c r="S35">
+        <v>0.05</v>
+      </c>
+      <c r="T35">
+        <v>0.03</v>
+      </c>
+      <c r="U35">
+        <v>0.05</v>
+      </c>
+      <c r="V35">
+        <v>0.05</v>
+      </c>
+      <c r="W35">
+        <v>0.09</v>
+      </c>
+      <c r="X35">
+        <v>0.05</v>
+      </c>
+      <c r="Y35">
+        <v>0.12</v>
+      </c>
+      <c r="Z35">
+        <v>0.05</v>
+      </c>
+      <c r="AA35">
+        <v>0.12</v>
+      </c>
+      <c r="AB35">
+        <v>0.05</v>
+      </c>
+      <c r="AC35">
+        <v>0.05</v>
+      </c>
+      <c r="AD35">
+        <v>0.04</v>
+      </c>
+      <c r="AE35">
+        <v>0.05</v>
+      </c>
+      <c r="AF35">
+        <v>0.05</v>
+      </c>
+      <c r="AG35">
+        <v>0.05</v>
+      </c>
+      <c r="AH35">
+        <v>0.04</v>
+      </c>
+      <c r="AI35">
+        <v>0.03</v>
+      </c>
+      <c r="AJ35">
+        <v>0.06</v>
+      </c>
+      <c r="AK35">
+        <v>0.06</v>
+      </c>
+      <c r="AL35">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="36" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P36" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q36">
+        <v>0.03</v>
+      </c>
+      <c r="R36">
+        <v>0.06</v>
+      </c>
+      <c r="S36">
+        <v>0.05</v>
+      </c>
+      <c r="T36">
+        <v>0.04</v>
+      </c>
+      <c r="U36">
+        <v>0.05</v>
+      </c>
+      <c r="V36">
+        <v>0.05</v>
+      </c>
+      <c r="W36">
+        <v>0.03</v>
+      </c>
+      <c r="X36">
+        <v>0.06</v>
+      </c>
+      <c r="Y36">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z36">
+        <v>0.05</v>
+      </c>
+      <c r="AA36">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB36">
+        <v>0.06</v>
+      </c>
+      <c r="AC36">
+        <v>0.06</v>
+      </c>
+      <c r="AD36">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AE36">
+        <v>0.02</v>
+      </c>
+      <c r="AF36">
+        <v>0.03</v>
+      </c>
+      <c r="AG36">
+        <v>0.04</v>
+      </c>
+      <c r="AH36">
+        <v>0.03</v>
+      </c>
+      <c r="AI36">
+        <v>0.02</v>
+      </c>
+      <c r="AJ36">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AK36">
+        <v>0.03</v>
+      </c>
+      <c r="AL36">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="37" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P37" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q37">
+        <v>0.01</v>
+      </c>
+      <c r="R37">
+        <v>0.03</v>
+      </c>
+      <c r="S37">
+        <v>0.03</v>
+      </c>
+      <c r="T37">
+        <v>0.02</v>
+      </c>
+      <c r="U37">
+        <v>0.02</v>
+      </c>
+      <c r="V37">
+        <v>0.02</v>
+      </c>
+      <c r="W37">
+        <v>0.01</v>
+      </c>
+      <c r="X37">
+        <v>0.03</v>
+      </c>
+      <c r="Y37">
+        <v>0.06</v>
+      </c>
+      <c r="Z37">
+        <v>0.03</v>
+      </c>
+      <c r="AA37">
+        <v>0.06</v>
+      </c>
+      <c r="AB37">
+        <v>0.02</v>
+      </c>
+      <c r="AC37">
+        <v>0.02</v>
+      </c>
+      <c r="AD37">
+        <v>0.03</v>
+      </c>
+      <c r="AE37">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AF37">
+        <v>0.04</v>
+      </c>
+      <c r="AG37">
+        <v>0.03</v>
+      </c>
+      <c r="AH37">
+        <v>0.05</v>
+      </c>
+      <c r="AI37">
+        <v>0.05</v>
+      </c>
+      <c r="AJ37">
+        <v>0.03</v>
+      </c>
+      <c r="AK37">
+        <v>0.05</v>
+      </c>
+      <c r="AL37">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="38" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P38" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q38">
+        <v>0.05</v>
+      </c>
+      <c r="R38">
+        <v>0.05</v>
+      </c>
+      <c r="S38">
+        <v>0.05</v>
+      </c>
+      <c r="T38">
+        <v>0.05</v>
+      </c>
+      <c r="U38">
+        <v>0.03</v>
+      </c>
+      <c r="V38">
+        <v>0.02</v>
+      </c>
+      <c r="W38">
+        <v>0.05</v>
+      </c>
+      <c r="X38">
+        <v>0.05</v>
+      </c>
+      <c r="Y38">
+        <v>0.1</v>
+      </c>
+      <c r="Z38">
+        <v>0.05</v>
+      </c>
+      <c r="AA38">
+        <v>0.1</v>
+      </c>
+      <c r="AB38">
+        <v>0.02</v>
+      </c>
+      <c r="AC38">
+        <v>0.02</v>
+      </c>
+      <c r="AD38">
+        <v>0.03</v>
+      </c>
+      <c r="AE38">
+        <v>0.04</v>
+      </c>
+      <c r="AF38">
+        <v>0.03</v>
+      </c>
+      <c r="AG38">
+        <v>0.03</v>
+      </c>
+      <c r="AH38">
+        <v>0.04</v>
+      </c>
+      <c r="AI38">
+        <v>0.05</v>
+      </c>
+      <c r="AJ38">
+        <v>0.03</v>
+      </c>
+      <c r="AK38">
+        <v>0.04</v>
+      </c>
+      <c r="AL38">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:38" ht="360" x14ac:dyDescent="0.3">
+      <c r="A39" s="11">
+        <v>44963</v>
+      </c>
+      <c r="B39" t="s">
+        <v>137</v>
+      </c>
+      <c r="C39" t="s">
+        <v>151</v>
+      </c>
+      <c r="D39">
+        <v>1E-3</v>
+      </c>
+      <c r="E39" t="s">
+        <v>142</v>
+      </c>
+      <c r="F39" t="s">
+        <v>149</v>
+      </c>
+      <c r="G39" t="s">
+        <v>147</v>
+      </c>
+      <c r="H39" t="s">
+        <v>148</v>
+      </c>
+      <c r="I39" t="s">
+        <v>148</v>
+      </c>
+      <c r="J39" s="2">
+        <v>1</v>
+      </c>
+      <c r="K39" s="2">
+        <v>1</v>
+      </c>
+      <c r="L39" t="s">
+        <v>127</v>
+      </c>
+      <c r="M39" t="s">
+        <v>40</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P39" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q39">
+        <v>0.06</v>
+      </c>
+      <c r="R39">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S39">
+        <v>0.04</v>
+      </c>
+      <c r="T39">
+        <v>0.04</v>
+      </c>
+      <c r="U39">
+        <v>0.09</v>
+      </c>
+      <c r="V39">
+        <v>0.02</v>
+      </c>
+      <c r="W39">
+        <v>0.06</v>
+      </c>
+      <c r="X39">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Y39">
+        <v>0.08</v>
+      </c>
+      <c r="Z39">
+        <v>0.04</v>
+      </c>
+      <c r="AA39">
+        <v>0.08</v>
+      </c>
+      <c r="AB39">
+        <v>0.02</v>
+      </c>
+      <c r="AC39">
+        <v>0.04</v>
+      </c>
+      <c r="AD39">
+        <v>0.03</v>
+      </c>
+      <c r="AE39">
+        <v>0.33</v>
+      </c>
+      <c r="AF39">
+        <v>0.12</v>
+      </c>
+      <c r="AG39">
+        <v>0.03</v>
+      </c>
+      <c r="AH39">
+        <v>0.25</v>
+      </c>
+      <c r="AI39">
+        <v>0.06</v>
+      </c>
+      <c r="AJ39">
+        <v>0.06</v>
+      </c>
+      <c r="AK39">
+        <v>0.23</v>
+      </c>
+      <c r="AL39">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P40" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q40">
+        <v>0.02</v>
+      </c>
+      <c r="R40">
+        <v>0.1</v>
+      </c>
+      <c r="S40">
+        <v>0.02</v>
+      </c>
+      <c r="T40">
+        <v>0.01</v>
+      </c>
+      <c r="U40">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V40">
+        <v>0.03</v>
+      </c>
+      <c r="W40">
+        <v>0.02</v>
+      </c>
+      <c r="X40">
+        <v>0.08</v>
+      </c>
+      <c r="Y40">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z40">
+        <v>0.02</v>
+      </c>
+      <c r="AA40">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB40">
+        <v>0.02</v>
+      </c>
+      <c r="AC40">
+        <v>0.01</v>
+      </c>
+      <c r="AD40">
+        <v>0.02</v>
+      </c>
+      <c r="AE40">
+        <v>0.21</v>
+      </c>
+      <c r="AF40">
+        <v>0.13</v>
+      </c>
+      <c r="AG40">
+        <v>0.02</v>
+      </c>
+      <c r="AH40">
+        <v>0.17</v>
+      </c>
+      <c r="AI40">
+        <v>0.05</v>
+      </c>
+      <c r="AJ40">
+        <v>0.06</v>
+      </c>
+      <c r="AK40">
+        <v>0.18</v>
+      </c>
+      <c r="AL40">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P41" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q41">
+        <v>0.04</v>
+      </c>
+      <c r="R41">
+        <v>0.08</v>
+      </c>
+      <c r="S41">
+        <v>0.02</v>
+      </c>
+      <c r="T41">
+        <v>0.05</v>
+      </c>
+      <c r="U41">
+        <v>0.08</v>
+      </c>
+      <c r="V41">
+        <v>0.01</v>
+      </c>
+      <c r="W41">
+        <v>0.04</v>
+      </c>
+      <c r="X41">
+        <v>0.08</v>
+      </c>
+      <c r="Y41">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z41">
+        <v>0.02</v>
+      </c>
+      <c r="AA41">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB41">
+        <v>0.04</v>
+      </c>
+      <c r="AC41">
+        <v>0.03</v>
+      </c>
+      <c r="AD41">
+        <v>0.03</v>
+      </c>
+      <c r="AE41">
+        <v>0.31</v>
+      </c>
+      <c r="AF41">
+        <v>0.17</v>
+      </c>
+      <c r="AG41">
+        <v>0.02</v>
+      </c>
+      <c r="AH41">
+        <v>0.25</v>
+      </c>
+      <c r="AI41">
+        <v>0.12</v>
+      </c>
+      <c r="AJ41">
+        <v>0.04</v>
+      </c>
+      <c r="AK41">
+        <v>0.26</v>
+      </c>
+      <c r="AL41">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P42" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q42">
+        <v>0.06</v>
+      </c>
+      <c r="R42">
+        <v>0.1</v>
+      </c>
+      <c r="S42">
+        <v>0.05</v>
+      </c>
+      <c r="T42">
+        <v>0.05</v>
+      </c>
+      <c r="U42">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V42">
+        <v>0.02</v>
+      </c>
+      <c r="W42">
+        <v>0.05</v>
+      </c>
+      <c r="X42">
+        <v>0.11</v>
+      </c>
+      <c r="Y42">
+        <v>0.08</v>
+      </c>
+      <c r="Z42">
+        <v>0.04</v>
+      </c>
+      <c r="AA42">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB42">
+        <v>0.02</v>
+      </c>
+      <c r="AC42">
+        <v>0.01</v>
+      </c>
+      <c r="AD42">
+        <v>0.04</v>
+      </c>
+      <c r="AE42">
+        <v>0.17</v>
+      </c>
+      <c r="AF42">
+        <v>0.05</v>
+      </c>
+      <c r="AG42">
+        <v>0.04</v>
+      </c>
+      <c r="AH42">
+        <v>0.16</v>
+      </c>
+      <c r="AI42">
+        <v>0.08</v>
+      </c>
+      <c r="AJ42">
+        <v>0.01</v>
+      </c>
+      <c r="AK42">
+        <v>0.21</v>
+      </c>
+      <c r="AL42">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P43" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q43">
+        <v>0.08</v>
+      </c>
+      <c r="R43">
+        <v>0.15</v>
+      </c>
+      <c r="S43">
+        <v>0.06</v>
+      </c>
+      <c r="T43">
+        <v>0.04</v>
+      </c>
+      <c r="U43">
+        <v>0.08</v>
+      </c>
+      <c r="V43">
+        <v>0.02</v>
+      </c>
+      <c r="W43">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="X43">
+        <v>0.15</v>
+      </c>
+      <c r="Y43">
+        <v>0.1</v>
+      </c>
+      <c r="Z43">
+        <v>0.06</v>
+      </c>
+      <c r="AA43">
+        <v>0.1</v>
+      </c>
+      <c r="AB43">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC43">
+        <v>0.03</v>
+      </c>
+      <c r="AD43">
+        <v>0.04</v>
+      </c>
+      <c r="AE43">
+        <v>0.34</v>
+      </c>
+      <c r="AF43">
+        <v>0.17</v>
+      </c>
+      <c r="AG43">
+        <v>0.03</v>
+      </c>
+      <c r="AH43">
+        <v>0.25</v>
+      </c>
+      <c r="AI43">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AJ43">
+        <v>0.03</v>
+      </c>
+      <c r="AK43">
+        <v>0.22</v>
+      </c>
+      <c r="AL43">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P44" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q44">
+        <v>0.02</v>
+      </c>
+      <c r="R44">
+        <v>0.04</v>
+      </c>
+      <c r="S44">
+        <v>0.03</v>
+      </c>
+      <c r="T44">
+        <v>0.01</v>
+      </c>
+      <c r="U44">
+        <v>0.02</v>
+      </c>
+      <c r="V44">
+        <v>0.04</v>
+      </c>
+      <c r="W44">
+        <v>0.02</v>
+      </c>
+      <c r="X44">
+        <v>0.04</v>
+      </c>
+      <c r="Y44">
+        <v>0.05</v>
+      </c>
+      <c r="Z44">
+        <v>0.02</v>
+      </c>
+      <c r="AA44">
+        <v>0.04</v>
+      </c>
+      <c r="AB44">
+        <v>0.04</v>
+      </c>
+      <c r="AC44">
+        <v>0.01</v>
+      </c>
+      <c r="AD44">
+        <v>0.08</v>
+      </c>
+      <c r="AE44">
+        <v>0.21</v>
+      </c>
+      <c r="AF44">
+        <v>0.09</v>
+      </c>
+      <c r="AG44">
+        <v>0.03</v>
+      </c>
+      <c r="AH44">
+        <v>0.2</v>
+      </c>
+      <c r="AI44">
+        <v>0.1</v>
+      </c>
+      <c r="AJ44">
+        <v>0.06</v>
+      </c>
+      <c r="AK44">
+        <v>0.18</v>
+      </c>
+      <c r="AL44">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="45" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P45" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q45">
+        <v>0.03</v>
+      </c>
+      <c r="R45">
+        <v>0.11</v>
+      </c>
+      <c r="S45">
+        <v>0.05</v>
+      </c>
+      <c r="T45">
+        <v>0.01</v>
+      </c>
+      <c r="U45">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V45">
+        <v>0.05</v>
+      </c>
+      <c r="W45">
+        <v>0.03</v>
+      </c>
+      <c r="X45">
+        <v>0.09</v>
+      </c>
+      <c r="Y45">
+        <v>0.05</v>
+      </c>
+      <c r="Z45">
+        <v>0.05</v>
+      </c>
+      <c r="AA45">
+        <v>0.06</v>
+      </c>
+      <c r="AB45">
+        <v>0.03</v>
+      </c>
+      <c r="AC45">
+        <v>0.03</v>
+      </c>
+      <c r="AD45">
+        <v>0.05</v>
+      </c>
+      <c r="AE45">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AF45">
+        <v>0.11</v>
+      </c>
+      <c r="AG45">
+        <v>0.04</v>
+      </c>
+      <c r="AH45">
+        <v>0.21</v>
+      </c>
+      <c r="AI45">
+        <v>0.1</v>
+      </c>
+      <c r="AJ45">
+        <v>0.06</v>
+      </c>
+      <c r="AK45">
+        <v>0.15</v>
+      </c>
+      <c r="AL45">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P46" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q46">
+        <v>1.35135135135135E-2</v>
+      </c>
+      <c r="R46">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="S46">
+        <v>6.5934065934065894E-2</v>
+      </c>
+      <c r="T46">
+        <v>1.4285714285714299E-2</v>
+      </c>
+      <c r="U46">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="V46">
+        <v>2.1978021978022001E-2</v>
+      </c>
+      <c r="W46">
+        <v>1.35135135135135E-2</v>
+      </c>
+      <c r="X46">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="Y46">
+        <v>3.03030303030303E-2</v>
+      </c>
+      <c r="Z46">
+        <v>3.2967032967033003E-2</v>
+      </c>
+      <c r="AA46">
+        <v>3.06122448979592E-2</v>
+      </c>
+      <c r="AB46">
+        <v>0.01</v>
+      </c>
+      <c r="AC46">
+        <v>0.01</v>
+      </c>
+      <c r="AD46">
+        <v>0.03</v>
+      </c>
+      <c r="AE46">
+        <v>0.2</v>
+      </c>
+      <c r="AF46">
+        <v>0.06</v>
+      </c>
+      <c r="AG46">
+        <v>0.06</v>
+      </c>
+      <c r="AH46">
+        <v>0.18</v>
+      </c>
+      <c r="AI46">
+        <v>0.09</v>
+      </c>
+      <c r="AJ46">
+        <v>0.01</v>
+      </c>
+      <c r="AK46">
+        <v>0.17</v>
+      </c>
+      <c r="AL46">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="47" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P47" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <v>0.12</v>
+      </c>
+      <c r="S47">
+        <v>0.04</v>
+      </c>
+      <c r="T47">
+        <v>0.01</v>
+      </c>
+      <c r="U47">
+        <v>0.1</v>
+      </c>
+      <c r="V47">
+        <v>0.03</v>
+      </c>
+      <c r="W47">
+        <v>0</v>
+      </c>
+      <c r="X47">
+        <v>0.11</v>
+      </c>
+      <c r="Y47">
+        <v>0.01</v>
+      </c>
+      <c r="Z47">
+        <v>0.02</v>
+      </c>
+      <c r="AA47">
+        <v>0.01</v>
+      </c>
+      <c r="AB47">
+        <v>0.06</v>
+      </c>
+      <c r="AC47">
+        <v>0.03</v>
+      </c>
+      <c r="AD47">
+        <v>0.01</v>
+      </c>
+      <c r="AE47">
+        <v>0.34</v>
+      </c>
+      <c r="AF47">
+        <v>0.17</v>
+      </c>
+      <c r="AG47">
+        <v>0.04</v>
+      </c>
+      <c r="AH47">
+        <v>0.3</v>
+      </c>
+      <c r="AI47">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AJ47">
+        <v>0.03</v>
+      </c>
+      <c r="AK47">
+        <v>0.26</v>
+      </c>
+      <c r="AL47">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P48" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q48">
+        <v>0.06</v>
+      </c>
+      <c r="R48">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S48">
+        <v>0.04</v>
+      </c>
+      <c r="T48">
+        <v>0.04</v>
+      </c>
+      <c r="U48">
+        <v>0.09</v>
+      </c>
+      <c r="V48">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W48">
+        <v>0.05</v>
+      </c>
+      <c r="X48">
+        <v>0.12</v>
+      </c>
+      <c r="Y48">
+        <v>0.11</v>
+      </c>
+      <c r="Z48">
+        <v>0.03</v>
+      </c>
+      <c r="AA48">
+        <v>0.11</v>
+      </c>
+      <c r="AB48">
+        <v>0.04</v>
+      </c>
+      <c r="AC48">
+        <v>0.05</v>
+      </c>
+      <c r="AD48">
+        <v>0.08</v>
+      </c>
+      <c r="AE48">
+        <v>0.27</v>
+      </c>
+      <c r="AF48">
+        <v>0.15</v>
+      </c>
+      <c r="AG48">
+        <v>0.05</v>
+      </c>
+      <c r="AH48">
+        <v>0.24</v>
+      </c>
+      <c r="AI48">
+        <v>0.08</v>
+      </c>
+      <c r="AJ48">
+        <v>0.06</v>
+      </c>
+      <c r="AK48">
+        <v>0.19</v>
+      </c>
+      <c r="AL48">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="16:38" x14ac:dyDescent="0.3">
+      <c r="P49" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q49">
+        <v>6.0606060606060601E-2</v>
+      </c>
+      <c r="R49">
+        <v>0.15</v>
+      </c>
+      <c r="S49">
+        <v>0.06</v>
+      </c>
+      <c r="T49">
+        <v>2.02020202020202E-2</v>
+      </c>
+      <c r="U49">
+        <v>0.13</v>
+      </c>
+      <c r="V49">
+        <v>0.05</v>
+      </c>
+      <c r="W49">
+        <v>4.0404040404040401E-2</v>
+      </c>
+      <c r="X49">
+        <v>0.13</v>
+      </c>
+      <c r="Y49">
+        <v>0.05</v>
+      </c>
+      <c r="Z49">
+        <v>0.04</v>
+      </c>
+      <c r="AA49">
+        <v>0.05</v>
+      </c>
+      <c r="AB49">
+        <v>0.04</v>
+      </c>
+      <c r="AC49">
+        <v>0.03</v>
+      </c>
+      <c r="AD49">
+        <v>0.03</v>
+      </c>
+      <c r="AE49">
+        <v>0.23</v>
+      </c>
+      <c r="AF49">
+        <v>0.13</v>
+      </c>
+      <c r="AG49">
+        <v>0.02</v>
+      </c>
+      <c r="AH49">
+        <v>0.21</v>
+      </c>
+      <c r="AI49">
+        <v>0.11</v>
+      </c>
+      <c r="AJ49">
+        <v>0.05</v>
+      </c>
+      <c r="AK49">
+        <v>0.2</v>
+      </c>
+      <c r="AL49">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="50" spans="16:38" x14ac:dyDescent="0.3">
+      <c r="P50" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q50">
+        <v>0.02</v>
+      </c>
+      <c r="R50">
+        <v>0.11</v>
+      </c>
+      <c r="S50">
+        <v>0.03</v>
+      </c>
+      <c r="T50">
+        <v>0.03</v>
+      </c>
+      <c r="U50">
+        <v>0.11</v>
+      </c>
+      <c r="V50">
+        <v>0.05</v>
+      </c>
+      <c r="W50">
+        <v>0.02</v>
+      </c>
+      <c r="X50">
+        <v>0.1</v>
+      </c>
+      <c r="Y50">
+        <v>0.05</v>
+      </c>
+      <c r="Z50">
+        <v>0.03</v>
+      </c>
+      <c r="AA50">
+        <v>0.05</v>
+      </c>
+      <c r="AB50">
+        <v>0.03</v>
+      </c>
+      <c r="AC50">
+        <v>0</v>
+      </c>
+      <c r="AD50">
+        <v>0.03</v>
+      </c>
+      <c r="AE50">
+        <v>0.43</v>
+      </c>
+      <c r="AF50">
+        <v>0.19</v>
+      </c>
+      <c r="AG50">
+        <v>0.05</v>
+      </c>
+      <c r="AH50">
+        <v>0.33</v>
+      </c>
+      <c r="AI50">
+        <v>0.13</v>
+      </c>
+      <c r="AJ50">
+        <v>0.03</v>
+      </c>
+      <c r="AK50">
+        <v>0.37</v>
+      </c>
+      <c r="AL50">
+        <v>0.23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="M1:Z1"/>
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="Q1:AD1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added 100v80 results for s1 and s2
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D923FBC5-4B60-4656-ABED-2CCDF93180E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5FDF80-7070-483F-B3D9-FF574053087C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="153">
   <si>
     <t>Population</t>
   </si>
@@ -842,9 +842,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -882,7 +882,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -988,7 +988,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1130,7 +1130,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -15340,11 +15340,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669C6091-A5A6-4DA3-95F0-78E591F91A2C}">
-  <dimension ref="A1:AM50"/>
+  <dimension ref="A1:AM74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
+      <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16673,7 +16673,7 @@
     </row>
     <row r="27" spans="1:38" ht="360" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
-        <v>44963</v>
+        <v>45328</v>
       </c>
       <c r="B27" t="s">
         <v>137</v>
@@ -17570,7 +17570,7 @@
     </row>
     <row r="39" spans="1:38" ht="360" x14ac:dyDescent="0.3">
       <c r="A39" s="11">
-        <v>44963</v>
+        <v>45328</v>
       </c>
       <c r="B39" t="s">
         <v>137</v>
@@ -18253,6 +18253,9 @@
       </c>
     </row>
     <row r="48" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="H48" t="s">
+        <v>84</v>
+      </c>
       <c r="P48" t="s">
         <v>115</v>
       </c>
@@ -18323,7 +18326,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="49" spans="16:38" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.3">
       <c r="P49" t="s">
         <v>116</v>
       </c>
@@ -18394,7 +18397,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="50" spans="16:38" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.3">
       <c r="P50" t="s">
         <v>117</v>
       </c>
@@ -18463,6 +18466,1800 @@
       </c>
       <c r="AL50">
         <v>0.23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:38" ht="360" x14ac:dyDescent="0.3">
+      <c r="A51" s="11">
+        <v>45356</v>
+      </c>
+      <c r="B51" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" t="s">
+        <v>151</v>
+      </c>
+      <c r="D51">
+        <v>1E-3</v>
+      </c>
+      <c r="E51" t="s">
+        <v>138</v>
+      </c>
+      <c r="F51" t="s">
+        <v>149</v>
+      </c>
+      <c r="G51" t="s">
+        <v>147</v>
+      </c>
+      <c r="H51" t="s">
+        <v>148</v>
+      </c>
+      <c r="I51" t="s">
+        <v>148</v>
+      </c>
+      <c r="J51" s="2">
+        <v>1</v>
+      </c>
+      <c r="K51" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L51" t="s">
+        <v>127</v>
+      </c>
+      <c r="M51" t="s">
+        <v>40</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P51" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q51">
+        <v>0.04</v>
+      </c>
+      <c r="R51">
+        <v>0.06</v>
+      </c>
+      <c r="S51">
+        <v>0.06</v>
+      </c>
+      <c r="T51">
+        <v>0.03</v>
+      </c>
+      <c r="U51">
+        <v>0.09</v>
+      </c>
+      <c r="V51">
+        <v>0.09</v>
+      </c>
+      <c r="W51">
+        <v>0.04</v>
+      </c>
+      <c r="X51">
+        <v>0.06</v>
+      </c>
+      <c r="Y51">
+        <v>0.04</v>
+      </c>
+      <c r="Z51">
+        <v>0.06</v>
+      </c>
+      <c r="AA51">
+        <v>0.04</v>
+      </c>
+      <c r="AB51">
+        <v>0.03</v>
+      </c>
+      <c r="AC51">
+        <v>0.03</v>
+      </c>
+      <c r="AD51">
+        <v>0.04</v>
+      </c>
+      <c r="AE51">
+        <v>0.47</v>
+      </c>
+      <c r="AF51">
+        <v>0.23</v>
+      </c>
+      <c r="AG51">
+        <v>0.03</v>
+      </c>
+      <c r="AH51">
+        <v>0.4</v>
+      </c>
+      <c r="AI51">
+        <v>0.21</v>
+      </c>
+      <c r="AJ51">
+        <v>0.06</v>
+      </c>
+      <c r="AK51">
+        <v>0.4</v>
+      </c>
+      <c r="AL51">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P52" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q52">
+        <v>0.03</v>
+      </c>
+      <c r="R52">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S52">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T52">
+        <v>0.02</v>
+      </c>
+      <c r="U52">
+        <v>0.03</v>
+      </c>
+      <c r="V52">
+        <v>0.03</v>
+      </c>
+      <c r="W52">
+        <v>0.03</v>
+      </c>
+      <c r="X52">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y52">
+        <v>0.03</v>
+      </c>
+      <c r="Z52">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA52">
+        <v>0.03</v>
+      </c>
+      <c r="AB52">
+        <v>0.02</v>
+      </c>
+      <c r="AC52">
+        <v>0.02</v>
+      </c>
+      <c r="AD52">
+        <v>0.02</v>
+      </c>
+      <c r="AE52">
+        <v>0.38</v>
+      </c>
+      <c r="AF52">
+        <v>0.17</v>
+      </c>
+      <c r="AG52">
+        <v>0.02</v>
+      </c>
+      <c r="AH52">
+        <v>0.31</v>
+      </c>
+      <c r="AI52">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AJ52">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AK52">
+        <v>0.35</v>
+      </c>
+      <c r="AL52">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P53" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q53">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R53">
+        <v>0.08</v>
+      </c>
+      <c r="S53">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T53">
+        <v>0.06</v>
+      </c>
+      <c r="U53">
+        <v>0.05</v>
+      </c>
+      <c r="V53">
+        <v>0.04</v>
+      </c>
+      <c r="W53">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="X53">
+        <v>0.08</v>
+      </c>
+      <c r="Y53">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z53">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA53">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB53">
+        <v>0.03</v>
+      </c>
+      <c r="AC53">
+        <v>0.03</v>
+      </c>
+      <c r="AD53">
+        <v>0.04</v>
+      </c>
+      <c r="AE53">
+        <v>0.4</v>
+      </c>
+      <c r="AF53">
+        <v>0.2</v>
+      </c>
+      <c r="AG53">
+        <v>0.02</v>
+      </c>
+      <c r="AH53">
+        <v>0.32</v>
+      </c>
+      <c r="AI53">
+        <v>0.16</v>
+      </c>
+      <c r="AJ53">
+        <v>0.04</v>
+      </c>
+      <c r="AK53">
+        <v>0.38</v>
+      </c>
+      <c r="AL53">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P54" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q54">
+        <v>0.03</v>
+      </c>
+      <c r="R54">
+        <v>0.1</v>
+      </c>
+      <c r="S54">
+        <v>0.1</v>
+      </c>
+      <c r="T54">
+        <v>0.01</v>
+      </c>
+      <c r="U54">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V54">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W54">
+        <v>0.02</v>
+      </c>
+      <c r="X54">
+        <v>0.1</v>
+      </c>
+      <c r="Y54">
+        <v>0.02</v>
+      </c>
+      <c r="Z54">
+        <v>0.1</v>
+      </c>
+      <c r="AA54">
+        <v>0.02</v>
+      </c>
+      <c r="AB54">
+        <v>0</v>
+      </c>
+      <c r="AC54">
+        <v>0</v>
+      </c>
+      <c r="AD54">
+        <v>0.02</v>
+      </c>
+      <c r="AE54">
+        <v>0.25</v>
+      </c>
+      <c r="AF54">
+        <v>0.12</v>
+      </c>
+      <c r="AG54">
+        <v>0.01</v>
+      </c>
+      <c r="AH54">
+        <v>0.17</v>
+      </c>
+      <c r="AI54">
+        <v>0.1</v>
+      </c>
+      <c r="AJ54">
+        <v>0.03</v>
+      </c>
+      <c r="AK54">
+        <v>0.22</v>
+      </c>
+      <c r="AL54">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P55" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q55">
+        <v>0.02</v>
+      </c>
+      <c r="R55">
+        <v>0.09</v>
+      </c>
+      <c r="S55">
+        <v>0.09</v>
+      </c>
+      <c r="T55">
+        <v>0</v>
+      </c>
+      <c r="U55">
+        <v>0.03</v>
+      </c>
+      <c r="V55">
+        <v>0.03</v>
+      </c>
+      <c r="W55">
+        <v>0.01</v>
+      </c>
+      <c r="X55">
+        <v>0.09</v>
+      </c>
+      <c r="Y55">
+        <v>0.01</v>
+      </c>
+      <c r="Z55">
+        <v>0.09</v>
+      </c>
+      <c r="AA55">
+        <v>0.01</v>
+      </c>
+      <c r="AB55">
+        <v>0.01</v>
+      </c>
+      <c r="AC55">
+        <v>0.01</v>
+      </c>
+      <c r="AD55">
+        <v>0.03</v>
+      </c>
+      <c r="AE55">
+        <v>0.27</v>
+      </c>
+      <c r="AF55">
+        <v>0.1</v>
+      </c>
+      <c r="AG55">
+        <v>0.05</v>
+      </c>
+      <c r="AH55">
+        <v>0.27</v>
+      </c>
+      <c r="AI55">
+        <v>0.11</v>
+      </c>
+      <c r="AJ55">
+        <v>0.06</v>
+      </c>
+      <c r="AK55">
+        <v>0.19</v>
+      </c>
+      <c r="AL55">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P56" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q56">
+        <v>0.03</v>
+      </c>
+      <c r="R56">
+        <v>0.11</v>
+      </c>
+      <c r="S56">
+        <v>0.11</v>
+      </c>
+      <c r="T56">
+        <v>0.02</v>
+      </c>
+      <c r="U56">
+        <v>0.09</v>
+      </c>
+      <c r="V56">
+        <v>0.1</v>
+      </c>
+      <c r="W56">
+        <v>0.02</v>
+      </c>
+      <c r="X56">
+        <v>0.1</v>
+      </c>
+      <c r="Y56">
+        <v>0.02</v>
+      </c>
+      <c r="Z56">
+        <v>0.1</v>
+      </c>
+      <c r="AA56">
+        <v>0.02</v>
+      </c>
+      <c r="AB56">
+        <v>0.03</v>
+      </c>
+      <c r="AC56">
+        <v>0.03</v>
+      </c>
+      <c r="AD56">
+        <v>0.05</v>
+      </c>
+      <c r="AE56">
+        <v>0.25</v>
+      </c>
+      <c r="AF56">
+        <v>0.1</v>
+      </c>
+      <c r="AG56">
+        <v>0.03</v>
+      </c>
+      <c r="AH56">
+        <v>0.25</v>
+      </c>
+      <c r="AI56">
+        <v>0.09</v>
+      </c>
+      <c r="AJ56">
+        <v>0.05</v>
+      </c>
+      <c r="AK56">
+        <v>0.16</v>
+      </c>
+      <c r="AL56">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P57" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q57">
+        <v>0.03</v>
+      </c>
+      <c r="R57">
+        <v>0.1</v>
+      </c>
+      <c r="S57">
+        <v>0.1</v>
+      </c>
+      <c r="T57">
+        <v>0.01</v>
+      </c>
+      <c r="U57">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V57">
+        <v>0.06</v>
+      </c>
+      <c r="W57">
+        <v>0.03</v>
+      </c>
+      <c r="X57">
+        <v>0.09</v>
+      </c>
+      <c r="Y57">
+        <v>0.04</v>
+      </c>
+      <c r="Z57">
+        <v>0.09</v>
+      </c>
+      <c r="AA57">
+        <v>0.04</v>
+      </c>
+      <c r="AB57">
+        <v>0.03</v>
+      </c>
+      <c r="AC57">
+        <v>0.03</v>
+      </c>
+      <c r="AD57">
+        <v>0.08</v>
+      </c>
+      <c r="AE57">
+        <v>0.27</v>
+      </c>
+      <c r="AF57">
+        <v>0.13</v>
+      </c>
+      <c r="AG57">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AH57">
+        <v>0.2</v>
+      </c>
+      <c r="AI57">
+        <v>0.12</v>
+      </c>
+      <c r="AJ57">
+        <v>0.05</v>
+      </c>
+      <c r="AK57">
+        <v>0.22</v>
+      </c>
+      <c r="AL57">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P58" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q58">
+        <v>4.3478260869565202E-2</v>
+      </c>
+      <c r="R58">
+        <v>0.102040816326531</v>
+      </c>
+      <c r="S58">
+        <v>0.102040816326531</v>
+      </c>
+      <c r="T58">
+        <v>3.2967032967033003E-2</v>
+      </c>
+      <c r="U58">
+        <v>6.25E-2</v>
+      </c>
+      <c r="V58">
+        <v>6.25E-2</v>
+      </c>
+      <c r="W58">
+        <v>2.1739130434782601E-2</v>
+      </c>
+      <c r="X58">
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="Y58">
+        <v>2.02020202020202E-2</v>
+      </c>
+      <c r="Z58">
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="AA58">
+        <v>2.02020202020202E-2</v>
+      </c>
+      <c r="AB58">
+        <v>0.02</v>
+      </c>
+      <c r="AC58">
+        <v>0.02</v>
+      </c>
+      <c r="AD58">
+        <v>0.06</v>
+      </c>
+      <c r="AE58">
+        <v>0.19</v>
+      </c>
+      <c r="AF58">
+        <v>0.06</v>
+      </c>
+      <c r="AG58">
+        <v>0.06</v>
+      </c>
+      <c r="AH58">
+        <v>0.17</v>
+      </c>
+      <c r="AI58">
+        <v>0.08</v>
+      </c>
+      <c r="AJ58">
+        <v>0.05</v>
+      </c>
+      <c r="AK58">
+        <v>0.16</v>
+      </c>
+      <c r="AL58">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="59" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P59" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q59">
+        <v>0.09</v>
+      </c>
+      <c r="R59">
+        <v>0.11</v>
+      </c>
+      <c r="S59">
+        <v>0.11</v>
+      </c>
+      <c r="T59">
+        <v>0.03</v>
+      </c>
+      <c r="U59">
+        <v>0.08</v>
+      </c>
+      <c r="V59">
+        <v>0.08</v>
+      </c>
+      <c r="W59">
+        <v>0.09</v>
+      </c>
+      <c r="X59">
+        <v>0.11</v>
+      </c>
+      <c r="Y59">
+        <v>0.1</v>
+      </c>
+      <c r="Z59">
+        <v>0.11</v>
+      </c>
+      <c r="AA59">
+        <v>0.1</v>
+      </c>
+      <c r="AB59">
+        <v>0.05</v>
+      </c>
+      <c r="AC59">
+        <v>0.05</v>
+      </c>
+      <c r="AD59">
+        <v>0.04</v>
+      </c>
+      <c r="AE59">
+        <v>0.41</v>
+      </c>
+      <c r="AF59">
+        <v>0.18</v>
+      </c>
+      <c r="AG59">
+        <v>0.05</v>
+      </c>
+      <c r="AH59">
+        <v>0.34</v>
+      </c>
+      <c r="AI59">
+        <v>0.19</v>
+      </c>
+      <c r="AJ59">
+        <v>0.06</v>
+      </c>
+      <c r="AK59">
+        <v>0.35</v>
+      </c>
+      <c r="AL59">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P60" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q60">
+        <v>0.03</v>
+      </c>
+      <c r="R60">
+        <v>0.11</v>
+      </c>
+      <c r="S60">
+        <v>0.11</v>
+      </c>
+      <c r="T60">
+        <v>0.04</v>
+      </c>
+      <c r="U60">
+        <v>0.08</v>
+      </c>
+      <c r="V60">
+        <v>0.08</v>
+      </c>
+      <c r="W60">
+        <v>0.03</v>
+      </c>
+      <c r="X60">
+        <v>0.11</v>
+      </c>
+      <c r="Y60">
+        <v>0.04</v>
+      </c>
+      <c r="Z60">
+        <v>0.11</v>
+      </c>
+      <c r="AA60">
+        <v>0.04</v>
+      </c>
+      <c r="AB60">
+        <v>0.06</v>
+      </c>
+      <c r="AC60">
+        <v>0.06</v>
+      </c>
+      <c r="AD60">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AE60">
+        <v>0.31</v>
+      </c>
+      <c r="AF60">
+        <v>0.12</v>
+      </c>
+      <c r="AG60">
+        <v>0.04</v>
+      </c>
+      <c r="AH60">
+        <v>0.32</v>
+      </c>
+      <c r="AI60">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AJ60">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AK60">
+        <v>0.23</v>
+      </c>
+      <c r="AL60">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="61" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P61" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q61">
+        <v>0.01</v>
+      </c>
+      <c r="R61">
+        <v>0.08</v>
+      </c>
+      <c r="S61">
+        <v>0.08</v>
+      </c>
+      <c r="T61">
+        <v>0.02</v>
+      </c>
+      <c r="U61">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V61">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W61">
+        <v>0.01</v>
+      </c>
+      <c r="X61">
+        <v>0.08</v>
+      </c>
+      <c r="Y61">
+        <v>0.01</v>
+      </c>
+      <c r="Z61">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA61">
+        <v>0.01</v>
+      </c>
+      <c r="AB61">
+        <v>0.03</v>
+      </c>
+      <c r="AC61">
+        <v>0.03</v>
+      </c>
+      <c r="AD61">
+        <v>0.03</v>
+      </c>
+      <c r="AE61">
+        <v>0.25</v>
+      </c>
+      <c r="AF61">
+        <v>0.18</v>
+      </c>
+      <c r="AG61">
+        <v>0.03</v>
+      </c>
+      <c r="AH61">
+        <v>0.24</v>
+      </c>
+      <c r="AI61">
+        <v>0.16</v>
+      </c>
+      <c r="AJ61">
+        <v>0.03</v>
+      </c>
+      <c r="AK61">
+        <v>0.2</v>
+      </c>
+      <c r="AL61">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P62" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q62">
+        <v>0.05</v>
+      </c>
+      <c r="R62">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S62">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="T62">
+        <v>0.05</v>
+      </c>
+      <c r="U62">
+        <v>0.08</v>
+      </c>
+      <c r="V62">
+        <v>0.08</v>
+      </c>
+      <c r="W62">
+        <v>0.05</v>
+      </c>
+      <c r="X62">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Y62">
+        <v>0.06</v>
+      </c>
+      <c r="Z62">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AA62">
+        <v>0.06</v>
+      </c>
+      <c r="AB62">
+        <v>0.04</v>
+      </c>
+      <c r="AC62">
+        <v>0.04</v>
+      </c>
+      <c r="AD62">
+        <v>0.03</v>
+      </c>
+      <c r="AE62">
+        <v>0.48</v>
+      </c>
+      <c r="AF62">
+        <v>0.25</v>
+      </c>
+      <c r="AG62">
+        <v>0.03</v>
+      </c>
+      <c r="AH62">
+        <v>0.39</v>
+      </c>
+      <c r="AI62">
+        <v>0.22</v>
+      </c>
+      <c r="AJ62">
+        <v>0.03</v>
+      </c>
+      <c r="AK62">
+        <v>0.42</v>
+      </c>
+      <c r="AL62">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="63" spans="1:38" ht="360" x14ac:dyDescent="0.3">
+      <c r="A63" s="11">
+        <v>45356</v>
+      </c>
+      <c r="B63" t="s">
+        <v>137</v>
+      </c>
+      <c r="C63" t="s">
+        <v>151</v>
+      </c>
+      <c r="D63">
+        <v>1E-3</v>
+      </c>
+      <c r="E63" t="s">
+        <v>142</v>
+      </c>
+      <c r="F63" t="s">
+        <v>149</v>
+      </c>
+      <c r="G63" t="s">
+        <v>147</v>
+      </c>
+      <c r="H63" t="s">
+        <v>148</v>
+      </c>
+      <c r="I63" t="s">
+        <v>148</v>
+      </c>
+      <c r="J63" s="2">
+        <v>1</v>
+      </c>
+      <c r="K63" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L63" t="s">
+        <v>127</v>
+      </c>
+      <c r="M63" t="s">
+        <v>40</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O63" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P63" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q63">
+        <v>0.06</v>
+      </c>
+      <c r="R63">
+        <v>0.12</v>
+      </c>
+      <c r="S63">
+        <v>0.08</v>
+      </c>
+      <c r="T63">
+        <v>0.04</v>
+      </c>
+      <c r="U63">
+        <v>0.13</v>
+      </c>
+      <c r="V63">
+        <v>0.04</v>
+      </c>
+      <c r="W63">
+        <v>0.06</v>
+      </c>
+      <c r="X63">
+        <v>0.11</v>
+      </c>
+      <c r="Y63">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z63">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA63">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB63">
+        <v>0.03</v>
+      </c>
+      <c r="AC63">
+        <v>0.03</v>
+      </c>
+      <c r="AD63">
+        <v>0.03</v>
+      </c>
+      <c r="AE63">
+        <v>0.49</v>
+      </c>
+      <c r="AF63">
+        <v>0.25</v>
+      </c>
+      <c r="AG63">
+        <v>0.03</v>
+      </c>
+      <c r="AH63">
+        <v>0.52</v>
+      </c>
+      <c r="AI63">
+        <v>0.31</v>
+      </c>
+      <c r="AJ63">
+        <v>0.06</v>
+      </c>
+      <c r="AK63">
+        <v>0.13</v>
+      </c>
+      <c r="AL63">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="P64" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q64">
+        <v>0.02</v>
+      </c>
+      <c r="R64">
+        <v>0.17</v>
+      </c>
+      <c r="S64">
+        <v>0.03</v>
+      </c>
+      <c r="T64">
+        <v>0.01</v>
+      </c>
+      <c r="U64">
+        <v>0.13</v>
+      </c>
+      <c r="V64">
+        <v>0.04</v>
+      </c>
+      <c r="W64">
+        <v>0.02</v>
+      </c>
+      <c r="X64">
+        <v>0.15</v>
+      </c>
+      <c r="Y64">
+        <v>0.02</v>
+      </c>
+      <c r="Z64">
+        <v>0.03</v>
+      </c>
+      <c r="AA64">
+        <v>0.02</v>
+      </c>
+      <c r="AB64">
+        <v>0.04</v>
+      </c>
+      <c r="AC64">
+        <v>0.01</v>
+      </c>
+      <c r="AD64">
+        <v>0.02</v>
+      </c>
+      <c r="AE64">
+        <v>0.47</v>
+      </c>
+      <c r="AF64">
+        <v>0.21</v>
+      </c>
+      <c r="AG64">
+        <v>0.02</v>
+      </c>
+      <c r="AH64">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AI64">
+        <v>0.25</v>
+      </c>
+      <c r="AJ64">
+        <v>0.06</v>
+      </c>
+      <c r="AK64">
+        <v>0.15</v>
+      </c>
+      <c r="AL64">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="65" spans="16:38" x14ac:dyDescent="0.3">
+      <c r="P65" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q65">
+        <v>0.04</v>
+      </c>
+      <c r="R65">
+        <v>0.16</v>
+      </c>
+      <c r="S65">
+        <v>0.04</v>
+      </c>
+      <c r="T65">
+        <v>0.05</v>
+      </c>
+      <c r="U65">
+        <v>0.12</v>
+      </c>
+      <c r="V65">
+        <v>0.04</v>
+      </c>
+      <c r="W65">
+        <v>0.04</v>
+      </c>
+      <c r="X65">
+        <v>0.16</v>
+      </c>
+      <c r="Y65">
+        <v>0.04</v>
+      </c>
+      <c r="Z65">
+        <v>0.04</v>
+      </c>
+      <c r="AA65">
+        <v>0.04</v>
+      </c>
+      <c r="AB65">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC65">
+        <v>0.04</v>
+      </c>
+      <c r="AD65">
+        <v>0.03</v>
+      </c>
+      <c r="AE65">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AF65">
+        <v>0.24</v>
+      </c>
+      <c r="AG65">
+        <v>0.02</v>
+      </c>
+      <c r="AH65">
+        <v>0.6</v>
+      </c>
+      <c r="AI65">
+        <v>0.3</v>
+      </c>
+      <c r="AJ65">
+        <v>0.04</v>
+      </c>
+      <c r="AK65">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AL65">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="66" spans="16:38" x14ac:dyDescent="0.3">
+      <c r="P66" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q66">
+        <v>0.06</v>
+      </c>
+      <c r="R66">
+        <v>0.16</v>
+      </c>
+      <c r="S66">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T66">
+        <v>0.05</v>
+      </c>
+      <c r="U66">
+        <v>0.08</v>
+      </c>
+      <c r="V66">
+        <v>0.03</v>
+      </c>
+      <c r="W66">
+        <v>0.05</v>
+      </c>
+      <c r="X66">
+        <v>0.16</v>
+      </c>
+      <c r="Y66">
+        <v>0.05</v>
+      </c>
+      <c r="Z66">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA66">
+        <v>0.05</v>
+      </c>
+      <c r="AB66">
+        <v>0.03</v>
+      </c>
+      <c r="AC66">
+        <v>0.02</v>
+      </c>
+      <c r="AD66">
+        <v>0.04</v>
+      </c>
+      <c r="AE66">
+        <v>0.36</v>
+      </c>
+      <c r="AF66">
+        <v>0.13</v>
+      </c>
+      <c r="AG66">
+        <v>0.04</v>
+      </c>
+      <c r="AH66">
+        <v>0.42</v>
+      </c>
+      <c r="AI66">
+        <v>0.18</v>
+      </c>
+      <c r="AJ66">
+        <v>0.01</v>
+      </c>
+      <c r="AK66">
+        <v>0.11</v>
+      </c>
+      <c r="AL66">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="16:38" x14ac:dyDescent="0.3">
+      <c r="P67" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q67">
+        <v>0.08</v>
+      </c>
+      <c r="R67">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S67">
+        <v>0.04</v>
+      </c>
+      <c r="T67">
+        <v>0.04</v>
+      </c>
+      <c r="U67">
+        <v>0.1</v>
+      </c>
+      <c r="V67">
+        <v>0.01</v>
+      </c>
+      <c r="W67">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="X67">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Y67">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z67">
+        <v>0.02</v>
+      </c>
+      <c r="AA67">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB67">
+        <v>0.06</v>
+      </c>
+      <c r="AC67">
+        <v>0.05</v>
+      </c>
+      <c r="AD67">
+        <v>0.04</v>
+      </c>
+      <c r="AE67">
+        <v>0.39</v>
+      </c>
+      <c r="AF67">
+        <v>0.2</v>
+      </c>
+      <c r="AG67">
+        <v>0.03</v>
+      </c>
+      <c r="AH67">
+        <v>0.43</v>
+      </c>
+      <c r="AI67">
+        <v>0.19</v>
+      </c>
+      <c r="AJ67">
+        <v>0.03</v>
+      </c>
+      <c r="AK67">
+        <v>0.1</v>
+      </c>
+      <c r="AL67">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="16:38" x14ac:dyDescent="0.3">
+      <c r="P68" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q68">
+        <v>0.02</v>
+      </c>
+      <c r="R68">
+        <v>0.09</v>
+      </c>
+      <c r="S68">
+        <v>0.04</v>
+      </c>
+      <c r="T68">
+        <v>0.01</v>
+      </c>
+      <c r="U68">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V68">
+        <v>0.03</v>
+      </c>
+      <c r="W68">
+        <v>0.02</v>
+      </c>
+      <c r="X68">
+        <v>0.08</v>
+      </c>
+      <c r="Y68">
+        <v>0.01</v>
+      </c>
+      <c r="Z68">
+        <v>0.04</v>
+      </c>
+      <c r="AA68">
+        <v>0.02</v>
+      </c>
+      <c r="AB68">
+        <v>0.04</v>
+      </c>
+      <c r="AC68">
+        <v>0.03</v>
+      </c>
+      <c r="AD68">
+        <v>0.08</v>
+      </c>
+      <c r="AE68">
+        <v>0.31</v>
+      </c>
+      <c r="AF68">
+        <v>0.12</v>
+      </c>
+      <c r="AG68">
+        <v>0.03</v>
+      </c>
+      <c r="AH68">
+        <v>0.4</v>
+      </c>
+      <c r="AI68">
+        <v>0.2</v>
+      </c>
+      <c r="AJ68">
+        <v>0.06</v>
+      </c>
+      <c r="AK68">
+        <v>0.1</v>
+      </c>
+      <c r="AL68">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="69" spans="16:38" x14ac:dyDescent="0.3">
+      <c r="P69" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q69">
+        <v>0.03</v>
+      </c>
+      <c r="R69">
+        <v>0.17</v>
+      </c>
+      <c r="S69">
+        <v>0.1</v>
+      </c>
+      <c r="T69">
+        <v>0.01</v>
+      </c>
+      <c r="U69">
+        <v>0.13</v>
+      </c>
+      <c r="V69">
+        <v>0.1</v>
+      </c>
+      <c r="W69">
+        <v>0.03</v>
+      </c>
+      <c r="X69">
+        <v>0.16</v>
+      </c>
+      <c r="Y69">
+        <v>0.03</v>
+      </c>
+      <c r="Z69">
+        <v>0.08</v>
+      </c>
+      <c r="AA69">
+        <v>0.03</v>
+      </c>
+      <c r="AB69">
+        <v>0.04</v>
+      </c>
+      <c r="AC69">
+        <v>0.04</v>
+      </c>
+      <c r="AD69">
+        <v>0.05</v>
+      </c>
+      <c r="AE69">
+        <v>0.4</v>
+      </c>
+      <c r="AF69">
+        <v>0.26</v>
+      </c>
+      <c r="AG69">
+        <v>0.04</v>
+      </c>
+      <c r="AH69">
+        <v>0.4</v>
+      </c>
+      <c r="AI69">
+        <v>0.26</v>
+      </c>
+      <c r="AJ69">
+        <v>0.06</v>
+      </c>
+      <c r="AK69">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AL69">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="70" spans="16:38" x14ac:dyDescent="0.3">
+      <c r="P70" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q70">
+        <v>1.35135135135135E-2</v>
+      </c>
+      <c r="R70">
+        <v>0.10752688172043</v>
+      </c>
+      <c r="S70">
+        <v>5.7471264367816098E-2</v>
+      </c>
+      <c r="T70">
+        <v>1.4285714285714299E-2</v>
+      </c>
+      <c r="U70">
+        <v>7.5268817204301106E-2</v>
+      </c>
+      <c r="V70">
+        <v>2.2988505747126398E-2</v>
+      </c>
+      <c r="W70">
+        <v>1.35135135135135E-2</v>
+      </c>
+      <c r="X70">
+        <v>7.5268817204301106E-2</v>
+      </c>
+      <c r="Y70">
+        <v>1.01010101010101E-2</v>
+      </c>
+      <c r="Z70">
+        <v>5.7471264367816098E-2</v>
+      </c>
+      <c r="AA70">
+        <v>1.05263157894737E-2</v>
+      </c>
+      <c r="AB70">
+        <v>0.02</v>
+      </c>
+      <c r="AC70">
+        <v>0.01</v>
+      </c>
+      <c r="AD70">
+        <v>0.03</v>
+      </c>
+      <c r="AE70">
+        <v>0.26</v>
+      </c>
+      <c r="AF70">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AG70">
+        <v>0.06</v>
+      </c>
+      <c r="AH70">
+        <v>0.26</v>
+      </c>
+      <c r="AI70">
+        <v>0.11</v>
+      </c>
+      <c r="AJ70">
+        <v>0.01</v>
+      </c>
+      <c r="AK70">
+        <v>0.15</v>
+      </c>
+      <c r="AL70">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="71" spans="16:38" x14ac:dyDescent="0.3">
+      <c r="P71" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q71">
+        <v>0</v>
+      </c>
+      <c r="R71">
+        <v>0.1</v>
+      </c>
+      <c r="S71">
+        <v>0.02</v>
+      </c>
+      <c r="T71">
+        <v>0.01</v>
+      </c>
+      <c r="U71">
+        <v>0.09</v>
+      </c>
+      <c r="V71">
+        <v>0.03</v>
+      </c>
+      <c r="W71">
+        <v>0</v>
+      </c>
+      <c r="X71">
+        <v>0.1</v>
+      </c>
+      <c r="Y71">
+        <v>0</v>
+      </c>
+      <c r="Z71">
+        <v>0.02</v>
+      </c>
+      <c r="AA71">
+        <v>0</v>
+      </c>
+      <c r="AB71">
+        <v>0.06</v>
+      </c>
+      <c r="AC71">
+        <v>0.04</v>
+      </c>
+      <c r="AD71">
+        <v>0.01</v>
+      </c>
+      <c r="AE71">
+        <v>0.47</v>
+      </c>
+      <c r="AF71">
+        <v>0.17</v>
+      </c>
+      <c r="AG71">
+        <v>0.04</v>
+      </c>
+      <c r="AH71">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AI71">
+        <v>0.26</v>
+      </c>
+      <c r="AJ71">
+        <v>0.03</v>
+      </c>
+      <c r="AK71">
+        <v>0.1</v>
+      </c>
+      <c r="AL71">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="72" spans="16:38" x14ac:dyDescent="0.3">
+      <c r="P72" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q72">
+        <v>0.06</v>
+      </c>
+      <c r="R72">
+        <v>0.17</v>
+      </c>
+      <c r="S72">
+        <v>0.06</v>
+      </c>
+      <c r="T72">
+        <v>0.04</v>
+      </c>
+      <c r="U72">
+        <v>0.12</v>
+      </c>
+      <c r="V72">
+        <v>0.06</v>
+      </c>
+      <c r="W72">
+        <v>0.05</v>
+      </c>
+      <c r="X72">
+        <v>0.17</v>
+      </c>
+      <c r="Y72">
+        <v>0.05</v>
+      </c>
+      <c r="Z72">
+        <v>0.06</v>
+      </c>
+      <c r="AA72">
+        <v>0.05</v>
+      </c>
+      <c r="AB72">
+        <v>0.04</v>
+      </c>
+      <c r="AC72">
+        <v>0.05</v>
+      </c>
+      <c r="AD72">
+        <v>0.08</v>
+      </c>
+      <c r="AE72">
+        <v>0.47</v>
+      </c>
+      <c r="AF72">
+        <v>0.19</v>
+      </c>
+      <c r="AG72">
+        <v>0.05</v>
+      </c>
+      <c r="AH72">
+        <v>0.51</v>
+      </c>
+      <c r="AI72">
+        <v>0.22</v>
+      </c>
+      <c r="AJ72">
+        <v>0.06</v>
+      </c>
+      <c r="AK72">
+        <v>0.19</v>
+      </c>
+      <c r="AL72">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="73" spans="16:38" x14ac:dyDescent="0.3">
+      <c r="P73" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q73">
+        <v>6.0606060606060601E-2</v>
+      </c>
+      <c r="R73">
+        <v>0.16</v>
+      </c>
+      <c r="S73">
+        <v>0.04</v>
+      </c>
+      <c r="T73">
+        <v>2.02020202020202E-2</v>
+      </c>
+      <c r="U73">
+        <v>0.1</v>
+      </c>
+      <c r="V73">
+        <v>0.05</v>
+      </c>
+      <c r="W73">
+        <v>4.0404040404040401E-2</v>
+      </c>
+      <c r="X73">
+        <v>0.13</v>
+      </c>
+      <c r="Y73">
+        <v>0.04</v>
+      </c>
+      <c r="Z73">
+        <v>0.03</v>
+      </c>
+      <c r="AA73">
+        <v>0.04</v>
+      </c>
+      <c r="AB73">
+        <v>0.02</v>
+      </c>
+      <c r="AC73">
+        <v>0.04</v>
+      </c>
+      <c r="AD73">
+        <v>0.03</v>
+      </c>
+      <c r="AE73">
+        <v>0.34</v>
+      </c>
+      <c r="AF73">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AG73">
+        <v>0.02</v>
+      </c>
+      <c r="AH73">
+        <v>0.38</v>
+      </c>
+      <c r="AI73">
+        <v>0.19</v>
+      </c>
+      <c r="AJ73">
+        <v>0.05</v>
+      </c>
+      <c r="AK73">
+        <v>0.1</v>
+      </c>
+      <c r="AL73">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="16:38" x14ac:dyDescent="0.3">
+      <c r="P74" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q74">
+        <v>0.02</v>
+      </c>
+      <c r="R74">
+        <v>0.15</v>
+      </c>
+      <c r="S74">
+        <v>0.02</v>
+      </c>
+      <c r="T74">
+        <v>0.03</v>
+      </c>
+      <c r="U74">
+        <v>0.12</v>
+      </c>
+      <c r="V74">
+        <v>0.03</v>
+      </c>
+      <c r="W74">
+        <v>0.02</v>
+      </c>
+      <c r="X74">
+        <v>0.15</v>
+      </c>
+      <c r="Y74">
+        <v>0.02</v>
+      </c>
+      <c r="Z74">
+        <v>0.02</v>
+      </c>
+      <c r="AA74">
+        <v>0.02</v>
+      </c>
+      <c r="AB74">
+        <v>0.02</v>
+      </c>
+      <c r="AC74">
+        <v>0.02</v>
+      </c>
+      <c r="AD74">
+        <v>0.03</v>
+      </c>
+      <c r="AE74">
+        <v>0.48</v>
+      </c>
+      <c r="AF74">
+        <v>0.21</v>
+      </c>
+      <c r="AG74">
+        <v>0.05</v>
+      </c>
+      <c r="AH74">
+        <v>0.52</v>
+      </c>
+      <c r="AI74">
+        <v>0.25</v>
+      </c>
+      <c r="AJ74">
+        <v>0.03</v>
+      </c>
+      <c r="AK74">
+        <v>0.15</v>
+      </c>
+      <c r="AL74">
+        <v>0.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added prox gene adjustment results
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5FDF80-7070-483F-B3D9-FF574053087C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB32C65-8D5B-47A8-A14E-06462D86F33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
   <sheets>
     <sheet name="t1e_gene_region" sheetId="1" r:id="rId1"/>
     <sheet name="t1e_by_gene" sheetId="2" r:id="rId2"/>
     <sheet name="power_by_gene" sheetId="3" r:id="rId3"/>
     <sheet name="admixed_t1e" sheetId="4" r:id="rId4"/>
+    <sheet name="prox_adj" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="165">
   <si>
     <t>Population</t>
   </si>
@@ -718,6 +719,42 @@
   <si>
     <t>New Simulated 100K haplotypes</t>
   </si>
+  <si>
+    <t>ProxECAT External Variant Adjusted Ncc</t>
+  </si>
+  <si>
+    <t>ProxECAT External Variant Adjusted Neff</t>
+  </si>
+  <si>
+    <t>ProxECAT External Gene Adjusted Ncc</t>
+  </si>
+  <si>
+    <t>ProxECAT-weighted Internal</t>
+  </si>
+  <si>
+    <t>ProxECAT-weighted External</t>
+  </si>
+  <si>
+    <t>ProxECAT-weighted External Variant Adjusted Ncc</t>
+  </si>
+  <si>
+    <t>ProxECAT-weighted External Variant Adjusted Neff</t>
+  </si>
+  <si>
+    <t>ProxECAT-weighted External Gene Adjusted Ncc</t>
+  </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>42k</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
 </sst>
 </file>
 
@@ -784,7 +821,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -814,6 +851,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1177,31 +1217,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
     </row>
     <row r="2" spans="1:35" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -7245,36 +7285,36 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="13" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
     </row>
     <row r="2" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -14430,37 +14470,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="13" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
       <c r="AB1" s="1"/>
     </row>
     <row r="2" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
@@ -15340,11 +15380,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669C6091-A5A6-4DA3-95F0-78E591F91A2C}">
-  <dimension ref="A1:AM74"/>
+  <dimension ref="A1:BU74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G72" sqref="G72"/>
+      <selection pane="bottomLeft" activeCell="L63" sqref="L63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15362,41 +15402,41 @@
     <col min="22" max="22" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="13" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
       <c r="AE1" s="12"/>
       <c r="AF1" s="12"/>
       <c r="AG1" s="12"/>
@@ -15406,7 +15446,7 @@
       <c r="AK1" s="12"/>
       <c r="AL1" s="1"/>
     </row>
-    <row r="2" spans="1:39" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:73" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -15525,7 +15565,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:39" ht="360" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:73" ht="360" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>45278</v>
       </c>
@@ -15613,8 +15653,11 @@
       <c r="AC3">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="BU3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:73" x14ac:dyDescent="0.3">
       <c r="P4" t="s">
         <v>107</v>
       </c>
@@ -15658,7 +15701,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:73" x14ac:dyDescent="0.3">
       <c r="P5" t="s">
         <v>108</v>
       </c>
@@ -15702,7 +15745,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:73" x14ac:dyDescent="0.3">
       <c r="P6" t="s">
         <v>109</v>
       </c>
@@ -15746,7 +15789,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:73" x14ac:dyDescent="0.3">
       <c r="P7" t="s">
         <v>110</v>
       </c>
@@ -15790,7 +15833,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:73" x14ac:dyDescent="0.3">
       <c r="P8" t="s">
         <v>111</v>
       </c>
@@ -15834,7 +15877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:73" x14ac:dyDescent="0.3">
       <c r="P9" t="s">
         <v>112</v>
       </c>
@@ -15878,7 +15921,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:73" x14ac:dyDescent="0.3">
       <c r="P10" t="s">
         <v>113</v>
       </c>
@@ -15922,7 +15965,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:73" x14ac:dyDescent="0.3">
       <c r="P11" t="s">
         <v>114</v>
       </c>
@@ -15966,7 +16009,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:73" x14ac:dyDescent="0.3">
       <c r="P12" t="s">
         <v>115</v>
       </c>
@@ -16010,7 +16053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:73" x14ac:dyDescent="0.3">
       <c r="P13" t="s">
         <v>116</v>
       </c>
@@ -16054,7 +16097,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:73" x14ac:dyDescent="0.3">
       <c r="P14" t="s">
         <v>117</v>
       </c>
@@ -16098,7 +16141,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:39" ht="360" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:73" ht="360" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>45279</v>
       </c>
@@ -16187,7 +16230,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:73" x14ac:dyDescent="0.3">
       <c r="P16" t="s">
         <v>107</v>
       </c>
@@ -20269,4 +20312,3398 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462CC3C0-91BE-442C-A1C6-C94A876D69AE}">
+  <dimension ref="A1:AH74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="14" max="14" width="15.109375" customWidth="1"/>
+    <col min="15" max="15" width="31.6640625" customWidth="1"/>
+    <col min="23" max="23" width="9.6640625" customWidth="1"/>
+    <col min="24" max="24" width="10.109375" customWidth="1"/>
+    <col min="25" max="25" width="10.44140625" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" customWidth="1"/>
+    <col min="27" max="27" width="9.77734375" customWidth="1"/>
+    <col min="28" max="28" width="10.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
+    </row>
+    <row r="2" spans="1:30" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>45376</v>
+      </c>
+      <c r="B3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3">
+        <v>1E-3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H3" t="s">
+        <v>148</v>
+      </c>
+      <c r="I3">
+        <v>500</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L3" t="s">
+        <v>127</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P3" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q3">
+        <v>0.05</v>
+      </c>
+      <c r="R3">
+        <v>0.11</v>
+      </c>
+      <c r="S3">
+        <v>0.11</v>
+      </c>
+      <c r="T3">
+        <v>0.13</v>
+      </c>
+      <c r="U3">
+        <v>0.11</v>
+      </c>
+      <c r="V3">
+        <v>0.12</v>
+      </c>
+      <c r="W3">
+        <v>0.01</v>
+      </c>
+      <c r="X3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z3">
+        <v>0.08</v>
+      </c>
+      <c r="AA3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="P4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q4">
+        <v>0.02</v>
+      </c>
+      <c r="R4">
+        <v>0.06</v>
+      </c>
+      <c r="S4">
+        <v>0.06</v>
+      </c>
+      <c r="T4">
+        <v>0.05</v>
+      </c>
+      <c r="U4">
+        <v>0.06</v>
+      </c>
+      <c r="V4">
+        <v>0.06</v>
+      </c>
+      <c r="W4">
+        <v>0.02</v>
+      </c>
+      <c r="X4">
+        <v>0.02</v>
+      </c>
+      <c r="Y4">
+        <v>0.02</v>
+      </c>
+      <c r="Z4">
+        <v>0.03</v>
+      </c>
+      <c r="AA4">
+        <v>0.03</v>
+      </c>
+      <c r="AB4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="P5" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q5">
+        <v>0.04</v>
+      </c>
+      <c r="R5">
+        <v>0.09</v>
+      </c>
+      <c r="S5">
+        <v>0.09</v>
+      </c>
+      <c r="T5">
+        <v>0.11</v>
+      </c>
+      <c r="U5">
+        <v>0.09</v>
+      </c>
+      <c r="V5">
+        <v>0.12</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0.06</v>
+      </c>
+      <c r="Y5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z5">
+        <v>0.08</v>
+      </c>
+      <c r="AA5">
+        <v>0.06</v>
+      </c>
+      <c r="AB5">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="P6" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q6">
+        <v>0.03</v>
+      </c>
+      <c r="R6">
+        <v>0.09</v>
+      </c>
+      <c r="S6">
+        <v>0.09</v>
+      </c>
+      <c r="T6">
+        <v>0.09</v>
+      </c>
+      <c r="U6">
+        <v>0.09</v>
+      </c>
+      <c r="V6">
+        <v>0.1</v>
+      </c>
+      <c r="W6">
+        <v>0.01</v>
+      </c>
+      <c r="X6">
+        <v>0.06</v>
+      </c>
+      <c r="Y6">
+        <v>0.05</v>
+      </c>
+      <c r="Z6">
+        <v>0.05</v>
+      </c>
+      <c r="AA6">
+        <v>0.06</v>
+      </c>
+      <c r="AB6">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="P7" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q7">
+        <v>0.02</v>
+      </c>
+      <c r="R7">
+        <v>0.11</v>
+      </c>
+      <c r="S7">
+        <v>0.1</v>
+      </c>
+      <c r="T7">
+        <v>0.11</v>
+      </c>
+      <c r="U7">
+        <v>0.1</v>
+      </c>
+      <c r="V7">
+        <v>0.1</v>
+      </c>
+      <c r="W7">
+        <v>0.03</v>
+      </c>
+      <c r="X7">
+        <v>0.08</v>
+      </c>
+      <c r="Y7">
+        <v>0.09</v>
+      </c>
+      <c r="Z7">
+        <v>0.08</v>
+      </c>
+      <c r="AA7">
+        <v>0.09</v>
+      </c>
+      <c r="AB7">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="P8" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q8">
+        <v>0.08</v>
+      </c>
+      <c r="R8">
+        <v>0.06</v>
+      </c>
+      <c r="S8">
+        <v>0.06</v>
+      </c>
+      <c r="T8">
+        <v>0.06</v>
+      </c>
+      <c r="U8">
+        <v>0.06</v>
+      </c>
+      <c r="V8">
+        <v>0.06</v>
+      </c>
+      <c r="W8">
+        <v>0.03</v>
+      </c>
+      <c r="X8">
+        <v>0.04</v>
+      </c>
+      <c r="Y8">
+        <v>0.05</v>
+      </c>
+      <c r="Z8">
+        <v>0.05</v>
+      </c>
+      <c r="AA8">
+        <v>0.05</v>
+      </c>
+      <c r="AB8">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="P9" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q9">
+        <v>0.04</v>
+      </c>
+      <c r="R9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S9">
+        <v>0.15</v>
+      </c>
+      <c r="T9">
+        <v>0.15</v>
+      </c>
+      <c r="U9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W9">
+        <v>0.04</v>
+      </c>
+      <c r="X9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z9">
+        <v>0.08</v>
+      </c>
+      <c r="AA9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB9">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="P10" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q10">
+        <v>3.1578947368421102E-2</v>
+      </c>
+      <c r="R10">
+        <v>8.2474226804123696E-2</v>
+      </c>
+      <c r="S10">
+        <v>8.2474226804123696E-2</v>
+      </c>
+      <c r="T10">
+        <v>8.2474226804123696E-2</v>
+      </c>
+      <c r="U10">
+        <v>8.2474226804123696E-2</v>
+      </c>
+      <c r="V10">
+        <v>9.2783505154639206E-2</v>
+      </c>
+      <c r="W10">
+        <v>1.0638297872340399E-2</v>
+      </c>
+      <c r="X10">
+        <v>6.3157894736842093E-2</v>
+      </c>
+      <c r="Y10">
+        <v>6.18556701030928E-2</v>
+      </c>
+      <c r="Z10">
+        <v>6.18556701030928E-2</v>
+      </c>
+      <c r="AA10">
+        <v>6.3157894736842093E-2</v>
+      </c>
+      <c r="AB10">
+        <v>6.3157894736842093E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="P11" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q11">
+        <v>0.04</v>
+      </c>
+      <c r="R11">
+        <v>0.11</v>
+      </c>
+      <c r="S11">
+        <v>0.1</v>
+      </c>
+      <c r="T11">
+        <v>0.12</v>
+      </c>
+      <c r="U11">
+        <v>0.11</v>
+      </c>
+      <c r="V11">
+        <v>0.12</v>
+      </c>
+      <c r="W11">
+        <v>0.02</v>
+      </c>
+      <c r="X11">
+        <v>0.13</v>
+      </c>
+      <c r="Y11">
+        <v>0.13</v>
+      </c>
+      <c r="Z11">
+        <v>0.13</v>
+      </c>
+      <c r="AA11">
+        <v>0.12</v>
+      </c>
+      <c r="AB11">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="P12" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q12">
+        <v>0.05</v>
+      </c>
+      <c r="R12">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S12">
+        <v>0.13</v>
+      </c>
+      <c r="T12">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U12">
+        <v>0.13</v>
+      </c>
+      <c r="V12">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W12">
+        <v>0.03</v>
+      </c>
+      <c r="X12">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y12">
+        <v>0.06</v>
+      </c>
+      <c r="Z12">
+        <v>0.06</v>
+      </c>
+      <c r="AA12">
+        <v>0.08</v>
+      </c>
+      <c r="AB12">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="P13" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R13">
+        <v>0.15</v>
+      </c>
+      <c r="S13">
+        <v>0.15</v>
+      </c>
+      <c r="T13">
+        <v>0.15</v>
+      </c>
+      <c r="U13">
+        <v>0.15</v>
+      </c>
+      <c r="V13">
+        <v>0.16</v>
+      </c>
+      <c r="W13">
+        <v>0.05</v>
+      </c>
+      <c r="X13">
+        <v>0.06</v>
+      </c>
+      <c r="Y13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z13">
+        <v>0.08</v>
+      </c>
+      <c r="AA13">
+        <v>0.06</v>
+      </c>
+      <c r="AB13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="P14" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q14">
+        <v>0.05</v>
+      </c>
+      <c r="R14">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S14">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="T14">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U14">
+        <v>0.15</v>
+      </c>
+      <c r="V14">
+        <v>0.15</v>
+      </c>
+      <c r="W14">
+        <v>0.05</v>
+      </c>
+      <c r="X14">
+        <v>0.08</v>
+      </c>
+      <c r="Y14">
+        <v>0.08</v>
+      </c>
+      <c r="Z14">
+        <v>0.1</v>
+      </c>
+      <c r="AA14">
+        <v>0.08</v>
+      </c>
+      <c r="AB14">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="11">
+        <v>45376</v>
+      </c>
+      <c r="B15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D15">
+        <v>1E-3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>163</v>
+      </c>
+      <c r="F15" t="s">
+        <v>162</v>
+      </c>
+      <c r="G15" t="s">
+        <v>147</v>
+      </c>
+      <c r="H15" t="s">
+        <v>148</v>
+      </c>
+      <c r="I15">
+        <v>500</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L15" t="s">
+        <v>127</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P15" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q15">
+        <v>0.08</v>
+      </c>
+      <c r="R15">
+        <v>0.16</v>
+      </c>
+      <c r="S15">
+        <v>0.2</v>
+      </c>
+      <c r="T15">
+        <v>0.19</v>
+      </c>
+      <c r="U15">
+        <v>0.31</v>
+      </c>
+      <c r="V15">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="W15">
+        <v>0.03</v>
+      </c>
+      <c r="X15">
+        <v>0.13</v>
+      </c>
+      <c r="Y15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Z15">
+        <v>0.13</v>
+      </c>
+      <c r="AA15">
+        <v>0.2</v>
+      </c>
+      <c r="AB15">
+        <v>0.2</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="P16" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q16">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R16">
+        <v>0.19</v>
+      </c>
+      <c r="S16">
+        <v>0.2</v>
+      </c>
+      <c r="T16">
+        <v>0.18</v>
+      </c>
+      <c r="U16">
+        <v>0.35</v>
+      </c>
+      <c r="V16">
+        <v>0.33</v>
+      </c>
+      <c r="W16">
+        <v>0.05</v>
+      </c>
+      <c r="X16">
+        <v>0.16</v>
+      </c>
+      <c r="Y16">
+        <v>0.18</v>
+      </c>
+      <c r="Z16">
+        <v>0.15</v>
+      </c>
+      <c r="AA16">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AB16">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="P17" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q17">
+        <v>0.03</v>
+      </c>
+      <c r="R17">
+        <v>0.26</v>
+      </c>
+      <c r="S17">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="T17">
+        <v>0.3</v>
+      </c>
+      <c r="U17">
+        <v>0.38</v>
+      </c>
+      <c r="V17">
+        <v>0.37</v>
+      </c>
+      <c r="W17">
+        <v>0.02</v>
+      </c>
+      <c r="X17">
+        <v>0.18</v>
+      </c>
+      <c r="Y17">
+        <v>0.22</v>
+      </c>
+      <c r="Z17">
+        <v>0.18</v>
+      </c>
+      <c r="AA17">
+        <v>0.37</v>
+      </c>
+      <c r="AB17">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="P18" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q18">
+        <v>6.0606060606060601E-2</v>
+      </c>
+      <c r="R18">
+        <v>0.12</v>
+      </c>
+      <c r="S18">
+        <v>0.15</v>
+      </c>
+      <c r="T18">
+        <v>0.16</v>
+      </c>
+      <c r="U18">
+        <v>0.18</v>
+      </c>
+      <c r="V18">
+        <v>0.16</v>
+      </c>
+      <c r="W18">
+        <v>3.03030303030303E-2</v>
+      </c>
+      <c r="X18">
+        <v>0.11</v>
+      </c>
+      <c r="Y18">
+        <v>0.11</v>
+      </c>
+      <c r="Z18">
+        <v>0.09</v>
+      </c>
+      <c r="AA18">
+        <v>0.17</v>
+      </c>
+      <c r="AB18">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="P19" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q19">
+        <v>0.03</v>
+      </c>
+      <c r="R19">
+        <v>0.15</v>
+      </c>
+      <c r="S19">
+        <v>0.18</v>
+      </c>
+      <c r="T19">
+        <v>0.17</v>
+      </c>
+      <c r="U19">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="V19">
+        <v>0.31313131313131298</v>
+      </c>
+      <c r="W19">
+        <v>0.01</v>
+      </c>
+      <c r="X19">
+        <v>0.1</v>
+      </c>
+      <c r="Y19">
+        <v>0.18</v>
+      </c>
+      <c r="Z19">
+        <v>0.18</v>
+      </c>
+      <c r="AA19">
+        <v>0.28282828282828298</v>
+      </c>
+      <c r="AB19">
+        <v>0.28282828282828298</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="P20" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q20">
+        <v>0.08</v>
+      </c>
+      <c r="R20">
+        <v>0.12</v>
+      </c>
+      <c r="S20">
+        <v>0.16</v>
+      </c>
+      <c r="T20">
+        <v>0.15</v>
+      </c>
+      <c r="U20">
+        <v>0.34</v>
+      </c>
+      <c r="V20">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="W20">
+        <v>0.06</v>
+      </c>
+      <c r="X20">
+        <v>0.12</v>
+      </c>
+      <c r="Y20">
+        <v>0.1</v>
+      </c>
+      <c r="Z20">
+        <v>0.08</v>
+      </c>
+      <c r="AA20">
+        <v>0.26</v>
+      </c>
+      <c r="AB20">
+        <v>0.27272727272727298</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="P21" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q21">
+        <v>0.06</v>
+      </c>
+      <c r="R21">
+        <v>0.17</v>
+      </c>
+      <c r="S21">
+        <v>0.2</v>
+      </c>
+      <c r="T21">
+        <v>0.2</v>
+      </c>
+      <c r="U21">
+        <v>0.30303030303030298</v>
+      </c>
+      <c r="V21">
+        <v>0.29292929292929298</v>
+      </c>
+      <c r="W21">
+        <v>0.03</v>
+      </c>
+      <c r="X21">
+        <v>0.11</v>
+      </c>
+      <c r="Y21">
+        <v>0.16</v>
+      </c>
+      <c r="Z21">
+        <v>0.16</v>
+      </c>
+      <c r="AA21">
+        <v>0.26262626262626299</v>
+      </c>
+      <c r="AB21">
+        <v>0.24242424242424199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="P22" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q22">
+        <v>1.3157894736842099E-2</v>
+      </c>
+      <c r="R22">
+        <v>0.17204301075268799</v>
+      </c>
+      <c r="S22">
+        <v>0.175824175824176</v>
+      </c>
+      <c r="T22">
+        <v>0.18681318681318701</v>
+      </c>
+      <c r="U22">
+        <v>0.358024691358025</v>
+      </c>
+      <c r="V22">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>0.108695652173913</v>
+      </c>
+      <c r="Y22">
+        <v>0.15730337078651699</v>
+      </c>
+      <c r="Z22">
+        <v>0.14606741573033699</v>
+      </c>
+      <c r="AA22">
+        <v>0.19230769230769201</v>
+      </c>
+      <c r="AB22">
+        <v>0.19480519480519501</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="P23" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q23">
+        <v>0.02</v>
+      </c>
+      <c r="R23">
+        <v>0.16</v>
+      </c>
+      <c r="S23">
+        <v>0.16</v>
+      </c>
+      <c r="T23">
+        <v>0.16</v>
+      </c>
+      <c r="U23">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="V23">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="W23">
+        <v>0.01</v>
+      </c>
+      <c r="X23">
+        <v>0.15</v>
+      </c>
+      <c r="Y23">
+        <v>0.13</v>
+      </c>
+      <c r="Z23">
+        <v>0.1</v>
+      </c>
+      <c r="AA23">
+        <v>0.19</v>
+      </c>
+      <c r="AB23">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="P24" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q24">
+        <v>0.05</v>
+      </c>
+      <c r="R24">
+        <v>0.13</v>
+      </c>
+      <c r="S24">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="T24">
+        <v>0.09</v>
+      </c>
+      <c r="U24">
+        <v>0.21</v>
+      </c>
+      <c r="V24">
+        <v>0.2</v>
+      </c>
+      <c r="W24">
+        <v>0.01</v>
+      </c>
+      <c r="X24">
+        <v>0.08</v>
+      </c>
+      <c r="Y24">
+        <v>0.13</v>
+      </c>
+      <c r="Z24">
+        <v>0.12</v>
+      </c>
+      <c r="AA24">
+        <v>0.16</v>
+      </c>
+      <c r="AB24">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="P25" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q25">
+        <v>0.05</v>
+      </c>
+      <c r="R25">
+        <v>0.18</v>
+      </c>
+      <c r="S25">
+        <v>0.26</v>
+      </c>
+      <c r="T25">
+        <v>0.25</v>
+      </c>
+      <c r="U25">
+        <v>0.38383838383838398</v>
+      </c>
+      <c r="V25">
+        <v>0.38383838383838398</v>
+      </c>
+      <c r="W25">
+        <v>0.02</v>
+      </c>
+      <c r="X25">
+        <v>0.13</v>
+      </c>
+      <c r="Y25">
+        <v>0.19</v>
+      </c>
+      <c r="Z25">
+        <v>0.13</v>
+      </c>
+      <c r="AA25">
+        <v>0.26262626262626299</v>
+      </c>
+      <c r="AB25">
+        <v>0.25252525252525299</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="P26" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q26">
+        <v>0.02</v>
+      </c>
+      <c r="R26">
+        <v>0.12</v>
+      </c>
+      <c r="S26">
+        <v>0.26</v>
+      </c>
+      <c r="T26">
+        <v>0.24</v>
+      </c>
+      <c r="U26">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="V26">
+        <v>0.27</v>
+      </c>
+      <c r="W26">
+        <v>0.01</v>
+      </c>
+      <c r="X26">
+        <v>0.11</v>
+      </c>
+      <c r="Y26">
+        <v>0.22</v>
+      </c>
+      <c r="Z26">
+        <v>0.19</v>
+      </c>
+      <c r="AA26">
+        <v>0.23</v>
+      </c>
+      <c r="AB26">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="11">
+        <v>45373</v>
+      </c>
+      <c r="B27" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" t="s">
+        <v>151</v>
+      </c>
+      <c r="D27">
+        <v>1E-3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>161</v>
+      </c>
+      <c r="F27" t="s">
+        <v>162</v>
+      </c>
+      <c r="G27" t="s">
+        <v>147</v>
+      </c>
+      <c r="H27" t="s">
+        <v>148</v>
+      </c>
+      <c r="I27" t="s">
+        <v>164</v>
+      </c>
+      <c r="J27" s="2">
+        <v>1</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L27" t="s">
+        <v>127</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P27" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q27">
+        <v>0.01</v>
+      </c>
+      <c r="R27">
+        <v>0.08</v>
+      </c>
+      <c r="S27">
+        <v>0.08</v>
+      </c>
+      <c r="T27">
+        <v>0.09</v>
+      </c>
+      <c r="U27">
+        <v>0.09</v>
+      </c>
+      <c r="V27">
+        <v>0.1</v>
+      </c>
+      <c r="W27">
+        <v>0.02</v>
+      </c>
+      <c r="X27">
+        <v>0.05</v>
+      </c>
+      <c r="Y27">
+        <v>0.04</v>
+      </c>
+      <c r="Z27">
+        <v>0.06</v>
+      </c>
+      <c r="AA27">
+        <v>0.02</v>
+      </c>
+      <c r="AB27">
+        <v>0.05</v>
+      </c>
+      <c r="AH27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="P28" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q28">
+        <v>0.01</v>
+      </c>
+      <c r="R28">
+        <v>0.1</v>
+      </c>
+      <c r="S28">
+        <v>0.11</v>
+      </c>
+      <c r="T28">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U28">
+        <v>0.11</v>
+      </c>
+      <c r="V28">
+        <v>0.15</v>
+      </c>
+      <c r="W28">
+        <v>0.02</v>
+      </c>
+      <c r="X28">
+        <v>0.03</v>
+      </c>
+      <c r="Y28">
+        <v>0.03</v>
+      </c>
+      <c r="Z28">
+        <v>0.05</v>
+      </c>
+      <c r="AA28">
+        <v>0.03</v>
+      </c>
+      <c r="AB28">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="P29" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q29">
+        <v>0.04</v>
+      </c>
+      <c r="R29">
+        <v>0.12</v>
+      </c>
+      <c r="S29">
+        <v>0.12</v>
+      </c>
+      <c r="T29">
+        <v>0.12</v>
+      </c>
+      <c r="U29">
+        <v>0.12</v>
+      </c>
+      <c r="V29">
+        <v>0.12</v>
+      </c>
+      <c r="W29">
+        <v>0.03</v>
+      </c>
+      <c r="X29">
+        <v>0.05</v>
+      </c>
+      <c r="Y29">
+        <v>0.06</v>
+      </c>
+      <c r="Z29">
+        <v>0.09</v>
+      </c>
+      <c r="AA29">
+        <v>0.04</v>
+      </c>
+      <c r="AB29">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="P30" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q30">
+        <v>0.04</v>
+      </c>
+      <c r="R30">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S30">
+        <v>0.08</v>
+      </c>
+      <c r="T30">
+        <v>0.11</v>
+      </c>
+      <c r="U30">
+        <v>0.08</v>
+      </c>
+      <c r="V30">
+        <v>0.08</v>
+      </c>
+      <c r="W30">
+        <v>0.03</v>
+      </c>
+      <c r="X30">
+        <v>0.06</v>
+      </c>
+      <c r="Y30">
+        <v>0.06</v>
+      </c>
+      <c r="Z30">
+        <v>0.06</v>
+      </c>
+      <c r="AA30">
+        <v>0.06</v>
+      </c>
+      <c r="AB30">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="P31" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q31">
+        <v>0.04</v>
+      </c>
+      <c r="R31">
+        <v>0.08</v>
+      </c>
+      <c r="S31">
+        <v>0.08</v>
+      </c>
+      <c r="T31">
+        <v>0.1</v>
+      </c>
+      <c r="U31">
+        <v>0.08</v>
+      </c>
+      <c r="V31">
+        <v>0.09</v>
+      </c>
+      <c r="W31">
+        <v>0.03</v>
+      </c>
+      <c r="X31">
+        <v>0.04</v>
+      </c>
+      <c r="Y31">
+        <v>0.04</v>
+      </c>
+      <c r="Z31">
+        <v>0.05</v>
+      </c>
+      <c r="AA31">
+        <v>0.04</v>
+      </c>
+      <c r="AB31">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="P32" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q32">
+        <v>0.05</v>
+      </c>
+      <c r="R32">
+        <v>0.09</v>
+      </c>
+      <c r="S32">
+        <v>0.09</v>
+      </c>
+      <c r="T32">
+        <v>0.09</v>
+      </c>
+      <c r="U32">
+        <v>0.09</v>
+      </c>
+      <c r="V32">
+        <v>0.1</v>
+      </c>
+      <c r="W32">
+        <v>0.01</v>
+      </c>
+      <c r="X32">
+        <v>0.06</v>
+      </c>
+      <c r="Y32">
+        <v>0.06</v>
+      </c>
+      <c r="Z32">
+        <v>0.06</v>
+      </c>
+      <c r="AA32">
+        <v>0.06</v>
+      </c>
+      <c r="AB32">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P33" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q33">
+        <v>0.06</v>
+      </c>
+      <c r="R33">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S33">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T33">
+        <v>0.11</v>
+      </c>
+      <c r="U33">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V33">
+        <v>0.12</v>
+      </c>
+      <c r="W33">
+        <v>0.02</v>
+      </c>
+      <c r="X33">
+        <v>0.05</v>
+      </c>
+      <c r="Y33">
+        <v>0.05</v>
+      </c>
+      <c r="Z33">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA33">
+        <v>0.05</v>
+      </c>
+      <c r="AB33">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P34" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q34">
+        <v>7.5268817204301106E-2</v>
+      </c>
+      <c r="R34">
+        <v>0.10752688172043</v>
+      </c>
+      <c r="S34">
+        <v>0.10752688172043</v>
+      </c>
+      <c r="T34">
+        <v>0.14893617021276601</v>
+      </c>
+      <c r="U34">
+        <v>0.10752688172043</v>
+      </c>
+      <c r="V34">
+        <v>0.123711340206186</v>
+      </c>
+      <c r="W34">
+        <v>5.4945054945054903E-2</v>
+      </c>
+      <c r="X34">
+        <v>6.4516129032258104E-2</v>
+      </c>
+      <c r="Y34">
+        <v>6.4516129032258104E-2</v>
+      </c>
+      <c r="Z34">
+        <v>8.5106382978723402E-2</v>
+      </c>
+      <c r="AA34">
+        <v>6.4516129032258104E-2</v>
+      </c>
+      <c r="AB34">
+        <v>7.2164948453608199E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P35" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q35">
+        <v>0.04</v>
+      </c>
+      <c r="R35">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S35">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T35">
+        <v>0.11</v>
+      </c>
+      <c r="U35">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V35">
+        <v>0.08</v>
+      </c>
+      <c r="W35">
+        <v>0.02</v>
+      </c>
+      <c r="X35">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y35">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z35">
+        <v>0.08</v>
+      </c>
+      <c r="AA35">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB35">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P36" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q36">
+        <v>0.05</v>
+      </c>
+      <c r="R36">
+        <v>0.15</v>
+      </c>
+      <c r="S36">
+        <v>0.15</v>
+      </c>
+      <c r="T36">
+        <v>0.16</v>
+      </c>
+      <c r="U36">
+        <v>0.15</v>
+      </c>
+      <c r="V36">
+        <v>0.18</v>
+      </c>
+      <c r="W36">
+        <v>0.04</v>
+      </c>
+      <c r="X36">
+        <v>0.09</v>
+      </c>
+      <c r="Y36">
+        <v>0.08</v>
+      </c>
+      <c r="Z36">
+        <v>0.1</v>
+      </c>
+      <c r="AA36">
+        <v>0.09</v>
+      </c>
+      <c r="AB36">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P37" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q37">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R37">
+        <v>0.08</v>
+      </c>
+      <c r="S37">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T37">
+        <v>0.11</v>
+      </c>
+      <c r="U37">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V37">
+        <v>0.11</v>
+      </c>
+      <c r="W37">
+        <v>0.03</v>
+      </c>
+      <c r="X37">
+        <v>0.03</v>
+      </c>
+      <c r="Y37">
+        <v>0.03</v>
+      </c>
+      <c r="Z37">
+        <v>0.03</v>
+      </c>
+      <c r="AA37">
+        <v>0.03</v>
+      </c>
+      <c r="AB37">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P38" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q38">
+        <v>0.06</v>
+      </c>
+      <c r="R38">
+        <v>0.11</v>
+      </c>
+      <c r="S38">
+        <v>0.11</v>
+      </c>
+      <c r="T38">
+        <v>0.13</v>
+      </c>
+      <c r="U38">
+        <v>0.11</v>
+      </c>
+      <c r="V38">
+        <v>0.13</v>
+      </c>
+      <c r="W38">
+        <v>0.05</v>
+      </c>
+      <c r="X38">
+        <v>0.09</v>
+      </c>
+      <c r="Y38">
+        <v>0.09</v>
+      </c>
+      <c r="Z38">
+        <v>0.1</v>
+      </c>
+      <c r="AA38">
+        <v>0.1</v>
+      </c>
+      <c r="AB38">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="11">
+        <v>45373</v>
+      </c>
+      <c r="B39" t="s">
+        <v>137</v>
+      </c>
+      <c r="C39" t="s">
+        <v>151</v>
+      </c>
+      <c r="D39">
+        <v>1E-3</v>
+      </c>
+      <c r="E39" t="s">
+        <v>163</v>
+      </c>
+      <c r="F39" t="s">
+        <v>162</v>
+      </c>
+      <c r="G39" t="s">
+        <v>147</v>
+      </c>
+      <c r="H39" t="s">
+        <v>148</v>
+      </c>
+      <c r="I39" t="s">
+        <v>164</v>
+      </c>
+      <c r="J39" s="2">
+        <v>1</v>
+      </c>
+      <c r="K39" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L39" t="s">
+        <v>127</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P39" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q39">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R39">
+        <v>0.12</v>
+      </c>
+      <c r="S39">
+        <v>0.08</v>
+      </c>
+      <c r="T39">
+        <v>0.08</v>
+      </c>
+      <c r="U39">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V39">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W39">
+        <v>0.03</v>
+      </c>
+      <c r="X39">
+        <v>0.06</v>
+      </c>
+      <c r="Y39">
+        <v>0.04</v>
+      </c>
+      <c r="Z39">
+        <v>0.05</v>
+      </c>
+      <c r="AA39">
+        <v>0.09</v>
+      </c>
+      <c r="AB39">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P40" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q40">
+        <v>0.04</v>
+      </c>
+      <c r="R40">
+        <v>0.12</v>
+      </c>
+      <c r="S40">
+        <v>0.1</v>
+      </c>
+      <c r="T40">
+        <v>0.09</v>
+      </c>
+      <c r="U40">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V40">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W40">
+        <v>0.04</v>
+      </c>
+      <c r="X40">
+        <v>0.13</v>
+      </c>
+      <c r="Y40">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z40">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA40">
+        <v>0.11</v>
+      </c>
+      <c r="AB40">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P41" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q41">
+        <v>0.03</v>
+      </c>
+      <c r="R41">
+        <v>0.2</v>
+      </c>
+      <c r="S41">
+        <v>0.12</v>
+      </c>
+      <c r="T41">
+        <v>0.11</v>
+      </c>
+      <c r="U41">
+        <v>0.21</v>
+      </c>
+      <c r="V41">
+        <v>0.21</v>
+      </c>
+      <c r="W41">
+        <v>0.02</v>
+      </c>
+      <c r="X41">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Y41">
+        <v>0.03</v>
+      </c>
+      <c r="Z41">
+        <v>0.04</v>
+      </c>
+      <c r="AA41">
+        <v>0.15</v>
+      </c>
+      <c r="AB41">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P42" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q42">
+        <v>0.05</v>
+      </c>
+      <c r="R42">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S42">
+        <v>0.08</v>
+      </c>
+      <c r="T42">
+        <v>0.09</v>
+      </c>
+      <c r="U42">
+        <v>0.16</v>
+      </c>
+      <c r="V42">
+        <v>0.16</v>
+      </c>
+      <c r="W42">
+        <v>0.02</v>
+      </c>
+      <c r="X42">
+        <v>0.12</v>
+      </c>
+      <c r="Y42">
+        <v>0.06</v>
+      </c>
+      <c r="Z42">
+        <v>0.06</v>
+      </c>
+      <c r="AA42">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AB42">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P43" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q43">
+        <v>0.03</v>
+      </c>
+      <c r="R43">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S43">
+        <v>0.08</v>
+      </c>
+      <c r="T43">
+        <v>0.09</v>
+      </c>
+      <c r="U43">
+        <v>0.13</v>
+      </c>
+      <c r="V43">
+        <v>0.13</v>
+      </c>
+      <c r="W43">
+        <v>0.01</v>
+      </c>
+      <c r="X43">
+        <v>0.08</v>
+      </c>
+      <c r="Y43">
+        <v>0.05</v>
+      </c>
+      <c r="Z43">
+        <v>0.05</v>
+      </c>
+      <c r="AA43">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AB43">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P44" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q44">
+        <v>0.06</v>
+      </c>
+      <c r="R44">
+        <v>0.19</v>
+      </c>
+      <c r="S44">
+        <v>0.1</v>
+      </c>
+      <c r="T44">
+        <v>0.1</v>
+      </c>
+      <c r="U44">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V44">
+        <v>0.13</v>
+      </c>
+      <c r="W44">
+        <v>0.04</v>
+      </c>
+      <c r="X44">
+        <v>0.12</v>
+      </c>
+      <c r="Y44">
+        <v>0.08</v>
+      </c>
+      <c r="Z44">
+        <v>0.08</v>
+      </c>
+      <c r="AA44">
+        <v>0.11</v>
+      </c>
+      <c r="AB44">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P45" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q45">
+        <v>0.06</v>
+      </c>
+      <c r="R45">
+        <v>0.1</v>
+      </c>
+      <c r="S45">
+        <v>0.06</v>
+      </c>
+      <c r="T45">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U45">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V45">
+        <v>0.13</v>
+      </c>
+      <c r="W45">
+        <v>0.01</v>
+      </c>
+      <c r="X45">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y45">
+        <v>0.05</v>
+      </c>
+      <c r="Z45">
+        <v>0.05</v>
+      </c>
+      <c r="AA45">
+        <v>0.09</v>
+      </c>
+      <c r="AB45">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P46" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q46">
+        <v>0.08</v>
+      </c>
+      <c r="R46">
+        <v>0.18279569892473099</v>
+      </c>
+      <c r="S46">
+        <v>8.7912087912087905E-2</v>
+      </c>
+      <c r="T46">
+        <v>9.8901098901098897E-2</v>
+      </c>
+      <c r="U46">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="V46">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="W46">
+        <v>2.8571428571428598E-2</v>
+      </c>
+      <c r="X46">
+        <v>0.13186813186813201</v>
+      </c>
+      <c r="Y46">
+        <v>6.6666666666666693E-2</v>
+      </c>
+      <c r="Z46">
+        <v>6.6666666666666693E-2</v>
+      </c>
+      <c r="AA46">
+        <v>8.2191780821917804E-2</v>
+      </c>
+      <c r="AB46">
+        <v>8.2191780821917804E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P47" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q47">
+        <v>0.04</v>
+      </c>
+      <c r="R47">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S47">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T47">
+        <v>0.08</v>
+      </c>
+      <c r="U47">
+        <v>0.13</v>
+      </c>
+      <c r="V47">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W47">
+        <v>0.03</v>
+      </c>
+      <c r="X47">
+        <v>0.16</v>
+      </c>
+      <c r="Y47">
+        <v>0.09</v>
+      </c>
+      <c r="Z47">
+        <v>0.09</v>
+      </c>
+      <c r="AA47">
+        <v>0.11</v>
+      </c>
+      <c r="AB47">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P48" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q48">
+        <v>0.05</v>
+      </c>
+      <c r="R48">
+        <v>0.1</v>
+      </c>
+      <c r="S48">
+        <v>0.03</v>
+      </c>
+      <c r="T48">
+        <v>0.04</v>
+      </c>
+      <c r="U48">
+        <v>0.08</v>
+      </c>
+      <c r="V48">
+        <v>0.09</v>
+      </c>
+      <c r="W48">
+        <v>0.03</v>
+      </c>
+      <c r="X48">
+        <v>0.09</v>
+      </c>
+      <c r="Y48">
+        <v>0.02</v>
+      </c>
+      <c r="Z48">
+        <v>0.03</v>
+      </c>
+      <c r="AA48">
+        <v>0.06</v>
+      </c>
+      <c r="AB48">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P49" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q49">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R49">
+        <v>0.21</v>
+      </c>
+      <c r="S49">
+        <v>0.05</v>
+      </c>
+      <c r="T49">
+        <v>0.06</v>
+      </c>
+      <c r="U49">
+        <v>0.10101010101010099</v>
+      </c>
+      <c r="V49">
+        <v>0.10101010101010099</v>
+      </c>
+      <c r="W49">
+        <v>0.04</v>
+      </c>
+      <c r="X49">
+        <v>0.15</v>
+      </c>
+      <c r="Y49">
+        <v>0.05</v>
+      </c>
+      <c r="Z49">
+        <v>0.03</v>
+      </c>
+      <c r="AA49">
+        <v>9.0909090909090898E-2</v>
+      </c>
+      <c r="AB49">
+        <v>9.0909090909090898E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P50" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q50">
+        <v>0.03</v>
+      </c>
+      <c r="R50">
+        <v>0.12</v>
+      </c>
+      <c r="S50">
+        <v>0.12</v>
+      </c>
+      <c r="T50">
+        <v>0.13</v>
+      </c>
+      <c r="U50">
+        <v>0.2</v>
+      </c>
+      <c r="V50">
+        <v>0.2</v>
+      </c>
+      <c r="W50">
+        <v>0.03</v>
+      </c>
+      <c r="X50">
+        <v>0.09</v>
+      </c>
+      <c r="Y50">
+        <v>0.08</v>
+      </c>
+      <c r="Z50">
+        <v>0.09</v>
+      </c>
+      <c r="AA50">
+        <v>0.13</v>
+      </c>
+      <c r="AB50">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:31" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="11">
+        <v>45373</v>
+      </c>
+      <c r="B51" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" t="s">
+        <v>151</v>
+      </c>
+      <c r="D51">
+        <v>1E-3</v>
+      </c>
+      <c r="E51" t="s">
+        <v>161</v>
+      </c>
+      <c r="F51" t="s">
+        <v>162</v>
+      </c>
+      <c r="G51" t="s">
+        <v>147</v>
+      </c>
+      <c r="H51" t="s">
+        <v>148</v>
+      </c>
+      <c r="I51" t="s">
+        <v>148</v>
+      </c>
+      <c r="J51" s="2">
+        <v>1</v>
+      </c>
+      <c r="K51" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L51" t="s">
+        <v>127</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P51" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q51">
+        <v>0.04</v>
+      </c>
+      <c r="R51">
+        <v>0.06</v>
+      </c>
+      <c r="S51">
+        <v>0.06</v>
+      </c>
+      <c r="T51">
+        <v>0.13</v>
+      </c>
+      <c r="U51">
+        <v>0.06</v>
+      </c>
+      <c r="V51">
+        <v>0.13</v>
+      </c>
+      <c r="W51">
+        <v>0.03</v>
+      </c>
+      <c r="X51">
+        <v>0.09</v>
+      </c>
+      <c r="Y51">
+        <v>0.09</v>
+      </c>
+      <c r="Z51">
+        <v>0.13</v>
+      </c>
+      <c r="AA51">
+        <v>0.09</v>
+      </c>
+      <c r="AB51">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P52" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q52">
+        <v>0.03</v>
+      </c>
+      <c r="R52">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S52">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T52">
+        <v>0.1</v>
+      </c>
+      <c r="U52">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V52">
+        <v>0.09</v>
+      </c>
+      <c r="W52">
+        <v>0.02</v>
+      </c>
+      <c r="X52">
+        <v>0.03</v>
+      </c>
+      <c r="Y52">
+        <v>0.03</v>
+      </c>
+      <c r="Z52">
+        <v>0.05</v>
+      </c>
+      <c r="AA52">
+        <v>0.03</v>
+      </c>
+      <c r="AB52">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P53" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q53">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R53">
+        <v>0.08</v>
+      </c>
+      <c r="S53">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T53">
+        <v>0.12</v>
+      </c>
+      <c r="U53">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V53">
+        <v>0.16</v>
+      </c>
+      <c r="W53">
+        <v>0.06</v>
+      </c>
+      <c r="X53">
+        <v>0.05</v>
+      </c>
+      <c r="Y53">
+        <v>0.04</v>
+      </c>
+      <c r="Z53">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA53">
+        <v>0.05</v>
+      </c>
+      <c r="AB53">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P54" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q54">
+        <v>0.03</v>
+      </c>
+      <c r="R54">
+        <v>0.1</v>
+      </c>
+      <c r="S54">
+        <v>0.1</v>
+      </c>
+      <c r="T54">
+        <v>0.18</v>
+      </c>
+      <c r="U54">
+        <v>0.1</v>
+      </c>
+      <c r="V54">
+        <v>0.17</v>
+      </c>
+      <c r="W54">
+        <v>0.01</v>
+      </c>
+      <c r="X54">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y54">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z54">
+        <v>0.1</v>
+      </c>
+      <c r="AA54">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB54">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="55" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P55" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q55">
+        <v>0.02</v>
+      </c>
+      <c r="R55">
+        <v>0.09</v>
+      </c>
+      <c r="S55">
+        <v>0.09</v>
+      </c>
+      <c r="T55">
+        <v>0.15</v>
+      </c>
+      <c r="U55">
+        <v>0.09</v>
+      </c>
+      <c r="V55">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W55">
+        <v>0</v>
+      </c>
+      <c r="X55">
+        <v>0.03</v>
+      </c>
+      <c r="Y55">
+        <v>0.03</v>
+      </c>
+      <c r="Z55">
+        <v>0.1</v>
+      </c>
+      <c r="AA55">
+        <v>0.03</v>
+      </c>
+      <c r="AB55">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="56" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P56" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q56">
+        <v>0.03</v>
+      </c>
+      <c r="R56">
+        <v>0.11</v>
+      </c>
+      <c r="S56">
+        <v>0.11</v>
+      </c>
+      <c r="T56">
+        <v>0.17</v>
+      </c>
+      <c r="U56">
+        <v>0.11</v>
+      </c>
+      <c r="V56">
+        <v>0.16</v>
+      </c>
+      <c r="W56">
+        <v>0.02</v>
+      </c>
+      <c r="X56">
+        <v>0.09</v>
+      </c>
+      <c r="Y56">
+        <v>0.1</v>
+      </c>
+      <c r="Z56">
+        <v>0.11</v>
+      </c>
+      <c r="AA56">
+        <v>0.09</v>
+      </c>
+      <c r="AB56">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P57" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q57">
+        <v>0.03</v>
+      </c>
+      <c r="R57">
+        <v>0.1</v>
+      </c>
+      <c r="S57">
+        <v>0.1</v>
+      </c>
+      <c r="T57">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U57">
+        <v>0.1</v>
+      </c>
+      <c r="V57">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W57">
+        <v>0.01</v>
+      </c>
+      <c r="X57">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y57">
+        <v>0.06</v>
+      </c>
+      <c r="Z57">
+        <v>0.1</v>
+      </c>
+      <c r="AA57">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB57">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P58" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q58">
+        <v>4.3478260869565202E-2</v>
+      </c>
+      <c r="R58">
+        <v>0.102040816326531</v>
+      </c>
+      <c r="S58">
+        <v>0.102040816326531</v>
+      </c>
+      <c r="T58">
+        <v>0.14141414141414099</v>
+      </c>
+      <c r="U58">
+        <v>0.102040816326531</v>
+      </c>
+      <c r="V58">
+        <v>0.13131313131313099</v>
+      </c>
+      <c r="W58">
+        <v>3.2967032967033003E-2</v>
+      </c>
+      <c r="X58">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Y58">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Z58">
+        <v>8.0808080808080801E-2</v>
+      </c>
+      <c r="AA58">
+        <v>6.25E-2</v>
+      </c>
+      <c r="AB58">
+        <v>7.0707070707070704E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P59" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q59">
+        <v>0.09</v>
+      </c>
+      <c r="R59">
+        <v>0.11</v>
+      </c>
+      <c r="S59">
+        <v>0.11</v>
+      </c>
+      <c r="T59">
+        <v>0.15</v>
+      </c>
+      <c r="U59">
+        <v>0.13</v>
+      </c>
+      <c r="V59">
+        <v>0.17</v>
+      </c>
+      <c r="W59">
+        <v>0.03</v>
+      </c>
+      <c r="X59">
+        <v>0.08</v>
+      </c>
+      <c r="Y59">
+        <v>0.08</v>
+      </c>
+      <c r="Z59">
+        <v>0.12</v>
+      </c>
+      <c r="AA59">
+        <v>0.08</v>
+      </c>
+      <c r="AB59">
+        <v>0.12</v>
+      </c>
+      <c r="AE59" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="60" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P60" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q60">
+        <v>0.03</v>
+      </c>
+      <c r="R60">
+        <v>0.11</v>
+      </c>
+      <c r="S60">
+        <v>0.11</v>
+      </c>
+      <c r="T60">
+        <v>0.16</v>
+      </c>
+      <c r="U60">
+        <v>0.11</v>
+      </c>
+      <c r="V60">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W60">
+        <v>0.04</v>
+      </c>
+      <c r="X60">
+        <v>0.08</v>
+      </c>
+      <c r="Y60">
+        <v>0.08</v>
+      </c>
+      <c r="Z60">
+        <v>0.12</v>
+      </c>
+      <c r="AA60">
+        <v>0.09</v>
+      </c>
+      <c r="AB60">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P61" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q61">
+        <v>0.01</v>
+      </c>
+      <c r="R61">
+        <v>0.08</v>
+      </c>
+      <c r="S61">
+        <v>0.08</v>
+      </c>
+      <c r="T61">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U61">
+        <v>0.09</v>
+      </c>
+      <c r="V61">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W61">
+        <v>0.02</v>
+      </c>
+      <c r="X61">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y61">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z61">
+        <v>0.09</v>
+      </c>
+      <c r="AA61">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB61">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="62" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P62" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q62">
+        <v>0.05</v>
+      </c>
+      <c r="R62">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S62">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="T62">
+        <v>0.17</v>
+      </c>
+      <c r="U62">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V62">
+        <v>0.19</v>
+      </c>
+      <c r="W62">
+        <v>0.05</v>
+      </c>
+      <c r="X62">
+        <v>0.08</v>
+      </c>
+      <c r="Y62">
+        <v>0.08</v>
+      </c>
+      <c r="Z62">
+        <v>0.16</v>
+      </c>
+      <c r="AA62">
+        <v>0.08</v>
+      </c>
+      <c r="AB62">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:31" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A63" s="11">
+        <v>45373</v>
+      </c>
+      <c r="B63" t="s">
+        <v>137</v>
+      </c>
+      <c r="C63" t="s">
+        <v>151</v>
+      </c>
+      <c r="D63">
+        <v>1E-3</v>
+      </c>
+      <c r="E63" t="s">
+        <v>163</v>
+      </c>
+      <c r="F63" t="s">
+        <v>162</v>
+      </c>
+      <c r="G63" t="s">
+        <v>147</v>
+      </c>
+      <c r="H63" t="s">
+        <v>148</v>
+      </c>
+      <c r="I63" t="s">
+        <v>148</v>
+      </c>
+      <c r="J63" s="2">
+        <v>1</v>
+      </c>
+      <c r="K63" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L63" t="s">
+        <v>127</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O63" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P63" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q63">
+        <v>0.06</v>
+      </c>
+      <c r="R63">
+        <v>0.12</v>
+      </c>
+      <c r="S63">
+        <v>0.08</v>
+      </c>
+      <c r="T63">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U63">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V63">
+        <v>0.08</v>
+      </c>
+      <c r="W63">
+        <v>0.04</v>
+      </c>
+      <c r="X63">
+        <v>0.13</v>
+      </c>
+      <c r="Y63">
+        <v>0.04</v>
+      </c>
+      <c r="Z63">
+        <v>0.06</v>
+      </c>
+      <c r="AA63">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB63">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="64" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P64" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q64">
+        <v>0.02</v>
+      </c>
+      <c r="R64">
+        <v>0.17</v>
+      </c>
+      <c r="S64">
+        <v>0.03</v>
+      </c>
+      <c r="T64">
+        <v>0.06</v>
+      </c>
+      <c r="U64">
+        <v>0.03</v>
+      </c>
+      <c r="V64">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W64">
+        <v>0.01</v>
+      </c>
+      <c r="X64">
+        <v>0.13</v>
+      </c>
+      <c r="Y64">
+        <v>0.04</v>
+      </c>
+      <c r="Z64">
+        <v>0.03</v>
+      </c>
+      <c r="AA64">
+        <v>0.02</v>
+      </c>
+      <c r="AB64">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="65" spans="16:31" x14ac:dyDescent="0.3">
+      <c r="P65" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q65">
+        <v>0.04</v>
+      </c>
+      <c r="R65">
+        <v>0.16</v>
+      </c>
+      <c r="S65">
+        <v>0.04</v>
+      </c>
+      <c r="T65">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U65">
+        <v>0.18</v>
+      </c>
+      <c r="V65">
+        <v>0.23</v>
+      </c>
+      <c r="W65">
+        <v>0.05</v>
+      </c>
+      <c r="X65">
+        <v>0.12</v>
+      </c>
+      <c r="Y65">
+        <v>0.04</v>
+      </c>
+      <c r="Z65">
+        <v>0.03</v>
+      </c>
+      <c r="AA65">
+        <v>0.1</v>
+      </c>
+      <c r="AB65">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="16:31" x14ac:dyDescent="0.3">
+      <c r="P66" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q66">
+        <v>0.06</v>
+      </c>
+      <c r="R66">
+        <v>0.16</v>
+      </c>
+      <c r="S66">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T66">
+        <v>0.11</v>
+      </c>
+      <c r="U66">
+        <v>0.08</v>
+      </c>
+      <c r="V66">
+        <v>0.11</v>
+      </c>
+      <c r="W66">
+        <v>0.05</v>
+      </c>
+      <c r="X66">
+        <v>0.08</v>
+      </c>
+      <c r="Y66">
+        <v>0.03</v>
+      </c>
+      <c r="Z66">
+        <v>0.05</v>
+      </c>
+      <c r="AA66">
+        <v>0.03</v>
+      </c>
+      <c r="AB66">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="67" spans="16:31" x14ac:dyDescent="0.3">
+      <c r="P67" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q67">
+        <v>0.08</v>
+      </c>
+      <c r="R67">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S67">
+        <v>0.04</v>
+      </c>
+      <c r="T67">
+        <v>0.03</v>
+      </c>
+      <c r="U67">
+        <v>0.06</v>
+      </c>
+      <c r="V67">
+        <v>0.08</v>
+      </c>
+      <c r="W67">
+        <v>0.04</v>
+      </c>
+      <c r="X67">
+        <v>0.1</v>
+      </c>
+      <c r="Y67">
+        <v>0.01</v>
+      </c>
+      <c r="Z67">
+        <v>0.03</v>
+      </c>
+      <c r="AA67">
+        <v>0.05</v>
+      </c>
+      <c r="AB67">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="68" spans="16:31" x14ac:dyDescent="0.3">
+      <c r="P68" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q68">
+        <v>0.02</v>
+      </c>
+      <c r="R68">
+        <v>0.09</v>
+      </c>
+      <c r="S68">
+        <v>0.04</v>
+      </c>
+      <c r="T68">
+        <v>0.05</v>
+      </c>
+      <c r="U68">
+        <v>0.09</v>
+      </c>
+      <c r="V68">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W68">
+        <v>0.01</v>
+      </c>
+      <c r="X68">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y68">
+        <v>0.03</v>
+      </c>
+      <c r="Z68">
+        <v>0.03</v>
+      </c>
+      <c r="AA68">
+        <v>0.08</v>
+      </c>
+      <c r="AB68">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="69" spans="16:31" x14ac:dyDescent="0.3">
+      <c r="P69" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q69">
+        <v>0.03</v>
+      </c>
+      <c r="R69">
+        <v>0.17</v>
+      </c>
+      <c r="S69">
+        <v>0.1</v>
+      </c>
+      <c r="T69">
+        <v>0.13</v>
+      </c>
+      <c r="U69">
+        <v>0.16</v>
+      </c>
+      <c r="V69">
+        <v>0.19</v>
+      </c>
+      <c r="W69">
+        <v>0.01</v>
+      </c>
+      <c r="X69">
+        <v>0.13</v>
+      </c>
+      <c r="Y69">
+        <v>0.1</v>
+      </c>
+      <c r="Z69">
+        <v>0.1</v>
+      </c>
+      <c r="AA69">
+        <v>0.06</v>
+      </c>
+      <c r="AB69">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="70" spans="16:31" x14ac:dyDescent="0.3">
+      <c r="P70" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q70">
+        <v>1.35135135135135E-2</v>
+      </c>
+      <c r="R70">
+        <v>0.10752688172043</v>
+      </c>
+      <c r="S70">
+        <v>5.7471264367816098E-2</v>
+      </c>
+      <c r="T70">
+        <v>9.375E-2</v>
+      </c>
+      <c r="U70">
+        <v>7.0588235294117604E-2</v>
+      </c>
+      <c r="V70">
+        <v>0.10989010989011</v>
+      </c>
+      <c r="W70">
+        <v>1.4285714285714299E-2</v>
+      </c>
+      <c r="X70">
+        <v>7.5268817204301106E-2</v>
+      </c>
+      <c r="Y70">
+        <v>2.2988505747126398E-2</v>
+      </c>
+      <c r="Z70">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="AA70">
+        <v>4.7619047619047603E-2</v>
+      </c>
+      <c r="AB70">
+        <v>8.7912087912087905E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="16:31" x14ac:dyDescent="0.3">
+      <c r="P71" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q71">
+        <v>0</v>
+      </c>
+      <c r="R71">
+        <v>0.1</v>
+      </c>
+      <c r="S71">
+        <v>0.02</v>
+      </c>
+      <c r="T71">
+        <v>0.03</v>
+      </c>
+      <c r="U71">
+        <v>0.02</v>
+      </c>
+      <c r="V71">
+        <v>0.06</v>
+      </c>
+      <c r="W71">
+        <v>0.01</v>
+      </c>
+      <c r="X71">
+        <v>0.09</v>
+      </c>
+      <c r="Y71">
+        <v>0.03</v>
+      </c>
+      <c r="Z71">
+        <v>0.02</v>
+      </c>
+      <c r="AA71">
+        <v>0.05</v>
+      </c>
+      <c r="AB71">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="72" spans="16:31" x14ac:dyDescent="0.3">
+      <c r="P72" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q72">
+        <v>0.06</v>
+      </c>
+      <c r="R72">
+        <v>0.17</v>
+      </c>
+      <c r="S72">
+        <v>0.06</v>
+      </c>
+      <c r="T72">
+        <v>0.09</v>
+      </c>
+      <c r="U72">
+        <v>0.12</v>
+      </c>
+      <c r="V72">
+        <v>0.13</v>
+      </c>
+      <c r="W72">
+        <v>0.04</v>
+      </c>
+      <c r="X72">
+        <v>0.12</v>
+      </c>
+      <c r="Y72">
+        <v>0.06</v>
+      </c>
+      <c r="Z72">
+        <v>0.09</v>
+      </c>
+      <c r="AA72">
+        <v>0.1</v>
+      </c>
+      <c r="AB72">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AE72" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="73" spans="16:31" x14ac:dyDescent="0.3">
+      <c r="P73" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q73">
+        <v>6.0606060606060601E-2</v>
+      </c>
+      <c r="R73">
+        <v>0.16</v>
+      </c>
+      <c r="S73">
+        <v>0.04</v>
+      </c>
+      <c r="T73">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U73">
+        <v>0.04</v>
+      </c>
+      <c r="V73">
+        <v>0.06</v>
+      </c>
+      <c r="W73">
+        <v>2.02020202020202E-2</v>
+      </c>
+      <c r="X73">
+        <v>0.1</v>
+      </c>
+      <c r="Y73">
+        <v>0.05</v>
+      </c>
+      <c r="Z73">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA73">
+        <v>0.03</v>
+      </c>
+      <c r="AB73">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="74" spans="16:31" x14ac:dyDescent="0.3">
+      <c r="P74" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q74">
+        <v>0.02</v>
+      </c>
+      <c r="R74">
+        <v>0.15</v>
+      </c>
+      <c r="S74">
+        <v>0.02</v>
+      </c>
+      <c r="T74">
+        <v>0.02</v>
+      </c>
+      <c r="U74">
+        <v>0.02</v>
+      </c>
+      <c r="V74">
+        <v>0.04</v>
+      </c>
+      <c r="W74">
+        <v>0.03</v>
+      </c>
+      <c r="X74">
+        <v>0.12</v>
+      </c>
+      <c r="Y74">
+        <v>0.03</v>
+      </c>
+      <c r="Z74">
+        <v>0.03</v>
+      </c>
+      <c r="AA74">
+        <v>0.03</v>
+      </c>
+      <c r="AB74">
+        <v>0.04</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="Q1:AB1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added updated Neff results using newer formula
</commit_message>
<xml_diff>
--- a/Results/t1e_simulation_tracker.xlsx
+++ b/Results/t1e_simulation_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagee\Documents\GitHub\masters_project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB32C65-8D5B-47A8-A14E-06462D86F33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEDF4A2-C082-4080-B18A-BCFAD857849C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{A2C378D7-6BEC-4566-B54E-29AFD33A9FE4}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="169">
   <si>
     <t>Population</t>
   </si>
@@ -755,6 +755,20 @@
   <si>
     <t>2k</t>
   </si>
+  <si>
+    <t>Neff calculated using v1 equation: 
+eff_samp_size = floor(sum(pmin(pi.observed, pi.target)*N_observed + N_reference*pmin(1,(pi.target*length(pi.target)))))</t>
+  </si>
+  <si>
+    <t>3/25/2024 and 4/1/2024 for Neff</t>
+  </si>
+  <si>
+    <t>3/22/2024 and 4/1/2024 for Neff</t>
+  </si>
+  <si>
+    <t>Neff calculated using v2 equation:
+eff_samp_size = floor(sum(pmin(pi.target, pi.observed)) * N_observed + sum(pi.target * N_reference))</t>
+  </si>
 </sst>
 </file>
 
@@ -821,7 +835,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -853,6 +867,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1217,31 +1234,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
     </row>
     <row r="2" spans="1:35" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -7285,36 +7302,36 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -14470,37 +14487,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="14" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
       <c r="AB1" s="1"/>
     </row>
     <row r="2" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
@@ -15404,39 +15421,39 @@
   <sheetData>
     <row r="1" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="14" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
       <c r="AE1" s="12"/>
       <c r="AF1" s="12"/>
       <c r="AG1" s="12"/>
@@ -20316,11 +20333,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462CC3C0-91BE-442C-A1C6-C94A876D69AE}">
-  <dimension ref="A1:AH74"/>
+  <dimension ref="A1:AH146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
+      <pane ySplit="2" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K150" sqref="K150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20338,42 +20355,43 @@
     <col min="26" max="26" width="9.6640625" customWidth="1"/>
     <col min="27" max="27" width="9.77734375" customWidth="1"/>
     <col min="28" max="28" width="10.21875" customWidth="1"/>
+    <col min="29" max="29" width="98.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="14" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="13"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="14"/>
       <c r="AD1" s="13"/>
     </row>
     <row r="2" spans="1:30" ht="86.4" x14ac:dyDescent="0.3">
@@ -20461,6 +20479,9 @@
       <c r="AB2" s="1" t="s">
         <v>160</v>
       </c>
+      <c r="AC2" s="1" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="3" spans="1:30" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
@@ -20547,6 +20568,9 @@
       <c r="AB3">
         <v>7.0000000000000007E-2</v>
       </c>
+      <c r="AC3" s="1" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="P4" t="s">
@@ -21084,6 +21108,9 @@
       <c r="AB15">
         <v>0.2</v>
       </c>
+      <c r="AC15" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="AD15" t="s">
         <v>84</v>
       </c>
@@ -21624,6 +21651,9 @@
       <c r="AB27">
         <v>0.05</v>
       </c>
+      <c r="AC27" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="AH27" t="s">
         <v>84</v>
       </c>
@@ -22164,6 +22194,9 @@
       <c r="AB39">
         <v>0.1</v>
       </c>
+      <c r="AC39" s="1" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="P40" t="s">
@@ -22704,6 +22737,9 @@
       <c r="AB51">
         <v>0.12</v>
       </c>
+      <c r="AC51" s="1" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.3">
       <c r="P52" t="s">
@@ -23244,6 +23280,9 @@
       <c r="AB63">
         <v>0.09</v>
       </c>
+      <c r="AC63" s="1" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="64" spans="1:31" x14ac:dyDescent="0.3">
       <c r="P64" t="s">
@@ -23286,7 +23325,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="65" spans="16:31" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.3">
       <c r="P65" t="s">
         <v>108</v>
       </c>
@@ -23327,7 +23366,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="66" spans="16:31" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.3">
       <c r="P66" t="s">
         <v>109</v>
       </c>
@@ -23368,7 +23407,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="67" spans="16:31" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.3">
       <c r="P67" t="s">
         <v>110</v>
       </c>
@@ -23409,7 +23448,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="68" spans="16:31" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.3">
       <c r="P68" t="s">
         <v>111</v>
       </c>
@@ -23450,7 +23489,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="69" spans="16:31" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.3">
       <c r="P69" t="s">
         <v>112</v>
       </c>
@@ -23491,7 +23530,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="70" spans="16:31" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.3">
       <c r="P70" t="s">
         <v>113</v>
       </c>
@@ -23532,7 +23571,7 @@
         <v>8.7912087912087905E-2</v>
       </c>
     </row>
-    <row r="71" spans="16:31" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.3">
       <c r="P71" t="s">
         <v>114</v>
       </c>
@@ -23573,7 +23612,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="72" spans="16:31" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.3">
       <c r="P72" t="s">
         <v>115</v>
       </c>
@@ -23617,7 +23656,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="16:31" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.3">
       <c r="P73" t="s">
         <v>116</v>
       </c>
@@ -23658,7 +23697,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="74" spans="16:31" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.3">
       <c r="P74" t="s">
         <v>117</v>
       </c>
@@ -23696,6 +23735,3246 @@
         <v>0.03</v>
       </c>
       <c r="AB74">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="75" spans="1:31" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A75" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B75" t="s">
+        <v>137</v>
+      </c>
+      <c r="C75" t="s">
+        <v>151</v>
+      </c>
+      <c r="D75">
+        <v>1E-3</v>
+      </c>
+      <c r="E75" t="s">
+        <v>161</v>
+      </c>
+      <c r="F75" t="s">
+        <v>162</v>
+      </c>
+      <c r="G75" t="s">
+        <v>147</v>
+      </c>
+      <c r="H75" t="s">
+        <v>148</v>
+      </c>
+      <c r="I75">
+        <v>500</v>
+      </c>
+      <c r="J75" s="2">
+        <v>1</v>
+      </c>
+      <c r="K75" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L75" t="s">
+        <v>127</v>
+      </c>
+      <c r="M75" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N75" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O75" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P75" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q75">
+        <v>0.05</v>
+      </c>
+      <c r="R75">
+        <v>0.11</v>
+      </c>
+      <c r="S75">
+        <v>0.11</v>
+      </c>
+      <c r="T75">
+        <v>0.12</v>
+      </c>
+      <c r="U75">
+        <v>0.11</v>
+      </c>
+      <c r="V75">
+        <v>0.12</v>
+      </c>
+      <c r="W75">
+        <v>0.01</v>
+      </c>
+      <c r="X75">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y75">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z75">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA75">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB75">
+        <v>0.08</v>
+      </c>
+      <c r="AC75" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="76" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P76" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q76">
+        <v>0.02</v>
+      </c>
+      <c r="R76">
+        <v>0.06</v>
+      </c>
+      <c r="S76">
+        <v>0.06</v>
+      </c>
+      <c r="T76">
+        <v>0.06</v>
+      </c>
+      <c r="U76">
+        <v>0.06</v>
+      </c>
+      <c r="V76">
+        <v>0.06</v>
+      </c>
+      <c r="W76">
+        <v>0.02</v>
+      </c>
+      <c r="X76">
+        <v>0.02</v>
+      </c>
+      <c r="Y76">
+        <v>0.02</v>
+      </c>
+      <c r="Z76">
+        <v>0.02</v>
+      </c>
+      <c r="AA76">
+        <v>0.03</v>
+      </c>
+      <c r="AB76">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="77" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P77" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q77">
+        <v>0.04</v>
+      </c>
+      <c r="R77">
+        <v>0.09</v>
+      </c>
+      <c r="S77">
+        <v>0.09</v>
+      </c>
+      <c r="T77">
+        <v>0.1</v>
+      </c>
+      <c r="U77">
+        <v>0.09</v>
+      </c>
+      <c r="V77">
+        <v>0.12</v>
+      </c>
+      <c r="W77">
+        <v>0</v>
+      </c>
+      <c r="X77">
+        <v>0.06</v>
+      </c>
+      <c r="Y77">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z77">
+        <v>0.08</v>
+      </c>
+      <c r="AA77">
+        <v>0.06</v>
+      </c>
+      <c r="AB77">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="78" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P78" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q78">
+        <v>0.03</v>
+      </c>
+      <c r="R78">
+        <v>0.09</v>
+      </c>
+      <c r="S78">
+        <v>0.09</v>
+      </c>
+      <c r="T78">
+        <v>0.09</v>
+      </c>
+      <c r="U78">
+        <v>0.09</v>
+      </c>
+      <c r="V78">
+        <v>0.09</v>
+      </c>
+      <c r="W78">
+        <v>0.01</v>
+      </c>
+      <c r="X78">
+        <v>0.06</v>
+      </c>
+      <c r="Y78">
+        <v>0.05</v>
+      </c>
+      <c r="Z78">
+        <v>0.06</v>
+      </c>
+      <c r="AA78">
+        <v>0.06</v>
+      </c>
+      <c r="AB78">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="79" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P79" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q79">
+        <v>0.02</v>
+      </c>
+      <c r="R79">
+        <v>0.11</v>
+      </c>
+      <c r="S79">
+        <v>0.1</v>
+      </c>
+      <c r="T79">
+        <v>0.11</v>
+      </c>
+      <c r="U79">
+        <v>0.1</v>
+      </c>
+      <c r="V79">
+        <v>0.1</v>
+      </c>
+      <c r="W79">
+        <v>0.03</v>
+      </c>
+      <c r="X79">
+        <v>0.08</v>
+      </c>
+      <c r="Y79">
+        <v>0.09</v>
+      </c>
+      <c r="Z79">
+        <v>0.09</v>
+      </c>
+      <c r="AA79">
+        <v>0.09</v>
+      </c>
+      <c r="AB79">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="80" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="P80" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q80">
+        <v>0.08</v>
+      </c>
+      <c r="R80">
+        <v>0.06</v>
+      </c>
+      <c r="S80">
+        <v>0.06</v>
+      </c>
+      <c r="T80">
+        <v>0.06</v>
+      </c>
+      <c r="U80">
+        <v>0.06</v>
+      </c>
+      <c r="V80">
+        <v>0.06</v>
+      </c>
+      <c r="W80">
+        <v>0.03</v>
+      </c>
+      <c r="X80">
+        <v>0.04</v>
+      </c>
+      <c r="Y80">
+        <v>0.05</v>
+      </c>
+      <c r="Z80">
+        <v>0.04</v>
+      </c>
+      <c r="AA80">
+        <v>0.05</v>
+      </c>
+      <c r="AB80">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="81" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P81" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q81">
+        <v>0.04</v>
+      </c>
+      <c r="R81">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S81">
+        <v>0.15</v>
+      </c>
+      <c r="T81">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U81">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V81">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W81">
+        <v>0.04</v>
+      </c>
+      <c r="X81">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y81">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z81">
+        <v>0.08</v>
+      </c>
+      <c r="AA81">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB81">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="82" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P82" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q82">
+        <v>3.1578947368421102E-2</v>
+      </c>
+      <c r="R82">
+        <v>8.2474226804123696E-2</v>
+      </c>
+      <c r="S82">
+        <v>8.2474226804123696E-2</v>
+      </c>
+      <c r="T82">
+        <v>8.2474226804123696E-2</v>
+      </c>
+      <c r="U82">
+        <v>8.2474226804123696E-2</v>
+      </c>
+      <c r="V82">
+        <v>9.2783505154639206E-2</v>
+      </c>
+      <c r="W82">
+        <v>1.0638297872340399E-2</v>
+      </c>
+      <c r="X82">
+        <v>6.3157894736842093E-2</v>
+      </c>
+      <c r="Y82">
+        <v>6.18556701030928E-2</v>
+      </c>
+      <c r="Z82">
+        <v>6.18556701030928E-2</v>
+      </c>
+      <c r="AA82">
+        <v>6.3157894736842093E-2</v>
+      </c>
+      <c r="AB82">
+        <v>6.3157894736842093E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P83" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q83">
+        <v>0.04</v>
+      </c>
+      <c r="R83">
+        <v>0.11</v>
+      </c>
+      <c r="S83">
+        <v>0.1</v>
+      </c>
+      <c r="T83">
+        <v>0.12</v>
+      </c>
+      <c r="U83">
+        <v>0.11</v>
+      </c>
+      <c r="V83">
+        <v>0.12</v>
+      </c>
+      <c r="W83">
+        <v>0.02</v>
+      </c>
+      <c r="X83">
+        <v>0.13</v>
+      </c>
+      <c r="Y83">
+        <v>0.13</v>
+      </c>
+      <c r="Z83">
+        <v>0.13</v>
+      </c>
+      <c r="AA83">
+        <v>0.12</v>
+      </c>
+      <c r="AB83">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P84" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q84">
+        <v>0.05</v>
+      </c>
+      <c r="R84">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S84">
+        <v>0.13</v>
+      </c>
+      <c r="T84">
+        <v>0.15</v>
+      </c>
+      <c r="U84">
+        <v>0.13</v>
+      </c>
+      <c r="V84">
+        <v>0.13</v>
+      </c>
+      <c r="W84">
+        <v>0.03</v>
+      </c>
+      <c r="X84">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y84">
+        <v>0.06</v>
+      </c>
+      <c r="Z84">
+        <v>0.06</v>
+      </c>
+      <c r="AA84">
+        <v>0.08</v>
+      </c>
+      <c r="AB84">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="85" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P85" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q85">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R85">
+        <v>0.15</v>
+      </c>
+      <c r="S85">
+        <v>0.15</v>
+      </c>
+      <c r="T85">
+        <v>0.15</v>
+      </c>
+      <c r="U85">
+        <v>0.15</v>
+      </c>
+      <c r="V85">
+        <v>0.15</v>
+      </c>
+      <c r="W85">
+        <v>0.05</v>
+      </c>
+      <c r="X85">
+        <v>0.06</v>
+      </c>
+      <c r="Y85">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z85">
+        <v>0.08</v>
+      </c>
+      <c r="AA85">
+        <v>0.06</v>
+      </c>
+      <c r="AB85">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P86" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q86">
+        <v>0.05</v>
+      </c>
+      <c r="R86">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S86">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="T86">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U86">
+        <v>0.15</v>
+      </c>
+      <c r="V86">
+        <v>0.15</v>
+      </c>
+      <c r="W86">
+        <v>0.05</v>
+      </c>
+      <c r="X86">
+        <v>0.08</v>
+      </c>
+      <c r="Y86">
+        <v>0.08</v>
+      </c>
+      <c r="Z86">
+        <v>0.09</v>
+      </c>
+      <c r="AA86">
+        <v>0.08</v>
+      </c>
+      <c r="AB86">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:29" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A87" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B87" t="s">
+        <v>137</v>
+      </c>
+      <c r="C87" t="s">
+        <v>151</v>
+      </c>
+      <c r="D87">
+        <v>1E-3</v>
+      </c>
+      <c r="E87" t="s">
+        <v>163</v>
+      </c>
+      <c r="F87" t="s">
+        <v>162</v>
+      </c>
+      <c r="G87" t="s">
+        <v>147</v>
+      </c>
+      <c r="H87" t="s">
+        <v>148</v>
+      </c>
+      <c r="I87">
+        <v>500</v>
+      </c>
+      <c r="J87" s="2">
+        <v>1</v>
+      </c>
+      <c r="K87" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L87" t="s">
+        <v>127</v>
+      </c>
+      <c r="M87" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N87" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O87" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P87" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q87">
+        <v>0.08</v>
+      </c>
+      <c r="R87">
+        <v>0.16</v>
+      </c>
+      <c r="S87">
+        <v>0.2</v>
+      </c>
+      <c r="T87">
+        <v>0.19</v>
+      </c>
+      <c r="U87">
+        <v>0.31</v>
+      </c>
+      <c r="V87">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="W87">
+        <v>0.03</v>
+      </c>
+      <c r="X87">
+        <v>0.13</v>
+      </c>
+      <c r="Y87">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Z87">
+        <v>0.13</v>
+      </c>
+      <c r="AA87">
+        <v>0.2</v>
+      </c>
+      <c r="AB87">
+        <v>0.2</v>
+      </c>
+      <c r="AC87" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="88" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P88" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q88">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R88">
+        <v>0.19</v>
+      </c>
+      <c r="S88">
+        <v>0.2</v>
+      </c>
+      <c r="T88">
+        <v>0.18</v>
+      </c>
+      <c r="U88">
+        <v>0.35</v>
+      </c>
+      <c r="V88">
+        <v>0.32</v>
+      </c>
+      <c r="W88">
+        <v>0.05</v>
+      </c>
+      <c r="X88">
+        <v>0.16</v>
+      </c>
+      <c r="Y88">
+        <v>0.18</v>
+      </c>
+      <c r="Z88">
+        <v>0.15</v>
+      </c>
+      <c r="AA88">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AB88">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="89" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P89" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q89">
+        <v>0.03</v>
+      </c>
+      <c r="R89">
+        <v>0.26</v>
+      </c>
+      <c r="S89">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="T89">
+        <v>0.3</v>
+      </c>
+      <c r="U89">
+        <v>0.38</v>
+      </c>
+      <c r="V89">
+        <v>0.37</v>
+      </c>
+      <c r="W89">
+        <v>0.02</v>
+      </c>
+      <c r="X89">
+        <v>0.18</v>
+      </c>
+      <c r="Y89">
+        <v>0.22</v>
+      </c>
+      <c r="Z89">
+        <v>0.18</v>
+      </c>
+      <c r="AA89">
+        <v>0.37</v>
+      </c>
+      <c r="AB89">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="90" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P90" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q90">
+        <v>6.0606060606060601E-2</v>
+      </c>
+      <c r="R90">
+        <v>0.12</v>
+      </c>
+      <c r="S90">
+        <v>0.15</v>
+      </c>
+      <c r="T90">
+        <v>0.16</v>
+      </c>
+      <c r="U90">
+        <v>0.18</v>
+      </c>
+      <c r="V90">
+        <v>0.16</v>
+      </c>
+      <c r="W90">
+        <v>3.03030303030303E-2</v>
+      </c>
+      <c r="X90">
+        <v>0.11</v>
+      </c>
+      <c r="Y90">
+        <v>0.11</v>
+      </c>
+      <c r="Z90">
+        <v>0.09</v>
+      </c>
+      <c r="AA90">
+        <v>0.17</v>
+      </c>
+      <c r="AB90">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P91" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q91">
+        <v>0.03</v>
+      </c>
+      <c r="R91">
+        <v>0.15</v>
+      </c>
+      <c r="S91">
+        <v>0.18</v>
+      </c>
+      <c r="T91">
+        <v>0.17</v>
+      </c>
+      <c r="U91">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="V91">
+        <v>0.31313131313131298</v>
+      </c>
+      <c r="W91">
+        <v>0.01</v>
+      </c>
+      <c r="X91">
+        <v>0.1</v>
+      </c>
+      <c r="Y91">
+        <v>0.18</v>
+      </c>
+      <c r="Z91">
+        <v>0.18</v>
+      </c>
+      <c r="AA91">
+        <v>0.28282828282828298</v>
+      </c>
+      <c r="AB91">
+        <v>0.28282828282828298</v>
+      </c>
+    </row>
+    <row r="92" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P92" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q92">
+        <v>0.08</v>
+      </c>
+      <c r="R92">
+        <v>0.12</v>
+      </c>
+      <c r="S92">
+        <v>0.16</v>
+      </c>
+      <c r="T92">
+        <v>0.15</v>
+      </c>
+      <c r="U92">
+        <v>0.34</v>
+      </c>
+      <c r="V92">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="W92">
+        <v>0.06</v>
+      </c>
+      <c r="X92">
+        <v>0.12</v>
+      </c>
+      <c r="Y92">
+        <v>0.1</v>
+      </c>
+      <c r="Z92">
+        <v>0.08</v>
+      </c>
+      <c r="AA92">
+        <v>0.26</v>
+      </c>
+      <c r="AB92">
+        <v>0.27272727272727298</v>
+      </c>
+    </row>
+    <row r="93" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P93" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q93">
+        <v>0.06</v>
+      </c>
+      <c r="R93">
+        <v>0.17</v>
+      </c>
+      <c r="S93">
+        <v>0.2</v>
+      </c>
+      <c r="T93">
+        <v>0.2</v>
+      </c>
+      <c r="U93">
+        <v>0.30303030303030298</v>
+      </c>
+      <c r="V93">
+        <v>0.29292929292929298</v>
+      </c>
+      <c r="W93">
+        <v>0.03</v>
+      </c>
+      <c r="X93">
+        <v>0.11</v>
+      </c>
+      <c r="Y93">
+        <v>0.16</v>
+      </c>
+      <c r="Z93">
+        <v>0.16</v>
+      </c>
+      <c r="AA93">
+        <v>0.26262626262626299</v>
+      </c>
+      <c r="AB93">
+        <v>0.25252525252525299</v>
+      </c>
+    </row>
+    <row r="94" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P94" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q94">
+        <v>1.3157894736842099E-2</v>
+      </c>
+      <c r="R94">
+        <v>0.17204301075268799</v>
+      </c>
+      <c r="S94">
+        <v>0.175824175824176</v>
+      </c>
+      <c r="T94">
+        <v>0.18681318681318701</v>
+      </c>
+      <c r="U94">
+        <v>0.358024691358025</v>
+      </c>
+      <c r="V94">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="W94">
+        <v>0</v>
+      </c>
+      <c r="X94">
+        <v>0.108695652173913</v>
+      </c>
+      <c r="Y94">
+        <v>0.15730337078651699</v>
+      </c>
+      <c r="Z94">
+        <v>0.14606741573033699</v>
+      </c>
+      <c r="AA94">
+        <v>0.19230769230769201</v>
+      </c>
+      <c r="AB94">
+        <v>0.19480519480519501</v>
+      </c>
+    </row>
+    <row r="95" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P95" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q95">
+        <v>0.02</v>
+      </c>
+      <c r="R95">
+        <v>0.16</v>
+      </c>
+      <c r="S95">
+        <v>0.16</v>
+      </c>
+      <c r="T95">
+        <v>0.16</v>
+      </c>
+      <c r="U95">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="V95">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="W95">
+        <v>0.01</v>
+      </c>
+      <c r="X95">
+        <v>0.15</v>
+      </c>
+      <c r="Y95">
+        <v>0.13</v>
+      </c>
+      <c r="Z95">
+        <v>0.1</v>
+      </c>
+      <c r="AA95">
+        <v>0.19</v>
+      </c>
+      <c r="AB95">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="96" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P96" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q96">
+        <v>0.05</v>
+      </c>
+      <c r="R96">
+        <v>0.13</v>
+      </c>
+      <c r="S96">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="T96">
+        <v>0.09</v>
+      </c>
+      <c r="U96">
+        <v>0.21</v>
+      </c>
+      <c r="V96">
+        <v>0.2</v>
+      </c>
+      <c r="W96">
+        <v>0.01</v>
+      </c>
+      <c r="X96">
+        <v>0.08</v>
+      </c>
+      <c r="Y96">
+        <v>0.13</v>
+      </c>
+      <c r="Z96">
+        <v>0.12</v>
+      </c>
+      <c r="AA96">
+        <v>0.16</v>
+      </c>
+      <c r="AB96">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P97" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q97">
+        <v>0.05</v>
+      </c>
+      <c r="R97">
+        <v>0.18</v>
+      </c>
+      <c r="S97">
+        <v>0.26</v>
+      </c>
+      <c r="T97">
+        <v>0.25</v>
+      </c>
+      <c r="U97">
+        <v>0.38383838383838398</v>
+      </c>
+      <c r="V97">
+        <v>0.38383838383838398</v>
+      </c>
+      <c r="W97">
+        <v>0.02</v>
+      </c>
+      <c r="X97">
+        <v>0.13</v>
+      </c>
+      <c r="Y97">
+        <v>0.19</v>
+      </c>
+      <c r="Z97">
+        <v>0.13</v>
+      </c>
+      <c r="AA97">
+        <v>0.26262626262626299</v>
+      </c>
+      <c r="AB97">
+        <v>0.25252525252525299</v>
+      </c>
+    </row>
+    <row r="98" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P98" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q98">
+        <v>0.02</v>
+      </c>
+      <c r="R98">
+        <v>0.12</v>
+      </c>
+      <c r="S98">
+        <v>0.26</v>
+      </c>
+      <c r="T98">
+        <v>0.24</v>
+      </c>
+      <c r="U98">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="V98">
+        <v>0.27</v>
+      </c>
+      <c r="W98">
+        <v>0.01</v>
+      </c>
+      <c r="X98">
+        <v>0.11</v>
+      </c>
+      <c r="Y98">
+        <v>0.22</v>
+      </c>
+      <c r="Z98">
+        <v>0.19</v>
+      </c>
+      <c r="AA98">
+        <v>0.23</v>
+      </c>
+      <c r="AB98">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="99" spans="1:29" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A99" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B99" t="s">
+        <v>137</v>
+      </c>
+      <c r="C99" t="s">
+        <v>151</v>
+      </c>
+      <c r="D99">
+        <v>1E-3</v>
+      </c>
+      <c r="E99" t="s">
+        <v>161</v>
+      </c>
+      <c r="F99" t="s">
+        <v>162</v>
+      </c>
+      <c r="G99" t="s">
+        <v>147</v>
+      </c>
+      <c r="H99" t="s">
+        <v>148</v>
+      </c>
+      <c r="I99" t="s">
+        <v>164</v>
+      </c>
+      <c r="J99" s="2">
+        <v>1</v>
+      </c>
+      <c r="K99" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L99" t="s">
+        <v>127</v>
+      </c>
+      <c r="M99" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N99" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O99" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P99" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q99">
+        <v>0.01</v>
+      </c>
+      <c r="R99">
+        <v>0.08</v>
+      </c>
+      <c r="S99">
+        <v>0.08</v>
+      </c>
+      <c r="T99">
+        <v>0.1</v>
+      </c>
+      <c r="U99">
+        <v>0.09</v>
+      </c>
+      <c r="V99">
+        <v>0.1</v>
+      </c>
+      <c r="W99">
+        <v>0.02</v>
+      </c>
+      <c r="X99">
+        <v>0.05</v>
+      </c>
+      <c r="Y99">
+        <v>0.04</v>
+      </c>
+      <c r="Z99">
+        <v>0.06</v>
+      </c>
+      <c r="AA99">
+        <v>0.02</v>
+      </c>
+      <c r="AB99">
+        <v>0.05</v>
+      </c>
+      <c r="AC99" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="100" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P100" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q100">
+        <v>0.01</v>
+      </c>
+      <c r="R100">
+        <v>0.1</v>
+      </c>
+      <c r="S100">
+        <v>0.11</v>
+      </c>
+      <c r="T100">
+        <v>0.15</v>
+      </c>
+      <c r="U100">
+        <v>0.11</v>
+      </c>
+      <c r="V100">
+        <v>0.13</v>
+      </c>
+      <c r="W100">
+        <v>0.02</v>
+      </c>
+      <c r="X100">
+        <v>0.03</v>
+      </c>
+      <c r="Y100">
+        <v>0.03</v>
+      </c>
+      <c r="Z100">
+        <v>0.05</v>
+      </c>
+      <c r="AA100">
+        <v>0.03</v>
+      </c>
+      <c r="AB100">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="101" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P101" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q101">
+        <v>0.04</v>
+      </c>
+      <c r="R101">
+        <v>0.12</v>
+      </c>
+      <c r="S101">
+        <v>0.12</v>
+      </c>
+      <c r="T101">
+        <v>0.13</v>
+      </c>
+      <c r="U101">
+        <v>0.12</v>
+      </c>
+      <c r="V101">
+        <v>0.12</v>
+      </c>
+      <c r="W101">
+        <v>0.03</v>
+      </c>
+      <c r="X101">
+        <v>0.05</v>
+      </c>
+      <c r="Y101">
+        <v>0.06</v>
+      </c>
+      <c r="Z101">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA101">
+        <v>0.04</v>
+      </c>
+      <c r="AB101">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P102" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q102">
+        <v>0.04</v>
+      </c>
+      <c r="R102">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S102">
+        <v>0.08</v>
+      </c>
+      <c r="T102">
+        <v>0.11</v>
+      </c>
+      <c r="U102">
+        <v>0.08</v>
+      </c>
+      <c r="V102">
+        <v>0.09</v>
+      </c>
+      <c r="W102">
+        <v>0.03</v>
+      </c>
+      <c r="X102">
+        <v>0.06</v>
+      </c>
+      <c r="Y102">
+        <v>0.06</v>
+      </c>
+      <c r="Z102">
+        <v>0.06</v>
+      </c>
+      <c r="AA102">
+        <v>0.06</v>
+      </c>
+      <c r="AB102">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="103" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P103" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q103">
+        <v>0.04</v>
+      </c>
+      <c r="R103">
+        <v>0.08</v>
+      </c>
+      <c r="S103">
+        <v>0.08</v>
+      </c>
+      <c r="T103">
+        <v>0.1</v>
+      </c>
+      <c r="U103">
+        <v>0.08</v>
+      </c>
+      <c r="V103">
+        <v>0.09</v>
+      </c>
+      <c r="W103">
+        <v>0.03</v>
+      </c>
+      <c r="X103">
+        <v>0.04</v>
+      </c>
+      <c r="Y103">
+        <v>0.04</v>
+      </c>
+      <c r="Z103">
+        <v>0.04</v>
+      </c>
+      <c r="AA103">
+        <v>0.04</v>
+      </c>
+      <c r="AB103">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="104" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P104" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q104">
+        <v>0.05</v>
+      </c>
+      <c r="R104">
+        <v>0.09</v>
+      </c>
+      <c r="S104">
+        <v>0.09</v>
+      </c>
+      <c r="T104">
+        <v>0.1</v>
+      </c>
+      <c r="U104">
+        <v>0.09</v>
+      </c>
+      <c r="V104">
+        <v>0.09</v>
+      </c>
+      <c r="W104">
+        <v>0.01</v>
+      </c>
+      <c r="X104">
+        <v>0.06</v>
+      </c>
+      <c r="Y104">
+        <v>0.06</v>
+      </c>
+      <c r="Z104">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA104">
+        <v>0.06</v>
+      </c>
+      <c r="AB104">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="105" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P105" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q105">
+        <v>0.06</v>
+      </c>
+      <c r="R105">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S105">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T105">
+        <v>0.11</v>
+      </c>
+      <c r="U105">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V105">
+        <v>0.1</v>
+      </c>
+      <c r="W105">
+        <v>0.02</v>
+      </c>
+      <c r="X105">
+        <v>0.05</v>
+      </c>
+      <c r="Y105">
+        <v>0.05</v>
+      </c>
+      <c r="Z105">
+        <v>0.06</v>
+      </c>
+      <c r="AA105">
+        <v>0.05</v>
+      </c>
+      <c r="AB105">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="106" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P106" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q106">
+        <v>7.5268817204301106E-2</v>
+      </c>
+      <c r="R106">
+        <v>0.10752688172043</v>
+      </c>
+      <c r="S106">
+        <v>0.10752688172043</v>
+      </c>
+      <c r="T106">
+        <v>0.12765957446808501</v>
+      </c>
+      <c r="U106">
+        <v>0.10752688172043</v>
+      </c>
+      <c r="V106">
+        <v>0.12765957446808501</v>
+      </c>
+      <c r="W106">
+        <v>5.4945054945054903E-2</v>
+      </c>
+      <c r="X106">
+        <v>6.4516129032258104E-2</v>
+      </c>
+      <c r="Y106">
+        <v>6.4516129032258104E-2</v>
+      </c>
+      <c r="Z106">
+        <v>7.4468085106383003E-2</v>
+      </c>
+      <c r="AA106">
+        <v>6.4516129032258104E-2</v>
+      </c>
+      <c r="AB106">
+        <v>9.5744680851063801E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P107" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q107">
+        <v>0.04</v>
+      </c>
+      <c r="R107">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S107">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T107">
+        <v>0.1</v>
+      </c>
+      <c r="U107">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V107">
+        <v>0.08</v>
+      </c>
+      <c r="W107">
+        <v>0.02</v>
+      </c>
+      <c r="X107">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y107">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z107">
+        <v>0.1</v>
+      </c>
+      <c r="AA107">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB107">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="108" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P108" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q108">
+        <v>0.05</v>
+      </c>
+      <c r="R108">
+        <v>0.15</v>
+      </c>
+      <c r="S108">
+        <v>0.15</v>
+      </c>
+      <c r="T108">
+        <v>0.17</v>
+      </c>
+      <c r="U108">
+        <v>0.15</v>
+      </c>
+      <c r="V108">
+        <v>0.16</v>
+      </c>
+      <c r="W108">
+        <v>0.04</v>
+      </c>
+      <c r="X108">
+        <v>0.09</v>
+      </c>
+      <c r="Y108">
+        <v>0.08</v>
+      </c>
+      <c r="Z108">
+        <v>0.11</v>
+      </c>
+      <c r="AA108">
+        <v>0.09</v>
+      </c>
+      <c r="AB108">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P109" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q109">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R109">
+        <v>0.08</v>
+      </c>
+      <c r="S109">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T109">
+        <v>0.1</v>
+      </c>
+      <c r="U109">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V109">
+        <v>0.1</v>
+      </c>
+      <c r="W109">
+        <v>0.03</v>
+      </c>
+      <c r="X109">
+        <v>0.03</v>
+      </c>
+      <c r="Y109">
+        <v>0.03</v>
+      </c>
+      <c r="Z109">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA109">
+        <v>0.03</v>
+      </c>
+      <c r="AB109">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="110" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P110" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q110">
+        <v>0.06</v>
+      </c>
+      <c r="R110">
+        <v>0.11</v>
+      </c>
+      <c r="S110">
+        <v>0.11</v>
+      </c>
+      <c r="T110">
+        <v>0.13</v>
+      </c>
+      <c r="U110">
+        <v>0.11</v>
+      </c>
+      <c r="V110">
+        <v>0.12</v>
+      </c>
+      <c r="W110">
+        <v>0.05</v>
+      </c>
+      <c r="X110">
+        <v>0.09</v>
+      </c>
+      <c r="Y110">
+        <v>0.09</v>
+      </c>
+      <c r="Z110">
+        <v>0.1</v>
+      </c>
+      <c r="AA110">
+        <v>0.1</v>
+      </c>
+      <c r="AB110">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:29" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A111" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B111" t="s">
+        <v>137</v>
+      </c>
+      <c r="C111" t="s">
+        <v>151</v>
+      </c>
+      <c r="D111">
+        <v>1E-3</v>
+      </c>
+      <c r="E111" t="s">
+        <v>163</v>
+      </c>
+      <c r="F111" t="s">
+        <v>162</v>
+      </c>
+      <c r="G111" t="s">
+        <v>147</v>
+      </c>
+      <c r="H111" t="s">
+        <v>148</v>
+      </c>
+      <c r="I111" t="s">
+        <v>164</v>
+      </c>
+      <c r="J111" s="2">
+        <v>1</v>
+      </c>
+      <c r="K111" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L111" t="s">
+        <v>127</v>
+      </c>
+      <c r="M111" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N111" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O111" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P111" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q111">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R111">
+        <v>0.12</v>
+      </c>
+      <c r="S111">
+        <v>0.08</v>
+      </c>
+      <c r="T111">
+        <v>0.08</v>
+      </c>
+      <c r="U111">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V111">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W111">
+        <v>0.03</v>
+      </c>
+      <c r="X111">
+        <v>0.06</v>
+      </c>
+      <c r="Y111">
+        <v>0.04</v>
+      </c>
+      <c r="Z111">
+        <v>0.05</v>
+      </c>
+      <c r="AA111">
+        <v>0.09</v>
+      </c>
+      <c r="AB111">
+        <v>0.1</v>
+      </c>
+      <c r="AC111" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="112" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P112" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q112">
+        <v>0.04</v>
+      </c>
+      <c r="R112">
+        <v>0.12</v>
+      </c>
+      <c r="S112">
+        <v>0.1</v>
+      </c>
+      <c r="T112">
+        <v>0.1</v>
+      </c>
+      <c r="U112">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V112">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W112">
+        <v>0.04</v>
+      </c>
+      <c r="X112">
+        <v>0.13</v>
+      </c>
+      <c r="Y112">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z112">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA112">
+        <v>0.11</v>
+      </c>
+      <c r="AB112">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P113" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q113">
+        <v>0.03</v>
+      </c>
+      <c r="R113">
+        <v>0.2</v>
+      </c>
+      <c r="S113">
+        <v>0.12</v>
+      </c>
+      <c r="T113">
+        <v>0.11</v>
+      </c>
+      <c r="U113">
+        <v>0.21</v>
+      </c>
+      <c r="V113">
+        <v>0.21</v>
+      </c>
+      <c r="W113">
+        <v>0.02</v>
+      </c>
+      <c r="X113">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Y113">
+        <v>0.03</v>
+      </c>
+      <c r="Z113">
+        <v>0.04</v>
+      </c>
+      <c r="AA113">
+        <v>0.15</v>
+      </c>
+      <c r="AB113">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="114" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P114" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q114">
+        <v>0.05</v>
+      </c>
+      <c r="R114">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S114">
+        <v>0.08</v>
+      </c>
+      <c r="T114">
+        <v>0.09</v>
+      </c>
+      <c r="U114">
+        <v>0.16</v>
+      </c>
+      <c r="V114">
+        <v>0.16</v>
+      </c>
+      <c r="W114">
+        <v>0.02</v>
+      </c>
+      <c r="X114">
+        <v>0.12</v>
+      </c>
+      <c r="Y114">
+        <v>0.06</v>
+      </c>
+      <c r="Z114">
+        <v>0.06</v>
+      </c>
+      <c r="AA114">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AB114">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P115" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q115">
+        <v>0.03</v>
+      </c>
+      <c r="R115">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S115">
+        <v>0.08</v>
+      </c>
+      <c r="T115">
+        <v>0.09</v>
+      </c>
+      <c r="U115">
+        <v>0.13</v>
+      </c>
+      <c r="V115">
+        <v>0.13</v>
+      </c>
+      <c r="W115">
+        <v>0.01</v>
+      </c>
+      <c r="X115">
+        <v>0.08</v>
+      </c>
+      <c r="Y115">
+        <v>0.05</v>
+      </c>
+      <c r="Z115">
+        <v>0.05</v>
+      </c>
+      <c r="AA115">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AB115">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P116" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q116">
+        <v>0.06</v>
+      </c>
+      <c r="R116">
+        <v>0.19</v>
+      </c>
+      <c r="S116">
+        <v>0.1</v>
+      </c>
+      <c r="T116">
+        <v>0.1</v>
+      </c>
+      <c r="U116">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V116">
+        <v>0.13</v>
+      </c>
+      <c r="W116">
+        <v>0.04</v>
+      </c>
+      <c r="X116">
+        <v>0.12</v>
+      </c>
+      <c r="Y116">
+        <v>0.08</v>
+      </c>
+      <c r="Z116">
+        <v>0.08</v>
+      </c>
+      <c r="AA116">
+        <v>0.11</v>
+      </c>
+      <c r="AB116">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="117" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P117" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q117">
+        <v>0.06</v>
+      </c>
+      <c r="R117">
+        <v>0.1</v>
+      </c>
+      <c r="S117">
+        <v>0.06</v>
+      </c>
+      <c r="T117">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U117">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V117">
+        <v>0.13</v>
+      </c>
+      <c r="W117">
+        <v>0.01</v>
+      </c>
+      <c r="X117">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y117">
+        <v>0.05</v>
+      </c>
+      <c r="Z117">
+        <v>0.05</v>
+      </c>
+      <c r="AA117">
+        <v>0.09</v>
+      </c>
+      <c r="AB117">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P118" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q118">
+        <v>0.08</v>
+      </c>
+      <c r="R118">
+        <v>0.18279569892473099</v>
+      </c>
+      <c r="S118">
+        <v>8.7912087912087905E-2</v>
+      </c>
+      <c r="T118">
+        <v>9.8901098901098897E-2</v>
+      </c>
+      <c r="U118">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="V118">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="W118">
+        <v>2.8571428571428598E-2</v>
+      </c>
+      <c r="X118">
+        <v>0.13186813186813201</v>
+      </c>
+      <c r="Y118">
+        <v>6.6666666666666693E-2</v>
+      </c>
+      <c r="Z118">
+        <v>6.6666666666666693E-2</v>
+      </c>
+      <c r="AA118">
+        <v>8.2191780821917804E-2</v>
+      </c>
+      <c r="AB118">
+        <v>6.8493150684931503E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P119" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q119">
+        <v>0.04</v>
+      </c>
+      <c r="R119">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S119">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T119">
+        <v>0.08</v>
+      </c>
+      <c r="U119">
+        <v>0.13</v>
+      </c>
+      <c r="V119">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W119">
+        <v>0.03</v>
+      </c>
+      <c r="X119">
+        <v>0.16</v>
+      </c>
+      <c r="Y119">
+        <v>0.09</v>
+      </c>
+      <c r="Z119">
+        <v>0.09</v>
+      </c>
+      <c r="AA119">
+        <v>0.11</v>
+      </c>
+      <c r="AB119">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="120" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P120" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q120">
+        <v>0.05</v>
+      </c>
+      <c r="R120">
+        <v>0.1</v>
+      </c>
+      <c r="S120">
+        <v>0.03</v>
+      </c>
+      <c r="T120">
+        <v>0.04</v>
+      </c>
+      <c r="U120">
+        <v>0.08</v>
+      </c>
+      <c r="V120">
+        <v>0.09</v>
+      </c>
+      <c r="W120">
+        <v>0.03</v>
+      </c>
+      <c r="X120">
+        <v>0.09</v>
+      </c>
+      <c r="Y120">
+        <v>0.02</v>
+      </c>
+      <c r="Z120">
+        <v>0.03</v>
+      </c>
+      <c r="AA120">
+        <v>0.06</v>
+      </c>
+      <c r="AB120">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="121" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P121" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q121">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R121">
+        <v>0.21</v>
+      </c>
+      <c r="S121">
+        <v>0.05</v>
+      </c>
+      <c r="T121">
+        <v>0.06</v>
+      </c>
+      <c r="U121">
+        <v>0.10101010101010099</v>
+      </c>
+      <c r="V121">
+        <v>0.10101010101010099</v>
+      </c>
+      <c r="W121">
+        <v>0.04</v>
+      </c>
+      <c r="X121">
+        <v>0.15</v>
+      </c>
+      <c r="Y121">
+        <v>0.05</v>
+      </c>
+      <c r="Z121">
+        <v>0.04</v>
+      </c>
+      <c r="AA121">
+        <v>9.0909090909090898E-2</v>
+      </c>
+      <c r="AB121">
+        <v>9.0909090909090898E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P122" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q122">
+        <v>0.03</v>
+      </c>
+      <c r="R122">
+        <v>0.12</v>
+      </c>
+      <c r="S122">
+        <v>0.12</v>
+      </c>
+      <c r="T122">
+        <v>0.13</v>
+      </c>
+      <c r="U122">
+        <v>0.2</v>
+      </c>
+      <c r="V122">
+        <v>0.2</v>
+      </c>
+      <c r="W122">
+        <v>0.03</v>
+      </c>
+      <c r="X122">
+        <v>0.09</v>
+      </c>
+      <c r="Y122">
+        <v>0.08</v>
+      </c>
+      <c r="Z122">
+        <v>0.09</v>
+      </c>
+      <c r="AA122">
+        <v>0.13</v>
+      </c>
+      <c r="AB122">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="123" spans="1:29" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A123" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B123" t="s">
+        <v>137</v>
+      </c>
+      <c r="C123" t="s">
+        <v>151</v>
+      </c>
+      <c r="D123">
+        <v>1E-3</v>
+      </c>
+      <c r="E123" t="s">
+        <v>161</v>
+      </c>
+      <c r="F123" t="s">
+        <v>162</v>
+      </c>
+      <c r="G123" t="s">
+        <v>147</v>
+      </c>
+      <c r="H123" t="s">
+        <v>148</v>
+      </c>
+      <c r="I123" t="s">
+        <v>148</v>
+      </c>
+      <c r="J123" s="2">
+        <v>1</v>
+      </c>
+      <c r="K123" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L123" t="s">
+        <v>127</v>
+      </c>
+      <c r="M123" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N123" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O123" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P123" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q123">
+        <v>0.04</v>
+      </c>
+      <c r="R123">
+        <v>0.06</v>
+      </c>
+      <c r="S123">
+        <v>0.06</v>
+      </c>
+      <c r="T123">
+        <v>0.11</v>
+      </c>
+      <c r="U123">
+        <v>0.06</v>
+      </c>
+      <c r="V123">
+        <v>0.11</v>
+      </c>
+      <c r="W123">
+        <v>0.03</v>
+      </c>
+      <c r="X123">
+        <v>0.09</v>
+      </c>
+      <c r="Y123">
+        <v>0.09</v>
+      </c>
+      <c r="Z123">
+        <v>0.11</v>
+      </c>
+      <c r="AA123">
+        <v>0.09</v>
+      </c>
+      <c r="AB123">
+        <v>0.11</v>
+      </c>
+      <c r="AC123" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="124" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P124" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q124">
+        <v>0.03</v>
+      </c>
+      <c r="R124">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S124">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T124">
+        <v>0.09</v>
+      </c>
+      <c r="U124">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V124">
+        <v>0.09</v>
+      </c>
+      <c r="W124">
+        <v>0.02</v>
+      </c>
+      <c r="X124">
+        <v>0.03</v>
+      </c>
+      <c r="Y124">
+        <v>0.03</v>
+      </c>
+      <c r="Z124">
+        <v>0.04</v>
+      </c>
+      <c r="AA124">
+        <v>0.03</v>
+      </c>
+      <c r="AB124">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="125" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P125" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q125">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R125">
+        <v>0.08</v>
+      </c>
+      <c r="S125">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T125">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U125">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V125">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W125">
+        <v>0.06</v>
+      </c>
+      <c r="X125">
+        <v>0.05</v>
+      </c>
+      <c r="Y125">
+        <v>0.04</v>
+      </c>
+      <c r="Z125">
+        <v>0.06</v>
+      </c>
+      <c r="AA125">
+        <v>0.05</v>
+      </c>
+      <c r="AB125">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="126" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P126" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q126">
+        <v>0.03</v>
+      </c>
+      <c r="R126">
+        <v>0.1</v>
+      </c>
+      <c r="S126">
+        <v>0.1</v>
+      </c>
+      <c r="T126">
+        <v>0.15</v>
+      </c>
+      <c r="U126">
+        <v>0.1</v>
+      </c>
+      <c r="V126">
+        <v>0.15</v>
+      </c>
+      <c r="W126">
+        <v>0.01</v>
+      </c>
+      <c r="X126">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y126">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z126">
+        <v>0.09</v>
+      </c>
+      <c r="AA126">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB126">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="127" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P127" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q127">
+        <v>0.02</v>
+      </c>
+      <c r="R127">
+        <v>0.09</v>
+      </c>
+      <c r="S127">
+        <v>0.09</v>
+      </c>
+      <c r="T127">
+        <v>0.15</v>
+      </c>
+      <c r="U127">
+        <v>0.09</v>
+      </c>
+      <c r="V127">
+        <v>0.13</v>
+      </c>
+      <c r="W127">
+        <v>0</v>
+      </c>
+      <c r="X127">
+        <v>0.03</v>
+      </c>
+      <c r="Y127">
+        <v>0.03</v>
+      </c>
+      <c r="Z127">
+        <v>0.09</v>
+      </c>
+      <c r="AA127">
+        <v>0.03</v>
+      </c>
+      <c r="AB127">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P128" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q128">
+        <v>0.03</v>
+      </c>
+      <c r="R128">
+        <v>0.11</v>
+      </c>
+      <c r="S128">
+        <v>0.11</v>
+      </c>
+      <c r="T128">
+        <v>0.16</v>
+      </c>
+      <c r="U128">
+        <v>0.11</v>
+      </c>
+      <c r="V128">
+        <v>0.16</v>
+      </c>
+      <c r="W128">
+        <v>0.02</v>
+      </c>
+      <c r="X128">
+        <v>0.09</v>
+      </c>
+      <c r="Y128">
+        <v>0.1</v>
+      </c>
+      <c r="Z128">
+        <v>0.11</v>
+      </c>
+      <c r="AA128">
+        <v>0.09</v>
+      </c>
+      <c r="AB128">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="129" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P129" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q129">
+        <v>0.03</v>
+      </c>
+      <c r="R129">
+        <v>0.1</v>
+      </c>
+      <c r="S129">
+        <v>0.1</v>
+      </c>
+      <c r="T129">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U129">
+        <v>0.1</v>
+      </c>
+      <c r="V129">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W129">
+        <v>0.01</v>
+      </c>
+      <c r="X129">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y129">
+        <v>0.06</v>
+      </c>
+      <c r="Z129">
+        <v>0.08</v>
+      </c>
+      <c r="AA129">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB129">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P130" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q130">
+        <v>4.3478260869565202E-2</v>
+      </c>
+      <c r="R130">
+        <v>0.102040816326531</v>
+      </c>
+      <c r="S130">
+        <v>0.102040816326531</v>
+      </c>
+      <c r="T130">
+        <v>0.12121212121212099</v>
+      </c>
+      <c r="U130">
+        <v>0.102040816326531</v>
+      </c>
+      <c r="V130">
+        <v>0.13131313131313099</v>
+      </c>
+      <c r="W130">
+        <v>3.2967032967033003E-2</v>
+      </c>
+      <c r="X130">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Y130">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Z130">
+        <v>7.0707070707070704E-2</v>
+      </c>
+      <c r="AA130">
+        <v>6.25E-2</v>
+      </c>
+      <c r="AB130">
+        <v>7.0707070707070704E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P131" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q131">
+        <v>0.09</v>
+      </c>
+      <c r="R131">
+        <v>0.11</v>
+      </c>
+      <c r="S131">
+        <v>0.11</v>
+      </c>
+      <c r="T131">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U131">
+        <v>0.13</v>
+      </c>
+      <c r="V131">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W131">
+        <v>0.03</v>
+      </c>
+      <c r="X131">
+        <v>0.08</v>
+      </c>
+      <c r="Y131">
+        <v>0.08</v>
+      </c>
+      <c r="Z131">
+        <v>0.12</v>
+      </c>
+      <c r="AA131">
+        <v>0.08</v>
+      </c>
+      <c r="AB131">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="132" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P132" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q132">
+        <v>0.03</v>
+      </c>
+      <c r="R132">
+        <v>0.11</v>
+      </c>
+      <c r="S132">
+        <v>0.11</v>
+      </c>
+      <c r="T132">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U132">
+        <v>0.11</v>
+      </c>
+      <c r="V132">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W132">
+        <v>0.04</v>
+      </c>
+      <c r="X132">
+        <v>0.08</v>
+      </c>
+      <c r="Y132">
+        <v>0.08</v>
+      </c>
+      <c r="Z132">
+        <v>0.1</v>
+      </c>
+      <c r="AA132">
+        <v>0.09</v>
+      </c>
+      <c r="AB132">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="133" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P133" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q133">
+        <v>0.01</v>
+      </c>
+      <c r="R133">
+        <v>0.08</v>
+      </c>
+      <c r="S133">
+        <v>0.08</v>
+      </c>
+      <c r="T133">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U133">
+        <v>0.09</v>
+      </c>
+      <c r="V133">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W133">
+        <v>0.02</v>
+      </c>
+      <c r="X133">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y133">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z133">
+        <v>0.08</v>
+      </c>
+      <c r="AA133">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB133">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="134" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P134" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q134">
+        <v>0.05</v>
+      </c>
+      <c r="R134">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S134">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="T134">
+        <v>0.19</v>
+      </c>
+      <c r="U134">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V134">
+        <v>0.19</v>
+      </c>
+      <c r="W134">
+        <v>0.05</v>
+      </c>
+      <c r="X134">
+        <v>0.08</v>
+      </c>
+      <c r="Y134">
+        <v>0.08</v>
+      </c>
+      <c r="Z134">
+        <v>0.12</v>
+      </c>
+      <c r="AA134">
+        <v>0.08</v>
+      </c>
+      <c r="AB134">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="135" spans="1:29" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A135" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B135" t="s">
+        <v>137</v>
+      </c>
+      <c r="C135" t="s">
+        <v>151</v>
+      </c>
+      <c r="D135">
+        <v>1E-3</v>
+      </c>
+      <c r="E135" t="s">
+        <v>163</v>
+      </c>
+      <c r="F135" t="s">
+        <v>162</v>
+      </c>
+      <c r="G135" t="s">
+        <v>147</v>
+      </c>
+      <c r="H135" t="s">
+        <v>148</v>
+      </c>
+      <c r="I135" t="s">
+        <v>148</v>
+      </c>
+      <c r="J135" s="2">
+        <v>1</v>
+      </c>
+      <c r="K135" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L135" t="s">
+        <v>127</v>
+      </c>
+      <c r="M135" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N135" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O135" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P135" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q135">
+        <v>0.06</v>
+      </c>
+      <c r="R135">
+        <v>0.12</v>
+      </c>
+      <c r="S135">
+        <v>0.08</v>
+      </c>
+      <c r="T135">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U135">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V135">
+        <v>0.08</v>
+      </c>
+      <c r="W135">
+        <v>0.04</v>
+      </c>
+      <c r="X135">
+        <v>0.13</v>
+      </c>
+      <c r="Y135">
+        <v>0.04</v>
+      </c>
+      <c r="Z135">
+        <v>0.06</v>
+      </c>
+      <c r="AA135">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB135">
+        <v>0.09</v>
+      </c>
+      <c r="AC135" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="136" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P136" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q136">
+        <v>0.02</v>
+      </c>
+      <c r="R136">
+        <v>0.17</v>
+      </c>
+      <c r="S136">
+        <v>0.03</v>
+      </c>
+      <c r="T136">
+        <v>0.05</v>
+      </c>
+      <c r="U136">
+        <v>0.03</v>
+      </c>
+      <c r="V136">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W136">
+        <v>0.01</v>
+      </c>
+      <c r="X136">
+        <v>0.13</v>
+      </c>
+      <c r="Y136">
+        <v>0.04</v>
+      </c>
+      <c r="Z136">
+        <v>0.03</v>
+      </c>
+      <c r="AA136">
+        <v>0.02</v>
+      </c>
+      <c r="AB136">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="137" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P137" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q137">
+        <v>0.04</v>
+      </c>
+      <c r="R137">
+        <v>0.16</v>
+      </c>
+      <c r="S137">
+        <v>0.04</v>
+      </c>
+      <c r="T137">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U137">
+        <v>0.18</v>
+      </c>
+      <c r="V137">
+        <v>0.23</v>
+      </c>
+      <c r="W137">
+        <v>0.05</v>
+      </c>
+      <c r="X137">
+        <v>0.12</v>
+      </c>
+      <c r="Y137">
+        <v>0.04</v>
+      </c>
+      <c r="Z137">
+        <v>0.03</v>
+      </c>
+      <c r="AA137">
+        <v>0.1</v>
+      </c>
+      <c r="AB137">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="138" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P138" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q138">
+        <v>0.06</v>
+      </c>
+      <c r="R138">
+        <v>0.16</v>
+      </c>
+      <c r="S138">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T138">
+        <v>0.11</v>
+      </c>
+      <c r="U138">
+        <v>0.08</v>
+      </c>
+      <c r="V138">
+        <v>0.11</v>
+      </c>
+      <c r="W138">
+        <v>0.05</v>
+      </c>
+      <c r="X138">
+        <v>0.08</v>
+      </c>
+      <c r="Y138">
+        <v>0.03</v>
+      </c>
+      <c r="Z138">
+        <v>0.05</v>
+      </c>
+      <c r="AA138">
+        <v>0.03</v>
+      </c>
+      <c r="AB138">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="139" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P139" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q139">
+        <v>0.08</v>
+      </c>
+      <c r="R139">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S139">
+        <v>0.04</v>
+      </c>
+      <c r="T139">
+        <v>0.03</v>
+      </c>
+      <c r="U139">
+        <v>0.06</v>
+      </c>
+      <c r="V139">
+        <v>0.08</v>
+      </c>
+      <c r="W139">
+        <v>0.04</v>
+      </c>
+      <c r="X139">
+        <v>0.1</v>
+      </c>
+      <c r="Y139">
+        <v>0.01</v>
+      </c>
+      <c r="Z139">
+        <v>0.03</v>
+      </c>
+      <c r="AA139">
+        <v>0.05</v>
+      </c>
+      <c r="AB139">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="140" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P140" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q140">
+        <v>0.02</v>
+      </c>
+      <c r="R140">
+        <v>0.09</v>
+      </c>
+      <c r="S140">
+        <v>0.04</v>
+      </c>
+      <c r="T140">
+        <v>0.04</v>
+      </c>
+      <c r="U140">
+        <v>0.09</v>
+      </c>
+      <c r="V140">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="W140">
+        <v>0.01</v>
+      </c>
+      <c r="X140">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y140">
+        <v>0.03</v>
+      </c>
+      <c r="Z140">
+        <v>0.03</v>
+      </c>
+      <c r="AA140">
+        <v>0.08</v>
+      </c>
+      <c r="AB140">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P141" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q141">
+        <v>0.03</v>
+      </c>
+      <c r="R141">
+        <v>0.17</v>
+      </c>
+      <c r="S141">
+        <v>0.1</v>
+      </c>
+      <c r="T141">
+        <v>0.13</v>
+      </c>
+      <c r="U141">
+        <v>0.16</v>
+      </c>
+      <c r="V141">
+        <v>0.19</v>
+      </c>
+      <c r="W141">
+        <v>0.01</v>
+      </c>
+      <c r="X141">
+        <v>0.13</v>
+      </c>
+      <c r="Y141">
+        <v>0.1</v>
+      </c>
+      <c r="Z141">
+        <v>0.1</v>
+      </c>
+      <c r="AA141">
+        <v>0.06</v>
+      </c>
+      <c r="AB141">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="142" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P142" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q142">
+        <v>1.35135135135135E-2</v>
+      </c>
+      <c r="R142">
+        <v>0.10752688172043</v>
+      </c>
+      <c r="S142">
+        <v>5.7471264367816098E-2</v>
+      </c>
+      <c r="T142">
+        <v>9.375E-2</v>
+      </c>
+      <c r="U142">
+        <v>7.0588235294117604E-2</v>
+      </c>
+      <c r="V142">
+        <v>0.10989010989011</v>
+      </c>
+      <c r="W142">
+        <v>1.4285714285714299E-2</v>
+      </c>
+      <c r="X142">
+        <v>7.5268817204301106E-2</v>
+      </c>
+      <c r="Y142">
+        <v>2.2988505747126398E-2</v>
+      </c>
+      <c r="Z142">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="AA142">
+        <v>4.7619047619047603E-2</v>
+      </c>
+      <c r="AB142">
+        <v>8.7912087912087905E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P143" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q143">
+        <v>0</v>
+      </c>
+      <c r="R143">
+        <v>0.1</v>
+      </c>
+      <c r="S143">
+        <v>0.02</v>
+      </c>
+      <c r="T143">
+        <v>0.03</v>
+      </c>
+      <c r="U143">
+        <v>0.02</v>
+      </c>
+      <c r="V143">
+        <v>0.06</v>
+      </c>
+      <c r="W143">
+        <v>0.01</v>
+      </c>
+      <c r="X143">
+        <v>0.09</v>
+      </c>
+      <c r="Y143">
+        <v>0.03</v>
+      </c>
+      <c r="Z143">
+        <v>0.03</v>
+      </c>
+      <c r="AA143">
+        <v>0.05</v>
+      </c>
+      <c r="AB143">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="144" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="P144" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q144">
+        <v>0.06</v>
+      </c>
+      <c r="R144">
+        <v>0.17</v>
+      </c>
+      <c r="S144">
+        <v>0.06</v>
+      </c>
+      <c r="T144">
+        <v>0.09</v>
+      </c>
+      <c r="U144">
+        <v>0.12</v>
+      </c>
+      <c r="V144">
+        <v>0.13</v>
+      </c>
+      <c r="W144">
+        <v>0.04</v>
+      </c>
+      <c r="X144">
+        <v>0.12</v>
+      </c>
+      <c r="Y144">
+        <v>0.06</v>
+      </c>
+      <c r="Z144">
+        <v>0.09</v>
+      </c>
+      <c r="AA144">
+        <v>0.1</v>
+      </c>
+      <c r="AB144">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="145" spans="16:28" x14ac:dyDescent="0.3">
+      <c r="P145" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q145">
+        <v>6.0606060606060601E-2</v>
+      </c>
+      <c r="R145">
+        <v>0.16</v>
+      </c>
+      <c r="S145">
+        <v>0.04</v>
+      </c>
+      <c r="T145">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U145">
+        <v>0.04</v>
+      </c>
+      <c r="V145">
+        <v>0.06</v>
+      </c>
+      <c r="W145">
+        <v>2.02020202020202E-2</v>
+      </c>
+      <c r="X145">
+        <v>0.1</v>
+      </c>
+      <c r="Y145">
+        <v>0.05</v>
+      </c>
+      <c r="Z145">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA145">
+        <v>0.03</v>
+      </c>
+      <c r="AB145">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="146" spans="16:28" x14ac:dyDescent="0.3">
+      <c r="P146" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q146">
+        <v>0.02</v>
+      </c>
+      <c r="R146">
+        <v>0.15</v>
+      </c>
+      <c r="S146">
+        <v>0.02</v>
+      </c>
+      <c r="T146">
+        <v>0.02</v>
+      </c>
+      <c r="U146">
+        <v>0.02</v>
+      </c>
+      <c r="V146">
+        <v>0.04</v>
+      </c>
+      <c r="W146">
+        <v>0.03</v>
+      </c>
+      <c r="X146">
+        <v>0.12</v>
+      </c>
+      <c r="Y146">
+        <v>0.03</v>
+      </c>
+      <c r="Z146">
+        <v>0.03</v>
+      </c>
+      <c r="AA146">
+        <v>0.03</v>
+      </c>
+      <c r="AB146">
         <v>0.04</v>
       </c>
     </row>

</xml_diff>